<commit_message>
Update JTOUSDT.json at 2024-09-30_16-37-36 bestfile_scores 0.002569582091560346 bestfile_sharp 0.21442701301531394
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="388">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -745,7 +745,7 @@
     <t>HNTUSDT</t>
   </si>
   <si>
-    <t>RENUSDT</t>
+    <t>DOGSUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1539,7 +1539,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU158"/>
+  <dimension ref="A1:CU146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -41590,169 +41590,169 @@
     </row>
     <row r="146" spans="10:99">
       <c r="J146" t="s">
-        <v>220</v>
+        <v>243</v>
       </c>
       <c r="K146">
-        <v>0.001476797697630428</v>
+        <v>0.008132907461073646</v>
       </c>
       <c r="L146">
-        <v>0.001476797697630428</v>
+        <v>0.008132907461073646</v>
       </c>
       <c r="M146">
-        <v>0.0006849787689617859</v>
+        <v>0.01470591882488992</v>
       </c>
       <c r="N146">
-        <v>0.0006849787689617859</v>
+        <v>0.01470591882488992</v>
       </c>
       <c r="O146">
-        <v>0.001132997748242803</v>
+        <v>0.01014692122048955</v>
       </c>
       <c r="P146">
-        <v>0.001132997748242803</v>
+        <v>0.01014692122048955</v>
       </c>
       <c r="Q146">
-        <v>0.0005858347096432626</v>
+        <v>0.01885597483453796</v>
       </c>
       <c r="R146">
-        <v>0.0005858347096432626</v>
+        <v>0.01885597483453796</v>
       </c>
       <c r="S146">
-        <v>11.22947894165205</v>
+        <v>6.438930067676441</v>
       </c>
       <c r="T146">
-        <v>5.941297336119808</v>
+        <v>48.08894618111505</v>
       </c>
       <c r="U146">
-        <v>0.989858202712437</v>
+        <v>0.999954001314926</v>
       </c>
       <c r="V146">
-        <v>0.7558922324765516</v>
+        <v>0.7899217884646401</v>
       </c>
       <c r="W146">
-        <v>0.09997637553531981</v>
+        <v>0.09362078117437235</v>
       </c>
       <c r="X146">
-        <v>0.0483292150191479</v>
+        <v>0.07718550642633364</v>
       </c>
       <c r="Y146">
-        <v>0.1998439776979348</v>
+        <v>0.1047847908401863</v>
       </c>
       <c r="Z146">
-        <v>0.1391639567656968</v>
+        <v>0.1177025551717131</v>
       </c>
       <c r="AA146">
-        <v>0.9984384873723651</v>
+        <v>0.9926316906383604</v>
       </c>
       <c r="AB146">
-        <v>0.8346951337665619</v>
+        <v>0.9193818057349388</v>
       </c>
       <c r="AC146">
-        <v>0.8972558791436146</v>
+        <v>0.9254028897944</v>
       </c>
       <c r="AD146">
-        <v>0.9988806859624895</v>
+        <v>0.9930630996665251</v>
       </c>
       <c r="AE146">
-        <v>0.8075997036392804</v>
+        <v>0.9051921112722948</v>
       </c>
       <c r="AF146">
-        <v>0.8609900598165279</v>
+        <v>0.8826429282397099</v>
       </c>
       <c r="AG146">
-        <v>0.009664363916657152</v>
+        <v>0.01607406978542908</v>
       </c>
       <c r="AH146">
-        <v>0.005378217302631533</v>
+        <v>0.01422843894993598</v>
       </c>
       <c r="AI146">
-        <v>0.9984384873723651</v>
+        <v>0.9926316906383604</v>
       </c>
       <c r="AJ146">
-        <v>0.9988806859624895</v>
+        <v>0.9930630996665251</v>
       </c>
       <c r="AK146">
-        <v>0.009664363916657152</v>
+        <v>0.01607406978542908</v>
       </c>
       <c r="AL146">
-        <v>0.005378217302631533</v>
+        <v>0.01422843894993598</v>
       </c>
       <c r="AM146" t="s">
         <v>244</v>
       </c>
       <c r="AN146">
-        <v>0.06761023312432207</v>
+        <v>0.3570285831928028</v>
       </c>
       <c r="AO146">
-        <v>0.04804155310831611</v>
+        <v>0.3842735807398202</v>
       </c>
       <c r="AP146">
-        <v>-1460.205405172</v>
+        <v>-37.04018483751999</v>
       </c>
       <c r="AQ146">
-        <v>-694.167403444</v>
+        <v>-311.74666843072</v>
       </c>
       <c r="AR146">
-        <v>64645.83203412539</v>
+        <v>13221.64899875173</v>
       </c>
       <c r="AS146">
-        <v>23773.84285655582</v>
+        <v>16542.29599256928</v>
       </c>
       <c r="AT146">
-        <v>61213.41891482817</v>
+        <v>13188.75076696247</v>
       </c>
       <c r="AU146">
-        <v>23773.84285655582</v>
+        <v>16537.67084536928</v>
       </c>
       <c r="AV146">
-        <v>5.464583203412539</v>
+        <v>0.3221648998751732</v>
       </c>
       <c r="AW146">
-        <v>1.377384285655582</v>
+        <v>0.654229599256928</v>
       </c>
       <c r="AX146">
-        <v>2.137193390136845</v>
+        <v>3.741704374057315</v>
       </c>
       <c r="AY146">
-        <v>4.039700075424819</v>
+        <v>0.4990545161939248</v>
       </c>
       <c r="AZ146">
-        <v>90.46666666666667</v>
+        <v>21.25</v>
       </c>
       <c r="BA146">
-        <v>92.91666666666667</v>
+        <v>20.85</v>
       </c>
       <c r="BB146">
-        <v>0.08627842267587477</v>
+        <v>0.01786524646848583</v>
       </c>
       <c r="BC146">
-        <v>0.07559359687889899</v>
+        <v>0.01292401837150051</v>
       </c>
       <c r="BD146">
-        <v>-5297.82871827594</v>
+        <v>-59.27627061324936</v>
       </c>
       <c r="BE146">
-        <v>-1183.125659386996</v>
+        <v>-89.74159529610705</v>
       </c>
       <c r="BF146">
-        <v>5088</v>
+        <v>133</v>
       </c>
       <c r="BG146">
-        <v>3243</v>
+        <v>620</v>
       </c>
       <c r="BH146">
-        <v>1264.706944444444</v>
+        <v>34.47777777777778</v>
       </c>
       <c r="BI146">
-        <v>9114</v>
+        <v>89</v>
       </c>
       <c r="BJ146">
-        <v>4271</v>
+        <v>1038</v>
       </c>
       <c r="BK146">
-        <v>14202</v>
+        <v>222</v>
       </c>
       <c r="BL146">
-        <v>7514</v>
+        <v>1658</v>
       </c>
       <c r="BM146">
         <v>0</v>
@@ -41761,10 +41761,10 @@
         <v>0</v>
       </c>
       <c r="BO146">
-        <v>927</v>
+        <v>91</v>
       </c>
       <c r="BP146">
-        <v>1696</v>
+        <v>574</v>
       </c>
       <c r="BQ146">
         <v>0</v>
@@ -41773,3316 +41773,88 @@
         <v>0</v>
       </c>
       <c r="BS146">
-        <v>4161</v>
+        <v>42</v>
       </c>
       <c r="BT146">
-        <v>1547</v>
+        <v>46</v>
       </c>
       <c r="BU146">
-        <v>9114</v>
+        <v>89</v>
       </c>
       <c r="BV146">
-        <v>4271</v>
+        <v>1038</v>
       </c>
       <c r="BW146">
-        <v>54645.83203412523</v>
+        <v>3221.648998751739</v>
       </c>
       <c r="BX146">
-        <v>13773.84285655599</v>
+        <v>6542.29599256929</v>
       </c>
       <c r="BY146">
-        <v>0.09624258572833584</v>
+        <v>0.09082937992426762</v>
       </c>
       <c r="BZ146">
-        <v>0.06231994724870232</v>
+        <v>0.09638833545707579</v>
       </c>
       <c r="CA146">
-        <v>0.2696665691770914</v>
+        <v>0.1047335790151753</v>
       </c>
       <c r="CB146">
-        <v>0.1220415181612061</v>
+        <v>0.1810017528328711</v>
       </c>
       <c r="CC146">
-        <v>0.0122364383855035</v>
+        <v>0.02140064093106624</v>
       </c>
       <c r="CD146">
-        <v>0.01316897058038698</v>
+        <v>0.01233261709852269</v>
       </c>
       <c r="CE146">
-        <v>0.01465300247227565</v>
+        <v>0.01711502500947822</v>
       </c>
       <c r="CF146">
-        <v>0.01309154129215727</v>
+        <v>0.01575380571662003</v>
       </c>
       <c r="CG146">
-        <v>56106.03743929722</v>
+        <v>3258.689183589259</v>
       </c>
       <c r="CH146">
-        <v>14468.01025999999</v>
+        <v>6854.04266100001</v>
       </c>
       <c r="CI146">
-        <v>61403.86615757316</v>
+        <v>3317.965454202509</v>
       </c>
       <c r="CJ146">
-        <v>15651.13591938698</v>
+        <v>6943.784256296118</v>
       </c>
       <c r="CK146">
-        <v>0.1107177189361315</v>
+        <v>0.3071541511866948</v>
       </c>
       <c r="CL146">
-        <v>0.09342915988791074</v>
+        <v>0.8460378628220039</v>
       </c>
       <c r="CM146">
         <v>10000</v>
       </c>
       <c r="CO146">
-        <v>0.0212492587467879</v>
+        <v>0.158021712907117</v>
       </c>
       <c r="CP146">
-        <v>0.009191539830005931</v>
+        <v>0.2448733413751508</v>
       </c>
       <c r="CQ146">
-        <v>77098772.95674427</v>
+        <v>984997.8581532167</v>
       </c>
       <c r="CR146">
-        <v>9904185.350622581</v>
+        <v>5014111.391096285</v>
       </c>
       <c r="CS146" s="2">
-        <v>45538.89718956128</v>
+        <v>45565.59730472715</v>
       </c>
       <c r="CT146">
-        <v>-0.6341016418874756</v>
+        <v>-0.05725379331569909</v>
       </c>
       <c r="CU146">
-        <v>-0.8182444829914358</v>
-      </c>
-    </row>
-    <row r="147" spans="10:99">
-      <c r="J147" t="s">
-        <v>206</v>
-      </c>
-      <c r="K147">
-        <v>0.001014229819630286</v>
-      </c>
-      <c r="L147">
-        <v>0.001014229819630286</v>
-      </c>
-      <c r="M147">
-        <v>0.000771048648971373</v>
-      </c>
-      <c r="N147">
-        <v>0.000771048648971373</v>
-      </c>
-      <c r="O147">
-        <v>0.0007826236082778104</v>
-      </c>
-      <c r="P147">
-        <v>0.0007826236082778104</v>
-      </c>
-      <c r="Q147">
-        <v>0.0007028386892377503</v>
-      </c>
-      <c r="R147">
-        <v>0.0007028386892377503</v>
-      </c>
-      <c r="S147">
-        <v>10.43832433568448</v>
-      </c>
-      <c r="T147">
-        <v>36.94412060598135</v>
-      </c>
-      <c r="U147">
-        <v>0.9911014868792343</v>
-      </c>
-      <c r="V147">
-        <v>0.8270499048743385</v>
-      </c>
-      <c r="W147">
-        <v>0.09932600349992228</v>
-      </c>
-      <c r="X147">
-        <v>0.03794766513934982</v>
-      </c>
-      <c r="Y147">
-        <v>0.2434829400847191</v>
-      </c>
-      <c r="Z147">
-        <v>0.1053068344105673</v>
-      </c>
-      <c r="AA147">
-        <v>0.998313112299717</v>
-      </c>
-      <c r="AB147">
-        <v>0.7792743281927834</v>
-      </c>
-      <c r="AC147">
-        <v>0.9104821173262169</v>
-      </c>
-      <c r="AD147">
-        <v>0.9992746114873325</v>
-      </c>
-      <c r="AE147">
-        <v>0.6520833642920584</v>
-      </c>
-      <c r="AF147">
-        <v>0.8946817475479407</v>
-      </c>
-      <c r="AG147">
-        <v>0.01113203793548537</v>
-      </c>
-      <c r="AH147">
-        <v>0.004353103387594826</v>
-      </c>
-      <c r="AI147">
-        <v>0.998313112299717</v>
-      </c>
-      <c r="AJ147">
-        <v>0.9992746114873325</v>
-      </c>
-      <c r="AK147">
-        <v>0.01113203793548537</v>
-      </c>
-      <c r="AL147">
-        <v>0.004353103387594826</v>
-      </c>
-      <c r="AM147" t="s">
-        <v>244</v>
-      </c>
-      <c r="AN147">
-        <v>0.04836557928147062</v>
-      </c>
-      <c r="AO147">
-        <v>0.03760458833670856</v>
-      </c>
-      <c r="AP147">
-        <v>-1008.432096288</v>
-      </c>
-      <c r="AQ147">
-        <v>-3193.833982976</v>
-      </c>
-      <c r="AR147">
-        <v>39884.40898371212</v>
-      </c>
-      <c r="AS147">
-        <v>28628.88987702379</v>
-      </c>
-      <c r="AT147">
-        <v>39884.40898371212</v>
-      </c>
-      <c r="AU147">
-        <v>28516.67859702379</v>
-      </c>
-      <c r="AV147">
-        <v>2.988440898371212</v>
-      </c>
-      <c r="AW147">
-        <v>1.862888987702379</v>
-      </c>
-      <c r="AX147">
-        <v>2.298743330525133</v>
-      </c>
-      <c r="AY147">
-        <v>0.6496390034909553</v>
-      </c>
-      <c r="AZ147">
-        <v>59.23333333333333</v>
-      </c>
-      <c r="BA147">
-        <v>102.3833333333333</v>
-      </c>
-      <c r="BB147">
-        <v>0.07174263209818849</v>
-      </c>
-      <c r="BC147">
-        <v>0.01701934882523052</v>
-      </c>
-      <c r="BD147">
-        <v>-2387.62848398385</v>
-      </c>
-      <c r="BE147">
-        <v>-377.8391255678808</v>
-      </c>
-      <c r="BF147">
-        <v>5370</v>
-      </c>
-      <c r="BG147">
-        <v>17518</v>
-      </c>
-      <c r="BH147">
-        <v>1364.682638888889</v>
-      </c>
-      <c r="BI147">
-        <v>8875</v>
-      </c>
-      <c r="BJ147">
-        <v>32899</v>
-      </c>
-      <c r="BK147">
-        <v>14245</v>
-      </c>
-      <c r="BL147">
-        <v>50417</v>
-      </c>
-      <c r="BM147">
-        <v>0</v>
-      </c>
-      <c r="BN147">
-        <v>0</v>
-      </c>
-      <c r="BO147">
-        <v>988</v>
-      </c>
-      <c r="BP147">
-        <v>16569</v>
-      </c>
-      <c r="BQ147">
-        <v>0</v>
-      </c>
-      <c r="BR147">
-        <v>0</v>
-      </c>
-      <c r="BS147">
-        <v>4382</v>
-      </c>
-      <c r="BT147">
-        <v>949</v>
-      </c>
-      <c r="BU147">
-        <v>8875</v>
-      </c>
-      <c r="BV147">
-        <v>32899</v>
-      </c>
-      <c r="BW147">
-        <v>29884.40898371196</v>
-      </c>
-      <c r="BX147">
-        <v>18628.88987702399</v>
-      </c>
-      <c r="BY147">
-        <v>0.1146989693078136</v>
-      </c>
-      <c r="BZ147">
-        <v>0.06742016340281778</v>
-      </c>
-      <c r="CA147">
-        <v>0.3974532124154436</v>
-      </c>
-      <c r="CB147">
-        <v>0.2061882003003253</v>
-      </c>
-      <c r="CC147">
-        <v>0.01462325354241527</v>
-      </c>
-      <c r="CD147">
-        <v>0.009718074555247098</v>
-      </c>
-      <c r="CE147">
-        <v>0.01761461970754639</v>
-      </c>
-      <c r="CF147">
-        <v>0.01366299079902771</v>
-      </c>
-      <c r="CG147">
-        <v>30892.84107999997</v>
-      </c>
-      <c r="CH147">
-        <v>21822.72385999999</v>
-      </c>
-      <c r="CI147">
-        <v>33280.46956398382</v>
-      </c>
-      <c r="CJ147">
-        <v>22200.56298556787</v>
-      </c>
-      <c r="CK147">
-        <v>0.09127680031236299</v>
-      </c>
-      <c r="CL147">
-        <v>0.1263326858427522</v>
-      </c>
-      <c r="CM147">
-        <v>10000</v>
-      </c>
-      <c r="CO147">
-        <v>0.01917323075044269</v>
-      </c>
-      <c r="CP147">
-        <v>0.01163216706356475</v>
-      </c>
-      <c r="CQ147">
-        <v>26186203.34920769</v>
-      </c>
-      <c r="CR147">
-        <v>33076028.4704131</v>
-      </c>
-      <c r="CS147" s="2">
-        <v>45539.07826618969</v>
-      </c>
-      <c r="CT147">
-        <v>-0.7352993376867214</v>
-      </c>
-      <c r="CU147">
-        <v>-0.8640112100798503</v>
-      </c>
-    </row>
-    <row r="148" spans="10:99">
-      <c r="J148" t="s">
-        <v>240</v>
-      </c>
-      <c r="K148">
-        <v>0.001043980302255276</v>
-      </c>
-      <c r="L148">
-        <v>0.001043980302255276</v>
-      </c>
-      <c r="M148">
-        <v>0.001118819137860605</v>
-      </c>
-      <c r="N148">
-        <v>0.001118819137860605</v>
-      </c>
-      <c r="O148">
-        <v>0.0007576810164051428</v>
-      </c>
-      <c r="P148">
-        <v>0.0007576810164051428</v>
-      </c>
-      <c r="Q148">
-        <v>0.0008276500578958013</v>
-      </c>
-      <c r="R148">
-        <v>0.0008276500578958013</v>
-      </c>
-      <c r="S148">
-        <v>7.948578552510321</v>
-      </c>
-      <c r="T148">
-        <v>23.97570380942227</v>
-      </c>
-      <c r="U148">
-        <v>0.9892200490245532</v>
-      </c>
-      <c r="V148">
-        <v>0.6261525309147947</v>
-      </c>
-      <c r="W148">
-        <v>0.08332267561648335</v>
-      </c>
-      <c r="X148">
-        <v>0.06110170446035521</v>
-      </c>
-      <c r="Y148">
-        <v>0.2274428612262671</v>
-      </c>
-      <c r="Z148">
-        <v>0.2272883356562123</v>
-      </c>
-      <c r="AA148">
-        <v>0.9987949487194659</v>
-      </c>
-      <c r="AB148">
-        <v>0.831845234829394</v>
-      </c>
-      <c r="AC148">
-        <v>0.7956433713700398</v>
-      </c>
-      <c r="AD148">
-        <v>0.9991530473480615</v>
-      </c>
-      <c r="AE148">
-        <v>0.7814626398845502</v>
-      </c>
-      <c r="AF148">
-        <v>0.7728673161191121</v>
-      </c>
-      <c r="AG148">
-        <v>0.0084055278262375</v>
-      </c>
-      <c r="AH148">
-        <v>0.008097880290040839</v>
-      </c>
-      <c r="AI148">
-        <v>0.9987949487194659</v>
-      </c>
-      <c r="AJ148">
-        <v>0.9991530473480615</v>
-      </c>
-      <c r="AK148">
-        <v>0.0084055278262375</v>
-      </c>
-      <c r="AL148">
-        <v>0.008097880290040839</v>
-      </c>
-      <c r="AM148" t="s">
-        <v>244</v>
-      </c>
-      <c r="AN148">
-        <v>0.03862144590411947</v>
-      </c>
-      <c r="AO148">
-        <v>0.03213660866764869</v>
-      </c>
-      <c r="AP148">
-        <v>-807.1987751476001</v>
-      </c>
-      <c r="AQ148">
-        <v>-2223.9511840864</v>
-      </c>
-      <c r="AR148">
-        <v>39466.04705485226</v>
-      </c>
-      <c r="AS148">
-        <v>43545.23765191371</v>
-      </c>
-      <c r="AT148">
-        <v>39466.04705485226</v>
-      </c>
-      <c r="AU148">
-        <v>43506.29687191371</v>
-      </c>
-      <c r="AV148">
-        <v>2.946604705485226</v>
-      </c>
-      <c r="AW148">
-        <v>3.354523765191371</v>
-      </c>
-      <c r="AX148">
-        <v>3.019400082879092</v>
-      </c>
-      <c r="AY148">
-        <v>1.000948410685603</v>
-      </c>
-      <c r="AZ148">
-        <v>50.18333333333333</v>
-      </c>
-      <c r="BA148">
-        <v>36.83333333333334</v>
-      </c>
-      <c r="BB148">
-        <v>0.09233635491843634</v>
-      </c>
-      <c r="BC148">
-        <v>0.03273602029387997</v>
-      </c>
-      <c r="BD148">
-        <v>-3079.688369848458</v>
-      </c>
-      <c r="BE148">
-        <v>-1210.570140311318</v>
-      </c>
-      <c r="BF148">
-        <v>4053</v>
-      </c>
-      <c r="BG148">
-        <v>9814</v>
-      </c>
-      <c r="BH148">
-        <v>1315.706944444444</v>
-      </c>
-      <c r="BI148">
-        <v>6405</v>
-      </c>
-      <c r="BJ148">
-        <v>21731</v>
-      </c>
-      <c r="BK148">
-        <v>10458</v>
-      </c>
-      <c r="BL148">
-        <v>31545</v>
-      </c>
-      <c r="BM148">
-        <v>0</v>
-      </c>
-      <c r="BN148">
-        <v>0</v>
-      </c>
-      <c r="BO148">
-        <v>155</v>
-      </c>
-      <c r="BP148">
-        <v>8222</v>
-      </c>
-      <c r="BQ148">
-        <v>0</v>
-      </c>
-      <c r="BR148">
-        <v>0</v>
-      </c>
-      <c r="BS148">
-        <v>3898</v>
-      </c>
-      <c r="BT148">
-        <v>1592</v>
-      </c>
-      <c r="BU148">
-        <v>6405</v>
-      </c>
-      <c r="BV148">
-        <v>21731</v>
-      </c>
-      <c r="BW148">
-        <v>29466.04705485237</v>
-      </c>
-      <c r="BX148">
-        <v>33545.23765191361</v>
-      </c>
-      <c r="BY148">
-        <v>0.08912400837164683</v>
-      </c>
-      <c r="BZ148">
-        <v>0.06562881901766722</v>
-      </c>
-      <c r="CA148">
-        <v>0.3032060874745139</v>
-      </c>
-      <c r="CB148">
-        <v>0.2730519736323765</v>
-      </c>
-      <c r="CC148">
-        <v>0.01375647983116006</v>
-      </c>
-      <c r="CD148">
-        <v>0.008653595506676808</v>
-      </c>
-      <c r="CE148">
-        <v>0.01442163639110036</v>
-      </c>
-      <c r="CF148">
-        <v>0.01015626277347712</v>
-      </c>
-      <c r="CG148">
-        <v>30273.24582999997</v>
-      </c>
-      <c r="CH148">
-        <v>35769.18883600001</v>
-      </c>
-      <c r="CI148">
-        <v>33352.93419984842</v>
-      </c>
-      <c r="CJ148">
-        <v>36979.75897631133</v>
-      </c>
-      <c r="CK148">
-        <v>0.09900868191806761</v>
-      </c>
-      <c r="CL148">
-        <v>0.1272734056878337</v>
-      </c>
-      <c r="CM148">
-        <v>10000</v>
-      </c>
-      <c r="CO148">
-        <v>0.01235037051111533</v>
-      </c>
-      <c r="CP148">
-        <v>0.008265247957438724</v>
-      </c>
-      <c r="CQ148">
-        <v>16588242.9701402</v>
-      </c>
-      <c r="CR148">
-        <v>47918642.04957736</v>
-      </c>
-      <c r="CS148" s="2">
-        <v>45539.21829002783</v>
-      </c>
-      <c r="CT148">
-        <v>-0.735755419851611</v>
-      </c>
-      <c r="CU148">
-        <v>-0.7623117469432787</v>
-      </c>
-    </row>
-    <row r="149" spans="10:99">
-      <c r="J149" t="s">
-        <v>209</v>
-      </c>
-      <c r="K149">
-        <v>0.0009594193172550725</v>
-      </c>
-      <c r="L149">
-        <v>0.0009594193172550725</v>
-      </c>
-      <c r="M149">
-        <v>0.0004586137350390818</v>
-      </c>
-      <c r="N149">
-        <v>0.0004586137350390818</v>
-      </c>
-      <c r="O149">
-        <v>0.0004002844140237771</v>
-      </c>
-      <c r="P149">
-        <v>0.0004002844140237771</v>
-      </c>
-      <c r="Q149">
-        <v>0.000111867747310157</v>
-      </c>
-      <c r="R149">
-        <v>0.000111867747310157</v>
-      </c>
-      <c r="S149">
-        <v>9.983331386892312</v>
-      </c>
-      <c r="T149">
-        <v>5.765815155021962</v>
-      </c>
-      <c r="U149">
-        <v>1</v>
-      </c>
-      <c r="V149">
-        <v>0.6901335639634388</v>
-      </c>
-      <c r="W149">
-        <v>0.09471351238170106</v>
-      </c>
-      <c r="X149">
-        <v>0.04588253762971296</v>
-      </c>
-      <c r="Y149">
-        <v>0.2183023774254544</v>
-      </c>
-      <c r="Z149">
-        <v>0.1840397618258545</v>
-      </c>
-      <c r="AA149">
-        <v>0.9977013166528762</v>
-      </c>
-      <c r="AB149">
-        <v>0.8266332438111783</v>
-      </c>
-      <c r="AC149">
-        <v>0.8530261982718146</v>
-      </c>
-      <c r="AD149">
-        <v>0.9991885716489726</v>
-      </c>
-      <c r="AE149">
-        <v>0.6481048484676548</v>
-      </c>
-      <c r="AF149">
-        <v>0.7940983685254002</v>
-      </c>
-      <c r="AG149">
-        <v>0.01097685173217941</v>
-      </c>
-      <c r="AH149">
-        <v>0.005474007347218681</v>
-      </c>
-      <c r="AI149">
-        <v>0.9977013166528762</v>
-      </c>
-      <c r="AJ149">
-        <v>0.9991885716489726</v>
-      </c>
-      <c r="AK149">
-        <v>0.01097685173217941</v>
-      </c>
-      <c r="AL149">
-        <v>0.005474007347218681</v>
-      </c>
-      <c r="AM149" t="s">
-        <v>244</v>
-      </c>
-      <c r="AN149">
-        <v>0.1016699776902103</v>
-      </c>
-      <c r="AO149">
-        <v>0.04485763468527489</v>
-      </c>
-      <c r="AP149">
-        <v>-951.859602792</v>
-      </c>
-      <c r="AQ149">
-        <v>-724.9581278860001</v>
-      </c>
-      <c r="AR149">
-        <v>39746.67908886574</v>
-      </c>
-      <c r="AS149">
-        <v>19343.9234621139</v>
-      </c>
-      <c r="AT149">
-        <v>39661.2646372079</v>
-      </c>
-      <c r="AU149">
-        <v>19343.9234621139</v>
-      </c>
-      <c r="AV149">
-        <v>2.974667908886574</v>
-      </c>
-      <c r="AW149">
-        <v>0.9343923462113901</v>
-      </c>
-      <c r="AX149">
-        <v>2.404078199327068</v>
-      </c>
-      <c r="AY149">
-        <v>4.161824975891996</v>
-      </c>
-      <c r="AZ149">
-        <v>47.91666666666666</v>
-      </c>
-      <c r="BA149">
-        <v>110.3</v>
-      </c>
-      <c r="BB149">
-        <v>0.0864080720136467</v>
-      </c>
-      <c r="BC149">
-        <v>0.2782607464466617</v>
-      </c>
-      <c r="BD149">
-        <v>-2903.486185379377</v>
-      </c>
-      <c r="BE149">
-        <v>-3881.97606451703</v>
-      </c>
-      <c r="BF149">
-        <v>4548</v>
-      </c>
-      <c r="BG149">
-        <v>4355</v>
-      </c>
-      <c r="BH149">
-        <v>1438.998611111111</v>
-      </c>
-      <c r="BI149">
-        <v>9818</v>
-      </c>
-      <c r="BJ149">
-        <v>3942</v>
-      </c>
-      <c r="BK149">
-        <v>14366</v>
-      </c>
-      <c r="BL149">
-        <v>8297</v>
-      </c>
-      <c r="BM149">
-        <v>0</v>
-      </c>
-      <c r="BN149">
-        <v>0</v>
-      </c>
-      <c r="BO149">
-        <v>526</v>
-      </c>
-      <c r="BP149">
-        <v>1858</v>
-      </c>
-      <c r="BQ149">
-        <v>0</v>
-      </c>
-      <c r="BR149">
-        <v>0</v>
-      </c>
-      <c r="BS149">
-        <v>4022</v>
-      </c>
-      <c r="BT149">
-        <v>2497</v>
-      </c>
-      <c r="BU149">
-        <v>9818</v>
-      </c>
-      <c r="BV149">
-        <v>3942</v>
-      </c>
-      <c r="BW149">
-        <v>29746.67908886581</v>
-      </c>
-      <c r="BX149">
-        <v>9343.923462113988</v>
-      </c>
-      <c r="BY149">
-        <v>0.1003179205659135</v>
-      </c>
-      <c r="BZ149">
-        <v>0.05345448741478384</v>
-      </c>
-      <c r="CA149">
-        <v>0.3355805945064965</v>
-      </c>
-      <c r="CB149">
-        <v>0.1549279952923401</v>
-      </c>
-      <c r="CC149">
-        <v>0.00929209131503835</v>
-      </c>
-      <c r="CD149">
-        <v>0.008302997929263874</v>
-      </c>
-      <c r="CE149">
-        <v>0.01321986003523268</v>
-      </c>
-      <c r="CF149">
-        <v>0.009374499341050202</v>
-      </c>
-      <c r="CG149">
-        <v>30698.53869165781</v>
-      </c>
-      <c r="CH149">
-        <v>10068.88158999999</v>
-      </c>
-      <c r="CI149">
-        <v>33602.02487703718</v>
-      </c>
-      <c r="CJ149">
-        <v>13950.85765451702</v>
-      </c>
-      <c r="CK149">
-        <v>0.1036859701323928</v>
-      </c>
-      <c r="CL149">
-        <v>0.05224521534246774</v>
-      </c>
-      <c r="CM149">
-        <v>10000</v>
-      </c>
-      <c r="CO149">
-        <v>0.04670353533891189</v>
-      </c>
-      <c r="CP149">
-        <v>0.006456843385354837</v>
-      </c>
-      <c r="CQ149">
-        <v>62123674.221907</v>
-      </c>
-      <c r="CR149">
-        <v>8972816.952993827</v>
-      </c>
-      <c r="CS149" s="2">
-        <v>45539.39437030051</v>
-      </c>
-      <c r="CT149">
-        <v>-0.7432041515252624</v>
-      </c>
-      <c r="CU149">
-        <v>-0.8000401109199134</v>
-      </c>
-    </row>
-    <row r="150" spans="10:99">
-      <c r="J150" t="s">
-        <v>175</v>
-      </c>
-      <c r="K150">
-        <v>0.0014995749146125</v>
-      </c>
-      <c r="L150">
-        <v>0.0014995749146125</v>
-      </c>
-      <c r="M150">
-        <v>0.0006212630536890362</v>
-      </c>
-      <c r="N150">
-        <v>0.0006212630536890362</v>
-      </c>
-      <c r="O150">
-        <v>0.000866381927922788</v>
-      </c>
-      <c r="P150">
-        <v>0.000866381927922788</v>
-      </c>
-      <c r="Q150">
-        <v>0.0004080107070856265</v>
-      </c>
-      <c r="R150">
-        <v>0.0004080107070856265</v>
-      </c>
-      <c r="S150">
-        <v>7.273618126560693</v>
-      </c>
-      <c r="T150">
-        <v>22.96252214749435</v>
-      </c>
-      <c r="U150">
-        <v>0.9925846500328536</v>
-      </c>
-      <c r="V150">
-        <v>0.7108944380863923</v>
-      </c>
-      <c r="W150">
-        <v>0.08101871973489233</v>
-      </c>
-      <c r="X150">
-        <v>0.0713155061628284</v>
-      </c>
-      <c r="Y150">
-        <v>0.2381933793153074</v>
-      </c>
-      <c r="Z150">
-        <v>0.1704779765509124</v>
-      </c>
-      <c r="AA150">
-        <v>0.9987178385896829</v>
-      </c>
-      <c r="AB150">
-        <v>0.8161999919868432</v>
-      </c>
-      <c r="AC150">
-        <v>0.8473240680715619</v>
-      </c>
-      <c r="AD150">
-        <v>0.9988971486549644</v>
-      </c>
-      <c r="AE150">
-        <v>0.7568816395548748</v>
-      </c>
-      <c r="AF150">
-        <v>0.8310222244591673</v>
-      </c>
-      <c r="AG150">
-        <v>0.008625831493960947</v>
-      </c>
-      <c r="AH150">
-        <v>0.007685838354184884</v>
-      </c>
-      <c r="AI150">
-        <v>0.9987178385896829</v>
-      </c>
-      <c r="AJ150">
-        <v>0.9988971486549644</v>
-      </c>
-      <c r="AK150">
-        <v>0.008625831493960947</v>
-      </c>
-      <c r="AL150">
-        <v>0.007685838354184884</v>
-      </c>
-      <c r="AM150" t="s">
-        <v>244</v>
-      </c>
-      <c r="AN150">
-        <v>0.07009917180099763</v>
-      </c>
-      <c r="AO150">
-        <v>0.0429808340201189</v>
-      </c>
-      <c r="AP150">
-        <v>-1752.08941275</v>
-      </c>
-      <c r="AQ150">
-        <v>-1608.391471576</v>
-      </c>
-      <c r="AR150">
-        <v>86518.08123501994</v>
-      </c>
-      <c r="AS150">
-        <v>24457.214548424</v>
-      </c>
-      <c r="AT150">
-        <v>86396.77777724982</v>
-      </c>
-      <c r="AU150">
-        <v>24457.082638424</v>
-      </c>
-      <c r="AV150">
-        <v>7.651808123501993</v>
-      </c>
-      <c r="AW150">
-        <v>1.4457214548424</v>
-      </c>
-      <c r="AX150">
-        <v>3.299899742194214</v>
-      </c>
-      <c r="AY150">
-        <v>1.045210948132466</v>
-      </c>
-      <c r="AZ150">
-        <v>41.18333333333333</v>
-      </c>
-      <c r="BA150">
-        <v>41.43333333333333</v>
-      </c>
-      <c r="BB150">
-        <v>0.02433726582011549</v>
-      </c>
-      <c r="BC150">
-        <v>0.09421864468452391</v>
-      </c>
-      <c r="BD150">
-        <v>-1952.397977403301</v>
-      </c>
-      <c r="BE150">
-        <v>-1671.131356764048</v>
-      </c>
-      <c r="BF150">
-        <v>4077</v>
-      </c>
-      <c r="BG150">
-        <v>13799</v>
-      </c>
-      <c r="BH150">
-        <v>1439.998611111111</v>
-      </c>
-      <c r="BI150">
-        <v>6397</v>
-      </c>
-      <c r="BJ150">
-        <v>19267</v>
-      </c>
-      <c r="BK150">
-        <v>10474</v>
-      </c>
-      <c r="BL150">
-        <v>33066</v>
-      </c>
-      <c r="BM150">
-        <v>0</v>
-      </c>
-      <c r="BN150">
-        <v>0</v>
-      </c>
-      <c r="BO150">
-        <v>841</v>
-      </c>
-      <c r="BP150">
-        <v>11424</v>
-      </c>
-      <c r="BQ150">
-        <v>0</v>
-      </c>
-      <c r="BR150">
-        <v>0</v>
-      </c>
-      <c r="BS150">
-        <v>3236</v>
-      </c>
-      <c r="BT150">
-        <v>2375</v>
-      </c>
-      <c r="BU150">
-        <v>6397</v>
-      </c>
-      <c r="BV150">
-        <v>19267</v>
-      </c>
-      <c r="BW150">
-        <v>76518.08123502007</v>
-      </c>
-      <c r="BX150">
-        <v>14457.21454842402</v>
-      </c>
-      <c r="BY150">
-        <v>0.08566530884267912</v>
-      </c>
-      <c r="BZ150">
-        <v>0.06741678347672533</v>
-      </c>
-      <c r="CA150">
-        <v>0.3212033159013191</v>
-      </c>
-      <c r="CB150">
-        <v>0.1445513215610652</v>
-      </c>
-      <c r="CC150">
-        <v>0.0103375825119956</v>
-      </c>
-      <c r="CD150">
-        <v>0.009949600912788664</v>
-      </c>
-      <c r="CE150">
-        <v>0.01167370057748904</v>
-      </c>
-      <c r="CF150">
-        <v>0.009373687370082942</v>
-      </c>
-      <c r="CG150">
-        <v>78270.17064777008</v>
-      </c>
-      <c r="CH150">
-        <v>16065.60602000002</v>
-      </c>
-      <c r="CI150">
-        <v>80222.56862517339</v>
-      </c>
-      <c r="CJ150">
-        <v>17736.73737676406</v>
-      </c>
-      <c r="CK150">
-        <v>0.1619194381255034</v>
-      </c>
-      <c r="CL150">
-        <v>0.08270623426214278</v>
-      </c>
-      <c r="CM150">
-        <v>10000</v>
-      </c>
-      <c r="CO150">
-        <v>0.0187205231330112</v>
-      </c>
-      <c r="CP150">
-        <v>0.01119759266224936</v>
-      </c>
-      <c r="CQ150">
-        <v>40395803.74727766</v>
-      </c>
-      <c r="CR150">
-        <v>14011581.24698414</v>
-      </c>
-      <c r="CS150" s="2">
-        <v>45539.58827701793</v>
-      </c>
-      <c r="CT150">
-        <v>-0.7561305054481315</v>
-      </c>
-      <c r="CU150">
-        <v>-0.8473151020033423</v>
-      </c>
-    </row>
-    <row r="151" spans="10:99">
-      <c r="J151" t="s">
-        <v>224</v>
-      </c>
-      <c r="K151">
-        <v>0.001100342047341885</v>
-      </c>
-      <c r="L151">
-        <v>0.001100342047341885</v>
-      </c>
-      <c r="M151">
-        <v>-2.872463366199174E-05</v>
-      </c>
-      <c r="N151">
-        <v>-2.872463366199174E-05</v>
-      </c>
-      <c r="O151">
-        <v>0.0007925903433322334</v>
-      </c>
-      <c r="P151">
-        <v>0.0007925903433322334</v>
-      </c>
-      <c r="Q151">
-        <v>1.972643475112168E-06</v>
-      </c>
-      <c r="R151">
-        <v>1.972643475112168E-06</v>
-      </c>
-      <c r="S151">
-        <v>12.03542827491153</v>
-      </c>
-      <c r="T151">
-        <v>5.512505316845406</v>
-      </c>
-      <c r="U151">
-        <v>0.9887697174512384</v>
-      </c>
-      <c r="V151">
-        <v>1</v>
-      </c>
-      <c r="W151">
-        <v>0.09937230146642329</v>
-      </c>
-      <c r="X151">
-        <v>0.06591441228009143</v>
-      </c>
-      <c r="Y151">
-        <v>0.2263478475720091</v>
-      </c>
-      <c r="Z151">
-        <v>0.0834064156812034</v>
-      </c>
-      <c r="AA151">
-        <v>0.9981412425233237</v>
-      </c>
-      <c r="AB151">
-        <v>0.7984741232052582</v>
-      </c>
-      <c r="AC151">
-        <v>0.9706591237504322</v>
-      </c>
-      <c r="AD151">
-        <v>0.9996582932945351</v>
-      </c>
-      <c r="AE151">
-        <v>0.7738094005776048</v>
-      </c>
-      <c r="AF151">
-        <v>0.9435950173268086</v>
-      </c>
-      <c r="AG151">
-        <v>0.01099361573530142</v>
-      </c>
-      <c r="AH151">
-        <v>0.0009388811709616013</v>
-      </c>
-      <c r="AI151">
-        <v>0.9981412425233237</v>
-      </c>
-      <c r="AJ151">
-        <v>0.9996582932945351</v>
-      </c>
-      <c r="AK151">
-        <v>0.01099361573530142</v>
-      </c>
-      <c r="AL151">
-        <v>0.0009388811709616013</v>
-      </c>
-      <c r="AM151" t="s">
-        <v>244</v>
-      </c>
-      <c r="AN151">
-        <v>0.05381833292422038</v>
-      </c>
-      <c r="AO151">
-        <v>0.01256153943738053</v>
-      </c>
-      <c r="AP151">
-        <v>-1465.5897298514</v>
-      </c>
-      <c r="AQ151">
-        <v>-185.7751726004</v>
-      </c>
-      <c r="AR151">
-        <v>48725.62199914842</v>
-      </c>
-      <c r="AS151">
-        <v>9594.797901399508</v>
-      </c>
-      <c r="AT151">
-        <v>48603.00859914842</v>
-      </c>
-      <c r="AU151">
-        <v>9594.978501399508</v>
-      </c>
-      <c r="AV151">
-        <v>3.872562199914842</v>
-      </c>
-      <c r="AW151">
-        <v>-0.04052020986004923</v>
-      </c>
-      <c r="AX151">
-        <v>1.994210425081746</v>
-      </c>
-      <c r="AY151">
-        <v>4.354275334929235</v>
-      </c>
-      <c r="AZ151">
-        <v>86.86666666666666</v>
-      </c>
-      <c r="BA151">
-        <v>18.9</v>
-      </c>
-      <c r="BB151">
-        <v>0.05142994950845454</v>
-      </c>
-      <c r="BC151">
-        <v>1.035211515588393</v>
-      </c>
-      <c r="BD151">
-        <v>-2179.103155149112</v>
-      </c>
-      <c r="BE151">
-        <v>-6451.107736476973</v>
-      </c>
-      <c r="BF151">
-        <v>5353</v>
-      </c>
-      <c r="BG151">
-        <v>3338</v>
-      </c>
-      <c r="BH151">
-        <v>1439.998611111111</v>
-      </c>
-      <c r="BI151">
-        <v>11978</v>
-      </c>
-      <c r="BJ151">
-        <v>4600</v>
-      </c>
-      <c r="BK151">
-        <v>17331</v>
-      </c>
-      <c r="BL151">
-        <v>7938</v>
-      </c>
-      <c r="BM151">
-        <v>0</v>
-      </c>
-      <c r="BN151">
-        <v>0</v>
-      </c>
-      <c r="BO151">
-        <v>3090</v>
-      </c>
-      <c r="BP151">
-        <v>1746</v>
-      </c>
-      <c r="BQ151">
-        <v>0</v>
-      </c>
-      <c r="BR151">
-        <v>0</v>
-      </c>
-      <c r="BS151">
-        <v>2263</v>
-      </c>
-      <c r="BT151">
-        <v>1592</v>
-      </c>
-      <c r="BU151">
-        <v>11978</v>
-      </c>
-      <c r="BV151">
-        <v>4600</v>
-      </c>
-      <c r="BW151">
-        <v>38725.62199914867</v>
-      </c>
-      <c r="BX151">
-        <v>-405.202098600401</v>
-      </c>
-      <c r="BY151">
-        <v>0.1094545955740971</v>
-      </c>
-      <c r="BZ151">
-        <v>0.2245772785989912</v>
-      </c>
-      <c r="CA151">
-        <v>0.3162144518428589</v>
-      </c>
-      <c r="CB151">
-        <v>0.6410193300702672</v>
-      </c>
-      <c r="CC151">
-        <v>0.01373791149179598</v>
-      </c>
-      <c r="CD151">
-        <v>0.02565032554759203</v>
-      </c>
-      <c r="CE151">
-        <v>0.01741526819893258</v>
-      </c>
-      <c r="CF151">
-        <v>0.03507472111070104</v>
-      </c>
-      <c r="CG151">
-        <v>40191.21172900007</v>
-      </c>
-      <c r="CH151">
-        <v>-219.426926000001</v>
-      </c>
-      <c r="CI151">
-        <v>42370.31488414918</v>
-      </c>
-      <c r="CJ151">
-        <v>6231.680810476972</v>
-      </c>
-      <c r="CK151">
-        <v>0.1234634230078177</v>
-      </c>
-      <c r="CL151">
-        <v>-0.02556835925803037</v>
-      </c>
-      <c r="CM151">
-        <v>10000</v>
-      </c>
-      <c r="CO151">
-        <v>0.02476780185758514</v>
-      </c>
-      <c r="CP151">
-        <v>0</v>
-      </c>
-      <c r="CQ151">
-        <v>41435419.99585532</v>
-      </c>
-      <c r="CR151">
-        <v>603432.5153436529</v>
-      </c>
-      <c r="CS151" s="2">
-        <v>45540.00083998014</v>
-      </c>
-      <c r="CT151">
-        <v>-0.7383216948663216</v>
-      </c>
-      <c r="CU151">
-        <v>-0.9943363761513067</v>
-      </c>
-    </row>
-    <row r="152" spans="10:99">
-      <c r="J152" t="s">
-        <v>228</v>
-      </c>
-      <c r="K152">
-        <v>0.0006889648218131317</v>
-      </c>
-      <c r="L152">
-        <v>0.0006889648218131317</v>
-      </c>
-      <c r="M152">
-        <v>0.001536655964846867</v>
-      </c>
-      <c r="N152">
-        <v>0.001536655964846867</v>
-      </c>
-      <c r="O152">
-        <v>0.0002933723056169013</v>
-      </c>
-      <c r="P152">
-        <v>0.0002933723056169013</v>
-      </c>
-      <c r="Q152">
-        <v>0.001042875489022177</v>
-      </c>
-      <c r="R152">
-        <v>0.001042875489022177</v>
-      </c>
-      <c r="S152">
-        <v>5.732738283511747</v>
-      </c>
-      <c r="T152">
-        <v>32.85826724490322</v>
-      </c>
-      <c r="U152">
-        <v>0.9999794662160716</v>
-      </c>
-      <c r="V152">
-        <v>0.7684244774598183</v>
-      </c>
-      <c r="W152">
-        <v>0.03236390712084835</v>
-      </c>
-      <c r="X152">
-        <v>0.04437183403018002</v>
-      </c>
-      <c r="Y152">
-        <v>0.2454399633786155</v>
-      </c>
-      <c r="Z152">
-        <v>0.1308072771384882</v>
-      </c>
-      <c r="AA152">
-        <v>0.9994130361074415</v>
-      </c>
-      <c r="AB152">
-        <v>0.9116995454295356</v>
-      </c>
-      <c r="AC152">
-        <v>0.889670914704431</v>
-      </c>
-      <c r="AD152">
-        <v>0.9991471960976822</v>
-      </c>
-      <c r="AE152">
-        <v>0.7168695499381326</v>
-      </c>
-      <c r="AF152">
-        <v>0.8690506867398055</v>
-      </c>
-      <c r="AG152">
-        <v>0.003361404753680459</v>
-      </c>
-      <c r="AH152">
-        <v>0.005017747852152942</v>
-      </c>
-      <c r="AI152">
-        <v>0.9994130361074415</v>
-      </c>
-      <c r="AJ152">
-        <v>0.9991471960976822</v>
-      </c>
-      <c r="AK152">
-        <v>0.003361404753680459</v>
-      </c>
-      <c r="AL152">
-        <v>0.005017747852152942</v>
-      </c>
-      <c r="AM152" t="s">
-        <v>244</v>
-      </c>
-      <c r="AN152">
-        <v>0.02206642486920156</v>
-      </c>
-      <c r="AO152">
-        <v>0.04841765670190545</v>
-      </c>
-      <c r="AP152">
-        <v>-682.6122474680001</v>
-      </c>
-      <c r="AQ152">
-        <v>-4908.613774936</v>
-      </c>
-      <c r="AR152">
-        <v>24850.58112253209</v>
-      </c>
-      <c r="AS152">
-        <v>76098.99578506412</v>
-      </c>
-      <c r="AT152">
-        <v>24832.57507253209</v>
-      </c>
-      <c r="AU152">
-        <v>76098.84416506412</v>
-      </c>
-      <c r="AV152">
-        <v>1.485058112253209</v>
-      </c>
-      <c r="AW152">
-        <v>6.609899578506412</v>
-      </c>
-      <c r="AX152">
-        <v>4.185511263639563</v>
-      </c>
-      <c r="AY152">
-        <v>0.7304250713825182</v>
-      </c>
-      <c r="AZ152">
-        <v>64.2</v>
-      </c>
-      <c r="BA152">
-        <v>27.96666666666667</v>
-      </c>
-      <c r="BB152">
-        <v>0.1823428078809934</v>
-      </c>
-      <c r="BC152">
-        <v>0.04420199055362796</v>
-      </c>
-      <c r="BD152">
-        <v>-3464.00193350466</v>
-      </c>
-      <c r="BE152">
-        <v>-3283.829486969573</v>
-      </c>
-      <c r="BF152">
-        <v>3621</v>
-      </c>
-      <c r="BG152">
-        <v>15818</v>
-      </c>
-      <c r="BH152">
-        <v>1321.706944444444</v>
-      </c>
-      <c r="BI152">
-        <v>3956</v>
-      </c>
-      <c r="BJ152">
-        <v>27611</v>
-      </c>
-      <c r="BK152">
-        <v>7577</v>
-      </c>
-      <c r="BL152">
-        <v>43429</v>
-      </c>
-      <c r="BM152">
-        <v>0</v>
-      </c>
-      <c r="BN152">
-        <v>0</v>
-      </c>
-      <c r="BO152">
-        <v>58</v>
-      </c>
-      <c r="BP152">
-        <v>14243</v>
-      </c>
-      <c r="BQ152">
-        <v>0</v>
-      </c>
-      <c r="BR152">
-        <v>0</v>
-      </c>
-      <c r="BS152">
-        <v>3563</v>
-      </c>
-      <c r="BT152">
-        <v>1575</v>
-      </c>
-      <c r="BU152">
-        <v>3956</v>
-      </c>
-      <c r="BV152">
-        <v>27611</v>
-      </c>
-      <c r="BW152">
-        <v>14850.581122532</v>
-      </c>
-      <c r="BX152">
-        <v>66098.99578506392</v>
-      </c>
-      <c r="BY152">
-        <v>0.07446835139682238</v>
-      </c>
-      <c r="BZ152">
-        <v>0.04970030167677591</v>
-      </c>
-      <c r="CA152">
-        <v>0.4806323632557072</v>
-      </c>
-      <c r="CB152">
-        <v>0.3999748099586756</v>
-      </c>
-      <c r="CC152">
-        <v>0.01922391630415166</v>
-      </c>
-      <c r="CD152">
-        <v>0.008607661146581855</v>
-      </c>
-      <c r="CE152">
-        <v>0.0175854482447623</v>
-      </c>
-      <c r="CF152">
-        <v>0.007666096373314267</v>
-      </c>
-      <c r="CG152">
-        <v>15533.19337</v>
-      </c>
-      <c r="CH152">
-        <v>71007.60955999992</v>
-      </c>
-      <c r="CI152">
-        <v>18997.19530350466</v>
-      </c>
-      <c r="CJ152">
-        <v>74291.43904696949</v>
-      </c>
-      <c r="CK152">
-        <v>0.1432439658117321</v>
-      </c>
-      <c r="CL152">
-        <v>0.218422062698417</v>
-      </c>
-      <c r="CM152">
-        <v>10000</v>
-      </c>
-      <c r="CO152">
-        <v>0.001166382951894584</v>
-      </c>
-      <c r="CP152">
-        <v>0.01361830905995839</v>
-      </c>
-      <c r="CQ152">
-        <v>4460437.951027548</v>
-      </c>
-      <c r="CR152">
-        <v>66744473.90759409</v>
-      </c>
-      <c r="CS152" s="2">
-        <v>45540.65858099446</v>
-      </c>
-      <c r="CT152">
-        <v>-0.9241762384078545</v>
-      </c>
-      <c r="CU152">
-        <v>-0.8168419123201983</v>
-      </c>
-    </row>
-    <row r="153" spans="10:99">
-      <c r="J153" t="s">
-        <v>237</v>
-      </c>
-      <c r="K153">
-        <v>0.001363895207304289</v>
-      </c>
-      <c r="L153">
-        <v>0.001363895207304289</v>
-      </c>
-      <c r="M153">
-        <v>0.00131510646043731</v>
-      </c>
-      <c r="N153">
-        <v>0.00131510646043731</v>
-      </c>
-      <c r="O153">
-        <v>0.0009596810146333734</v>
-      </c>
-      <c r="P153">
-        <v>0.0009596810146333734</v>
-      </c>
-      <c r="Q153">
-        <v>0.0006730526161528472</v>
-      </c>
-      <c r="R153">
-        <v>0.0006730526161528472</v>
-      </c>
-      <c r="S153">
-        <v>12.48403981871125</v>
-      </c>
-      <c r="T153">
-        <v>28.50558304936636</v>
-      </c>
-      <c r="U153">
-        <v>0.996384734366299</v>
-      </c>
-      <c r="V153">
-        <v>0.6862216716354762</v>
-      </c>
-      <c r="W153">
-        <v>0.07787462701468174</v>
-      </c>
-      <c r="X153">
-        <v>0.07636508241688436</v>
-      </c>
-      <c r="Y153">
-        <v>0.1675117941291408</v>
-      </c>
-      <c r="Z153">
-        <v>0.1884206273728783</v>
-      </c>
-      <c r="AA153">
-        <v>0.9985524899474487</v>
-      </c>
-      <c r="AB153">
-        <v>0.8421952050776198</v>
-      </c>
-      <c r="AC153">
-        <v>0.8318309742131449</v>
-      </c>
-      <c r="AD153">
-        <v>0.9985060231121184</v>
-      </c>
-      <c r="AE153">
-        <v>0.7870724390564318</v>
-      </c>
-      <c r="AF153">
-        <v>0.8139167779782349</v>
-      </c>
-      <c r="AG153">
-        <v>0.0087516756243736</v>
-      </c>
-      <c r="AH153">
-        <v>0.008477139319420332</v>
-      </c>
-      <c r="AI153">
-        <v>0.9985524899474487</v>
-      </c>
-      <c r="AJ153">
-        <v>0.9985060231121184</v>
-      </c>
-      <c r="AK153">
-        <v>0.0087516756243736</v>
-      </c>
-      <c r="AL153">
-        <v>0.008477139319420332</v>
-      </c>
-      <c r="AM153" t="s">
-        <v>244</v>
-      </c>
-      <c r="AN153">
-        <v>0.05965595413851525</v>
-      </c>
-      <c r="AO153">
-        <v>0.06569108848759826</v>
-      </c>
-      <c r="AP153">
-        <v>-2527.972262422</v>
-      </c>
-      <c r="AQ153">
-        <v>-8077.206215980001</v>
-      </c>
-      <c r="AR153">
-        <v>71183.00981757799</v>
-      </c>
-      <c r="AS153">
-        <v>66359.86412402045</v>
-      </c>
-      <c r="AT153">
-        <v>71184.76971757799</v>
-      </c>
-      <c r="AU153">
-        <v>66355.53628402045</v>
-      </c>
-      <c r="AV153">
-        <v>6.118300981757798</v>
-      </c>
-      <c r="AW153">
-        <v>5.635986412402045</v>
-      </c>
-      <c r="AX153">
-        <v>1.922550437620531</v>
-      </c>
-      <c r="AY153">
-        <v>0.8419571872893674</v>
-      </c>
-      <c r="AZ153">
-        <v>75.96666666666667</v>
-      </c>
-      <c r="BA153">
-        <v>38.35</v>
-      </c>
-      <c r="BB153">
-        <v>0.0119231640291018</v>
-      </c>
-      <c r="BC153">
-        <v>0.07972402355996953</v>
-      </c>
-      <c r="BD153">
-        <v>-768.8030547225367</v>
-      </c>
-      <c r="BE153">
-        <v>-5582.219513970262</v>
-      </c>
-      <c r="BF153">
-        <v>6282</v>
-      </c>
-      <c r="BG153">
-        <v>17216</v>
-      </c>
-      <c r="BH153">
-        <v>1439.998611111111</v>
-      </c>
-      <c r="BI153">
-        <v>11695</v>
-      </c>
-      <c r="BJ153">
-        <v>23832</v>
-      </c>
-      <c r="BK153">
-        <v>17977</v>
-      </c>
-      <c r="BL153">
-        <v>41048</v>
-      </c>
-      <c r="BM153">
-        <v>0</v>
-      </c>
-      <c r="BN153">
-        <v>0</v>
-      </c>
-      <c r="BO153">
-        <v>5297</v>
-      </c>
-      <c r="BP153">
-        <v>15670</v>
-      </c>
-      <c r="BQ153">
-        <v>0</v>
-      </c>
-      <c r="BR153">
-        <v>0</v>
-      </c>
-      <c r="BS153">
-        <v>985</v>
-      </c>
-      <c r="BT153">
-        <v>1546</v>
-      </c>
-      <c r="BU153">
-        <v>11695</v>
-      </c>
-      <c r="BV153">
-        <v>23832</v>
-      </c>
-      <c r="BW153">
-        <v>61183.00981757801</v>
-      </c>
-      <c r="BX153">
-        <v>56359.86412402001</v>
-      </c>
-      <c r="BY153">
-        <v>0.0825482504461246</v>
-      </c>
-      <c r="BZ153">
-        <v>0.06845783195325277</v>
-      </c>
-      <c r="CA153">
-        <v>0.2010601196676451</v>
-      </c>
-      <c r="CB153">
-        <v>0.1568886932104819</v>
-      </c>
-      <c r="CC153">
-        <v>0.009236451697664624</v>
-      </c>
-      <c r="CD153">
-        <v>0.01018854513380211</v>
-      </c>
-      <c r="CE153">
-        <v>0.01294118899758029</v>
-      </c>
-      <c r="CF153">
-        <v>0.009968466131137551</v>
-      </c>
-      <c r="CG153">
-        <v>63710.98208000002</v>
-      </c>
-      <c r="CH153">
-        <v>64437.07034000001</v>
-      </c>
-      <c r="CI153">
-        <v>64479.78513472255</v>
-      </c>
-      <c r="CJ153">
-        <v>70019.28985397027</v>
-      </c>
-      <c r="CK153">
-        <v>0.2091801955866159</v>
-      </c>
-      <c r="CL153">
-        <v>0.1462312238727882</v>
-      </c>
-      <c r="CM153">
-        <v>10000</v>
-      </c>
-      <c r="CO153">
-        <v>0.03124909580162611</v>
-      </c>
-      <c r="CP153">
-        <v>0.01854691704522439</v>
-      </c>
-      <c r="CQ153">
-        <v>48932006.51948117</v>
-      </c>
-      <c r="CR153">
-        <v>56740598.89710363</v>
-      </c>
-      <c r="CS153" s="2">
-        <v>45541.01923338153</v>
-      </c>
-      <c r="CT153">
-        <v>-0.8064255886182842</v>
-      </c>
-      <c r="CU153">
-        <v>-0.7724972631530349</v>
-      </c>
-    </row>
-    <row r="154" spans="10:99">
-      <c r="J154" t="s">
-        <v>232</v>
-      </c>
-      <c r="K154">
-        <v>0.0007843565991936252</v>
-      </c>
-      <c r="L154">
-        <v>0.0007843565991936252</v>
-      </c>
-      <c r="M154">
-        <v>0.00153633942446274</v>
-      </c>
-      <c r="N154">
-        <v>0.00153633942446274</v>
-      </c>
-      <c r="O154">
-        <v>0.0007094521679432697</v>
-      </c>
-      <c r="P154">
-        <v>0.0007094521679432697</v>
-      </c>
-      <c r="Q154">
-        <v>0.0009943027425494578</v>
-      </c>
-      <c r="R154">
-        <v>0.0009943027425494578</v>
-      </c>
-      <c r="S154">
-        <v>6.120246048786336</v>
-      </c>
-      <c r="T154">
-        <v>9.644277180937504</v>
-      </c>
-      <c r="U154">
-        <v>0.9944710117642555</v>
-      </c>
-      <c r="V154">
-        <v>0.707962058385367</v>
-      </c>
-      <c r="W154">
-        <v>0.059065585869127</v>
-      </c>
-      <c r="X154">
-        <v>0.0993364132816321</v>
-      </c>
-      <c r="Y154">
-        <v>0.2198769519029539</v>
-      </c>
-      <c r="Z154">
-        <v>0.1792287518479593</v>
-      </c>
-      <c r="AA154">
-        <v>0.9992345958731407</v>
-      </c>
-      <c r="AB154">
-        <v>0.8097850414303209</v>
-      </c>
-      <c r="AC154">
-        <v>0.8386283536897322</v>
-      </c>
-      <c r="AD154">
-        <v>0.9982324656575681</v>
-      </c>
-      <c r="AE154">
-        <v>0.7366940451455581</v>
-      </c>
-      <c r="AF154">
-        <v>0.8290195899625088</v>
-      </c>
-      <c r="AG154">
-        <v>0.006665919517405538</v>
-      </c>
-      <c r="AH154">
-        <v>0.009974970531181647</v>
-      </c>
-      <c r="AI154">
-        <v>0.9992345958731407</v>
-      </c>
-      <c r="AJ154">
-        <v>0.9982324656575681</v>
-      </c>
-      <c r="AK154">
-        <v>0.006665919517405538</v>
-      </c>
-      <c r="AL154">
-        <v>0.009974970531181647</v>
-      </c>
-      <c r="AM154" t="s">
-        <v>244</v>
-      </c>
-      <c r="AN154">
-        <v>0.02571118579126636</v>
-      </c>
-      <c r="AO154">
-        <v>0.0612139838128191</v>
-      </c>
-      <c r="AP154">
-        <v>-545.844836524</v>
-      </c>
-      <c r="AQ154">
-        <v>-2827.512254194</v>
-      </c>
-      <c r="AR154">
-        <v>30846.82892347604</v>
-      </c>
-      <c r="AS154">
-        <v>90754.74789580594</v>
-      </c>
-      <c r="AT154">
-        <v>30846.82892347604</v>
-      </c>
-      <c r="AU154">
-        <v>90692.94501580593</v>
-      </c>
-      <c r="AV154">
-        <v>2.084682892347604</v>
-      </c>
-      <c r="AW154">
-        <v>8.075474789580595</v>
-      </c>
-      <c r="AX154">
-        <v>3.920511070670306</v>
-      </c>
-      <c r="AY154">
-        <v>2.488549260194875</v>
-      </c>
-      <c r="AZ154">
-        <v>94.34999999999999</v>
-      </c>
-      <c r="BA154">
-        <v>51.83333333333334</v>
-      </c>
-      <c r="BB154">
-        <v>0.07367997301171074</v>
-      </c>
-      <c r="BC154">
-        <v>0.06677813608918472</v>
-      </c>
-      <c r="BD154">
-        <v>-1701.584311428319</v>
-      </c>
-      <c r="BE154">
-        <v>-5980.858099003707</v>
-      </c>
-      <c r="BF154">
-        <v>4136</v>
-      </c>
-      <c r="BG154">
-        <v>4854</v>
-      </c>
-      <c r="BH154">
-        <v>1436.706944444444</v>
-      </c>
-      <c r="BI154">
-        <v>4657</v>
-      </c>
-      <c r="BJ154">
-        <v>9002</v>
-      </c>
-      <c r="BK154">
-        <v>8793</v>
-      </c>
-      <c r="BL154">
-        <v>13856</v>
-      </c>
-      <c r="BM154">
-        <v>0</v>
-      </c>
-      <c r="BN154">
-        <v>0</v>
-      </c>
-      <c r="BO154">
-        <v>71</v>
-      </c>
-      <c r="BP154">
-        <v>3003</v>
-      </c>
-      <c r="BQ154">
-        <v>0</v>
-      </c>
-      <c r="BR154">
-        <v>0</v>
-      </c>
-      <c r="BS154">
-        <v>4065</v>
-      </c>
-      <c r="BT154">
-        <v>1851</v>
-      </c>
-      <c r="BU154">
-        <v>4657</v>
-      </c>
-      <c r="BV154">
-        <v>9002</v>
-      </c>
-      <c r="BW154">
-        <v>20846.82892347597</v>
-      </c>
-      <c r="BX154">
-        <v>80754.74789580592</v>
-      </c>
-      <c r="BY154">
-        <v>0.08329926461958016</v>
-      </c>
-      <c r="BZ154">
-        <v>0.08408573892944785</v>
-      </c>
-      <c r="CA154">
-        <v>0.2683138366192507</v>
-      </c>
-      <c r="CB154">
-        <v>0.1708521324593514</v>
-      </c>
-      <c r="CC154">
-        <v>0.0172489774041921</v>
-      </c>
-      <c r="CD154">
-        <v>0.01199360158031172</v>
-      </c>
-      <c r="CE154">
-        <v>0.01687145019977058</v>
-      </c>
-      <c r="CF154">
-        <v>0.01279764853236176</v>
-      </c>
-      <c r="CG154">
-        <v>21392.67375999997</v>
-      </c>
-      <c r="CH154">
-        <v>83582.26014999991</v>
-      </c>
-      <c r="CI154">
-        <v>23094.25807142829</v>
-      </c>
-      <c r="CJ154">
-        <v>89563.11824900362</v>
-      </c>
-      <c r="CK154">
-        <v>0.1171785543307918</v>
-      </c>
-      <c r="CL154">
-        <v>0.1491951124597834</v>
-      </c>
-      <c r="CM154">
-        <v>10000</v>
-      </c>
-      <c r="CO154">
-        <v>0.004582100806217737</v>
-      </c>
-      <c r="CP154">
-        <v>0.01586334899367786</v>
-      </c>
-      <c r="CQ154">
-        <v>8559234.822575567</v>
-      </c>
-      <c r="CR154">
-        <v>63330179.18358867</v>
-      </c>
-      <c r="CS154" s="2">
-        <v>45541.42294348889</v>
-      </c>
-      <c r="CT154">
-        <v>-0.8563809420370235</v>
-      </c>
-      <c r="CU154">
-        <v>-0.7090733064609169</v>
-      </c>
-    </row>
-    <row r="155" spans="10:99">
-      <c r="J155" t="s">
-        <v>243</v>
-      </c>
-      <c r="K155">
-        <v>0.0007874408358226059</v>
-      </c>
-      <c r="L155">
-        <v>0.0007874408358226059</v>
-      </c>
-      <c r="M155">
-        <v>0.001461924244027246</v>
-      </c>
-      <c r="N155">
-        <v>0.001461924244027246</v>
-      </c>
-      <c r="O155">
-        <v>0.0007091576196501581</v>
-      </c>
-      <c r="P155">
-        <v>0.0007091576196501581</v>
-      </c>
-      <c r="Q155">
-        <v>0.001316948283100494</v>
-      </c>
-      <c r="R155">
-        <v>0.001316948283100494</v>
-      </c>
-      <c r="S155">
-        <v>6.917153869641946</v>
-      </c>
-      <c r="T155">
-        <v>7.540175344293897</v>
-      </c>
-      <c r="U155">
-        <v>0.9946753372141043</v>
-      </c>
-      <c r="V155">
-        <v>0.6356886397446692</v>
-      </c>
-      <c r="W155">
-        <v>0.09225337502510826</v>
-      </c>
-      <c r="X155">
-        <v>0.09980855305094893</v>
-      </c>
-      <c r="Y155">
-        <v>0.2362253934726235</v>
-      </c>
-      <c r="Z155">
-        <v>0.2234705581314674</v>
-      </c>
-      <c r="AA155">
-        <v>0.9986273278577874</v>
-      </c>
-      <c r="AB155">
-        <v>0.7762653653814799</v>
-      </c>
-      <c r="AC155">
-        <v>0.8063659044589523</v>
-      </c>
-      <c r="AD155">
-        <v>0.9970840801340662</v>
-      </c>
-      <c r="AE155">
-        <v>0.7661900432002213</v>
-      </c>
-      <c r="AF155">
-        <v>0.7772653897943246</v>
-      </c>
-      <c r="AG155">
-        <v>0.01088172376438835</v>
-      </c>
-      <c r="AH155">
-        <v>0.01175773765724271</v>
-      </c>
-      <c r="AI155">
-        <v>0.9986273278577874</v>
-      </c>
-      <c r="AJ155">
-        <v>0.9970840801340662</v>
-      </c>
-      <c r="AK155">
-        <v>0.01088172376438835</v>
-      </c>
-      <c r="AL155">
-        <v>0.01175773765724271</v>
-      </c>
-      <c r="AM155" t="s">
-        <v>244</v>
-      </c>
-      <c r="AN155">
-        <v>0.03244426465269235</v>
-      </c>
-      <c r="AO155">
-        <v>0.07987066753881372</v>
-      </c>
-      <c r="AP155">
-        <v>-534.628112</v>
-      </c>
-      <c r="AQ155">
-        <v>-1375.056872564</v>
-      </c>
-      <c r="AR155">
-        <v>30668.28064799989</v>
-      </c>
-      <c r="AS155">
-        <v>80031.22598743613</v>
-      </c>
-      <c r="AT155">
-        <v>30664.26637799989</v>
-      </c>
-      <c r="AU155">
-        <v>80031.22598743613</v>
-      </c>
-      <c r="AV155">
-        <v>2.066828064799989</v>
-      </c>
-      <c r="AW155">
-        <v>7.003122598743614</v>
-      </c>
-      <c r="AX155">
-        <v>3.469049795199892</v>
-      </c>
-      <c r="AY155">
-        <v>3.182395503384883</v>
-      </c>
-      <c r="AZ155">
-        <v>84.13333333333334</v>
-      </c>
-      <c r="BA155">
-        <v>80.41666666666667</v>
-      </c>
-      <c r="BB155">
-        <v>0.0650775197558405</v>
-      </c>
-      <c r="BC155">
-        <v>0.04376090618998604</v>
-      </c>
-      <c r="BD155">
-        <v>-1475.879276482725</v>
-      </c>
-      <c r="BE155">
-        <v>-3267.805788154597</v>
-      </c>
-      <c r="BF155">
-        <v>4736</v>
-      </c>
-      <c r="BG155">
-        <v>8315</v>
-      </c>
-      <c r="BH155">
-        <v>1423.706944444444</v>
-      </c>
-      <c r="BI155">
-        <v>5112</v>
-      </c>
-      <c r="BJ155">
-        <v>2420</v>
-      </c>
-      <c r="BK155">
-        <v>9848</v>
-      </c>
-      <c r="BL155">
-        <v>10735</v>
-      </c>
-      <c r="BM155">
-        <v>0</v>
-      </c>
-      <c r="BN155">
-        <v>0</v>
-      </c>
-      <c r="BO155">
-        <v>151</v>
-      </c>
-      <c r="BP155">
-        <v>445</v>
-      </c>
-      <c r="BQ155">
-        <v>0</v>
-      </c>
-      <c r="BR155">
-        <v>0</v>
-      </c>
-      <c r="BS155">
-        <v>4585</v>
-      </c>
-      <c r="BT155">
-        <v>7870</v>
-      </c>
-      <c r="BU155">
-        <v>5112</v>
-      </c>
-      <c r="BV155">
-        <v>2420</v>
-      </c>
-      <c r="BW155">
-        <v>20668.28064800002</v>
-      </c>
-      <c r="BX155">
-        <v>70031.22598743605</v>
-      </c>
-      <c r="BY155">
-        <v>0.1170193221367332</v>
-      </c>
-      <c r="BZ155">
-        <v>0.1008678239126301</v>
-      </c>
-      <c r="CA155">
-        <v>0.3117112869774564</v>
-      </c>
-      <c r="CB155">
-        <v>0.1821641144000655</v>
-      </c>
-      <c r="CC155">
-        <v>0.0199837559293953</v>
-      </c>
-      <c r="CD155">
-        <v>0.02334639384316032</v>
-      </c>
-      <c r="CE155">
-        <v>0.02148495729427865</v>
-      </c>
-      <c r="CF155">
-        <v>0.02090287506928901</v>
-      </c>
-      <c r="CG155">
-        <v>21202.90876000002</v>
-      </c>
-      <c r="CH155">
-        <v>71406.28286000005</v>
-      </c>
-      <c r="CI155">
-        <v>22678.78803648274</v>
-      </c>
-      <c r="CJ155">
-        <v>74674.08864815465</v>
-      </c>
-      <c r="CK155">
-        <v>0.07939574083908092</v>
-      </c>
-      <c r="CL155">
-        <v>0.1067798788311242</v>
-      </c>
-      <c r="CM155">
-        <v>10000</v>
-      </c>
-      <c r="CO155">
-        <v>0.008838162130523851</v>
-      </c>
-      <c r="CP155">
-        <v>0.01984196663740123</v>
-      </c>
-      <c r="CQ155">
-        <v>13053001.74351714</v>
-      </c>
-      <c r="CR155">
-        <v>39462546.04624498</v>
-      </c>
-      <c r="CS155" s="2">
-        <v>45541.60396500168</v>
-      </c>
-      <c r="CT155">
-        <v>-0.7675437736784942</v>
-      </c>
-      <c r="CU155">
-        <v>-0.6130242688530818</v>
-      </c>
-    </row>
-    <row r="156" spans="10:99">
-      <c r="J156" t="s">
-        <v>222</v>
-      </c>
-      <c r="K156">
-        <v>0.001019362423848813</v>
-      </c>
-      <c r="L156">
-        <v>0.001019362423848813</v>
-      </c>
-      <c r="M156">
-        <v>0.0009737504407758557</v>
-      </c>
-      <c r="N156">
-        <v>0.0009737504407758557</v>
-      </c>
-      <c r="O156">
-        <v>0.0009057864588954301</v>
-      </c>
-      <c r="P156">
-        <v>0.0009057864588954301</v>
-      </c>
-      <c r="Q156">
-        <v>0.000373093361672372</v>
-      </c>
-      <c r="R156">
-        <v>0.000373093361672372</v>
-      </c>
-      <c r="S156">
-        <v>5.555560913928351</v>
-      </c>
-      <c r="T156">
-        <v>6.092366987236677</v>
-      </c>
-      <c r="U156">
-        <v>0.9999672408283798</v>
-      </c>
-      <c r="V156">
-        <v>0.6362413483200143</v>
-      </c>
-      <c r="W156">
-        <v>0.09531144901077192</v>
-      </c>
-      <c r="X156">
-        <v>0.05975277972079557</v>
-      </c>
-      <c r="Y156">
-        <v>0.2434019552580584</v>
-      </c>
-      <c r="Z156">
-        <v>0.2252194507762023</v>
-      </c>
-      <c r="AA156">
-        <v>0.9975560777150345</v>
-      </c>
-      <c r="AB156">
-        <v>0.796858356866104</v>
-      </c>
-      <c r="AC156">
-        <v>0.8031428080226751</v>
-      </c>
-      <c r="AD156">
-        <v>0.9990411314488882</v>
-      </c>
-      <c r="AE156">
-        <v>0.7584930254447194</v>
-      </c>
-      <c r="AF156">
-        <v>0.7776905392432638</v>
-      </c>
-      <c r="AG156">
-        <v>0.01112742793926059</v>
-      </c>
-      <c r="AH156">
-        <v>0.007282914863473273</v>
-      </c>
-      <c r="AI156">
-        <v>0.9975560777150345</v>
-      </c>
-      <c r="AJ156">
-        <v>0.9990411314488882</v>
-      </c>
-      <c r="AK156">
-        <v>0.01112742793926059</v>
-      </c>
-      <c r="AL156">
-        <v>0.007282914863473273</v>
-      </c>
-      <c r="AM156" t="s">
-        <v>244</v>
-      </c>
-      <c r="AN156">
-        <v>0.06697457918144563</v>
-      </c>
-      <c r="AO156">
-        <v>0.03405234731275385</v>
-      </c>
-      <c r="AP156">
-        <v>-803.7593923200001</v>
-      </c>
-      <c r="AQ156">
-        <v>-786.01610246</v>
-      </c>
-      <c r="AR156">
-        <v>43367.83010768007</v>
-      </c>
-      <c r="AS156">
-        <v>40613.56491679172</v>
-      </c>
-      <c r="AT156">
-        <v>43358.25450768007</v>
-      </c>
-      <c r="AU156">
-        <v>40618.21129753976</v>
-      </c>
-      <c r="AV156">
-        <v>3.336783010768007</v>
-      </c>
-      <c r="AW156">
-        <v>3.061356491679172</v>
-      </c>
-      <c r="AX156">
-        <v>4.319408676084511</v>
-      </c>
-      <c r="AY156">
-        <v>3.938641890864873</v>
-      </c>
-      <c r="AZ156">
-        <v>66.71666666666667</v>
-      </c>
-      <c r="BA156">
-        <v>60.36666666666667</v>
-      </c>
-      <c r="BB156">
-        <v>0.07246768829662328</v>
-      </c>
-      <c r="BC156">
-        <v>0.106263022336795</v>
-      </c>
-      <c r="BD156">
-        <v>-2669.811137833539</v>
-      </c>
-      <c r="BE156">
-        <v>-3733.329226165388</v>
-      </c>
-      <c r="BF156">
-        <v>4481</v>
-      </c>
-      <c r="BG156">
-        <v>3153</v>
-      </c>
-      <c r="BH156">
-        <v>1439.998611111111</v>
-      </c>
-      <c r="BI156">
-        <v>3519</v>
-      </c>
-      <c r="BJ156">
-        <v>5620</v>
-      </c>
-      <c r="BK156">
-        <v>8000</v>
-      </c>
-      <c r="BL156">
-        <v>8773</v>
-      </c>
-      <c r="BM156">
-        <v>0</v>
-      </c>
-      <c r="BN156">
-        <v>0</v>
-      </c>
-      <c r="BO156">
-        <v>183</v>
-      </c>
-      <c r="BP156">
-        <v>1035</v>
-      </c>
-      <c r="BQ156">
-        <v>0</v>
-      </c>
-      <c r="BR156">
-        <v>0</v>
-      </c>
-      <c r="BS156">
-        <v>4298</v>
-      </c>
-      <c r="BT156">
-        <v>2118</v>
-      </c>
-      <c r="BU156">
-        <v>3519</v>
-      </c>
-      <c r="BV156">
-        <v>5620</v>
-      </c>
-      <c r="BW156">
-        <v>33367.83010768</v>
-      </c>
-      <c r="BX156">
-        <v>30613.56491679188</v>
-      </c>
-      <c r="BY156">
-        <v>0.1099570854519043</v>
-      </c>
-      <c r="BZ156">
-        <v>0.0695498981197728</v>
-      </c>
-      <c r="CA156">
-        <v>0.3184027205808249</v>
-      </c>
-      <c r="CB156">
-        <v>0.1818750054408434</v>
-      </c>
-      <c r="CC156">
-        <v>0.02412767197452832</v>
-      </c>
-      <c r="CD156">
-        <v>0.01598763713030481</v>
-      </c>
-      <c r="CE156">
-        <v>0.02185689162478268</v>
-      </c>
-      <c r="CF156">
-        <v>0.01346670727632281</v>
-      </c>
-      <c r="CG156">
-        <v>34171.58949999999</v>
-      </c>
-      <c r="CH156">
-        <v>31399.58101925188</v>
-      </c>
-      <c r="CI156">
-        <v>36841.40063783353</v>
-      </c>
-      <c r="CJ156">
-        <v>35132.91024541727</v>
-      </c>
-      <c r="CK156">
-        <v>0.09078370111895454</v>
-      </c>
-      <c r="CL156">
-        <v>0.1362059278628572</v>
-      </c>
-      <c r="CM156">
-        <v>10000</v>
-      </c>
-      <c r="CO156">
-        <v>0.02265559445617893</v>
-      </c>
-      <c r="CP156">
-        <v>0.006625965683863314</v>
-      </c>
-      <c r="CQ156">
-        <v>20520037.44911024</v>
-      </c>
-      <c r="CR156">
-        <v>15098410.24104184</v>
-      </c>
-      <c r="CS156" s="2">
-        <v>45541.83903305073</v>
-      </c>
-      <c r="CT156">
-        <v>-0.6908626175691092</v>
-      </c>
-      <c r="CU156">
-        <v>-0.8400892136604561</v>
-      </c>
-    </row>
-    <row r="157" spans="10:99">
-      <c r="J157" t="s">
-        <v>176</v>
-      </c>
-      <c r="K157">
-        <v>0.0009219562221054467</v>
-      </c>
-      <c r="L157">
-        <v>0.0009219562221054467</v>
-      </c>
-      <c r="M157">
-        <v>0.001021606238448935</v>
-      </c>
-      <c r="N157">
-        <v>0.001021606238448935</v>
-      </c>
-      <c r="O157">
-        <v>0.0007158017042718567</v>
-      </c>
-      <c r="P157">
-        <v>0.0007158017042718567</v>
-      </c>
-      <c r="Q157">
-        <v>0.0007548130339735337</v>
-      </c>
-      <c r="R157">
-        <v>0.0007548130339735337</v>
-      </c>
-      <c r="S157">
-        <v>6.888895533271155</v>
-      </c>
-      <c r="T157">
-        <v>20.81738118960377</v>
-      </c>
-      <c r="U157">
-        <v>0.9913923732653491</v>
-      </c>
-      <c r="V157">
-        <v>0.697305638645183</v>
-      </c>
-      <c r="W157">
-        <v>0.09543438929411133</v>
-      </c>
-      <c r="X157">
-        <v>0.05761063337171857</v>
-      </c>
-      <c r="Y157">
-        <v>0.1490198533961702</v>
-      </c>
-      <c r="Z157">
-        <v>0.184757176897363</v>
-      </c>
-      <c r="AA157">
-        <v>0.9982906150915102</v>
-      </c>
-      <c r="AB157">
-        <v>0.8643420436194059</v>
-      </c>
-      <c r="AC157">
-        <v>0.8385236033265329</v>
-      </c>
-      <c r="AD157">
-        <v>0.9990468047365818</v>
-      </c>
-      <c r="AE157">
-        <v>0.7273492459647685</v>
-      </c>
-      <c r="AF157">
-        <v>0.8216620167261901</v>
-      </c>
-      <c r="AG157">
-        <v>0.009952275419430463</v>
-      </c>
-      <c r="AH157">
-        <v>0.006177937815664242</v>
-      </c>
-      <c r="AI157">
-        <v>0.9982906150915102</v>
-      </c>
-      <c r="AJ157">
-        <v>0.9990468047365818</v>
-      </c>
-      <c r="AK157">
-        <v>0.009952275419430463</v>
-      </c>
-      <c r="AL157">
-        <v>0.006177937815664242</v>
-      </c>
-      <c r="AM157" t="s">
-        <v>244</v>
-      </c>
-      <c r="AN157">
-        <v>0.06577318605636155</v>
-      </c>
-      <c r="AO157">
-        <v>0.05239122198265308</v>
-      </c>
-      <c r="AP157">
-        <v>-950.4398444000001</v>
-      </c>
-      <c r="AQ157">
-        <v>-2548.68232334</v>
-      </c>
-      <c r="AR157">
-        <v>37697.32535560007</v>
-      </c>
-      <c r="AS157">
-        <v>43508.03877665997</v>
-      </c>
-      <c r="AT157">
-        <v>37688.36435560007</v>
-      </c>
-      <c r="AU157">
-        <v>43508.03877665997</v>
-      </c>
-      <c r="AV157">
-        <v>2.769732535560007</v>
-      </c>
-      <c r="AW157">
-        <v>3.350803877665997</v>
-      </c>
-      <c r="AX157">
-        <v>3.483361898040797</v>
-      </c>
-      <c r="AY157">
-        <v>1.15259429766035</v>
-      </c>
-      <c r="AZ157">
-        <v>52.4</v>
-      </c>
-      <c r="BA157">
-        <v>57.28333333333333</v>
-      </c>
-      <c r="BB157">
-        <v>0.03826578617569007</v>
-      </c>
-      <c r="BC157">
-        <v>0.04996460626527787</v>
-      </c>
-      <c r="BD157">
-        <v>-1139.846375221954</v>
-      </c>
-      <c r="BE157">
-        <v>-1896.3081637372</v>
-      </c>
-      <c r="BF157">
-        <v>3276</v>
-      </c>
-      <c r="BG157">
-        <v>9163</v>
-      </c>
-      <c r="BH157">
-        <v>1439.998611111111</v>
-      </c>
-      <c r="BI157">
-        <v>6644</v>
-      </c>
-      <c r="BJ157">
-        <v>20814</v>
-      </c>
-      <c r="BK157">
-        <v>9920</v>
-      </c>
-      <c r="BL157">
-        <v>29977</v>
-      </c>
-      <c r="BM157">
-        <v>0</v>
-      </c>
-      <c r="BN157">
-        <v>0</v>
-      </c>
-      <c r="BO157">
-        <v>2061</v>
-      </c>
-      <c r="BP157">
-        <v>5502</v>
-      </c>
-      <c r="BQ157">
-        <v>0</v>
-      </c>
-      <c r="BR157">
-        <v>0</v>
-      </c>
-      <c r="BS157">
-        <v>1215</v>
-      </c>
-      <c r="BT157">
-        <v>3661</v>
-      </c>
-      <c r="BU157">
-        <v>6644</v>
-      </c>
-      <c r="BV157">
-        <v>20814</v>
-      </c>
-      <c r="BW157">
-        <v>27697.32535559999</v>
-      </c>
-      <c r="BX157">
-        <v>33508.03877666004</v>
-      </c>
-      <c r="BY157">
-        <v>0.0984925899152552</v>
-      </c>
-      <c r="BZ157">
-        <v>0.04967606411233294</v>
-      </c>
-      <c r="CA157">
-        <v>0.2981715057061041</v>
-      </c>
-      <c r="CB157">
-        <v>0.1513470000924703</v>
-      </c>
-      <c r="CC157">
-        <v>0.01128669015859226</v>
-      </c>
-      <c r="CD157">
-        <v>0.0073849163798192</v>
-      </c>
-      <c r="CE157">
-        <v>0.01393803250499442</v>
-      </c>
-      <c r="CF157">
-        <v>0.008301299482969062</v>
-      </c>
-      <c r="CG157">
-        <v>28647.76519999999</v>
-      </c>
-      <c r="CH157">
-        <v>36056.72110000004</v>
-      </c>
-      <c r="CI157">
-        <v>29787.61157522195</v>
-      </c>
-      <c r="CJ157">
-        <v>37953.02926373724</v>
-      </c>
-      <c r="CK157">
-        <v>0.1353554399173141</v>
-      </c>
-      <c r="CL157">
-        <v>0.1480319356586776</v>
-      </c>
-      <c r="CM157">
-        <v>10000</v>
-      </c>
-      <c r="CO157">
-        <v>0.02592517577616388</v>
-      </c>
-      <c r="CP157">
-        <v>0.01955961922398079</v>
-      </c>
-      <c r="CQ157">
-        <v>17125292.63383621</v>
-      </c>
-      <c r="CR157">
-        <v>51239540.92325264</v>
-      </c>
-      <c r="CS157" s="2">
-        <v>45542.05352771992</v>
-      </c>
-      <c r="CT157">
-        <v>-0.8207165518084033</v>
-      </c>
-      <c r="CU157">
-        <v>-0.8156135517063872</v>
-      </c>
-    </row>
-    <row r="158" spans="10:99">
-      <c r="J158" t="s">
-        <v>196</v>
-      </c>
-      <c r="K158">
-        <v>0.0009847133187756985</v>
-      </c>
-      <c r="L158">
-        <v>0.0009847133187756985</v>
-      </c>
-      <c r="M158">
-        <v>0.000177110550394044</v>
-      </c>
-      <c r="N158">
-        <v>0.000177110550394044</v>
-      </c>
-      <c r="O158">
-        <v>0.0006828386426430244</v>
-      </c>
-      <c r="P158">
-        <v>0.0006828386426430244</v>
-      </c>
-      <c r="Q158">
-        <v>9.784127854464141E-05</v>
-      </c>
-      <c r="R158">
-        <v>9.784127854464141E-05</v>
-      </c>
-      <c r="S158">
-        <v>8.193892550664573</v>
-      </c>
-      <c r="T158">
-        <v>9.89090600234152</v>
-      </c>
-      <c r="U158">
-        <v>0.9996496993042026</v>
-      </c>
-      <c r="V158">
-        <v>0.6728781863269108</v>
-      </c>
-      <c r="W158">
-        <v>0.08568016570009003</v>
-      </c>
-      <c r="X158">
-        <v>0.08058409999872683</v>
-      </c>
-      <c r="Y158">
-        <v>0.2449095637395339</v>
-      </c>
-      <c r="Z158">
-        <v>0.2291436549757783</v>
-      </c>
-      <c r="AA158">
-        <v>0.9985659742954034</v>
-      </c>
-      <c r="AB158">
-        <v>0.7826209792439608</v>
-      </c>
-      <c r="AC158">
-        <v>0.8192282510584151</v>
-      </c>
-      <c r="AD158">
-        <v>0.9988904077698645</v>
-      </c>
-      <c r="AE158">
-        <v>0.6509511769182851</v>
-      </c>
-      <c r="AF158">
-        <v>0.8044017719449525</v>
-      </c>
-      <c r="AG158">
-        <v>0.009666184227992071</v>
-      </c>
-      <c r="AH158">
-        <v>0.008008559287370893</v>
-      </c>
-      <c r="AI158">
-        <v>0.9985659742954034</v>
-      </c>
-      <c r="AJ158">
-        <v>0.9988904077698645</v>
-      </c>
-      <c r="AK158">
-        <v>0.009666184227992071</v>
-      </c>
-      <c r="AL158">
-        <v>0.008008559287370893</v>
-      </c>
-      <c r="AM158" t="s">
-        <v>244</v>
-      </c>
-      <c r="AN158">
-        <v>0.03970236948954436</v>
-      </c>
-      <c r="AO158">
-        <v>0.02693207923708976</v>
-      </c>
-      <c r="AP158">
-        <v>-799.1750500400001</v>
-      </c>
-      <c r="AQ158">
-        <v>-446.49869214</v>
-      </c>
-      <c r="AR158">
-        <v>41218.57394995987</v>
-      </c>
-      <c r="AS158">
-        <v>12902.54220786004</v>
-      </c>
-      <c r="AT158">
-        <v>41189.87794995987</v>
-      </c>
-      <c r="AU158">
-        <v>12902.25420786004</v>
-      </c>
-      <c r="AV158">
-        <v>3.121857394995987</v>
-      </c>
-      <c r="AW158">
-        <v>0.2902542207860039</v>
-      </c>
-      <c r="AX158">
-        <v>2.928481764206955</v>
-      </c>
-      <c r="AY158">
-        <v>2.426415823496346</v>
-      </c>
-      <c r="AZ158">
-        <v>63.38333333333333</v>
-      </c>
-      <c r="BA158">
-        <v>17.51666666666667</v>
-      </c>
-      <c r="BB158">
-        <v>0.04957865386558762</v>
-      </c>
-      <c r="BC158">
-        <v>0.6872977584247519</v>
-      </c>
-      <c r="BD158">
-        <v>-1670.203327905652</v>
-      </c>
-      <c r="BE158">
-        <v>-7360.958756955096</v>
-      </c>
-      <c r="BF158">
-        <v>3754</v>
-      </c>
-      <c r="BG158">
-        <v>5951</v>
-      </c>
-      <c r="BH158">
-        <v>1438.998611111111</v>
-      </c>
-      <c r="BI158">
-        <v>8037</v>
-      </c>
-      <c r="BJ158">
-        <v>8282</v>
-      </c>
-      <c r="BK158">
-        <v>11791</v>
-      </c>
-      <c r="BL158">
-        <v>14233</v>
-      </c>
-      <c r="BM158">
-        <v>0</v>
-      </c>
-      <c r="BN158">
-        <v>0</v>
-      </c>
-      <c r="BO158">
-        <v>342</v>
-      </c>
-      <c r="BP158">
-        <v>375</v>
-      </c>
-      <c r="BQ158">
-        <v>0</v>
-      </c>
-      <c r="BR158">
-        <v>0</v>
-      </c>
-      <c r="BS158">
-        <v>3412</v>
-      </c>
-      <c r="BT158">
-        <v>5576</v>
-      </c>
-      <c r="BU158">
-        <v>8037</v>
-      </c>
-      <c r="BV158">
-        <v>8282</v>
-      </c>
-      <c r="BW158">
-        <v>31218.57394996002</v>
-      </c>
-      <c r="BX158">
-        <v>2902.542207859995</v>
-      </c>
-      <c r="BY158">
-        <v>0.1026209814452904</v>
-      </c>
-      <c r="BZ158">
-        <v>0.08737954624307426</v>
-      </c>
-      <c r="CA158">
-        <v>0.4338108286825653</v>
-      </c>
-      <c r="CB158">
-        <v>0.1636169704402945</v>
-      </c>
-      <c r="CC158">
-        <v>0.01697239760920564</v>
-      </c>
-      <c r="CD158">
-        <v>0.01752988379469588</v>
-      </c>
-      <c r="CE158">
-        <v>0.01804362000486143</v>
-      </c>
-      <c r="CF158">
-        <v>0.01692213429709064</v>
-      </c>
-      <c r="CG158">
-        <v>32017.74900000002</v>
-      </c>
-      <c r="CH158">
-        <v>3349.040899999995</v>
-      </c>
-      <c r="CI158">
-        <v>33687.95232790567</v>
-      </c>
-      <c r="CJ158">
-        <v>10709.99965695509</v>
-      </c>
-      <c r="CK158">
-        <v>0.09137706781739408</v>
-      </c>
-      <c r="CL158">
-        <v>0.0278078392752082</v>
-      </c>
-      <c r="CM158">
-        <v>10000</v>
-      </c>
-      <c r="CO158">
-        <v>0.01024987694356777</v>
-      </c>
-      <c r="CP158">
-        <v>0.005385528563569505</v>
-      </c>
-      <c r="CQ158">
-        <v>43542700.35438982</v>
-      </c>
-      <c r="CR158">
-        <v>5330975.417100843</v>
-      </c>
-      <c r="CS158" s="2">
-        <v>45542.27691519913</v>
-      </c>
-      <c r="CT158">
-        <v>-0.7215228330432941</v>
-      </c>
-      <c r="CU158">
-        <v>-0.8758916606232978</v>
+        <v>0.2347171187836478</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update STORJUSDT.json at 2024-09-30_20-53-23 bestfile_scores 0.0006923105369634642 bestfile_sharp 0.08595485485965598
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="389">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -746,6 +746,9 @@
   </si>
   <si>
     <t>DOGSUSDT</t>
+  </si>
+  <si>
+    <t>JTOUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1539,7 +1542,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU146"/>
+  <dimension ref="A1:CU147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1957,7 +1960,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2122,7 +2125,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2238,7 +2241,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2403,7 +2406,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2519,7 +2522,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2684,7 +2687,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2800,7 +2803,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -2965,7 +2968,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3081,7 +3084,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3246,7 +3249,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3362,7 +3365,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3527,7 +3530,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3643,7 +3646,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3808,7 +3811,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3924,7 +3927,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4089,7 +4092,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4205,7 +4208,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4370,7 +4373,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4486,7 +4489,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4651,7 +4654,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4767,7 +4770,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4932,7 +4935,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5048,7 +5051,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5213,7 +5216,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5329,7 +5332,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5494,7 +5497,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5610,7 +5613,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5775,7 +5778,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5891,7 +5894,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6056,7 +6059,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6172,7 +6175,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6337,7 +6340,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6453,7 +6456,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6618,7 +6621,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6734,7 +6737,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6899,7 +6902,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7015,7 +7018,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7180,7 +7183,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7296,7 +7299,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7461,7 +7464,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7577,7 +7580,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7742,7 +7745,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7858,7 +7861,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8023,7 +8026,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8139,7 +8142,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8304,7 +8307,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8420,7 +8423,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8585,7 +8588,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8701,7 +8704,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8866,7 +8869,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -8982,7 +8985,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9147,7 +9150,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9263,7 +9266,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9428,7 +9431,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9544,7 +9547,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9709,7 +9712,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9825,7 +9828,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -9990,7 +9993,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10106,7 +10109,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10271,7 +10274,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10387,7 +10390,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10552,7 +10555,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10668,7 +10671,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10833,7 +10836,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10949,7 +10952,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11114,7 +11117,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11236,7 +11239,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11401,7 +11404,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11523,7 +11526,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11688,7 +11691,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11810,7 +11813,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -11975,7 +11978,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12097,7 +12100,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12262,7 +12265,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12384,7 +12387,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12549,7 +12552,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12671,7 +12674,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12836,7 +12839,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12958,7 +12961,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13123,7 +13126,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13245,7 +13248,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13410,7 +13413,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13532,7 +13535,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13697,7 +13700,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13819,7 +13822,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -13984,7 +13987,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14106,7 +14109,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14271,7 +14274,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14393,7 +14396,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14558,7 +14561,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14680,7 +14683,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14845,7 +14848,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -14967,7 +14970,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15132,7 +15135,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15254,7 +15257,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15419,7 +15422,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15541,7 +15544,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15706,7 +15709,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15828,7 +15831,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -15993,7 +15996,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16115,7 +16118,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16280,7 +16283,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16402,7 +16405,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16567,7 +16570,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16689,7 +16692,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16854,7 +16857,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -16973,7 +16976,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17138,7 +17141,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17254,7 +17257,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17419,7 +17422,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17532,7 +17535,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17697,7 +17700,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17810,7 +17813,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -17975,7 +17978,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18088,7 +18091,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18253,7 +18256,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18366,7 +18369,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18531,7 +18534,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18644,7 +18647,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18809,7 +18812,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18922,7 +18925,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19087,7 +19090,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19200,7 +19203,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19365,7 +19368,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19478,7 +19481,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19643,7 +19646,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19756,7 +19759,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19921,7 +19924,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20034,7 +20037,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20205,7 +20208,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20318,7 +20321,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20489,7 +20492,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20602,7 +20605,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20773,7 +20776,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20886,7 +20889,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21057,7 +21060,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21167,7 +21170,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21338,7 +21341,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21445,7 +21448,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21616,7 +21619,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21720,7 +21723,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21891,7 +21894,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -21995,7 +21998,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22166,7 +22169,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22270,7 +22273,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22441,7 +22444,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22545,7 +22548,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22716,7 +22719,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22820,7 +22823,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -22991,7 +22994,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23095,7 +23098,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23266,7 +23269,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23367,7 +23370,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23538,7 +23541,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23639,7 +23642,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23810,7 +23813,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23911,7 +23914,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24082,7 +24085,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24183,7 +24186,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24354,7 +24357,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24455,7 +24458,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24626,7 +24629,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24727,7 +24730,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24898,7 +24901,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -24999,7 +25002,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25170,7 +25173,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25268,7 +25271,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25439,7 +25442,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25537,7 +25540,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25708,7 +25711,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25806,7 +25809,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -25977,7 +25980,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26075,7 +26078,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26246,7 +26249,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26344,7 +26347,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26515,7 +26518,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26613,7 +26616,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26784,7 +26787,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26882,7 +26885,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27053,7 +27056,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27151,7 +27154,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27322,7 +27325,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27420,7 +27423,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27591,7 +27594,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27689,7 +27692,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27860,7 +27863,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27958,7 +27961,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28129,7 +28132,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28227,7 +28230,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28398,7 +28401,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28496,7 +28499,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28667,7 +28670,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28765,7 +28768,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28936,7 +28939,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29034,7 +29037,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29205,7 +29208,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29303,7 +29306,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29474,7 +29477,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29572,7 +29575,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29743,7 +29746,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29841,7 +29844,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30012,7 +30015,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30110,7 +30113,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30281,7 +30284,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30379,7 +30382,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30550,7 +30553,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30648,7 +30651,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30819,7 +30822,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30917,7 +30920,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31088,7 +31091,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31186,7 +31189,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31357,7 +31360,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31455,7 +31458,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31626,7 +31629,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31724,7 +31727,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31895,7 +31898,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -31993,7 +31996,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32164,7 +32167,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32262,7 +32265,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32433,7 +32436,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32531,7 +32534,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32702,7 +32705,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32800,7 +32803,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -32971,7 +32974,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33069,7 +33072,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33240,7 +33243,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33338,7 +33341,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33509,7 +33512,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33607,7 +33610,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33778,7 +33781,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33876,7 +33879,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34047,7 +34050,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34145,7 +34148,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34316,7 +34319,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34414,7 +34417,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34585,7 +34588,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34683,7 +34686,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34854,7 +34857,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34952,7 +34955,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35123,7 +35126,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35221,7 +35224,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35392,7 +35395,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35490,7 +35493,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35661,7 +35664,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35759,7 +35762,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35930,7 +35933,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36028,7 +36031,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36199,7 +36202,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36297,7 +36300,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36468,7 +36471,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36566,7 +36569,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36737,7 +36740,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36835,7 +36838,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37006,7 +37009,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37104,7 +37107,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37275,7 +37278,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37373,7 +37376,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37544,7 +37547,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37642,7 +37645,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37813,7 +37816,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37911,7 +37914,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38082,7 +38085,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38180,7 +38183,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38351,7 +38354,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38449,7 +38452,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38620,7 +38623,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38718,7 +38721,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38889,7 +38892,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -38987,7 +38990,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39158,7 +39161,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39256,7 +39259,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39427,7 +39430,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39525,7 +39528,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39696,7 +39699,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39794,7 +39797,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -39965,7 +39968,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40063,7 +40066,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40234,7 +40237,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40332,7 +40335,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40503,7 +40506,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40601,7 +40604,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40772,7 +40775,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40870,7 +40873,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41041,7 +41044,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41139,7 +41142,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41310,7 +41313,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41408,7 +41411,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41579,7 +41582,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41677,7 +41680,7 @@
         <v>0.01422843894993598</v>
       </c>
       <c r="AM146" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN146">
         <v>0.3570285831928028</v>
@@ -41855,6 +41858,275 @@
       </c>
       <c r="CU146">
         <v>0.2347171187836478</v>
+      </c>
+    </row>
+    <row r="147" spans="10:99">
+      <c r="J147" t="s">
+        <v>244</v>
+      </c>
+      <c r="K147">
+        <v>0.003022867801742768</v>
+      </c>
+      <c r="L147">
+        <v>0.003022867801742768</v>
+      </c>
+      <c r="M147">
+        <v>0.002770215014981536</v>
+      </c>
+      <c r="N147">
+        <v>0.002770215014981536</v>
+      </c>
+      <c r="O147">
+        <v>0.002299720220082513</v>
+      </c>
+      <c r="P147">
+        <v>0.002299720220082513</v>
+      </c>
+      <c r="Q147">
+        <v>0.002185525329434568</v>
+      </c>
+      <c r="R147">
+        <v>0.002185525329434568</v>
+      </c>
+      <c r="S147">
+        <v>8.581122373717152</v>
+      </c>
+      <c r="T147">
+        <v>14.00965165532211</v>
+      </c>
+      <c r="U147">
+        <v>0.9978766692895592</v>
+      </c>
+      <c r="V147">
+        <v>0.6592921762857294</v>
+      </c>
+      <c r="W147">
+        <v>0.0887175250587791</v>
+      </c>
+      <c r="X147">
+        <v>0.09616245673173855</v>
+      </c>
+      <c r="Y147">
+        <v>0.1902540328836635</v>
+      </c>
+      <c r="Z147">
+        <v>0.205869103450395</v>
+      </c>
+      <c r="AA147">
+        <v>0.9976470758551494</v>
+      </c>
+      <c r="AB147">
+        <v>0.8426177102200922</v>
+      </c>
+      <c r="AC147">
+        <v>0.8581546891098478</v>
+      </c>
+      <c r="AD147">
+        <v>0.9957411675388217</v>
+      </c>
+      <c r="AE147">
+        <v>0.809906319431881</v>
+      </c>
+      <c r="AF147">
+        <v>0.7947221067317487</v>
+      </c>
+      <c r="AG147">
+        <v>0.01071361379258181</v>
+      </c>
+      <c r="AH147">
+        <v>0.01287672421329242</v>
+      </c>
+      <c r="AI147">
+        <v>0.9976470758551494</v>
+      </c>
+      <c r="AJ147">
+        <v>0.9957411675388217</v>
+      </c>
+      <c r="AK147">
+        <v>0.01071361379258181</v>
+      </c>
+      <c r="AL147">
+        <v>0.01287672421329242</v>
+      </c>
+      <c r="AM147" t="s">
+        <v>245</v>
+      </c>
+      <c r="AN147">
+        <v>0.1138938544209247</v>
+      </c>
+      <c r="AO147">
+        <v>0.1347190359775772</v>
+      </c>
+      <c r="AP147">
+        <v>-236.16315634</v>
+      </c>
+      <c r="AQ147">
+        <v>-427.6444658200001</v>
+      </c>
+      <c r="AR147">
+        <v>24477.60674366003</v>
+      </c>
+      <c r="AS147">
+        <v>22715.39813417995</v>
+      </c>
+      <c r="AT147">
+        <v>24475.34044366003</v>
+      </c>
+      <c r="AU147">
+        <v>22694.39093417995</v>
+      </c>
+      <c r="AV147">
+        <v>1.447760674366003</v>
+      </c>
+      <c r="AW147">
+        <v>1.271539813417995</v>
+      </c>
+      <c r="AX147">
+        <v>2.797444968553459</v>
+      </c>
+      <c r="AY147">
+        <v>1.71254614026641</v>
+      </c>
+      <c r="AZ147">
+        <v>33.56666666666667</v>
+      </c>
+      <c r="BA147">
+        <v>32.95</v>
+      </c>
+      <c r="BB147">
+        <v>0.04075503202233647</v>
+      </c>
+      <c r="BC147">
+        <v>0.02223195468360725</v>
+      </c>
+      <c r="BD147">
+        <v>-625.1376691691473</v>
+      </c>
+      <c r="BE147">
+        <v>-298.8393094738224</v>
+      </c>
+      <c r="BF147">
+        <v>1111</v>
+      </c>
+      <c r="BG147">
+        <v>2773</v>
+      </c>
+      <c r="BH147">
+        <v>296.58125</v>
+      </c>
+      <c r="BI147">
+        <v>1434</v>
+      </c>
+      <c r="BJ147">
+        <v>1382</v>
+      </c>
+      <c r="BK147">
+        <v>2545</v>
+      </c>
+      <c r="BL147">
+        <v>4155</v>
+      </c>
+      <c r="BM147">
+        <v>0</v>
+      </c>
+      <c r="BN147">
+        <v>0</v>
+      </c>
+      <c r="BO147">
+        <v>194</v>
+      </c>
+      <c r="BP147">
+        <v>400</v>
+      </c>
+      <c r="BQ147">
+        <v>0</v>
+      </c>
+      <c r="BR147">
+        <v>0</v>
+      </c>
+      <c r="BS147">
+        <v>917</v>
+      </c>
+      <c r="BT147">
+        <v>2373</v>
+      </c>
+      <c r="BU147">
+        <v>1434</v>
+      </c>
+      <c r="BV147">
+        <v>1382</v>
+      </c>
+      <c r="BW147">
+        <v>14477.60674365999</v>
+      </c>
+      <c r="BX147">
+        <v>12715.39813418001</v>
+      </c>
+      <c r="BY147">
+        <v>0.09565801326647466</v>
+      </c>
+      <c r="BZ147">
+        <v>0.08829846837465503</v>
+      </c>
+      <c r="CA147">
+        <v>0.2376034515328641</v>
+      </c>
+      <c r="CB147">
+        <v>0.1702961423241965</v>
+      </c>
+      <c r="CC147">
+        <v>0.01687906605202549</v>
+      </c>
+      <c r="CD147">
+        <v>0.01865278405012467</v>
+      </c>
+      <c r="CE147">
+        <v>0.01539769414779864</v>
+      </c>
+      <c r="CF147">
+        <v>0.0172679029203921</v>
+      </c>
+      <c r="CG147">
+        <v>14713.76989999999</v>
+      </c>
+      <c r="CH147">
+        <v>13143.04260000001</v>
+      </c>
+      <c r="CI147">
+        <v>15338.90756916913</v>
+      </c>
+      <c r="CJ147">
+        <v>13441.88190947383</v>
+      </c>
+      <c r="CK147">
+        <v>0.2144270130153139</v>
+      </c>
+      <c r="CL147">
+        <v>0.1928104639516788</v>
+      </c>
+      <c r="CM147">
+        <v>10000</v>
+      </c>
+      <c r="CO147">
+        <v>0.0337126000842815</v>
+      </c>
+      <c r="CP147">
+        <v>0.04087652760219132</v>
+      </c>
+      <c r="CQ147">
+        <v>6808931.255047252</v>
+      </c>
+      <c r="CR147">
+        <v>6035210.07833078</v>
+      </c>
+      <c r="CS147" s="2">
+        <v>45565.69279742855</v>
+      </c>
+      <c r="CT147">
+        <v>-0.5227728639837005</v>
+      </c>
+      <c r="CU147">
+        <v>-0.4881984724812514</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update TOKENUSDT.json at 2024-09-30_22-41-24 bestfile_scores 0.0007780932306859223 bestfile_sharp 0.20582752930630005
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="390">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -749,6 +749,9 @@
   </si>
   <si>
     <t>JTOUSDT</t>
+  </si>
+  <si>
+    <t>STORJUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1542,7 +1545,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU147"/>
+  <dimension ref="A1:CU148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1960,7 +1963,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2125,7 +2128,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2241,7 +2244,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2406,7 +2409,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2522,7 +2525,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2687,7 +2690,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2803,7 +2806,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -2968,7 +2971,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3084,7 +3087,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3249,7 +3252,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3365,7 +3368,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3530,7 +3533,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3646,7 +3649,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3811,7 +3814,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3927,7 +3930,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4092,7 +4095,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4208,7 +4211,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4373,7 +4376,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4489,7 +4492,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4654,7 +4657,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4770,7 +4773,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4935,7 +4938,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5051,7 +5054,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5216,7 +5219,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5332,7 +5335,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5497,7 +5500,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5613,7 +5616,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5778,7 +5781,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5894,7 +5897,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6059,7 +6062,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6175,7 +6178,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6340,7 +6343,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6456,7 +6459,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6621,7 +6624,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6737,7 +6740,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6902,7 +6905,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7018,7 +7021,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7183,7 +7186,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7299,7 +7302,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7464,7 +7467,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7580,7 +7583,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7745,7 +7748,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7861,7 +7864,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8026,7 +8029,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8142,7 +8145,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8307,7 +8310,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8423,7 +8426,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8588,7 +8591,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8704,7 +8707,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8869,7 +8872,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -8985,7 +8988,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9150,7 +9153,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9266,7 +9269,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9431,7 +9434,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9547,7 +9550,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9712,7 +9715,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9828,7 +9831,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -9993,7 +9996,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10109,7 +10112,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10274,7 +10277,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10390,7 +10393,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10555,7 +10558,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10671,7 +10674,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10836,7 +10839,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10952,7 +10955,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11117,7 +11120,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11239,7 +11242,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11404,7 +11407,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11526,7 +11529,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11691,7 +11694,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11813,7 +11816,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -11978,7 +11981,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12100,7 +12103,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12265,7 +12268,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12387,7 +12390,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12552,7 +12555,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12674,7 +12677,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12839,7 +12842,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12961,7 +12964,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13126,7 +13129,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13248,7 +13251,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13413,7 +13416,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13535,7 +13538,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13700,7 +13703,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13822,7 +13825,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -13987,7 +13990,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14109,7 +14112,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14274,7 +14277,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14396,7 +14399,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14561,7 +14564,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14683,7 +14686,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14848,7 +14851,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -14970,7 +14973,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15135,7 +15138,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15257,7 +15260,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15422,7 +15425,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15544,7 +15547,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15709,7 +15712,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15831,7 +15834,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -15996,7 +15999,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16118,7 +16121,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16283,7 +16286,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16405,7 +16408,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16570,7 +16573,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16692,7 +16695,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16857,7 +16860,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -16976,7 +16979,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17141,7 +17144,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17257,7 +17260,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17422,7 +17425,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17535,7 +17538,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17700,7 +17703,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17813,7 +17816,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -17978,7 +17981,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18091,7 +18094,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18256,7 +18259,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18369,7 +18372,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18534,7 +18537,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18647,7 +18650,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18812,7 +18815,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18925,7 +18928,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19090,7 +19093,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19203,7 +19206,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19368,7 +19371,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19481,7 +19484,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19646,7 +19649,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19759,7 +19762,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19924,7 +19927,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20037,7 +20040,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20208,7 +20211,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20321,7 +20324,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20492,7 +20495,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20605,7 +20608,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20776,7 +20779,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20889,7 +20892,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21060,7 +21063,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21170,7 +21173,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21341,7 +21344,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21448,7 +21451,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21619,7 +21622,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21723,7 +21726,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21894,7 +21897,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -21998,7 +22001,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22169,7 +22172,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22273,7 +22276,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22444,7 +22447,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22548,7 +22551,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22719,7 +22722,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22823,7 +22826,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -22994,7 +22997,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23098,7 +23101,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23269,7 +23272,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23370,7 +23373,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23541,7 +23544,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23642,7 +23645,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23813,7 +23816,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23914,7 +23917,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24085,7 +24088,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24186,7 +24189,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24357,7 +24360,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24458,7 +24461,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24629,7 +24632,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24730,7 +24733,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24901,7 +24904,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25002,7 +25005,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25173,7 +25176,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25271,7 +25274,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25442,7 +25445,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25540,7 +25543,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25711,7 +25714,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25809,7 +25812,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -25980,7 +25983,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26078,7 +26081,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26249,7 +26252,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26347,7 +26350,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26518,7 +26521,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26616,7 +26619,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26787,7 +26790,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26885,7 +26888,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27056,7 +27059,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27154,7 +27157,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27325,7 +27328,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27423,7 +27426,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27594,7 +27597,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27692,7 +27695,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27863,7 +27866,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27961,7 +27964,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28132,7 +28135,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28230,7 +28233,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28401,7 +28404,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28499,7 +28502,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28670,7 +28673,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28768,7 +28771,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28939,7 +28942,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29037,7 +29040,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29208,7 +29211,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29306,7 +29309,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29477,7 +29480,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29575,7 +29578,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29746,7 +29749,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29844,7 +29847,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30015,7 +30018,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30113,7 +30116,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30284,7 +30287,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30382,7 +30385,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30553,7 +30556,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30651,7 +30654,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30822,7 +30825,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30920,7 +30923,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31091,7 +31094,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31189,7 +31192,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31360,7 +31363,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31458,7 +31461,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31629,7 +31632,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31727,7 +31730,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31898,7 +31901,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -31996,7 +31999,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32167,7 +32170,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32265,7 +32268,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32436,7 +32439,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32534,7 +32537,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32705,7 +32708,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32803,7 +32806,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -32974,7 +32977,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33072,7 +33075,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33243,7 +33246,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33341,7 +33344,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33512,7 +33515,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33610,7 +33613,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33781,7 +33784,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33879,7 +33882,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34050,7 +34053,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34148,7 +34151,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34319,7 +34322,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34417,7 +34420,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34588,7 +34591,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34686,7 +34689,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34857,7 +34860,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34955,7 +34958,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35126,7 +35129,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35224,7 +35227,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35395,7 +35398,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35493,7 +35496,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35664,7 +35667,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35762,7 +35765,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35933,7 +35936,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36031,7 +36034,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36202,7 +36205,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36300,7 +36303,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36471,7 +36474,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36569,7 +36572,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36740,7 +36743,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36838,7 +36841,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37009,7 +37012,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37107,7 +37110,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37278,7 +37281,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37376,7 +37379,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37547,7 +37550,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37645,7 +37648,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37816,7 +37819,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37914,7 +37917,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38085,7 +38088,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38183,7 +38186,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38354,7 +38357,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38452,7 +38455,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38623,7 +38626,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38721,7 +38724,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38892,7 +38895,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -38990,7 +38993,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39161,7 +39164,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39259,7 +39262,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39430,7 +39433,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39528,7 +39531,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39699,7 +39702,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39797,7 +39800,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -39968,7 +39971,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40066,7 +40069,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40237,7 +40240,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40335,7 +40338,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40506,7 +40509,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40604,7 +40607,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40775,7 +40778,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40873,7 +40876,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41044,7 +41047,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41142,7 +41145,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41313,7 +41316,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41411,7 +41414,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41582,7 +41585,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41680,7 +41683,7 @@
         <v>0.01422843894993598</v>
       </c>
       <c r="AM146" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN146">
         <v>0.3570285831928028</v>
@@ -41949,7 +41952,7 @@
         <v>0.01287672421329242</v>
       </c>
       <c r="AM147" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN147">
         <v>0.1138938544209247</v>
@@ -42127,6 +42130,275 @@
       </c>
       <c r="CU147">
         <v>-0.4881984724812514</v>
+      </c>
+    </row>
+    <row r="148" spans="10:99">
+      <c r="J148" t="s">
+        <v>245</v>
+      </c>
+      <c r="K148">
+        <v>0.0005412352606239956</v>
+      </c>
+      <c r="L148">
+        <v>0.0005412352606239956</v>
+      </c>
+      <c r="M148">
+        <v>0.0009563393066240877</v>
+      </c>
+      <c r="N148">
+        <v>0.0009563393066240877</v>
+      </c>
+      <c r="O148">
+        <v>0.0002753474014253632</v>
+      </c>
+      <c r="P148">
+        <v>0.0002753474014253632</v>
+      </c>
+      <c r="Q148">
+        <v>0.0009963201791804099</v>
+      </c>
+      <c r="R148">
+        <v>0.0009963201791804099</v>
+      </c>
+      <c r="S148">
+        <v>9.329870109828423</v>
+      </c>
+      <c r="T148">
+        <v>6.650700859086476</v>
+      </c>
+      <c r="U148">
+        <v>0.9909843259094337</v>
+      </c>
+      <c r="V148">
+        <v>0.7234444097459056</v>
+      </c>
+      <c r="W148">
+        <v>0.07118703117668049</v>
+      </c>
+      <c r="X148">
+        <v>0.09982323566528147</v>
+      </c>
+      <c r="Y148">
+        <v>0.203753774447213</v>
+      </c>
+      <c r="Z148">
+        <v>0.2301846485678385</v>
+      </c>
+      <c r="AA148">
+        <v>0.9992707910747977</v>
+      </c>
+      <c r="AB148">
+        <v>0.8242387975538019</v>
+      </c>
+      <c r="AC148">
+        <v>0.7927441602141755</v>
+      </c>
+      <c r="AD148">
+        <v>0.9974172453653362</v>
+      </c>
+      <c r="AE148">
+        <v>0.7234605207312226</v>
+      </c>
+      <c r="AF148">
+        <v>0.7599623980457865</v>
+      </c>
+      <c r="AG148">
+        <v>0.007331567654725139</v>
+      </c>
+      <c r="AH148">
+        <v>0.01129449859594168</v>
+      </c>
+      <c r="AI148">
+        <v>0.9992707910747977</v>
+      </c>
+      <c r="AJ148">
+        <v>0.9974172453653362</v>
+      </c>
+      <c r="AK148">
+        <v>0.007331567654725139</v>
+      </c>
+      <c r="AL148">
+        <v>0.01129449859594168</v>
+      </c>
+      <c r="AM148" t="s">
+        <v>246</v>
+      </c>
+      <c r="AN148">
+        <v>0.01929055864963264</v>
+      </c>
+      <c r="AO148">
+        <v>0.07294730335302833</v>
+      </c>
+      <c r="AP148">
+        <v>-627.80448362</v>
+      </c>
+      <c r="AQ148">
+        <v>-1295.0238795</v>
+      </c>
+      <c r="AR148">
+        <v>21796.56261637979</v>
+      </c>
+      <c r="AS148">
+        <v>39608.91762050003</v>
+      </c>
+      <c r="AT148">
+        <v>21796.56261637979</v>
+      </c>
+      <c r="AU148">
+        <v>39605.29202050003</v>
+      </c>
+      <c r="AV148">
+        <v>1.179656261637979</v>
+      </c>
+      <c r="AW148">
+        <v>2.960891762050003</v>
+      </c>
+      <c r="AX148">
+        <v>2.572038608505781</v>
+      </c>
+      <c r="AY148">
+        <v>3.608711013645224</v>
+      </c>
+      <c r="AZ148">
+        <v>101.5166666666667</v>
+      </c>
+      <c r="BA148">
+        <v>89.51666666666667</v>
+      </c>
+      <c r="BB148">
+        <v>0.2208748031202999</v>
+      </c>
+      <c r="BC148">
+        <v>0.1384300906673257</v>
+      </c>
+      <c r="BD148">
+        <v>-3522.193413968806</v>
+      </c>
+      <c r="BE148">
+        <v>-4965.395584829866</v>
+      </c>
+      <c r="BF148">
+        <v>5592</v>
+      </c>
+      <c r="BG148">
+        <v>4088</v>
+      </c>
+      <c r="BH148">
+        <v>1439.998611111111</v>
+      </c>
+      <c r="BI148">
+        <v>7843</v>
+      </c>
+      <c r="BJ148">
+        <v>5489</v>
+      </c>
+      <c r="BK148">
+        <v>13435</v>
+      </c>
+      <c r="BL148">
+        <v>9577</v>
+      </c>
+      <c r="BM148">
+        <v>0</v>
+      </c>
+      <c r="BN148">
+        <v>0</v>
+      </c>
+      <c r="BO148">
+        <v>170</v>
+      </c>
+      <c r="BP148">
+        <v>1500</v>
+      </c>
+      <c r="BQ148">
+        <v>0</v>
+      </c>
+      <c r="BR148">
+        <v>0</v>
+      </c>
+      <c r="BS148">
+        <v>5422</v>
+      </c>
+      <c r="BT148">
+        <v>2588</v>
+      </c>
+      <c r="BU148">
+        <v>7843</v>
+      </c>
+      <c r="BV148">
+        <v>5489</v>
+      </c>
+      <c r="BW148">
+        <v>11796.56261637999</v>
+      </c>
+      <c r="BX148">
+        <v>29608.9176205</v>
+      </c>
+      <c r="BY148">
+        <v>0.08181764723730447</v>
+      </c>
+      <c r="BZ148">
+        <v>0.1749942615512397</v>
+      </c>
+      <c r="CA148">
+        <v>0.3210867194853485</v>
+      </c>
+      <c r="CB148">
+        <v>0.4174610136088927</v>
+      </c>
+      <c r="CC148">
+        <v>0.01436258647122857</v>
+      </c>
+      <c r="CD148">
+        <v>0.0205508763337746</v>
+      </c>
+      <c r="CE148">
+        <v>0.01573117919882239</v>
+      </c>
+      <c r="CF148">
+        <v>0.02954917926588643</v>
+      </c>
+      <c r="CG148">
+        <v>12424.36709999999</v>
+      </c>
+      <c r="CH148">
+        <v>30903.9415</v>
+      </c>
+      <c r="CI148">
+        <v>15946.5605139688</v>
+      </c>
+      <c r="CJ148">
+        <v>35869.33708482987</v>
+      </c>
+      <c r="CK148">
+        <v>0.08595485485965598</v>
+      </c>
+      <c r="CL148">
+        <v>0.07943205910231327</v>
+      </c>
+      <c r="CM148">
+        <v>10000</v>
+      </c>
+      <c r="CO148">
+        <v>0.006220884812360754</v>
+      </c>
+      <c r="CP148">
+        <v>0.01605856312028009</v>
+      </c>
+      <c r="CQ148">
+        <v>9303670.593166731</v>
+      </c>
+      <c r="CR148">
+        <v>20925212.50933231</v>
+      </c>
+      <c r="CS148" s="2">
+        <v>45565.87042912793</v>
+      </c>
+      <c r="CT148">
+        <v>-0.8702493236754036</v>
+      </c>
+      <c r="CU148">
+        <v>-0.622450264906648</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update FLOWUSDT.json at 2024-10-01_01-57-25 bestfile_scores 0.0009353493902786725 bestfile_sharp 0.08200999793692151
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="391">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -752,6 +752,9 @@
   </si>
   <si>
     <t>STORJUSDT</t>
+  </si>
+  <si>
+    <t>TOKENUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1545,7 +1548,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU148"/>
+  <dimension ref="A1:CU149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1963,7 +1966,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2128,7 +2131,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2244,7 +2247,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2409,7 +2412,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2525,7 +2528,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2690,7 +2693,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2806,7 +2809,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -2971,7 +2974,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3087,7 +3090,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3252,7 +3255,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3368,7 +3371,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3533,7 +3536,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3649,7 +3652,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3814,7 +3817,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3930,7 +3933,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4095,7 +4098,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4211,7 +4214,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4376,7 +4379,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4492,7 +4495,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4657,7 +4660,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4773,7 +4776,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4938,7 +4941,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5054,7 +5057,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5219,7 +5222,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5335,7 +5338,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5500,7 +5503,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5616,7 +5619,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5781,7 +5784,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5897,7 +5900,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6062,7 +6065,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6178,7 +6181,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6343,7 +6346,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6459,7 +6462,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6624,7 +6627,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6740,7 +6743,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6905,7 +6908,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7021,7 +7024,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7186,7 +7189,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7302,7 +7305,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7467,7 +7470,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7583,7 +7586,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7748,7 +7751,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7864,7 +7867,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8029,7 +8032,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8145,7 +8148,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8310,7 +8313,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8426,7 +8429,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8591,7 +8594,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8707,7 +8710,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8872,7 +8875,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -8988,7 +8991,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9153,7 +9156,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9269,7 +9272,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9434,7 +9437,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9550,7 +9553,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9715,7 +9718,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9831,7 +9834,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -9996,7 +9999,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10112,7 +10115,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10277,7 +10280,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10393,7 +10396,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10558,7 +10561,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10674,7 +10677,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10839,7 +10842,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10955,7 +10958,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11120,7 +11123,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11242,7 +11245,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11407,7 +11410,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11529,7 +11532,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11694,7 +11697,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11816,7 +11819,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -11981,7 +11984,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12103,7 +12106,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12268,7 +12271,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12390,7 +12393,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12555,7 +12558,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12677,7 +12680,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12842,7 +12845,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12964,7 +12967,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13129,7 +13132,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13251,7 +13254,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13416,7 +13419,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13538,7 +13541,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13703,7 +13706,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13825,7 +13828,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -13990,7 +13993,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14112,7 +14115,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14277,7 +14280,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14399,7 +14402,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14564,7 +14567,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14686,7 +14689,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14851,7 +14854,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -14973,7 +14976,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15138,7 +15141,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15260,7 +15263,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15425,7 +15428,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15547,7 +15550,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15712,7 +15715,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15834,7 +15837,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -15999,7 +16002,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16121,7 +16124,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16286,7 +16289,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16408,7 +16411,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16573,7 +16576,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16695,7 +16698,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16860,7 +16863,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -16979,7 +16982,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17144,7 +17147,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17260,7 +17263,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17425,7 +17428,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17538,7 +17541,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17703,7 +17706,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17816,7 +17819,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -17981,7 +17984,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18094,7 +18097,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18259,7 +18262,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18372,7 +18375,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18537,7 +18540,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18650,7 +18653,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18815,7 +18818,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18928,7 +18931,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19093,7 +19096,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19206,7 +19209,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19371,7 +19374,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19484,7 +19487,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19649,7 +19652,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19762,7 +19765,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19927,7 +19930,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20040,7 +20043,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20211,7 +20214,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20324,7 +20327,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20495,7 +20498,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20608,7 +20611,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20779,7 +20782,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20892,7 +20895,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21063,7 +21066,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21173,7 +21176,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21344,7 +21347,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21451,7 +21454,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21622,7 +21625,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21726,7 +21729,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21897,7 +21900,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22001,7 +22004,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22172,7 +22175,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22276,7 +22279,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22447,7 +22450,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22551,7 +22554,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22722,7 +22725,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22826,7 +22829,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -22997,7 +23000,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23101,7 +23104,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23272,7 +23275,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23373,7 +23376,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23544,7 +23547,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23645,7 +23648,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23816,7 +23819,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23917,7 +23920,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24088,7 +24091,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24189,7 +24192,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24360,7 +24363,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24461,7 +24464,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24632,7 +24635,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24733,7 +24736,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24904,7 +24907,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25005,7 +25008,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25176,7 +25179,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25274,7 +25277,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25445,7 +25448,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25543,7 +25546,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25714,7 +25717,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25812,7 +25815,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -25983,7 +25986,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26081,7 +26084,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26252,7 +26255,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26350,7 +26353,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26521,7 +26524,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26619,7 +26622,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26790,7 +26793,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26888,7 +26891,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27059,7 +27062,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27157,7 +27160,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27328,7 +27331,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27426,7 +27429,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27597,7 +27600,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27695,7 +27698,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27866,7 +27869,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27964,7 +27967,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28135,7 +28138,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28233,7 +28236,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28404,7 +28407,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28502,7 +28505,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28673,7 +28676,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28771,7 +28774,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28942,7 +28945,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29040,7 +29043,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29211,7 +29214,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29309,7 +29312,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29480,7 +29483,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29578,7 +29581,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29749,7 +29752,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29847,7 +29850,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30018,7 +30021,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30116,7 +30119,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30287,7 +30290,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30385,7 +30388,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30556,7 +30559,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30654,7 +30657,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30825,7 +30828,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30923,7 +30926,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31094,7 +31097,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31192,7 +31195,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31363,7 +31366,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31461,7 +31464,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31632,7 +31635,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31730,7 +31733,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31901,7 +31904,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -31999,7 +32002,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32170,7 +32173,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32268,7 +32271,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32439,7 +32442,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32537,7 +32540,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32708,7 +32711,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32806,7 +32809,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -32977,7 +32980,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33075,7 +33078,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33246,7 +33249,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33344,7 +33347,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33515,7 +33518,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33613,7 +33616,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33784,7 +33787,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33882,7 +33885,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34053,7 +34056,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34151,7 +34154,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34322,7 +34325,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34420,7 +34423,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34591,7 +34594,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34689,7 +34692,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34860,7 +34863,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34958,7 +34961,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35129,7 +35132,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35227,7 +35230,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35398,7 +35401,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35496,7 +35499,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35667,7 +35670,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35765,7 +35768,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35936,7 +35939,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36034,7 +36037,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36205,7 +36208,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36303,7 +36306,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36474,7 +36477,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36572,7 +36575,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36743,7 +36746,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36841,7 +36844,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37012,7 +37015,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37110,7 +37113,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37281,7 +37284,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37379,7 +37382,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37550,7 +37553,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37648,7 +37651,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37819,7 +37822,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37917,7 +37920,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38088,7 +38091,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38186,7 +38189,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38357,7 +38360,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38455,7 +38458,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38626,7 +38629,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38724,7 +38727,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38895,7 +38898,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -38993,7 +38996,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39164,7 +39167,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39262,7 +39265,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39433,7 +39436,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39531,7 +39534,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39702,7 +39705,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39800,7 +39803,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -39971,7 +39974,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40069,7 +40072,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40240,7 +40243,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40338,7 +40341,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40509,7 +40512,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40607,7 +40610,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40778,7 +40781,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40876,7 +40879,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41047,7 +41050,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41145,7 +41148,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41316,7 +41319,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41414,7 +41417,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41585,7 +41588,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41683,7 +41686,7 @@
         <v>0.01422843894993598</v>
       </c>
       <c r="AM146" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN146">
         <v>0.3570285831928028</v>
@@ -41952,7 +41955,7 @@
         <v>0.01287672421329242</v>
       </c>
       <c r="AM147" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN147">
         <v>0.1138938544209247</v>
@@ -42221,7 +42224,7 @@
         <v>0.01129449859594168</v>
       </c>
       <c r="AM148" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN148">
         <v>0.01929055864963264</v>
@@ -42399,6 +42402,275 @@
       </c>
       <c r="CU148">
         <v>-0.622450264906648</v>
+      </c>
+    </row>
+    <row r="149" spans="10:99">
+      <c r="J149" t="s">
+        <v>246</v>
+      </c>
+      <c r="K149">
+        <v>0.001335038280820156</v>
+      </c>
+      <c r="L149">
+        <v>0.001335038280820156</v>
+      </c>
+      <c r="M149">
+        <v>0.0004640257007291204</v>
+      </c>
+      <c r="N149">
+        <v>0.0004640257007291204</v>
+      </c>
+      <c r="O149">
+        <v>0.001015037883052217</v>
+      </c>
+      <c r="P149">
+        <v>0.001015037883052217</v>
+      </c>
+      <c r="Q149">
+        <v>0.0002982710581421966</v>
+      </c>
+      <c r="R149">
+        <v>0.0002982710581421966</v>
+      </c>
+      <c r="S149">
+        <v>15.52929933903072</v>
+      </c>
+      <c r="T149">
+        <v>5.570751375796873</v>
+      </c>
+      <c r="U149">
+        <v>0.9955406418324396</v>
+      </c>
+      <c r="V149">
+        <v>1</v>
+      </c>
+      <c r="W149">
+        <v>0.03362416844596645</v>
+      </c>
+      <c r="X149">
+        <v>0.09996130962536967</v>
+      </c>
+      <c r="Y149">
+        <v>0.1318138602916397</v>
+      </c>
+      <c r="Z149">
+        <v>0.1332091416968328</v>
+      </c>
+      <c r="AA149">
+        <v>0.9994696754662277</v>
+      </c>
+      <c r="AB149">
+        <v>0.9112136115309515</v>
+      </c>
+      <c r="AC149">
+        <v>0.8846314994881338</v>
+      </c>
+      <c r="AD149">
+        <v>0.9955063023357636</v>
+      </c>
+      <c r="AE149">
+        <v>0.8683478955845328</v>
+      </c>
+      <c r="AF149">
+        <v>0.8703700338539395</v>
+      </c>
+      <c r="AG149">
+        <v>0.004429156240955837</v>
+      </c>
+      <c r="AH149">
+        <v>0.01268293743279473</v>
+      </c>
+      <c r="AI149">
+        <v>0.9994696754662277</v>
+      </c>
+      <c r="AJ149">
+        <v>0.9955063023357636</v>
+      </c>
+      <c r="AK149">
+        <v>0.004429156240955837</v>
+      </c>
+      <c r="AL149">
+        <v>0.01268293743279473</v>
+      </c>
+      <c r="AM149" t="s">
+        <v>247</v>
+      </c>
+      <c r="AN149">
+        <v>0.02713293780673231</v>
+      </c>
+      <c r="AO149">
+        <v>0.04896594609088707</v>
+      </c>
+      <c r="AP149">
+        <v>-270.941614298</v>
+      </c>
+      <c r="AQ149">
+        <v>-46.98059296</v>
+      </c>
+      <c r="AR149">
+        <v>15559.73524570206</v>
+      </c>
+      <c r="AS149">
+        <v>11661.76218704002</v>
+      </c>
+      <c r="AT149">
+        <v>15559.42874570206</v>
+      </c>
+      <c r="AU149">
+        <v>11658.23943704002</v>
+      </c>
+      <c r="AV149">
+        <v>0.5559735245702058</v>
+      </c>
+      <c r="AW149">
+        <v>0.1661762187040023</v>
+      </c>
+      <c r="AX149">
+        <v>1.545565273728539</v>
+      </c>
+      <c r="AY149">
+        <v>4.304760614272809</v>
+      </c>
+      <c r="AZ149">
+        <v>51.03333333333333</v>
+      </c>
+      <c r="BA149">
+        <v>18.4</v>
+      </c>
+      <c r="BB149">
+        <v>0.002755812858638183</v>
+      </c>
+      <c r="BC149">
+        <v>0.3604768730676468</v>
+      </c>
+      <c r="BD149">
+        <v>-16.11265773472432</v>
+      </c>
+      <c r="BE149">
+        <v>-963.1586853878894</v>
+      </c>
+      <c r="BF149">
+        <v>1910</v>
+      </c>
+      <c r="BG149">
+        <v>996</v>
+      </c>
+      <c r="BH149">
+        <v>331.3736111111111</v>
+      </c>
+      <c r="BI149">
+        <v>3236</v>
+      </c>
+      <c r="BJ149">
+        <v>850</v>
+      </c>
+      <c r="BK149">
+        <v>5146</v>
+      </c>
+      <c r="BL149">
+        <v>1846</v>
+      </c>
+      <c r="BM149">
+        <v>0</v>
+      </c>
+      <c r="BN149">
+        <v>0</v>
+      </c>
+      <c r="BO149">
+        <v>1106</v>
+      </c>
+      <c r="BP149">
+        <v>23</v>
+      </c>
+      <c r="BQ149">
+        <v>0</v>
+      </c>
+      <c r="BR149">
+        <v>0</v>
+      </c>
+      <c r="BS149">
+        <v>804</v>
+      </c>
+      <c r="BT149">
+        <v>973</v>
+      </c>
+      <c r="BU149">
+        <v>3236</v>
+      </c>
+      <c r="BV149">
+        <v>850</v>
+      </c>
+      <c r="BW149">
+        <v>5559.735245702009</v>
+      </c>
+      <c r="BX149">
+        <v>1661.762187039999</v>
+      </c>
+      <c r="BY149">
+        <v>0.05016566190961703</v>
+      </c>
+      <c r="BZ149">
+        <v>0.3576838290985885</v>
+      </c>
+      <c r="CA149">
+        <v>0.1509360720453389</v>
+      </c>
+      <c r="CB149">
+        <v>0.4915875044837255</v>
+      </c>
+      <c r="CC149">
+        <v>0.01056007572448148</v>
+      </c>
+      <c r="CD149">
+        <v>0.0496751478244886</v>
+      </c>
+      <c r="CE149">
+        <v>0.01007885059921431</v>
+      </c>
+      <c r="CF149">
+        <v>0.06039960406159971</v>
+      </c>
+      <c r="CG149">
+        <v>5830.676860000009</v>
+      </c>
+      <c r="CH149">
+        <v>1708.742779999999</v>
+      </c>
+      <c r="CI149">
+        <v>5846.789517734733</v>
+      </c>
+      <c r="CJ149">
+        <v>2671.901465387888</v>
+      </c>
+      <c r="CK149">
+        <v>0.2058275293063</v>
+      </c>
+      <c r="CL149">
+        <v>0.04926671039821775</v>
+      </c>
+      <c r="CM149">
+        <v>10000</v>
+      </c>
+      <c r="CO149">
+        <v>0.005154639175257732</v>
+      </c>
+      <c r="CP149">
+        <v>0</v>
+      </c>
+      <c r="CQ149">
+        <v>2482545.740378607</v>
+      </c>
+      <c r="CR149">
+        <v>842544.0492511673</v>
+      </c>
+      <c r="CS149" s="2">
+        <v>45565.94544501081</v>
+      </c>
+      <c r="CT149">
+        <v>-0.8600491294508058</v>
+      </c>
+      <c r="CU149">
+        <v>-0.7553213861826504</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update REEFUSDT.json at 2024-10-01_06-30-50 bestfile_scores 0.0009317939731238844 bestfile_sharp 0.10604715225512427
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="392">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -755,6 +755,9 @@
   </si>
   <si>
     <t>TOKENUSDT</t>
+  </si>
+  <si>
+    <t>FLOWUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1548,7 +1551,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU149"/>
+  <dimension ref="A1:CU150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1966,7 +1969,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2131,7 +2134,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2247,7 +2250,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2412,7 +2415,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2528,7 +2531,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2693,7 +2696,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2809,7 +2812,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -2974,7 +2977,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3090,7 +3093,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3255,7 +3258,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3371,7 +3374,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3536,7 +3539,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3652,7 +3655,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3817,7 +3820,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3933,7 +3936,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4098,7 +4101,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4214,7 +4217,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4379,7 +4382,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4495,7 +4498,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4660,7 +4663,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4776,7 +4779,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4941,7 +4944,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5057,7 +5060,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5222,7 +5225,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5338,7 +5341,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5503,7 +5506,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5619,7 +5622,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5784,7 +5787,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5900,7 +5903,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6065,7 +6068,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6181,7 +6184,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6346,7 +6349,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6462,7 +6465,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6627,7 +6630,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6743,7 +6746,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6908,7 +6911,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7024,7 +7027,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7189,7 +7192,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7305,7 +7308,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7470,7 +7473,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7586,7 +7589,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7751,7 +7754,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7867,7 +7870,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8032,7 +8035,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8148,7 +8151,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8313,7 +8316,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8429,7 +8432,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8594,7 +8597,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8710,7 +8713,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8875,7 +8878,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -8991,7 +8994,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9156,7 +9159,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9272,7 +9275,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9437,7 +9440,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9553,7 +9556,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9718,7 +9721,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9834,7 +9837,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -9999,7 +10002,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10115,7 +10118,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10280,7 +10283,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10396,7 +10399,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10561,7 +10564,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10677,7 +10680,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10842,7 +10845,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10958,7 +10961,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11123,7 +11126,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11245,7 +11248,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11410,7 +11413,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11532,7 +11535,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11697,7 +11700,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11819,7 +11822,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -11984,7 +11987,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12106,7 +12109,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12271,7 +12274,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12393,7 +12396,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12558,7 +12561,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12680,7 +12683,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12845,7 +12848,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12967,7 +12970,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13132,7 +13135,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13254,7 +13257,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13419,7 +13422,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13541,7 +13544,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13706,7 +13709,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13828,7 +13831,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -13993,7 +13996,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14115,7 +14118,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14280,7 +14283,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14402,7 +14405,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14567,7 +14570,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14689,7 +14692,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14854,7 +14857,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -14976,7 +14979,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15141,7 +15144,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15263,7 +15266,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15428,7 +15431,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15550,7 +15553,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15715,7 +15718,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15837,7 +15840,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16002,7 +16005,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16124,7 +16127,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16289,7 +16292,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16411,7 +16414,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16576,7 +16579,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16698,7 +16701,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16863,7 +16866,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -16982,7 +16985,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17147,7 +17150,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17263,7 +17266,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17428,7 +17431,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17541,7 +17544,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17706,7 +17709,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17819,7 +17822,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -17984,7 +17987,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18097,7 +18100,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18262,7 +18265,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18375,7 +18378,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18540,7 +18543,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18653,7 +18656,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18818,7 +18821,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18931,7 +18934,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19096,7 +19099,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19209,7 +19212,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19374,7 +19377,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19487,7 +19490,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19652,7 +19655,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19765,7 +19768,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19930,7 +19933,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20043,7 +20046,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20214,7 +20217,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20327,7 +20330,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20498,7 +20501,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20611,7 +20614,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20782,7 +20785,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20895,7 +20898,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21066,7 +21069,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21176,7 +21179,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21347,7 +21350,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21454,7 +21457,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21625,7 +21628,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21729,7 +21732,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21900,7 +21903,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22004,7 +22007,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22175,7 +22178,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22279,7 +22282,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22450,7 +22453,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22554,7 +22557,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22725,7 +22728,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22829,7 +22832,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23000,7 +23003,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23104,7 +23107,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23275,7 +23278,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23376,7 +23379,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23547,7 +23550,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23648,7 +23651,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23819,7 +23822,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23920,7 +23923,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24091,7 +24094,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24192,7 +24195,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24363,7 +24366,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24464,7 +24467,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24635,7 +24638,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24736,7 +24739,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24907,7 +24910,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25008,7 +25011,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25179,7 +25182,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25277,7 +25280,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25448,7 +25451,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25546,7 +25549,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25717,7 +25720,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25815,7 +25818,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -25986,7 +25989,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26084,7 +26087,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26255,7 +26258,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26353,7 +26356,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26524,7 +26527,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26622,7 +26625,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26793,7 +26796,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26891,7 +26894,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27062,7 +27065,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27160,7 +27163,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27331,7 +27334,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27429,7 +27432,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27600,7 +27603,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27698,7 +27701,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27869,7 +27872,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27967,7 +27970,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28138,7 +28141,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28236,7 +28239,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28407,7 +28410,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28505,7 +28508,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28676,7 +28679,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28774,7 +28777,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28945,7 +28948,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29043,7 +29046,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29214,7 +29217,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29312,7 +29315,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29483,7 +29486,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29581,7 +29584,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29752,7 +29755,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29850,7 +29853,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30021,7 +30024,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30119,7 +30122,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30290,7 +30293,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30388,7 +30391,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30559,7 +30562,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30657,7 +30660,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30828,7 +30831,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30926,7 +30929,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31097,7 +31100,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31195,7 +31198,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31366,7 +31369,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31464,7 +31467,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31635,7 +31638,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31733,7 +31736,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31904,7 +31907,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32002,7 +32005,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32173,7 +32176,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32271,7 +32274,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32442,7 +32445,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32540,7 +32543,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32711,7 +32714,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32809,7 +32812,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -32980,7 +32983,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33078,7 +33081,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33249,7 +33252,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33347,7 +33350,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33518,7 +33521,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33616,7 +33619,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33787,7 +33790,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33885,7 +33888,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34056,7 +34059,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34154,7 +34157,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34325,7 +34328,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34423,7 +34426,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34594,7 +34597,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34692,7 +34695,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34863,7 +34866,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34961,7 +34964,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35132,7 +35135,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35230,7 +35233,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35401,7 +35404,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35499,7 +35502,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35670,7 +35673,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35768,7 +35771,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35939,7 +35942,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36037,7 +36040,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36208,7 +36211,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36306,7 +36309,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36477,7 +36480,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36575,7 +36578,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36746,7 +36749,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36844,7 +36847,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37015,7 +37018,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37113,7 +37116,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37284,7 +37287,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37382,7 +37385,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37553,7 +37556,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37651,7 +37654,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37822,7 +37825,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37920,7 +37923,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38091,7 +38094,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38189,7 +38192,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38360,7 +38363,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38458,7 +38461,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38629,7 +38632,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38727,7 +38730,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38898,7 +38901,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -38996,7 +38999,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39167,7 +39170,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39265,7 +39268,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39436,7 +39439,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39534,7 +39537,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39705,7 +39708,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39803,7 +39806,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -39974,7 +39977,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40072,7 +40075,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40243,7 +40246,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40341,7 +40344,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40512,7 +40515,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40610,7 +40613,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40781,7 +40784,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40879,7 +40882,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41050,7 +41053,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41148,7 +41151,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41319,7 +41322,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41417,7 +41420,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41588,7 +41591,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41686,7 +41689,7 @@
         <v>0.01422843894993598</v>
       </c>
       <c r="AM146" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN146">
         <v>0.3570285831928028</v>
@@ -41955,7 +41958,7 @@
         <v>0.01287672421329242</v>
       </c>
       <c r="AM147" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN147">
         <v>0.1138938544209247</v>
@@ -42224,7 +42227,7 @@
         <v>0.01129449859594168</v>
       </c>
       <c r="AM148" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN148">
         <v>0.01929055864963264</v>
@@ -42493,7 +42496,7 @@
         <v>0.01268293743279473</v>
       </c>
       <c r="AM149" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN149">
         <v>0.02713293780673231</v>
@@ -42671,6 +42674,275 @@
       </c>
       <c r="CU149">
         <v>-0.7553213861826504</v>
+      </c>
+    </row>
+    <row r="150" spans="10:99">
+      <c r="J150" t="s">
+        <v>247</v>
+      </c>
+      <c r="K150">
+        <v>0.0007352864416327876</v>
+      </c>
+      <c r="L150">
+        <v>0.0007352864416327876</v>
+      </c>
+      <c r="M150">
+        <v>0.001332749455440485</v>
+      </c>
+      <c r="N150">
+        <v>0.001332749455440485</v>
+      </c>
+      <c r="O150">
+        <v>0.0005396326847290301</v>
+      </c>
+      <c r="P150">
+        <v>0.0005396326847290301</v>
+      </c>
+      <c r="Q150">
+        <v>0.001133728979312387</v>
+      </c>
+      <c r="R150">
+        <v>0.001133728979312387</v>
+      </c>
+      <c r="S150">
+        <v>7.434158331578325</v>
+      </c>
+      <c r="T150">
+        <v>11.57290113003315</v>
+      </c>
+      <c r="U150">
+        <v>0.9948902799949997</v>
+      </c>
+      <c r="V150">
+        <v>0.6932991385243087</v>
+      </c>
+      <c r="W150">
+        <v>0.09453379826850457</v>
+      </c>
+      <c r="X150">
+        <v>0.05969356293428486</v>
+      </c>
+      <c r="Y150">
+        <v>0.2220365291291444</v>
+      </c>
+      <c r="Z150">
+        <v>0.1795884199920777</v>
+      </c>
+      <c r="AA150">
+        <v>0.9980157868655635</v>
+      </c>
+      <c r="AB150">
+        <v>0.806393104081625</v>
+      </c>
+      <c r="AC150">
+        <v>0.8706270444657092</v>
+      </c>
+      <c r="AD150">
+        <v>0.9988205727200993</v>
+      </c>
+      <c r="AE150">
+        <v>0.7851912680962984</v>
+      </c>
+      <c r="AF150">
+        <v>0.8205961401009024</v>
+      </c>
+      <c r="AG150">
+        <v>0.01072690755203363</v>
+      </c>
+      <c r="AH150">
+        <v>0.006815186142663594</v>
+      </c>
+      <c r="AI150">
+        <v>0.9980157868655635</v>
+      </c>
+      <c r="AJ150">
+        <v>0.9988205727200993</v>
+      </c>
+      <c r="AK150">
+        <v>0.01072690755203363</v>
+      </c>
+      <c r="AL150">
+        <v>0.006815186142663594</v>
+      </c>
+      <c r="AM150" t="s">
+        <v>248</v>
+      </c>
+      <c r="AN150">
+        <v>0.06060596226028341</v>
+      </c>
+      <c r="AO150">
+        <v>0.0618869151945509</v>
+      </c>
+      <c r="AP150">
+        <v>-361.06342652</v>
+      </c>
+      <c r="AQ150">
+        <v>-871.7094364000001</v>
+      </c>
+      <c r="AR150">
+        <v>20293.43697347998</v>
+      </c>
+      <c r="AS150">
+        <v>36052.35716360011</v>
+      </c>
+      <c r="AT150">
+        <v>20294.04507347998</v>
+      </c>
+      <c r="AU150">
+        <v>36052.34466360012</v>
+      </c>
+      <c r="AV150">
+        <v>1.029343697347997</v>
+      </c>
+      <c r="AW150">
+        <v>2.605235716360011</v>
+      </c>
+      <c r="AX150">
+        <v>3.2287899958083</v>
+      </c>
+      <c r="AY150">
+        <v>2.073958894273918</v>
+      </c>
+      <c r="AZ150">
+        <v>70.81666666666666</v>
+      </c>
+      <c r="BA150">
+        <v>117.7666666666667</v>
+      </c>
+      <c r="BB150">
+        <v>0.07698668169237588</v>
+      </c>
+      <c r="BC150">
+        <v>0.009071402888860453</v>
+      </c>
+      <c r="BD150">
+        <v>-888.6704174432243</v>
+      </c>
+      <c r="BE150">
+        <v>-246.4749289173232</v>
+      </c>
+      <c r="BF150">
+        <v>4722</v>
+      </c>
+      <c r="BG150">
+        <v>3678</v>
+      </c>
+      <c r="BH150">
+        <v>962.8527777777778</v>
+      </c>
+      <c r="BI150">
+        <v>2436</v>
+      </c>
+      <c r="BJ150">
+        <v>7465</v>
+      </c>
+      <c r="BK150">
+        <v>7158</v>
+      </c>
+      <c r="BL150">
+        <v>11143</v>
+      </c>
+      <c r="BM150">
+        <v>0</v>
+      </c>
+      <c r="BN150">
+        <v>0</v>
+      </c>
+      <c r="BO150">
+        <v>434</v>
+      </c>
+      <c r="BP150">
+        <v>1654</v>
+      </c>
+      <c r="BQ150">
+        <v>0</v>
+      </c>
+      <c r="BR150">
+        <v>0</v>
+      </c>
+      <c r="BS150">
+        <v>4288</v>
+      </c>
+      <c r="BT150">
+        <v>2024</v>
+      </c>
+      <c r="BU150">
+        <v>2436</v>
+      </c>
+      <c r="BV150">
+        <v>7465</v>
+      </c>
+      <c r="BW150">
+        <v>10293.43697348001</v>
+      </c>
+      <c r="BX150">
+        <v>26052.35716359996</v>
+      </c>
+      <c r="BY150">
+        <v>0.1019802450399231</v>
+      </c>
+      <c r="BZ150">
+        <v>0.05540513783245231</v>
+      </c>
+      <c r="CA150">
+        <v>0.2735835321077433</v>
+      </c>
+      <c r="CB150">
+        <v>0.1515733933390011</v>
+      </c>
+      <c r="CC150">
+        <v>0.01548419087607043</v>
+      </c>
+      <c r="CD150">
+        <v>0.008383958044188249</v>
+      </c>
+      <c r="CE150">
+        <v>0.01751035625972605</v>
+      </c>
+      <c r="CF150">
+        <v>0.009211682235785536</v>
+      </c>
+      <c r="CG150">
+        <v>10654.50040000001</v>
+      </c>
+      <c r="CH150">
+        <v>26924.06659999996</v>
+      </c>
+      <c r="CI150">
+        <v>11543.17081744323</v>
+      </c>
+      <c r="CJ150">
+        <v>27170.54152891728</v>
+      </c>
+      <c r="CK150">
+        <v>0.08200999793692151</v>
+      </c>
+      <c r="CL150">
+        <v>0.1888511468351138</v>
+      </c>
+      <c r="CM150">
+        <v>10000</v>
+      </c>
+      <c r="CO150">
+        <v>0.02436174816096928</v>
+      </c>
+      <c r="CP150">
+        <v>0.02695802682821289</v>
+      </c>
+      <c r="CQ150">
+        <v>9632829.255098492</v>
+      </c>
+      <c r="CR150">
+        <v>39501191.44773848</v>
+      </c>
+      <c r="CS150" s="2">
+        <v>45566.08158654243</v>
+      </c>
+      <c r="CT150">
+        <v>-0.7762655293196914</v>
+      </c>
+      <c r="CU150">
+        <v>-0.7924465252031915</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update VIDTUSDT.json at 2024-10-01_07-01-21 bestfile_scores 0.00720858608850129 bestfile_sharp 0.21052956941367068
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="393">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -758,6 +758,9 @@
   </si>
   <si>
     <t>FLOWUSDT</t>
+  </si>
+  <si>
+    <t>REEFUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1551,7 +1554,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU150"/>
+  <dimension ref="A1:CU151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1969,7 +1972,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2134,7 +2137,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2250,7 +2253,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2415,7 +2418,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2531,7 +2534,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2696,7 +2699,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2812,7 +2815,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -2977,7 +2980,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3093,7 +3096,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3258,7 +3261,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3374,7 +3377,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3539,7 +3542,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3655,7 +3658,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3820,7 +3823,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3936,7 +3939,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4101,7 +4104,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4217,7 +4220,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4382,7 +4385,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4498,7 +4501,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4663,7 +4666,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4779,7 +4782,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4944,7 +4947,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5060,7 +5063,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5225,7 +5228,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5341,7 +5344,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5506,7 +5509,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5622,7 +5625,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5787,7 +5790,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5903,7 +5906,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6068,7 +6071,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6184,7 +6187,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6349,7 +6352,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6465,7 +6468,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6630,7 +6633,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6746,7 +6749,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6911,7 +6914,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7027,7 +7030,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7192,7 +7195,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7308,7 +7311,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7473,7 +7476,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7589,7 +7592,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7754,7 +7757,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7870,7 +7873,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8035,7 +8038,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8151,7 +8154,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8316,7 +8319,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8432,7 +8435,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8597,7 +8600,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8713,7 +8716,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8878,7 +8881,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -8994,7 +8997,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9159,7 +9162,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9275,7 +9278,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9440,7 +9443,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9556,7 +9559,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9721,7 +9724,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9837,7 +9840,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10002,7 +10005,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10118,7 +10121,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10283,7 +10286,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10399,7 +10402,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10564,7 +10567,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10680,7 +10683,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10845,7 +10848,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10961,7 +10964,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11126,7 +11129,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11248,7 +11251,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11413,7 +11416,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11535,7 +11538,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11700,7 +11703,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11822,7 +11825,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -11987,7 +11990,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12109,7 +12112,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12274,7 +12277,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12396,7 +12399,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12561,7 +12564,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12683,7 +12686,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12848,7 +12851,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12970,7 +12973,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13135,7 +13138,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13257,7 +13260,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13422,7 +13425,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13544,7 +13547,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13709,7 +13712,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13831,7 +13834,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -13996,7 +13999,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14118,7 +14121,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14283,7 +14286,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14405,7 +14408,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14570,7 +14573,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14692,7 +14695,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14857,7 +14860,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -14979,7 +14982,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15144,7 +15147,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15266,7 +15269,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15431,7 +15434,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15553,7 +15556,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15718,7 +15721,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15840,7 +15843,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16005,7 +16008,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16127,7 +16130,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16292,7 +16295,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16414,7 +16417,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16579,7 +16582,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16701,7 +16704,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16866,7 +16869,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -16985,7 +16988,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17150,7 +17153,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17266,7 +17269,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17431,7 +17434,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17544,7 +17547,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17709,7 +17712,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17822,7 +17825,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -17987,7 +17990,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18100,7 +18103,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18265,7 +18268,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18378,7 +18381,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18543,7 +18546,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18656,7 +18659,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18821,7 +18824,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18934,7 +18937,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19099,7 +19102,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19212,7 +19215,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19377,7 +19380,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19490,7 +19493,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19655,7 +19658,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19768,7 +19771,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19933,7 +19936,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20046,7 +20049,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20217,7 +20220,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20330,7 +20333,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20501,7 +20504,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20614,7 +20617,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20785,7 +20788,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20898,7 +20901,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21069,7 +21072,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21179,7 +21182,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21350,7 +21353,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21457,7 +21460,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21628,7 +21631,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21732,7 +21735,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21903,7 +21906,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22007,7 +22010,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22178,7 +22181,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22282,7 +22285,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22453,7 +22456,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22557,7 +22560,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22728,7 +22731,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22832,7 +22835,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23003,7 +23006,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23107,7 +23110,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23278,7 +23281,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23379,7 +23382,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23550,7 +23553,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23651,7 +23654,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23822,7 +23825,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23923,7 +23926,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24094,7 +24097,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24195,7 +24198,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24366,7 +24369,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24467,7 +24470,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24638,7 +24641,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24739,7 +24742,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24910,7 +24913,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25011,7 +25014,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25182,7 +25185,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25280,7 +25283,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25451,7 +25454,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25549,7 +25552,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25720,7 +25723,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25818,7 +25821,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -25989,7 +25992,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26087,7 +26090,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26258,7 +26261,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26356,7 +26359,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26527,7 +26530,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26625,7 +26628,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26796,7 +26799,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26894,7 +26897,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27065,7 +27068,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27163,7 +27166,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27334,7 +27337,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27432,7 +27435,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27603,7 +27606,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27701,7 +27704,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27872,7 +27875,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27970,7 +27973,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28141,7 +28144,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28239,7 +28242,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28410,7 +28413,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28508,7 +28511,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28679,7 +28682,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28777,7 +28780,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28948,7 +28951,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29046,7 +29049,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29217,7 +29220,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29315,7 +29318,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29486,7 +29489,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29584,7 +29587,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29755,7 +29758,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29853,7 +29856,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30024,7 +30027,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30122,7 +30125,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30293,7 +30296,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30391,7 +30394,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30562,7 +30565,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30660,7 +30663,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30831,7 +30834,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30929,7 +30932,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31100,7 +31103,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31198,7 +31201,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31369,7 +31372,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31467,7 +31470,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31638,7 +31641,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31736,7 +31739,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31907,7 +31910,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32005,7 +32008,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32176,7 +32179,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32274,7 +32277,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32445,7 +32448,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32543,7 +32546,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32714,7 +32717,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32812,7 +32815,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -32983,7 +32986,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33081,7 +33084,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33252,7 +33255,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33350,7 +33353,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33521,7 +33524,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33619,7 +33622,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33790,7 +33793,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33888,7 +33891,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34059,7 +34062,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34157,7 +34160,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34328,7 +34331,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34426,7 +34429,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34597,7 +34600,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34695,7 +34698,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34866,7 +34869,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34964,7 +34967,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35135,7 +35138,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35233,7 +35236,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35404,7 +35407,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35502,7 +35505,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35673,7 +35676,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35771,7 +35774,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35942,7 +35945,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36040,7 +36043,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36211,7 +36214,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36309,7 +36312,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36480,7 +36483,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36578,7 +36581,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36749,7 +36752,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36847,7 +36850,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37018,7 +37021,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37116,7 +37119,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37287,7 +37290,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37385,7 +37388,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37556,7 +37559,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37654,7 +37657,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37825,7 +37828,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37923,7 +37926,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38094,7 +38097,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38192,7 +38195,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38363,7 +38366,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38461,7 +38464,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38632,7 +38635,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38730,7 +38733,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38901,7 +38904,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -38999,7 +39002,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39170,7 +39173,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39268,7 +39271,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39439,7 +39442,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39537,7 +39540,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39708,7 +39711,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39806,7 +39809,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -39977,7 +39980,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40075,7 +40078,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40246,7 +40249,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40344,7 +40347,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40515,7 +40518,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40613,7 +40616,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40784,7 +40787,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40882,7 +40885,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41053,7 +41056,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41151,7 +41154,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41322,7 +41325,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41420,7 +41423,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41591,7 +41594,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41689,7 +41692,7 @@
         <v>0.01422843894993598</v>
       </c>
       <c r="AM146" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN146">
         <v>0.3570285831928028</v>
@@ -41958,7 +41961,7 @@
         <v>0.01287672421329242</v>
       </c>
       <c r="AM147" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN147">
         <v>0.1138938544209247</v>
@@ -42227,7 +42230,7 @@
         <v>0.01129449859594168</v>
       </c>
       <c r="AM148" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN148">
         <v>0.01929055864963264</v>
@@ -42496,7 +42499,7 @@
         <v>0.01268293743279473</v>
       </c>
       <c r="AM149" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN149">
         <v>0.02713293780673231</v>
@@ -42765,7 +42768,7 @@
         <v>0.006815186142663594</v>
       </c>
       <c r="AM150" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN150">
         <v>0.06060596226028341</v>
@@ -42943,6 +42946,275 @@
       </c>
       <c r="CU150">
         <v>-0.7924465252031915</v>
+      </c>
+    </row>
+    <row r="151" spans="10:99">
+      <c r="J151" t="s">
+        <v>248</v>
+      </c>
+      <c r="K151">
+        <v>0.001094339230302221</v>
+      </c>
+      <c r="L151">
+        <v>0.001094339230302221</v>
+      </c>
+      <c r="M151">
+        <v>0.0006562286858040611</v>
+      </c>
+      <c r="N151">
+        <v>0.0006562286858040611</v>
+      </c>
+      <c r="O151">
+        <v>0.001246630954638395</v>
+      </c>
+      <c r="P151">
+        <v>0.001246630954638395</v>
+      </c>
+      <c r="Q151">
+        <v>0.0007299770217508606</v>
+      </c>
+      <c r="R151">
+        <v>0.0007299770217508606</v>
+      </c>
+      <c r="S151">
+        <v>7.672713645552383</v>
+      </c>
+      <c r="T151">
+        <v>6.550878544924813</v>
+      </c>
+      <c r="U151">
+        <v>0.9883108632696075</v>
+      </c>
+      <c r="V151">
+        <v>0.633975070829861</v>
+      </c>
+      <c r="W151">
+        <v>0.09591588850592812</v>
+      </c>
+      <c r="X151">
+        <v>0.09510039260031514</v>
+      </c>
+      <c r="Y151">
+        <v>0.2415237372443393</v>
+      </c>
+      <c r="Z151">
+        <v>0.2266541513131684</v>
+      </c>
+      <c r="AA151">
+        <v>0.9969104622098344</v>
+      </c>
+      <c r="AB151">
+        <v>0.8391560953924968</v>
+      </c>
+      <c r="AC151">
+        <v>0.858197671828157</v>
+      </c>
+      <c r="AD151">
+        <v>0.9962937052465543</v>
+      </c>
+      <c r="AE151">
+        <v>0.7164621070883913</v>
+      </c>
+      <c r="AF151">
+        <v>0.775995301411877</v>
+      </c>
+      <c r="AG151">
+        <v>0.01209515522086237</v>
+      </c>
+      <c r="AH151">
+        <v>0.01172718359151741</v>
+      </c>
+      <c r="AI151">
+        <v>0.9969104622098344</v>
+      </c>
+      <c r="AJ151">
+        <v>0.9962937052465543</v>
+      </c>
+      <c r="AK151">
+        <v>0.01209515522086237</v>
+      </c>
+      <c r="AL151">
+        <v>0.01172718359151741</v>
+      </c>
+      <c r="AM151" t="s">
+        <v>249</v>
+      </c>
+      <c r="AN151">
+        <v>0.09142880750409497</v>
+      </c>
+      <c r="AO151">
+        <v>0.0848327349970343</v>
+      </c>
+      <c r="AP151">
+        <v>-717.5978317708</v>
+      </c>
+      <c r="AQ151">
+        <v>-508.1040573034001</v>
+      </c>
+      <c r="AR151">
+        <v>42166.30678687176</v>
+      </c>
+      <c r="AS151">
+        <v>23705.4010826966</v>
+      </c>
+      <c r="AT151">
+        <v>42165.83663922911</v>
+      </c>
+      <c r="AU151">
+        <v>23694.3455246966</v>
+      </c>
+      <c r="AV151">
+        <v>3.216630678687176</v>
+      </c>
+      <c r="AW151">
+        <v>1.37054010826966</v>
+      </c>
+      <c r="AX151">
+        <v>3.127798692292451</v>
+      </c>
+      <c r="AY151">
+        <v>3.662872282818906</v>
+      </c>
+      <c r="AZ151">
+        <v>37.31666666666667</v>
+      </c>
+      <c r="BA151">
+        <v>18.91666666666667</v>
+      </c>
+      <c r="BB151">
+        <v>0.06715981570901546</v>
+      </c>
+      <c r="BC151">
+        <v>0.3063248359503895</v>
+      </c>
+      <c r="BD151">
+        <v>-2367.476242095489</v>
+      </c>
+      <c r="BE151">
+        <v>-6276.640502555354</v>
+      </c>
+      <c r="BF151">
+        <v>4113</v>
+      </c>
+      <c r="BG151">
+        <v>5083</v>
+      </c>
+      <c r="BH151">
+        <v>1315.701388888889</v>
+      </c>
+      <c r="BI151">
+        <v>5982</v>
+      </c>
+      <c r="BJ151">
+        <v>3536</v>
+      </c>
+      <c r="BK151">
+        <v>10095</v>
+      </c>
+      <c r="BL151">
+        <v>8619</v>
+      </c>
+      <c r="BM151">
+        <v>0</v>
+      </c>
+      <c r="BN151">
+        <v>0</v>
+      </c>
+      <c r="BO151">
+        <v>516</v>
+      </c>
+      <c r="BP151">
+        <v>542</v>
+      </c>
+      <c r="BQ151">
+        <v>0</v>
+      </c>
+      <c r="BR151">
+        <v>0</v>
+      </c>
+      <c r="BS151">
+        <v>3597</v>
+      </c>
+      <c r="BT151">
+        <v>4541</v>
+      </c>
+      <c r="BU151">
+        <v>5982</v>
+      </c>
+      <c r="BV151">
+        <v>3536</v>
+      </c>
+      <c r="BW151">
+        <v>32166.30678687187</v>
+      </c>
+      <c r="BX151">
+        <v>13705.40108269659</v>
+      </c>
+      <c r="BY151">
+        <v>0.1055230111497342</v>
+      </c>
+      <c r="BZ151">
+        <v>0.1346573875535489</v>
+      </c>
+      <c r="CA151">
+        <v>0.5934733159961176</v>
+      </c>
+      <c r="CB151">
+        <v>0.2109147350507256</v>
+      </c>
+      <c r="CC151">
+        <v>0.0170634728790017</v>
+      </c>
+      <c r="CD151">
+        <v>0.02422087203215548</v>
+      </c>
+      <c r="CE151">
+        <v>0.01754635720680244</v>
+      </c>
+      <c r="CF151">
+        <v>0.02416840888963699</v>
+      </c>
+      <c r="CG151">
+        <v>32883.90461864267</v>
+      </c>
+      <c r="CH151">
+        <v>14213.50513999999</v>
+      </c>
+      <c r="CI151">
+        <v>35251.38086073816</v>
+      </c>
+      <c r="CJ151">
+        <v>20490.14564255534</v>
+      </c>
+      <c r="CK151">
+        <v>0.1060471522551243</v>
+      </c>
+      <c r="CL151">
+        <v>0.06105110705965381</v>
+      </c>
+      <c r="CM151">
+        <v>10000</v>
+      </c>
+      <c r="CO151">
+        <v>0.0407562226866806</v>
+      </c>
+      <c r="CP151">
+        <v>0.01311039331179935</v>
+      </c>
+      <c r="CQ151">
+        <v>35083089.05468039</v>
+      </c>
+      <c r="CR151">
+        <v>9875316.658029791</v>
+      </c>
+      <c r="CS151" s="2">
+        <v>45566.27144988522</v>
+      </c>
+      <c r="CT151">
+        <v>-0.7041943597283349</v>
+      </c>
+      <c r="CU151">
+        <v>-0.7162345042259899</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update BBUSDT.json at 2024-10-01_07-57-56 bestfile_scores 0.003487510306613717 bestfile_sharp 0.10470291873114007
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="394">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -761,6 +761,9 @@
   </si>
   <si>
     <t>REEFUSDT</t>
+  </si>
+  <si>
+    <t>VIDTUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1554,7 +1557,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU151"/>
+  <dimension ref="A1:CU152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1972,7 +1975,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2137,7 +2140,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2253,7 +2256,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2418,7 +2421,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2534,7 +2537,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2699,7 +2702,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2815,7 +2818,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -2980,7 +2983,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3096,7 +3099,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3261,7 +3264,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3377,7 +3380,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3542,7 +3545,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3658,7 +3661,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3823,7 +3826,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3939,7 +3942,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4104,7 +4107,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4220,7 +4223,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4385,7 +4388,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4501,7 +4504,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4666,7 +4669,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4782,7 +4785,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4947,7 +4950,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5063,7 +5066,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5228,7 +5231,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5344,7 +5347,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5509,7 +5512,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5625,7 +5628,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5790,7 +5793,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5906,7 +5909,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6071,7 +6074,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6187,7 +6190,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6352,7 +6355,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6468,7 +6471,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6633,7 +6636,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6749,7 +6752,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6914,7 +6917,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7030,7 +7033,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7195,7 +7198,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7311,7 +7314,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7476,7 +7479,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7592,7 +7595,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7757,7 +7760,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7873,7 +7876,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8038,7 +8041,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8154,7 +8157,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8319,7 +8322,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8435,7 +8438,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8600,7 +8603,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8716,7 +8719,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8881,7 +8884,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -8997,7 +9000,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9162,7 +9165,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9278,7 +9281,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9443,7 +9446,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9559,7 +9562,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9724,7 +9727,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9840,7 +9843,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10005,7 +10008,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10121,7 +10124,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10286,7 +10289,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10402,7 +10405,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10567,7 +10570,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10683,7 +10686,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10848,7 +10851,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10964,7 +10967,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11129,7 +11132,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11251,7 +11254,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11416,7 +11419,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11538,7 +11541,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11703,7 +11706,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11825,7 +11828,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -11990,7 +11993,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12112,7 +12115,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12277,7 +12280,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12399,7 +12402,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12564,7 +12567,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12686,7 +12689,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12851,7 +12854,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12973,7 +12976,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13138,7 +13141,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13260,7 +13263,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13425,7 +13428,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13547,7 +13550,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13712,7 +13715,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13834,7 +13837,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -13999,7 +14002,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14121,7 +14124,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14286,7 +14289,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14408,7 +14411,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14573,7 +14576,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14695,7 +14698,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14860,7 +14863,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -14982,7 +14985,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15147,7 +15150,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15269,7 +15272,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15434,7 +15437,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15556,7 +15559,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15721,7 +15724,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15843,7 +15846,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16008,7 +16011,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16130,7 +16133,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16295,7 +16298,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16417,7 +16420,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16582,7 +16585,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16704,7 +16707,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16869,7 +16872,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -16988,7 +16991,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17153,7 +17156,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17269,7 +17272,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17434,7 +17437,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17547,7 +17550,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17712,7 +17715,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17825,7 +17828,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -17990,7 +17993,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18103,7 +18106,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18268,7 +18271,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18381,7 +18384,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18546,7 +18549,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18659,7 +18662,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18824,7 +18827,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18937,7 +18940,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19102,7 +19105,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19215,7 +19218,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19380,7 +19383,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19493,7 +19496,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19658,7 +19661,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19771,7 +19774,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19936,7 +19939,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20049,7 +20052,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20220,7 +20223,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20333,7 +20336,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20504,7 +20507,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20617,7 +20620,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20788,7 +20791,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20901,7 +20904,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21072,7 +21075,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21182,7 +21185,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21353,7 +21356,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21460,7 +21463,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21631,7 +21634,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21735,7 +21738,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21906,7 +21909,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22010,7 +22013,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22181,7 +22184,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22285,7 +22288,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22456,7 +22459,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22560,7 +22563,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22731,7 +22734,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22835,7 +22838,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23006,7 +23009,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23110,7 +23113,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23281,7 +23284,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23382,7 +23385,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23553,7 +23556,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23654,7 +23657,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23825,7 +23828,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23926,7 +23929,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24097,7 +24100,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24198,7 +24201,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24369,7 +24372,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24470,7 +24473,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24641,7 +24644,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24742,7 +24745,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24913,7 +24916,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25014,7 +25017,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25185,7 +25188,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25283,7 +25286,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25454,7 +25457,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25552,7 +25555,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25723,7 +25726,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25821,7 +25824,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -25992,7 +25995,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26090,7 +26093,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26261,7 +26264,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26359,7 +26362,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26530,7 +26533,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26628,7 +26631,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26799,7 +26802,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26897,7 +26900,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27068,7 +27071,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27166,7 +27169,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27337,7 +27340,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27435,7 +27438,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27606,7 +27609,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27704,7 +27707,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27875,7 +27878,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27973,7 +27976,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28144,7 +28147,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28242,7 +28245,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28413,7 +28416,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28511,7 +28514,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28682,7 +28685,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28780,7 +28783,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28951,7 +28954,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29049,7 +29052,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29220,7 +29223,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29318,7 +29321,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29489,7 +29492,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29587,7 +29590,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29758,7 +29761,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29856,7 +29859,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30027,7 +30030,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30125,7 +30128,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30296,7 +30299,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30394,7 +30397,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30565,7 +30568,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30663,7 +30666,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30834,7 +30837,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30932,7 +30935,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31103,7 +31106,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31201,7 +31204,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31372,7 +31375,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31470,7 +31473,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31641,7 +31644,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31739,7 +31742,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31910,7 +31913,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32008,7 +32011,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32179,7 +32182,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32277,7 +32280,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32448,7 +32451,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32546,7 +32549,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32717,7 +32720,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32815,7 +32818,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -32986,7 +32989,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33084,7 +33087,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33255,7 +33258,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33353,7 +33356,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33524,7 +33527,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33622,7 +33625,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33793,7 +33796,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33891,7 +33894,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34062,7 +34065,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34160,7 +34163,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34331,7 +34334,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34429,7 +34432,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34600,7 +34603,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34698,7 +34701,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34869,7 +34872,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34967,7 +34970,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35138,7 +35141,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35236,7 +35239,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35407,7 +35410,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35505,7 +35508,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35676,7 +35679,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35774,7 +35777,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35945,7 +35948,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36043,7 +36046,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36214,7 +36217,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36312,7 +36315,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36483,7 +36486,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36581,7 +36584,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36752,7 +36755,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36850,7 +36853,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37021,7 +37024,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37119,7 +37122,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37290,7 +37293,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37388,7 +37391,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37559,7 +37562,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37657,7 +37660,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37828,7 +37831,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37926,7 +37929,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38097,7 +38100,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38195,7 +38198,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38366,7 +38369,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38464,7 +38467,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38635,7 +38638,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38733,7 +38736,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38904,7 +38907,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -39002,7 +39005,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39173,7 +39176,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39271,7 +39274,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39442,7 +39445,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39540,7 +39543,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39711,7 +39714,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39809,7 +39812,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -39980,7 +39983,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40078,7 +40081,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40249,7 +40252,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40347,7 +40350,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40518,7 +40521,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40616,7 +40619,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40787,7 +40790,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40885,7 +40888,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41056,7 +41059,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41154,7 +41157,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41325,7 +41328,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41423,7 +41426,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41594,7 +41597,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41692,7 +41695,7 @@
         <v>0.01422843894993598</v>
       </c>
       <c r="AM146" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN146">
         <v>0.3570285831928028</v>
@@ -41961,7 +41964,7 @@
         <v>0.01287672421329242</v>
       </c>
       <c r="AM147" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN147">
         <v>0.1138938544209247</v>
@@ -42230,7 +42233,7 @@
         <v>0.01129449859594168</v>
       </c>
       <c r="AM148" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN148">
         <v>0.01929055864963264</v>
@@ -42499,7 +42502,7 @@
         <v>0.01268293743279473</v>
       </c>
       <c r="AM149" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN149">
         <v>0.02713293780673231</v>
@@ -42768,7 +42771,7 @@
         <v>0.006815186142663594</v>
       </c>
       <c r="AM150" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN150">
         <v>0.06060596226028341</v>
@@ -43037,7 +43040,7 @@
         <v>0.01172718359151741</v>
       </c>
       <c r="AM151" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN151">
         <v>0.09142880750409497</v>
@@ -43215,6 +43218,275 @@
       </c>
       <c r="CU151">
         <v>-0.7162345042259899</v>
+      </c>
+    </row>
+    <row r="152" spans="10:99">
+      <c r="J152" t="s">
+        <v>249</v>
+      </c>
+      <c r="K152">
+        <v>0.004628604379359746</v>
+      </c>
+      <c r="L152">
+        <v>0.004628604379359746</v>
+      </c>
+      <c r="M152">
+        <v>0.007537649702437976</v>
+      </c>
+      <c r="N152">
+        <v>0.007537649702437976</v>
+      </c>
+      <c r="O152">
+        <v>0.007303512340594498</v>
+      </c>
+      <c r="P152">
+        <v>0.007303512340594498</v>
+      </c>
+      <c r="Q152">
+        <v>0.009364577931612938</v>
+      </c>
+      <c r="R152">
+        <v>0.009364577931612938</v>
+      </c>
+      <c r="S152">
+        <v>3.696535421437541</v>
+      </c>
+      <c r="T152">
+        <v>23.10999482898722</v>
+      </c>
+      <c r="U152">
+        <v>0.9956116636622782</v>
+      </c>
+      <c r="V152">
+        <v>0.7897924622269059</v>
+      </c>
+      <c r="W152">
+        <v>0.09999733885011025</v>
+      </c>
+      <c r="X152">
+        <v>0.09451574461716997</v>
+      </c>
+      <c r="Y152">
+        <v>0.1069501739871326</v>
+      </c>
+      <c r="Z152">
+        <v>0.1187033680841537</v>
+      </c>
+      <c r="AA152">
+        <v>0.9824530069386523</v>
+      </c>
+      <c r="AB152">
+        <v>0.9036766197611241</v>
+      </c>
+      <c r="AC152">
+        <v>0.9086523548279904</v>
+      </c>
+      <c r="AD152">
+        <v>0.9955626532703593</v>
+      </c>
+      <c r="AE152">
+        <v>0.8974069958886675</v>
+      </c>
+      <c r="AF152">
+        <v>0.8825532597660568</v>
+      </c>
+      <c r="AG152">
+        <v>0.02781150289803924</v>
+      </c>
+      <c r="AH152">
+        <v>0.01464508407647874</v>
+      </c>
+      <c r="AI152">
+        <v>0.9824530069386523</v>
+      </c>
+      <c r="AJ152">
+        <v>0.9955626532703593</v>
+      </c>
+      <c r="AK152">
+        <v>0.02781150289803924</v>
+      </c>
+      <c r="AL152">
+        <v>0.01464508407647874</v>
+      </c>
+      <c r="AM152" t="s">
+        <v>250</v>
+      </c>
+      <c r="AN152">
+        <v>0.3981395839245215</v>
+      </c>
+      <c r="AO152">
+        <v>0.1964166228833482</v>
+      </c>
+      <c r="AP152">
+        <v>-20.331237688</v>
+      </c>
+      <c r="AQ152">
+        <v>-59.486731742</v>
+      </c>
+      <c r="AR152">
+        <v>11896.35336189734</v>
+      </c>
+      <c r="AS152">
+        <v>13262.74231825799</v>
+      </c>
+      <c r="AT152">
+        <v>11929.68179231201</v>
+      </c>
+      <c r="AU152">
+        <v>13266.46275825799</v>
+      </c>
+      <c r="AV152">
+        <v>0.189635336189734</v>
+      </c>
+      <c r="AW152">
+        <v>0.3262742318257992</v>
+      </c>
+      <c r="AX152">
+        <v>6.510144927536231</v>
+      </c>
+      <c r="AY152">
+        <v>1.034754224270353</v>
+      </c>
+      <c r="AZ152">
+        <v>23.81666666666667</v>
+      </c>
+      <c r="BA152">
+        <v>18.7</v>
+      </c>
+      <c r="BB152">
+        <v>0.0476034285662398</v>
+      </c>
+      <c r="BC152">
+        <v>0.008337582419549946</v>
+      </c>
+      <c r="BD152">
+        <v>-95.80122520077572</v>
+      </c>
+      <c r="BE152">
+        <v>-27.9322459235488</v>
+      </c>
+      <c r="BF152">
+        <v>89</v>
+      </c>
+      <c r="BG152">
+        <v>398</v>
+      </c>
+      <c r="BH152">
+        <v>37.60277777777778</v>
+      </c>
+      <c r="BI152">
+        <v>50</v>
+      </c>
+      <c r="BJ152">
+        <v>471</v>
+      </c>
+      <c r="BK152">
+        <v>139</v>
+      </c>
+      <c r="BL152">
+        <v>869</v>
+      </c>
+      <c r="BM152">
+        <v>0</v>
+      </c>
+      <c r="BN152">
+        <v>0</v>
+      </c>
+      <c r="BO152">
+        <v>48</v>
+      </c>
+      <c r="BP152">
+        <v>80</v>
+      </c>
+      <c r="BQ152">
+        <v>0</v>
+      </c>
+      <c r="BR152">
+        <v>0</v>
+      </c>
+      <c r="BS152">
+        <v>41</v>
+      </c>
+      <c r="BT152">
+        <v>318</v>
+      </c>
+      <c r="BU152">
+        <v>50</v>
+      </c>
+      <c r="BV152">
+        <v>471</v>
+      </c>
+      <c r="BW152">
+        <v>1896.353361897333</v>
+      </c>
+      <c r="BX152">
+        <v>3262.742318257995</v>
+      </c>
+      <c r="BY152">
+        <v>0.1175321372209945</v>
+      </c>
+      <c r="BZ152">
+        <v>0.084942739986385</v>
+      </c>
+      <c r="CA152">
+        <v>0.1259214159167363</v>
+      </c>
+      <c r="CB152">
+        <v>0.1051024956550246</v>
+      </c>
+      <c r="CC152">
+        <v>0.04051888288167163</v>
+      </c>
+      <c r="CD152">
+        <v>0.01250691688980898</v>
+      </c>
+      <c r="CE152">
+        <v>0.02798156179946276</v>
+      </c>
+      <c r="CF152">
+        <v>0.01421662694897063</v>
+      </c>
+      <c r="CG152">
+        <v>1916.684599585333</v>
+      </c>
+      <c r="CH152">
+        <v>3322.229049999995</v>
+      </c>
+      <c r="CI152">
+        <v>2012.485824786109</v>
+      </c>
+      <c r="CJ152">
+        <v>3350.161295923544</v>
+      </c>
+      <c r="CK152">
+        <v>0.2105295694136707</v>
+      </c>
+      <c r="CL152">
+        <v>0.3206870364919667</v>
+      </c>
+      <c r="CM152">
+        <v>10000</v>
+      </c>
+      <c r="CO152">
+        <v>0.2367256637168142</v>
+      </c>
+      <c r="CP152">
+        <v>0.120575221238938</v>
+      </c>
+      <c r="CQ152">
+        <v>592843.0053132395</v>
+      </c>
+      <c r="CR152">
+        <v>2338303.893655388</v>
+      </c>
+      <c r="CS152" s="2">
+        <v>45566.29262072441</v>
+      </c>
+      <c r="CT152">
+        <v>-0.2458369562066722</v>
+      </c>
+      <c r="CU152">
+        <v>-0.09923207859327181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update SFPUSDT.json at 2024-10-01_23-05-46 bestfile_scores 0.0009300990691284705 bestfile_sharp 0.10216393432740803
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="396">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -767,6 +767,9 @@
   </si>
   <si>
     <t>BBUSDT</t>
+  </si>
+  <si>
+    <t>QTUMUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1560,7 +1563,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU153"/>
+  <dimension ref="A1:CU154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1978,7 +1981,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2143,7 +2146,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2259,7 +2262,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2424,7 +2427,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2540,7 +2543,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2705,7 +2708,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2821,7 +2824,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -2986,7 +2989,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3102,7 +3105,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3267,7 +3270,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3383,7 +3386,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3548,7 +3551,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3664,7 +3667,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3829,7 +3832,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3945,7 +3948,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4110,7 +4113,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4226,7 +4229,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4391,7 +4394,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4507,7 +4510,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4672,7 +4675,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4788,7 +4791,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4953,7 +4956,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5069,7 +5072,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5234,7 +5237,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5350,7 +5353,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5515,7 +5518,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5631,7 +5634,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5796,7 +5799,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5912,7 +5915,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6077,7 +6080,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6193,7 +6196,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6358,7 +6361,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6474,7 +6477,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6639,7 +6642,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6755,7 +6758,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6920,7 +6923,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7036,7 +7039,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7201,7 +7204,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7317,7 +7320,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7482,7 +7485,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7598,7 +7601,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7763,7 +7766,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7879,7 +7882,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8044,7 +8047,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8160,7 +8163,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8325,7 +8328,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8441,7 +8444,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8606,7 +8609,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8722,7 +8725,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8887,7 +8890,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -9003,7 +9006,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9168,7 +9171,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9284,7 +9287,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9449,7 +9452,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9565,7 +9568,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9730,7 +9733,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9846,7 +9849,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10011,7 +10014,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10127,7 +10130,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10292,7 +10295,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10408,7 +10411,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10573,7 +10576,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10689,7 +10692,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10854,7 +10857,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10970,7 +10973,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11135,7 +11138,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11257,7 +11260,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11422,7 +11425,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11544,7 +11547,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11709,7 +11712,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11831,7 +11834,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -11996,7 +11999,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12118,7 +12121,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12283,7 +12286,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12405,7 +12408,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12570,7 +12573,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12692,7 +12695,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12857,7 +12860,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12979,7 +12982,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13144,7 +13147,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13266,7 +13269,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13431,7 +13434,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13553,7 +13556,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13718,7 +13721,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13840,7 +13843,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -14005,7 +14008,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14127,7 +14130,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14292,7 +14295,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14414,7 +14417,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14579,7 +14582,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14701,7 +14704,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14866,7 +14869,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -14988,7 +14991,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15153,7 +15156,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15275,7 +15278,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15440,7 +15443,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15562,7 +15565,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15727,7 +15730,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15849,7 +15852,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16014,7 +16017,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16136,7 +16139,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16301,7 +16304,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16423,7 +16426,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16588,7 +16591,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16710,7 +16713,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16875,7 +16878,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -16994,7 +16997,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17159,7 +17162,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17275,7 +17278,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17440,7 +17443,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17553,7 +17556,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17718,7 +17721,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17831,7 +17834,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -17996,7 +17999,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18109,7 +18112,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18274,7 +18277,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18387,7 +18390,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18552,7 +18555,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18665,7 +18668,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18830,7 +18833,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18943,7 +18946,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19108,7 +19111,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19221,7 +19224,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19386,7 +19389,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19499,7 +19502,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19664,7 +19667,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19777,7 +19780,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19942,7 +19945,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20055,7 +20058,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20226,7 +20229,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20339,7 +20342,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20510,7 +20513,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20623,7 +20626,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20794,7 +20797,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20907,7 +20910,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21078,7 +21081,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21188,7 +21191,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21359,7 +21362,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21466,7 +21469,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21637,7 +21640,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21741,7 +21744,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21912,7 +21915,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22016,7 +22019,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22187,7 +22190,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22291,7 +22294,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22462,7 +22465,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22566,7 +22569,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22737,7 +22740,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22841,7 +22844,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23012,7 +23015,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23116,7 +23119,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23287,7 +23290,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23388,7 +23391,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23559,7 +23562,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23660,7 +23663,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23831,7 +23834,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23932,7 +23935,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24103,7 +24106,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24204,7 +24207,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24375,7 +24378,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24476,7 +24479,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24647,7 +24650,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24748,7 +24751,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24919,7 +24922,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25020,7 +25023,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25191,7 +25194,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25289,7 +25292,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25460,7 +25463,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25558,7 +25561,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25729,7 +25732,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25827,7 +25830,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -25998,7 +26001,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26096,7 +26099,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26267,7 +26270,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26365,7 +26368,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26536,7 +26539,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26634,7 +26637,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26805,7 +26808,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26903,7 +26906,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27074,7 +27077,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27172,7 +27175,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27343,7 +27346,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27441,7 +27444,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27612,7 +27615,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27710,7 +27713,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27881,7 +27884,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27979,7 +27982,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28150,7 +28153,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28248,7 +28251,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28419,7 +28422,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28517,7 +28520,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28688,7 +28691,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28786,7 +28789,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28957,7 +28960,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29055,7 +29058,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29226,7 +29229,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29324,7 +29327,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29495,7 +29498,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29593,7 +29596,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29764,7 +29767,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29862,7 +29865,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30033,7 +30036,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30131,7 +30134,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30302,7 +30305,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30400,7 +30403,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30571,7 +30574,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30669,7 +30672,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30840,7 +30843,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30938,7 +30941,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31109,7 +31112,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31207,7 +31210,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31378,7 +31381,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31476,7 +31479,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31647,7 +31650,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31745,7 +31748,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31916,7 +31919,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32014,7 +32017,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32185,7 +32188,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32283,7 +32286,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32454,7 +32457,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32552,7 +32555,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32723,7 +32726,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32821,7 +32824,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -32992,7 +32995,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33090,7 +33093,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33261,7 +33264,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33359,7 +33362,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33530,7 +33533,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33628,7 +33631,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33799,7 +33802,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33897,7 +33900,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34068,7 +34071,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34166,7 +34169,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34337,7 +34340,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34435,7 +34438,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34606,7 +34609,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34704,7 +34707,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34875,7 +34878,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34973,7 +34976,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35144,7 +35147,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35242,7 +35245,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35413,7 +35416,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35511,7 +35514,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35682,7 +35685,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35780,7 +35783,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35951,7 +35954,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36049,7 +36052,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36220,7 +36223,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36318,7 +36321,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36489,7 +36492,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36587,7 +36590,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36758,7 +36761,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36856,7 +36859,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37027,7 +37030,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37125,7 +37128,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37296,7 +37299,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37394,7 +37397,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37565,7 +37568,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37663,7 +37666,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37834,7 +37837,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37932,7 +37935,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38103,7 +38106,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38201,7 +38204,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38372,7 +38375,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38470,7 +38473,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38641,7 +38644,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38739,7 +38742,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38910,7 +38913,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -39008,7 +39011,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39179,7 +39182,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39277,7 +39280,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39448,7 +39451,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39546,7 +39549,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39717,7 +39720,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39815,7 +39818,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -39986,7 +39989,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40084,7 +40087,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40255,7 +40258,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40353,7 +40356,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40524,7 +40527,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40622,7 +40625,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40793,7 +40796,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40891,7 +40894,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41062,7 +41065,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41160,7 +41163,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41331,7 +41334,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41429,7 +41432,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41600,7 +41603,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41698,7 +41701,7 @@
         <v>0.01422843894993598</v>
       </c>
       <c r="AM146" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN146">
         <v>0.3570285831928028</v>
@@ -41967,7 +41970,7 @@
         <v>0.01287672421329242</v>
       </c>
       <c r="AM147" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN147">
         <v>0.1138938544209247</v>
@@ -42236,7 +42239,7 @@
         <v>0.01129449859594168</v>
       </c>
       <c r="AM148" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN148">
         <v>0.01929055864963264</v>
@@ -42505,7 +42508,7 @@
         <v>0.01268293743279473</v>
       </c>
       <c r="AM149" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN149">
         <v>0.02713293780673231</v>
@@ -42774,7 +42777,7 @@
         <v>0.006815186142663594</v>
       </c>
       <c r="AM150" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN150">
         <v>0.06060596226028341</v>
@@ -43043,7 +43046,7 @@
         <v>0.01172718359151741</v>
       </c>
       <c r="AM151" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN151">
         <v>0.09142880750409497</v>
@@ -43312,7 +43315,7 @@
         <v>0.01464508407647874</v>
       </c>
       <c r="AM152" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN152">
         <v>0.3981395839245215</v>
@@ -43581,7 +43584,7 @@
         <v>0.01424145384485694</v>
       </c>
       <c r="AM153" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN153">
         <v>0.1335188651800471</v>
@@ -43759,6 +43762,275 @@
       </c>
       <c r="CU153">
         <v>-0.2834712011312049</v>
+      </c>
+    </row>
+    <row r="154" spans="10:99">
+      <c r="J154" t="s">
+        <v>251</v>
+      </c>
+      <c r="K154">
+        <v>0.001310550855838866</v>
+      </c>
+      <c r="L154">
+        <v>0.001310550855838866</v>
+      </c>
+      <c r="M154">
+        <v>0.0005547042943281344</v>
+      </c>
+      <c r="N154">
+        <v>0.0005547042943281344</v>
+      </c>
+      <c r="O154">
+        <v>0.0009449200156608217</v>
+      </c>
+      <c r="P154">
+        <v>0.0009449200156608217</v>
+      </c>
+      <c r="Q154">
+        <v>0.0004369928898233288</v>
+      </c>
+      <c r="R154">
+        <v>0.0004369928898233288</v>
+      </c>
+      <c r="S154">
+        <v>6.74079872287731</v>
+      </c>
+      <c r="T154">
+        <v>12.3210681810943</v>
+      </c>
+      <c r="U154">
+        <v>0.9898073033907518</v>
+      </c>
+      <c r="V154">
+        <v>0.6324092725343671</v>
+      </c>
+      <c r="W154">
+        <v>0.08979195537706917</v>
+      </c>
+      <c r="X154">
+        <v>0.0806566095662971</v>
+      </c>
+      <c r="Y154">
+        <v>0.2357391322001378</v>
+      </c>
+      <c r="Z154">
+        <v>0.2293171629649537</v>
+      </c>
+      <c r="AA154">
+        <v>0.9984806413598178</v>
+      </c>
+      <c r="AB154">
+        <v>0.8079074430175333</v>
+      </c>
+      <c r="AC154">
+        <v>0.8090924772302086</v>
+      </c>
+      <c r="AD154">
+        <v>0.9988266364825759</v>
+      </c>
+      <c r="AE154">
+        <v>0.7104316699771203</v>
+      </c>
+      <c r="AF154">
+        <v>0.7709527026797399</v>
+      </c>
+      <c r="AG154">
+        <v>0.009486398822474689</v>
+      </c>
+      <c r="AH154">
+        <v>0.008636072468123625</v>
+      </c>
+      <c r="AI154">
+        <v>0.9984806413598178</v>
+      </c>
+      <c r="AJ154">
+        <v>0.9988266364825759</v>
+      </c>
+      <c r="AK154">
+        <v>0.009486398822474689</v>
+      </c>
+      <c r="AL154">
+        <v>0.008636072468123625</v>
+      </c>
+      <c r="AM154" t="s">
+        <v>252</v>
+      </c>
+      <c r="AN154">
+        <v>0.06745759346973818</v>
+      </c>
+      <c r="AO154">
+        <v>0.0353603039309605</v>
+      </c>
+      <c r="AP154">
+        <v>-1284.9050483</v>
+      </c>
+      <c r="AQ154">
+        <v>-811.6936034200002</v>
+      </c>
+      <c r="AR154">
+        <v>65840.24395170035</v>
+      </c>
+      <c r="AS154">
+        <v>22210.88527195222</v>
+      </c>
+      <c r="AT154">
+        <v>65835.79925170036</v>
+      </c>
+      <c r="AU154">
+        <v>22211.01809658024</v>
+      </c>
+      <c r="AV154">
+        <v>5.584024395170035</v>
+      </c>
+      <c r="AW154">
+        <v>1.221088527195222</v>
+      </c>
+      <c r="AX154">
+        <v>3.560408289514382</v>
+      </c>
+      <c r="AY154">
+        <v>1.947944046477523</v>
+      </c>
+      <c r="AZ154">
+        <v>34.38333333333333</v>
+      </c>
+      <c r="BA154">
+        <v>95.2</v>
+      </c>
+      <c r="BB154">
+        <v>0.1079692261440423</v>
+      </c>
+      <c r="BC154">
+        <v>0.05319420273052464</v>
+      </c>
+      <c r="BD154">
+        <v>-6914.288510733679</v>
+      </c>
+      <c r="BE154">
+        <v>-731.6449717234095</v>
+      </c>
+      <c r="BF154">
+        <v>3783</v>
+      </c>
+      <c r="BG154">
+        <v>8854</v>
+      </c>
+      <c r="BH154">
+        <v>1438.998611111111</v>
+      </c>
+      <c r="BI154">
+        <v>5917</v>
+      </c>
+      <c r="BJ154">
+        <v>8876</v>
+      </c>
+      <c r="BK154">
+        <v>9700</v>
+      </c>
+      <c r="BL154">
+        <v>17730</v>
+      </c>
+      <c r="BM154">
+        <v>0</v>
+      </c>
+      <c r="BN154">
+        <v>0</v>
+      </c>
+      <c r="BO154">
+        <v>186</v>
+      </c>
+      <c r="BP154">
+        <v>3765</v>
+      </c>
+      <c r="BQ154">
+        <v>0</v>
+      </c>
+      <c r="BR154">
+        <v>0</v>
+      </c>
+      <c r="BS154">
+        <v>3597</v>
+      </c>
+      <c r="BT154">
+        <v>5089</v>
+      </c>
+      <c r="BU154">
+        <v>5917</v>
+      </c>
+      <c r="BV154">
+        <v>8876</v>
+      </c>
+      <c r="BW154">
+        <v>55840.24395170009</v>
+      </c>
+      <c r="BX154">
+        <v>12210.88527195199</v>
+      </c>
+      <c r="BY154">
+        <v>0.0950373463777691</v>
+      </c>
+      <c r="BZ154">
+        <v>0.07418767024140233</v>
+      </c>
+      <c r="CA154">
+        <v>0.3516386657733838</v>
+      </c>
+      <c r="CB154">
+        <v>0.1878865385266587</v>
+      </c>
+      <c r="CC154">
+        <v>0.01357086897229917</v>
+      </c>
+      <c r="CD154">
+        <v>0.01113096283372704</v>
+      </c>
+      <c r="CE154">
+        <v>0.01454666252422261</v>
+      </c>
+      <c r="CF154">
+        <v>0.01268101666128819</v>
+      </c>
+      <c r="CG154">
+        <v>57125.14900000009</v>
+      </c>
+      <c r="CH154">
+        <v>13022.57887537199</v>
+      </c>
+      <c r="CI154">
+        <v>64039.43751073377</v>
+      </c>
+      <c r="CJ154">
+        <v>13754.2238470954</v>
+      </c>
+      <c r="CK154">
+        <v>0.1227722005586904</v>
+      </c>
+      <c r="CL154">
+        <v>0.075227385871015</v>
+      </c>
+      <c r="CM154">
+        <v>10000</v>
+      </c>
+      <c r="CO154">
+        <v>0.01534586096070881</v>
+      </c>
+      <c r="CP154">
+        <v>0.01103164721892463</v>
+      </c>
+      <c r="CQ154">
+        <v>45715024.24007426</v>
+      </c>
+      <c r="CR154">
+        <v>10585406.58084074</v>
+      </c>
+      <c r="CS154" s="2">
+        <v>45566.58953914532</v>
+      </c>
+      <c r="CT154">
+        <v>-0.6947171497334547</v>
+      </c>
+      <c r="CU154">
+        <v>-0.8339343080179423</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update POLYXUSDT.json at 2024-10-02_02-05-07 bestfile_scores 0.0012700171433919216 bestfile_sharp 0.1251524929448511
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="398">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -773,6 +773,9 @@
   </si>
   <si>
     <t>SFPUSDT</t>
+  </si>
+  <si>
+    <t>BEAMXUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1566,7 +1569,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU155"/>
+  <dimension ref="A1:CU156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1984,7 +1987,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2149,7 +2152,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2265,7 +2268,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2430,7 +2433,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2546,7 +2549,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2711,7 +2714,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2827,7 +2830,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -2992,7 +2995,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3108,7 +3111,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3273,7 +3276,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3389,7 +3392,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3554,7 +3557,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3670,7 +3673,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3835,7 +3838,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3951,7 +3954,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4116,7 +4119,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4232,7 +4235,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4397,7 +4400,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4513,7 +4516,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4678,7 +4681,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4794,7 +4797,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4959,7 +4962,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5075,7 +5078,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5240,7 +5243,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5356,7 +5359,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5521,7 +5524,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5637,7 +5640,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5802,7 +5805,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5918,7 +5921,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6083,7 +6086,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6199,7 +6202,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6364,7 +6367,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6480,7 +6483,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6645,7 +6648,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6761,7 +6764,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6926,7 +6929,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7042,7 +7045,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7207,7 +7210,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7323,7 +7326,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7488,7 +7491,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7604,7 +7607,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7769,7 +7772,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7885,7 +7888,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8050,7 +8053,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8166,7 +8169,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8331,7 +8334,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8447,7 +8450,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8612,7 +8615,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8728,7 +8731,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8893,7 +8896,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -9009,7 +9012,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9174,7 +9177,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9290,7 +9293,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9455,7 +9458,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9571,7 +9574,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9736,7 +9739,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9852,7 +9855,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10017,7 +10020,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10133,7 +10136,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10298,7 +10301,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10414,7 +10417,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10579,7 +10582,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10695,7 +10698,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10860,7 +10863,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10976,7 +10979,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11141,7 +11144,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11263,7 +11266,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11428,7 +11431,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11550,7 +11553,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11715,7 +11718,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11837,7 +11840,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -12002,7 +12005,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12124,7 +12127,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12289,7 +12292,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12411,7 +12414,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12576,7 +12579,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12698,7 +12701,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12863,7 +12866,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12985,7 +12988,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13150,7 +13153,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13272,7 +13275,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13437,7 +13440,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13559,7 +13562,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13724,7 +13727,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13846,7 +13849,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -14011,7 +14014,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14133,7 +14136,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14298,7 +14301,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14420,7 +14423,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14585,7 +14588,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14707,7 +14710,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14872,7 +14875,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -14994,7 +14997,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15159,7 +15162,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15281,7 +15284,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15446,7 +15449,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15568,7 +15571,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15733,7 +15736,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15855,7 +15858,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16020,7 +16023,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16142,7 +16145,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16307,7 +16310,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16429,7 +16432,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16594,7 +16597,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16716,7 +16719,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16881,7 +16884,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -17000,7 +17003,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17165,7 +17168,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17281,7 +17284,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17446,7 +17449,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17559,7 +17562,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17724,7 +17727,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17837,7 +17840,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -18002,7 +18005,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18115,7 +18118,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18280,7 +18283,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18393,7 +18396,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18558,7 +18561,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18671,7 +18674,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18836,7 +18839,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18949,7 +18952,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19114,7 +19117,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19227,7 +19230,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19392,7 +19395,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19505,7 +19508,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19670,7 +19673,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19783,7 +19786,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19948,7 +19951,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20061,7 +20064,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20232,7 +20235,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20345,7 +20348,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20516,7 +20519,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20629,7 +20632,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20800,7 +20803,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20913,7 +20916,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21084,7 +21087,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21194,7 +21197,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21365,7 +21368,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21472,7 +21475,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21643,7 +21646,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21747,7 +21750,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21918,7 +21921,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22022,7 +22025,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22193,7 +22196,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22297,7 +22300,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22468,7 +22471,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22572,7 +22575,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22743,7 +22746,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22847,7 +22850,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23018,7 +23021,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23122,7 +23125,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23293,7 +23296,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23394,7 +23397,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23565,7 +23568,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23666,7 +23669,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23837,7 +23840,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23938,7 +23941,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24109,7 +24112,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24210,7 +24213,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24381,7 +24384,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24482,7 +24485,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24653,7 +24656,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24754,7 +24757,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24925,7 +24928,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25026,7 +25029,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25197,7 +25200,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25295,7 +25298,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25466,7 +25469,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25564,7 +25567,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25735,7 +25738,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25833,7 +25836,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -26004,7 +26007,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26102,7 +26105,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26273,7 +26276,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26371,7 +26374,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26542,7 +26545,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26640,7 +26643,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26811,7 +26814,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26909,7 +26912,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27080,7 +27083,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27178,7 +27181,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27349,7 +27352,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27447,7 +27450,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27618,7 +27621,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27716,7 +27719,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27887,7 +27890,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27985,7 +27988,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28156,7 +28159,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28254,7 +28257,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28425,7 +28428,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28523,7 +28526,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28694,7 +28697,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28792,7 +28795,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28963,7 +28966,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29061,7 +29064,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29232,7 +29235,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29330,7 +29333,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29501,7 +29504,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29599,7 +29602,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29770,7 +29773,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29868,7 +29871,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30039,7 +30042,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30137,7 +30140,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30308,7 +30311,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30406,7 +30409,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30577,7 +30580,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30675,7 +30678,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30846,7 +30849,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30944,7 +30947,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31115,7 +31118,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31213,7 +31216,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31384,7 +31387,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31482,7 +31485,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31653,7 +31656,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31751,7 +31754,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31922,7 +31925,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32020,7 +32023,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32191,7 +32194,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32289,7 +32292,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32460,7 +32463,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32558,7 +32561,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32729,7 +32732,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32827,7 +32830,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -32998,7 +33001,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33096,7 +33099,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33267,7 +33270,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33365,7 +33368,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33536,7 +33539,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33634,7 +33637,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33805,7 +33808,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33903,7 +33906,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34074,7 +34077,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34172,7 +34175,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34343,7 +34346,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34441,7 +34444,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34612,7 +34615,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34710,7 +34713,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34881,7 +34884,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34979,7 +34982,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35150,7 +35153,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35248,7 +35251,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35419,7 +35422,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35517,7 +35520,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35688,7 +35691,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35786,7 +35789,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35957,7 +35960,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36055,7 +36058,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36226,7 +36229,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36324,7 +36327,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36495,7 +36498,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36593,7 +36596,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36764,7 +36767,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36862,7 +36865,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37033,7 +37036,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37131,7 +37134,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37302,7 +37305,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37400,7 +37403,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37571,7 +37574,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37669,7 +37672,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37840,7 +37843,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37938,7 +37941,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38109,7 +38112,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38207,7 +38210,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38378,7 +38381,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38476,7 +38479,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38647,7 +38650,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38745,7 +38748,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38916,7 +38919,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -39014,7 +39017,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39185,7 +39188,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39283,7 +39286,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39454,7 +39457,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39552,7 +39555,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39723,7 +39726,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39821,7 +39824,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -39992,7 +39995,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40090,7 +40093,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40261,7 +40264,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40359,7 +40362,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40530,7 +40533,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40628,7 +40631,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40799,7 +40802,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40897,7 +40900,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41068,7 +41071,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41166,7 +41169,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41337,7 +41340,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41435,7 +41438,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41606,7 +41609,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41704,7 +41707,7 @@
         <v>0.01422843894993598</v>
       </c>
       <c r="AM146" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN146">
         <v>0.3570285831928028</v>
@@ -41973,7 +41976,7 @@
         <v>0.01287672421329242</v>
       </c>
       <c r="AM147" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN147">
         <v>0.1138938544209247</v>
@@ -42242,7 +42245,7 @@
         <v>0.01129449859594168</v>
       </c>
       <c r="AM148" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN148">
         <v>0.01929055864963264</v>
@@ -42511,7 +42514,7 @@
         <v>0.01268293743279473</v>
       </c>
       <c r="AM149" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN149">
         <v>0.02713293780673231</v>
@@ -42780,7 +42783,7 @@
         <v>0.006815186142663594</v>
       </c>
       <c r="AM150" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN150">
         <v>0.06060596226028341</v>
@@ -43049,7 +43052,7 @@
         <v>0.01172718359151741</v>
       </c>
       <c r="AM151" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN151">
         <v>0.09142880750409497</v>
@@ -43318,7 +43321,7 @@
         <v>0.01464508407647874</v>
       </c>
       <c r="AM152" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN152">
         <v>0.3981395839245215</v>
@@ -43587,7 +43590,7 @@
         <v>0.01424145384485694</v>
       </c>
       <c r="AM153" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN153">
         <v>0.1335188651800471</v>
@@ -43856,7 +43859,7 @@
         <v>0.008636072468123625</v>
       </c>
       <c r="AM154" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN154">
         <v>0.06745759346973818</v>
@@ -44125,7 +44128,7 @@
         <v>0.01257263323646787</v>
       </c>
       <c r="AM155" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN155">
         <v>0.1015263162251083</v>
@@ -44303,6 +44306,275 @@
       </c>
       <c r="CU155">
         <v>-0.7441439765161092</v>
+      </c>
+    </row>
+    <row r="156" spans="10:99">
+      <c r="J156" t="s">
+        <v>253</v>
+      </c>
+      <c r="K156">
+        <v>0.0009795810651451742</v>
+      </c>
+      <c r="L156">
+        <v>0.0009795810651451742</v>
+      </c>
+      <c r="M156">
+        <v>0.002310159794659317</v>
+      </c>
+      <c r="N156">
+        <v>0.002310159794659317</v>
+      </c>
+      <c r="O156">
+        <v>0.0008429629072500111</v>
+      </c>
+      <c r="P156">
+        <v>0.0008429629072500111</v>
+      </c>
+      <c r="Q156">
+        <v>0.001681958021810748</v>
+      </c>
+      <c r="R156">
+        <v>0.001681958021810748</v>
+      </c>
+      <c r="S156">
+        <v>6.120536999398101</v>
+      </c>
+      <c r="T156">
+        <v>14.44245749627084</v>
+      </c>
+      <c r="U156">
+        <v>0.9999557869189082</v>
+      </c>
+      <c r="V156">
+        <v>0.6625918036596424</v>
+      </c>
+      <c r="W156">
+        <v>0.090919596659514</v>
+      </c>
+      <c r="X156">
+        <v>0.09681512620459506</v>
+      </c>
+      <c r="Y156">
+        <v>0.2032620001954608</v>
+      </c>
+      <c r="Z156">
+        <v>0.2041441349500067</v>
+      </c>
+      <c r="AA156">
+        <v>0.9968221111456839</v>
+      </c>
+      <c r="AB156">
+        <v>0.8442133485417239</v>
+      </c>
+      <c r="AC156">
+        <v>0.8272179544205936</v>
+      </c>
+      <c r="AD156">
+        <v>0.997252069327898</v>
+      </c>
+      <c r="AE156">
+        <v>0.7967173233566714</v>
+      </c>
+      <c r="AF156">
+        <v>0.7970607394262412</v>
+      </c>
+      <c r="AG156">
+        <v>0.01100696035524265</v>
+      </c>
+      <c r="AH156">
+        <v>0.01192789588635882</v>
+      </c>
+      <c r="AI156">
+        <v>0.9968221111456839</v>
+      </c>
+      <c r="AJ156">
+        <v>0.997252069327898</v>
+      </c>
+      <c r="AK156">
+        <v>0.01100696035524265</v>
+      </c>
+      <c r="AL156">
+        <v>0.01192789588635882</v>
+      </c>
+      <c r="AM156" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN156">
+        <v>0.08086717939318311</v>
+      </c>
+      <c r="AO156">
+        <v>0.09519154878928729</v>
+      </c>
+      <c r="AP156">
+        <v>-155.3841260214</v>
+      </c>
+      <c r="AQ156">
+        <v>-330.9298560732</v>
+      </c>
+      <c r="AR156">
+        <v>13658.55950797861</v>
+      </c>
+      <c r="AS156">
+        <v>20850.43850492673</v>
+      </c>
+      <c r="AT156">
+        <v>13653.8989949786</v>
+      </c>
+      <c r="AU156">
+        <v>20849.04412992673</v>
+      </c>
+      <c r="AV156">
+        <v>0.3658559507978605</v>
+      </c>
+      <c r="AW156">
+        <v>1.085043850492672</v>
+      </c>
+      <c r="AX156">
+        <v>3.922553045859</v>
+      </c>
+      <c r="AY156">
+        <v>1.662081339712919</v>
+      </c>
+      <c r="AZ156">
+        <v>76.84999999999999</v>
+      </c>
+      <c r="BA156">
+        <v>46.76666666666667</v>
+      </c>
+      <c r="BB156">
+        <v>0.1195173769002607</v>
+      </c>
+      <c r="BC156">
+        <v>0.04197758944855858</v>
+      </c>
+      <c r="BD156">
+        <v>-517.7075922025235</v>
+      </c>
+      <c r="BE156">
+        <v>-489.9331011066757</v>
+      </c>
+      <c r="BF156">
+        <v>1283</v>
+      </c>
+      <c r="BG156">
+        <v>1317</v>
+      </c>
+      <c r="BH156">
+        <v>318.4361111111111</v>
+      </c>
+      <c r="BI156">
+        <v>666</v>
+      </c>
+      <c r="BJ156">
+        <v>3282</v>
+      </c>
+      <c r="BK156">
+        <v>1949</v>
+      </c>
+      <c r="BL156">
+        <v>4599</v>
+      </c>
+      <c r="BM156">
+        <v>0</v>
+      </c>
+      <c r="BN156">
+        <v>0</v>
+      </c>
+      <c r="BO156">
+        <v>14</v>
+      </c>
+      <c r="BP156">
+        <v>724</v>
+      </c>
+      <c r="BQ156">
+        <v>0</v>
+      </c>
+      <c r="BR156">
+        <v>0</v>
+      </c>
+      <c r="BS156">
+        <v>1269</v>
+      </c>
+      <c r="BT156">
+        <v>593</v>
+      </c>
+      <c r="BU156">
+        <v>666</v>
+      </c>
+      <c r="BV156">
+        <v>3282</v>
+      </c>
+      <c r="BW156">
+        <v>3658.559507978599</v>
+      </c>
+      <c r="BX156">
+        <v>10850.4385049268</v>
+      </c>
+      <c r="BY156">
+        <v>0.1285508344024863</v>
+      </c>
+      <c r="BZ156">
+        <v>0.08753963982458492</v>
+      </c>
+      <c r="CA156">
+        <v>0.2551398218912022</v>
+      </c>
+      <c r="CB156">
+        <v>0.1687021879834596</v>
+      </c>
+      <c r="CC156">
+        <v>0.03021605123497878</v>
+      </c>
+      <c r="CD156">
+        <v>0.01318201578128399</v>
+      </c>
+      <c r="CE156">
+        <v>0.02639882012024189</v>
+      </c>
+      <c r="CF156">
+        <v>0.01341778189217475</v>
+      </c>
+      <c r="CG156">
+        <v>3813.943633999999</v>
+      </c>
+      <c r="CH156">
+        <v>11181.368361</v>
+      </c>
+      <c r="CI156">
+        <v>4331.651226202523</v>
+      </c>
+      <c r="CJ156">
+        <v>11671.30146210668</v>
+      </c>
+      <c r="CK156">
+        <v>0.09369694943724141</v>
+      </c>
+      <c r="CL156">
+        <v>0.18136203061593</v>
+      </c>
+      <c r="CM156">
+        <v>10000</v>
+      </c>
+      <c r="CO156">
+        <v>0.02158555729984301</v>
+      </c>
+      <c r="CP156">
+        <v>0.04160125588697017</v>
+      </c>
+      <c r="CQ156">
+        <v>1589740.657260704</v>
+      </c>
+      <c r="CR156">
+        <v>11729469.70403232</v>
+      </c>
+      <c r="CS156" s="2">
+        <v>45567.02705131168</v>
+      </c>
+      <c r="CT156">
+        <v>-0.7383044949042414</v>
+      </c>
+      <c r="CU156">
+        <v>-0.5439358604604325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update CFXUSDT.json at 2024-10-02_04-14-22 bestfile_scores 0.0008921042653760869 bestfile_sharp 0.09205743165258203
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="399">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -776,6 +776,9 @@
   </si>
   <si>
     <t>BEAMXUSDT</t>
+  </si>
+  <si>
+    <t>POLYXUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1569,7 +1572,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU156"/>
+  <dimension ref="A1:CU157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1987,7 +1990,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2152,7 +2155,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2268,7 +2271,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2433,7 +2436,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2549,7 +2552,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2714,7 +2717,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2830,7 +2833,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -2995,7 +2998,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3111,7 +3114,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3276,7 +3279,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3392,7 +3395,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3557,7 +3560,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3673,7 +3676,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3838,7 +3841,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3954,7 +3957,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4119,7 +4122,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4235,7 +4238,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4400,7 +4403,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4516,7 +4519,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4681,7 +4684,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4797,7 +4800,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4962,7 +4965,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5078,7 +5081,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5243,7 +5246,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5359,7 +5362,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5524,7 +5527,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5640,7 +5643,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5805,7 +5808,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5921,7 +5924,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6086,7 +6089,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6202,7 +6205,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6367,7 +6370,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6483,7 +6486,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6648,7 +6651,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6764,7 +6767,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6929,7 +6932,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7045,7 +7048,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7210,7 +7213,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7326,7 +7329,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7491,7 +7494,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7607,7 +7610,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7772,7 +7775,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7888,7 +7891,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8053,7 +8056,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8169,7 +8172,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8334,7 +8337,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8450,7 +8453,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8615,7 +8618,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8731,7 +8734,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8896,7 +8899,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -9012,7 +9015,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9177,7 +9180,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9293,7 +9296,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9458,7 +9461,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9574,7 +9577,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9739,7 +9742,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9855,7 +9858,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10020,7 +10023,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10136,7 +10139,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10301,7 +10304,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10417,7 +10420,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10582,7 +10585,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10698,7 +10701,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10863,7 +10866,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10979,7 +10982,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11144,7 +11147,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11266,7 +11269,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11431,7 +11434,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11553,7 +11556,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11718,7 +11721,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11840,7 +11843,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -12005,7 +12008,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12127,7 +12130,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12292,7 +12295,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12414,7 +12417,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12579,7 +12582,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12701,7 +12704,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12866,7 +12869,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12988,7 +12991,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13153,7 +13156,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13275,7 +13278,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13440,7 +13443,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13562,7 +13565,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13727,7 +13730,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13849,7 +13852,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -14014,7 +14017,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14136,7 +14139,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14301,7 +14304,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14423,7 +14426,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14588,7 +14591,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14710,7 +14713,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14875,7 +14878,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -14997,7 +15000,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15162,7 +15165,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15284,7 +15287,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15449,7 +15452,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15571,7 +15574,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15736,7 +15739,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15858,7 +15861,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16023,7 +16026,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16145,7 +16148,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16310,7 +16313,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16432,7 +16435,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16597,7 +16600,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16719,7 +16722,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16884,7 +16887,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -17003,7 +17006,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17168,7 +17171,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17284,7 +17287,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17449,7 +17452,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17562,7 +17565,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17727,7 +17730,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17840,7 +17843,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -18005,7 +18008,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18118,7 +18121,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18283,7 +18286,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18396,7 +18399,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18561,7 +18564,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18674,7 +18677,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18839,7 +18842,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18952,7 +18955,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19117,7 +19120,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19230,7 +19233,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19395,7 +19398,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19508,7 +19511,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19673,7 +19676,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19786,7 +19789,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19951,7 +19954,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20064,7 +20067,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20235,7 +20238,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20348,7 +20351,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20519,7 +20522,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20632,7 +20635,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20803,7 +20806,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20916,7 +20919,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21087,7 +21090,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21197,7 +21200,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21368,7 +21371,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21475,7 +21478,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21646,7 +21649,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21750,7 +21753,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21921,7 +21924,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22025,7 +22028,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22196,7 +22199,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22300,7 +22303,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22471,7 +22474,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22575,7 +22578,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22746,7 +22749,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22850,7 +22853,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23021,7 +23024,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23125,7 +23128,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23296,7 +23299,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23397,7 +23400,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23568,7 +23571,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23669,7 +23672,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23840,7 +23843,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23941,7 +23944,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24112,7 +24115,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24213,7 +24216,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24384,7 +24387,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24485,7 +24488,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24656,7 +24659,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24757,7 +24760,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24928,7 +24931,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25029,7 +25032,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25200,7 +25203,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25298,7 +25301,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25469,7 +25472,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25567,7 +25570,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25738,7 +25741,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25836,7 +25839,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -26007,7 +26010,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26105,7 +26108,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26276,7 +26279,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26374,7 +26377,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26545,7 +26548,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26643,7 +26646,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26814,7 +26817,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26912,7 +26915,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27083,7 +27086,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27181,7 +27184,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27352,7 +27355,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27450,7 +27453,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27621,7 +27624,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27719,7 +27722,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27890,7 +27893,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27988,7 +27991,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28159,7 +28162,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28257,7 +28260,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28428,7 +28431,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28526,7 +28529,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28697,7 +28700,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28795,7 +28798,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28966,7 +28969,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29064,7 +29067,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29235,7 +29238,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29333,7 +29336,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29504,7 +29507,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29602,7 +29605,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29773,7 +29776,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29871,7 +29874,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30042,7 +30045,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30140,7 +30143,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30311,7 +30314,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30409,7 +30412,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30580,7 +30583,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30678,7 +30681,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30849,7 +30852,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30947,7 +30950,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31118,7 +31121,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31216,7 +31219,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31387,7 +31390,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31485,7 +31488,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31656,7 +31659,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31754,7 +31757,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31925,7 +31928,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32023,7 +32026,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32194,7 +32197,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32292,7 +32295,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32463,7 +32466,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32561,7 +32564,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32732,7 +32735,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32830,7 +32833,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -33001,7 +33004,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33099,7 +33102,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33270,7 +33273,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33368,7 +33371,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33539,7 +33542,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33637,7 +33640,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33808,7 +33811,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33906,7 +33909,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34077,7 +34080,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34175,7 +34178,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34346,7 +34349,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34444,7 +34447,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34615,7 +34618,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34713,7 +34716,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34884,7 +34887,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34982,7 +34985,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35153,7 +35156,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35251,7 +35254,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35422,7 +35425,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35520,7 +35523,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35691,7 +35694,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35789,7 +35792,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35960,7 +35963,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36058,7 +36061,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36229,7 +36232,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36327,7 +36330,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36498,7 +36501,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36596,7 +36599,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36767,7 +36770,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36865,7 +36868,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37036,7 +37039,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37134,7 +37137,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37305,7 +37308,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37403,7 +37406,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37574,7 +37577,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37672,7 +37675,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37843,7 +37846,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37941,7 +37944,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38112,7 +38115,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38210,7 +38213,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38381,7 +38384,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38479,7 +38482,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38650,7 +38653,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38748,7 +38751,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38919,7 +38922,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -39017,7 +39020,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39188,7 +39191,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39286,7 +39289,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39457,7 +39460,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39555,7 +39558,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39726,7 +39729,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39824,7 +39827,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -39995,7 +39998,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40093,7 +40096,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40264,7 +40267,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40362,7 +40365,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40533,7 +40536,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40631,7 +40634,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40802,7 +40805,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40900,7 +40903,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41071,7 +41074,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41169,7 +41172,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41340,7 +41343,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41438,7 +41441,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41609,7 +41612,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41707,7 +41710,7 @@
         <v>0.01422843894993598</v>
       </c>
       <c r="AM146" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN146">
         <v>0.3570285831928028</v>
@@ -41976,7 +41979,7 @@
         <v>0.01287672421329242</v>
       </c>
       <c r="AM147" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN147">
         <v>0.1138938544209247</v>
@@ -42245,7 +42248,7 @@
         <v>0.01129449859594168</v>
       </c>
       <c r="AM148" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN148">
         <v>0.01929055864963264</v>
@@ -42514,7 +42517,7 @@
         <v>0.01268293743279473</v>
       </c>
       <c r="AM149" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN149">
         <v>0.02713293780673231</v>
@@ -42783,7 +42786,7 @@
         <v>0.006815186142663594</v>
       </c>
       <c r="AM150" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN150">
         <v>0.06060596226028341</v>
@@ -43052,7 +43055,7 @@
         <v>0.01172718359151741</v>
       </c>
       <c r="AM151" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN151">
         <v>0.09142880750409497</v>
@@ -43321,7 +43324,7 @@
         <v>0.01464508407647874</v>
       </c>
       <c r="AM152" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN152">
         <v>0.3981395839245215</v>
@@ -43590,7 +43593,7 @@
         <v>0.01424145384485694</v>
       </c>
       <c r="AM153" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN153">
         <v>0.1335188651800471</v>
@@ -43859,7 +43862,7 @@
         <v>0.008636072468123625</v>
       </c>
       <c r="AM154" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN154">
         <v>0.06745759346973818</v>
@@ -44128,7 +44131,7 @@
         <v>0.01257263323646787</v>
       </c>
       <c r="AM155" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN155">
         <v>0.1015263162251083</v>
@@ -44397,7 +44400,7 @@
         <v>0.01192789588635882</v>
       </c>
       <c r="AM156" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN156">
         <v>0.08086717939318311</v>
@@ -44575,6 +44578,275 @@
       </c>
       <c r="CU156">
         <v>-0.5439358604604325</v>
+      </c>
+    </row>
+    <row r="157" spans="10:99">
+      <c r="J157" t="s">
+        <v>254</v>
+      </c>
+      <c r="K157">
+        <v>0.001210565022821131</v>
+      </c>
+      <c r="L157">
+        <v>0.001210565022821131</v>
+      </c>
+      <c r="M157">
+        <v>0.001455271942118141</v>
+      </c>
+      <c r="N157">
+        <v>0.001455271942118141</v>
+      </c>
+      <c r="O157">
+        <v>0.0009134206994793504</v>
+      </c>
+      <c r="P157">
+        <v>0.0009134206994793504</v>
+      </c>
+      <c r="Q157">
+        <v>0.001500810909149064</v>
+      </c>
+      <c r="R157">
+        <v>0.001500810909149064</v>
+      </c>
+      <c r="S157">
+        <v>140.6018751726491</v>
+      </c>
+      <c r="T157">
+        <v>15.19182333728734</v>
+      </c>
+      <c r="U157">
+        <v>0.9999822790693662</v>
+      </c>
+      <c r="V157">
+        <v>0.714375572464524</v>
+      </c>
+      <c r="W157">
+        <v>0.09973908793800433</v>
+      </c>
+      <c r="X157">
+        <v>0.09905716628560957</v>
+      </c>
+      <c r="Y157">
+        <v>0.2209664894559913</v>
+      </c>
+      <c r="Z157">
+        <v>0.2050252525299883</v>
+      </c>
+      <c r="AA157">
+        <v>0.9979937638358292</v>
+      </c>
+      <c r="AB157">
+        <v>0.8110340943990056</v>
+      </c>
+      <c r="AC157">
+        <v>0.832267197285708</v>
+      </c>
+      <c r="AD157">
+        <v>0.9967349608988088</v>
+      </c>
+      <c r="AE157">
+        <v>0.77918931772499</v>
+      </c>
+      <c r="AF157">
+        <v>0.8014756747611035</v>
+      </c>
+      <c r="AG157">
+        <v>0.01172985884434391</v>
+      </c>
+      <c r="AH157">
+        <v>0.01186799249853062</v>
+      </c>
+      <c r="AI157">
+        <v>0.9979937638358292</v>
+      </c>
+      <c r="AJ157">
+        <v>0.9967349608988088</v>
+      </c>
+      <c r="AK157">
+        <v>0.01172985884434391</v>
+      </c>
+      <c r="AL157">
+        <v>0.01186799249853062</v>
+      </c>
+      <c r="AM157" t="s">
+        <v>255</v>
+      </c>
+      <c r="AN157">
+        <v>0.07213994227012922</v>
+      </c>
+      <c r="AO157">
+        <v>0.1093422173064931</v>
+      </c>
+      <c r="AP157">
+        <v>-1899.03637015</v>
+      </c>
+      <c r="AQ157">
+        <v>-332.804998822</v>
+      </c>
+      <c r="AR157">
+        <v>15123.05246985014</v>
+      </c>
+      <c r="AS157">
+        <v>16440.91099117805</v>
+      </c>
+      <c r="AT157">
+        <v>15107.59955985014</v>
+      </c>
+      <c r="AU157">
+        <v>16441.66693117805</v>
+      </c>
+      <c r="AV157">
+        <v>0.5123052469850138</v>
+      </c>
+      <c r="AW157">
+        <v>0.6440910991178046</v>
+      </c>
+      <c r="AX157">
+        <v>0.1706937799043062</v>
+      </c>
+      <c r="AY157">
+        <v>1.580024391809487</v>
+      </c>
+      <c r="AZ157">
+        <v>32.76666666666667</v>
+      </c>
+      <c r="BA157">
+        <v>31.03333333333333</v>
+      </c>
+      <c r="BB157">
+        <v>0.03247654340231827</v>
+      </c>
+      <c r="BC157">
+        <v>0.2438406946299834</v>
+      </c>
+      <c r="BD157">
+        <v>-235.7081592514037</v>
+      </c>
+      <c r="BE157">
+        <v>-2184.338142105632</v>
+      </c>
+      <c r="BF157">
+        <v>18692</v>
+      </c>
+      <c r="BG157">
+        <v>3575</v>
+      </c>
+      <c r="BH157">
+        <v>341.8944444444444</v>
+      </c>
+      <c r="BI157">
+        <v>29379</v>
+      </c>
+      <c r="BJ157">
+        <v>1619</v>
+      </c>
+      <c r="BK157">
+        <v>48071</v>
+      </c>
+      <c r="BL157">
+        <v>5194</v>
+      </c>
+      <c r="BM157">
+        <v>0</v>
+      </c>
+      <c r="BN157">
+        <v>0</v>
+      </c>
+      <c r="BO157">
+        <v>18273</v>
+      </c>
+      <c r="BP157">
+        <v>124</v>
+      </c>
+      <c r="BQ157">
+        <v>0</v>
+      </c>
+      <c r="BR157">
+        <v>0</v>
+      </c>
+      <c r="BS157">
+        <v>419</v>
+      </c>
+      <c r="BT157">
+        <v>3451</v>
+      </c>
+      <c r="BU157">
+        <v>29379</v>
+      </c>
+      <c r="BV157">
+        <v>1619</v>
+      </c>
+      <c r="BW157">
+        <v>5123.052469850006</v>
+      </c>
+      <c r="BX157">
+        <v>6440.910991178005</v>
+      </c>
+      <c r="BY157">
+        <v>0.1110132153026563</v>
+      </c>
+      <c r="BZ157">
+        <v>0.2094650326787421</v>
+      </c>
+      <c r="CA157">
+        <v>0.283384032956019</v>
+      </c>
+      <c r="CB157">
+        <v>0.3384513235049592</v>
+      </c>
+      <c r="CC157">
+        <v>0.006601019097538856</v>
+      </c>
+      <c r="CD157">
+        <v>0.01952261014767784</v>
+      </c>
+      <c r="CE157">
+        <v>0.01389184090812786</v>
+      </c>
+      <c r="CF157">
+        <v>0.02820450551920261</v>
+      </c>
+      <c r="CG157">
+        <v>7022.088840000006</v>
+      </c>
+      <c r="CH157">
+        <v>6773.715990000005</v>
+      </c>
+      <c r="CI157">
+        <v>7257.79699925141</v>
+      </c>
+      <c r="CJ157">
+        <v>8958.054132105637</v>
+      </c>
+      <c r="CK157">
+        <v>0.1251524929448511</v>
+      </c>
+      <c r="CL157">
+        <v>0.09484019382731924</v>
+      </c>
+      <c r="CM157">
+        <v>10000</v>
+      </c>
+      <c r="CO157">
+        <v>0.04203728524430364</v>
+      </c>
+      <c r="CP157">
+        <v>0.01462166443280127</v>
+      </c>
+      <c r="CQ157">
+        <v>16965841.93971542</v>
+      </c>
+      <c r="CR157">
+        <v>7546607.730239696</v>
+      </c>
+      <c r="CS157" s="2">
+        <v>45567.08692644227</v>
+      </c>
+      <c r="CT157">
+        <v>-0.7384737891802428</v>
+      </c>
+      <c r="CU157">
+        <v>-0.5699801868436853</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update ZROUSDT.json at 2024-10-02_05-03-47 bestfile_scores 0.0020720678794981353 bestfile_sharp 0.14643270779848253
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="400">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -779,6 +779,9 @@
   </si>
   <si>
     <t>POLYXUSDT</t>
+  </si>
+  <si>
+    <t>CFXUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1572,7 +1575,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU157"/>
+  <dimension ref="A1:CU158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1990,7 +1993,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2155,7 +2158,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2271,7 +2274,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2436,7 +2439,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2552,7 +2555,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2717,7 +2720,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2833,7 +2836,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -2998,7 +3001,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3114,7 +3117,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3279,7 +3282,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3395,7 +3398,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3560,7 +3563,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3676,7 +3679,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3841,7 +3844,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3957,7 +3960,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4122,7 +4125,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4238,7 +4241,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4403,7 +4406,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4519,7 +4522,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4684,7 +4687,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4800,7 +4803,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4965,7 +4968,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5081,7 +5084,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5246,7 +5249,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5362,7 +5365,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5527,7 +5530,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5643,7 +5646,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5808,7 +5811,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5924,7 +5927,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6089,7 +6092,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6205,7 +6208,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6370,7 +6373,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6486,7 +6489,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6651,7 +6654,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6767,7 +6770,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6932,7 +6935,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7048,7 +7051,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7213,7 +7216,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7329,7 +7332,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7494,7 +7497,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7610,7 +7613,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7775,7 +7778,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7891,7 +7894,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8056,7 +8059,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8172,7 +8175,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8337,7 +8340,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8453,7 +8456,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8618,7 +8621,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8734,7 +8737,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8899,7 +8902,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -9015,7 +9018,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9180,7 +9183,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9296,7 +9299,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9461,7 +9464,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9577,7 +9580,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9742,7 +9745,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9858,7 +9861,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10023,7 +10026,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10139,7 +10142,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10304,7 +10307,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10420,7 +10423,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10585,7 +10588,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10701,7 +10704,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10866,7 +10869,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10982,7 +10985,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11147,7 +11150,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11269,7 +11272,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11434,7 +11437,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11556,7 +11559,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11721,7 +11724,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11843,7 +11846,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -12008,7 +12011,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12130,7 +12133,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12295,7 +12298,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12417,7 +12420,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12582,7 +12585,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12704,7 +12707,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12869,7 +12872,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12991,7 +12994,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13156,7 +13159,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13278,7 +13281,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13443,7 +13446,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13565,7 +13568,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13730,7 +13733,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13852,7 +13855,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -14017,7 +14020,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14139,7 +14142,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14304,7 +14307,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14426,7 +14429,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14591,7 +14594,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14713,7 +14716,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14878,7 +14881,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -15000,7 +15003,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15165,7 +15168,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15287,7 +15290,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15452,7 +15455,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15574,7 +15577,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15739,7 +15742,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15861,7 +15864,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16026,7 +16029,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16148,7 +16151,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16313,7 +16316,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16435,7 +16438,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16600,7 +16603,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16722,7 +16725,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16887,7 +16890,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -17006,7 +17009,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17171,7 +17174,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17287,7 +17290,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17452,7 +17455,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17565,7 +17568,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17730,7 +17733,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17843,7 +17846,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -18008,7 +18011,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18121,7 +18124,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18286,7 +18289,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18399,7 +18402,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18564,7 +18567,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18677,7 +18680,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18842,7 +18845,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18955,7 +18958,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19120,7 +19123,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19233,7 +19236,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19398,7 +19401,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19511,7 +19514,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19676,7 +19679,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19789,7 +19792,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19954,7 +19957,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20067,7 +20070,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20238,7 +20241,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20351,7 +20354,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20522,7 +20525,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20635,7 +20638,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20806,7 +20809,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20919,7 +20922,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21090,7 +21093,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21200,7 +21203,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21371,7 +21374,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21478,7 +21481,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21649,7 +21652,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21753,7 +21756,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21924,7 +21927,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22028,7 +22031,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22199,7 +22202,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22303,7 +22306,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22474,7 +22477,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22578,7 +22581,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22749,7 +22752,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22853,7 +22856,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23024,7 +23027,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23128,7 +23131,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23299,7 +23302,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23400,7 +23403,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23571,7 +23574,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23672,7 +23675,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23843,7 +23846,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23944,7 +23947,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24115,7 +24118,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24216,7 +24219,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24387,7 +24390,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24488,7 +24491,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24659,7 +24662,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24760,7 +24763,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24931,7 +24934,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25032,7 +25035,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25203,7 +25206,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25301,7 +25304,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25472,7 +25475,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25570,7 +25573,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25741,7 +25744,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25839,7 +25842,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -26010,7 +26013,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26108,7 +26111,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26279,7 +26282,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26377,7 +26380,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26548,7 +26551,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26646,7 +26649,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26817,7 +26820,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26915,7 +26918,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27086,7 +27089,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27184,7 +27187,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27355,7 +27358,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27453,7 +27456,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27624,7 +27627,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27722,7 +27725,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27893,7 +27896,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27991,7 +27994,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28162,7 +28165,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28260,7 +28263,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28431,7 +28434,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28529,7 +28532,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28700,7 +28703,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28798,7 +28801,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28969,7 +28972,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29067,7 +29070,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29238,7 +29241,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29336,7 +29339,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29507,7 +29510,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29605,7 +29608,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29776,7 +29779,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29874,7 +29877,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30045,7 +30048,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30143,7 +30146,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30314,7 +30317,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30412,7 +30415,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30583,7 +30586,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30681,7 +30684,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30852,7 +30855,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30950,7 +30953,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31121,7 +31124,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31219,7 +31222,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31390,7 +31393,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31488,7 +31491,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31659,7 +31662,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31757,7 +31760,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31928,7 +31931,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32026,7 +32029,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32197,7 +32200,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32295,7 +32298,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32466,7 +32469,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32564,7 +32567,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32735,7 +32738,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32833,7 +32836,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -33004,7 +33007,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33102,7 +33105,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33273,7 +33276,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33371,7 +33374,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33542,7 +33545,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33640,7 +33643,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33811,7 +33814,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33909,7 +33912,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34080,7 +34083,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34178,7 +34181,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34349,7 +34352,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34447,7 +34450,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34618,7 +34621,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34716,7 +34719,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34887,7 +34890,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34985,7 +34988,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35156,7 +35159,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35254,7 +35257,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35425,7 +35428,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35523,7 +35526,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35694,7 +35697,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35792,7 +35795,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35963,7 +35966,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36061,7 +36064,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36232,7 +36235,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36330,7 +36333,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36501,7 +36504,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36599,7 +36602,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36770,7 +36773,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36868,7 +36871,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37039,7 +37042,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37137,7 +37140,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37308,7 +37311,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37406,7 +37409,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37577,7 +37580,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37675,7 +37678,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37846,7 +37849,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37944,7 +37947,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38115,7 +38118,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38213,7 +38216,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38384,7 +38387,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38482,7 +38485,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38653,7 +38656,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38751,7 +38754,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38922,7 +38925,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -39020,7 +39023,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39191,7 +39194,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39289,7 +39292,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39460,7 +39463,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39558,7 +39561,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39729,7 +39732,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39827,7 +39830,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -39998,7 +40001,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40096,7 +40099,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40267,7 +40270,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40365,7 +40368,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40536,7 +40539,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40634,7 +40637,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40805,7 +40808,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40903,7 +40906,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41074,7 +41077,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41172,7 +41175,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41343,7 +41346,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41441,7 +41444,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41612,7 +41615,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41710,7 +41713,7 @@
         <v>0.01422843894993598</v>
       </c>
       <c r="AM146" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN146">
         <v>0.3570285831928028</v>
@@ -41979,7 +41982,7 @@
         <v>0.01287672421329242</v>
       </c>
       <c r="AM147" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN147">
         <v>0.1138938544209247</v>
@@ -42248,7 +42251,7 @@
         <v>0.01129449859594168</v>
       </c>
       <c r="AM148" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN148">
         <v>0.01929055864963264</v>
@@ -42517,7 +42520,7 @@
         <v>0.01268293743279473</v>
       </c>
       <c r="AM149" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN149">
         <v>0.02713293780673231</v>
@@ -42786,7 +42789,7 @@
         <v>0.006815186142663594</v>
       </c>
       <c r="AM150" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN150">
         <v>0.06060596226028341</v>
@@ -43055,7 +43058,7 @@
         <v>0.01172718359151741</v>
       </c>
       <c r="AM151" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN151">
         <v>0.09142880750409497</v>
@@ -43324,7 +43327,7 @@
         <v>0.01464508407647874</v>
       </c>
       <c r="AM152" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN152">
         <v>0.3981395839245215</v>
@@ -43593,7 +43596,7 @@
         <v>0.01424145384485694</v>
       </c>
       <c r="AM153" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN153">
         <v>0.1335188651800471</v>
@@ -43862,7 +43865,7 @@
         <v>0.008636072468123625</v>
       </c>
       <c r="AM154" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN154">
         <v>0.06745759346973818</v>
@@ -44131,7 +44134,7 @@
         <v>0.01257263323646787</v>
       </c>
       <c r="AM155" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN155">
         <v>0.1015263162251083</v>
@@ -44400,7 +44403,7 @@
         <v>0.01192789588635882</v>
       </c>
       <c r="AM156" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN156">
         <v>0.08086717939318311</v>
@@ -44669,7 +44672,7 @@
         <v>0.01186799249853062</v>
       </c>
       <c r="AM157" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN157">
         <v>0.07213994227012922</v>
@@ -44847,6 +44850,275 @@
       </c>
       <c r="CU157">
         <v>-0.5699801868436853</v>
+      </c>
+    </row>
+    <row r="158" spans="10:99">
+      <c r="J158" t="s">
+        <v>255</v>
+      </c>
+      <c r="K158">
+        <v>0.0009835749309967667</v>
+      </c>
+      <c r="L158">
+        <v>0.0009835749309967667</v>
+      </c>
+      <c r="M158">
+        <v>0.0008667274962923521</v>
+      </c>
+      <c r="N158">
+        <v>0.0008667274962923521</v>
+      </c>
+      <c r="O158">
+        <v>0.0009687918231672699</v>
+      </c>
+      <c r="P158">
+        <v>0.0009687918231672699</v>
+      </c>
+      <c r="Q158">
+        <v>0.0007493228110479588</v>
+      </c>
+      <c r="R158">
+        <v>0.0007493228110479588</v>
+      </c>
+      <c r="S158">
+        <v>6.808357960929459</v>
+      </c>
+      <c r="T158">
+        <v>6.18462671488325</v>
+      </c>
+      <c r="U158">
+        <v>0.9999783692880325</v>
+      </c>
+      <c r="V158">
+        <v>0.7606993163737109</v>
+      </c>
+      <c r="W158">
+        <v>0.09785022012563692</v>
+      </c>
+      <c r="X158">
+        <v>0.09915926083758629</v>
+      </c>
+      <c r="Y158">
+        <v>0.1470618385785596</v>
+      </c>
+      <c r="Z158">
+        <v>0.1540355777038485</v>
+      </c>
+      <c r="AA158">
+        <v>0.9955224454258492</v>
+      </c>
+      <c r="AB158">
+        <v>0.8748319943824363</v>
+      </c>
+      <c r="AC158">
+        <v>0.8652356756052295</v>
+      </c>
+      <c r="AD158">
+        <v>0.9942781749121928</v>
+      </c>
+      <c r="AE158">
+        <v>0.8379751074153157</v>
+      </c>
+      <c r="AF158">
+        <v>0.8550196228023297</v>
+      </c>
+      <c r="AG158">
+        <v>0.01315633511505271</v>
+      </c>
+      <c r="AH158">
+        <v>0.01449742321347242</v>
+      </c>
+      <c r="AI158">
+        <v>0.9955224454258492</v>
+      </c>
+      <c r="AJ158">
+        <v>0.9942781749121928</v>
+      </c>
+      <c r="AK158">
+        <v>0.01315633511505271</v>
+      </c>
+      <c r="AL158">
+        <v>0.01449742321347242</v>
+      </c>
+      <c r="AM158" t="s">
+        <v>256</v>
+      </c>
+      <c r="AN158">
+        <v>0.1112845525409627</v>
+      </c>
+      <c r="AO158">
+        <v>0.1143849072260816</v>
+      </c>
+      <c r="AP158">
+        <v>-222.651178824</v>
+      </c>
+      <c r="AQ158">
+        <v>-133.557420746</v>
+      </c>
+      <c r="AR158">
+        <v>17832.643681176</v>
+      </c>
+      <c r="AS158">
+        <v>16648.86187867387</v>
+      </c>
+      <c r="AT158">
+        <v>17811.003781176</v>
+      </c>
+      <c r="AU158">
+        <v>16368.91042925397</v>
+      </c>
+      <c r="AV158">
+        <v>0.7832643681175999</v>
+      </c>
+      <c r="AW158">
+        <v>0.6648861878673866</v>
+      </c>
+      <c r="AX158">
+        <v>3.523524760715772</v>
+      </c>
+      <c r="AY158">
+        <v>3.881358805204325</v>
+      </c>
+      <c r="AZ158">
+        <v>76.81666666666666</v>
+      </c>
+      <c r="BA158">
+        <v>38.88333333333333</v>
+      </c>
+      <c r="BB158">
+        <v>0.07922114923943935</v>
+      </c>
+      <c r="BC158">
+        <v>0.1418485610802387</v>
+      </c>
+      <c r="BD158">
+        <v>-693.0542722007988</v>
+      </c>
+      <c r="BE158">
+        <v>-1121.103309547102</v>
+      </c>
+      <c r="BF158">
+        <v>2942</v>
+      </c>
+      <c r="BG158">
+        <v>1991</v>
+      </c>
+      <c r="BH158">
+        <v>588.3944444444445</v>
+      </c>
+      <c r="BI158">
+        <v>1064</v>
+      </c>
+      <c r="BJ158">
+        <v>1648</v>
+      </c>
+      <c r="BK158">
+        <v>4006</v>
+      </c>
+      <c r="BL158">
+        <v>3639</v>
+      </c>
+      <c r="BM158">
+        <v>0</v>
+      </c>
+      <c r="BN158">
+        <v>0</v>
+      </c>
+      <c r="BO158">
+        <v>253</v>
+      </c>
+      <c r="BP158">
+        <v>147</v>
+      </c>
+      <c r="BQ158">
+        <v>0</v>
+      </c>
+      <c r="BR158">
+        <v>0</v>
+      </c>
+      <c r="BS158">
+        <v>2689</v>
+      </c>
+      <c r="BT158">
+        <v>1844</v>
+      </c>
+      <c r="BU158">
+        <v>1064</v>
+      </c>
+      <c r="BV158">
+        <v>1648</v>
+      </c>
+      <c r="BW158">
+        <v>7832.643681175995</v>
+      </c>
+      <c r="BX158">
+        <v>6648.861878673893</v>
+      </c>
+      <c r="BY158">
+        <v>0.1185541481794694</v>
+      </c>
+      <c r="BZ158">
+        <v>0.2442504937979565</v>
+      </c>
+      <c r="CA158">
+        <v>0.1717703138756532</v>
+      </c>
+      <c r="CB158">
+        <v>0.3483949843722079</v>
+      </c>
+      <c r="CC158">
+        <v>0.02577833847887394</v>
+      </c>
+      <c r="CD158">
+        <v>0.03428641473363415</v>
+      </c>
+      <c r="CE158">
+        <v>0.02514262724609685</v>
+      </c>
+      <c r="CF158">
+        <v>0.04079896074537769</v>
+      </c>
+      <c r="CG158">
+        <v>8055.294859999995</v>
+      </c>
+      <c r="CH158">
+        <v>6782.419299419894</v>
+      </c>
+      <c r="CI158">
+        <v>8748.349132200794</v>
+      </c>
+      <c r="CJ158">
+        <v>7903.522608966996</v>
+      </c>
+      <c r="CK158">
+        <v>0.09205743165258203</v>
+      </c>
+      <c r="CL158">
+        <v>0.07440435688515409</v>
+      </c>
+      <c r="CM158">
+        <v>10000</v>
+      </c>
+      <c r="CO158">
+        <v>0.03051759541173972</v>
+      </c>
+      <c r="CP158">
+        <v>0.01855129929901579</v>
+      </c>
+      <c r="CQ158">
+        <v>5871599.863546415</v>
+      </c>
+      <c r="CR158">
+        <v>5398351.975391543</v>
+      </c>
+      <c r="CS158" s="2">
+        <v>45567.17667942392</v>
+      </c>
+      <c r="CT158">
+        <v>-0.7008697410150677</v>
+      </c>
+      <c r="CU158">
+        <v>-0.6649766371082574</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update RDNTUSDT.json at 2024-10-02_06-45-24 bestfile_scores 0.0015001738414448852 bestfile_sharp 0.04413544954082176
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="401">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -782,6 +782,9 @@
   </si>
   <si>
     <t>CFXUSDT</t>
+  </si>
+  <si>
+    <t>ZROUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1575,7 +1578,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU158"/>
+  <dimension ref="A1:CU159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1993,7 +1996,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2158,7 +2161,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2274,7 +2277,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2439,7 +2442,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2555,7 +2558,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2720,7 +2723,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2836,7 +2839,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -3001,7 +3004,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3117,7 +3120,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3282,7 +3285,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3398,7 +3401,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3563,7 +3566,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3679,7 +3682,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3844,7 +3847,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3960,7 +3963,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4125,7 +4128,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4241,7 +4244,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4406,7 +4409,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4522,7 +4525,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4687,7 +4690,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4803,7 +4806,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4968,7 +4971,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5084,7 +5087,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5249,7 +5252,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5365,7 +5368,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5530,7 +5533,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5646,7 +5649,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5811,7 +5814,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5927,7 +5930,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6092,7 +6095,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6208,7 +6211,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6373,7 +6376,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6489,7 +6492,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6654,7 +6657,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6770,7 +6773,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6935,7 +6938,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7051,7 +7054,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7216,7 +7219,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7332,7 +7335,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7497,7 +7500,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7613,7 +7616,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7778,7 +7781,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7894,7 +7897,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8059,7 +8062,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8175,7 +8178,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8340,7 +8343,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8456,7 +8459,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8621,7 +8624,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8737,7 +8740,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8902,7 +8905,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -9018,7 +9021,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9183,7 +9186,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9299,7 +9302,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9464,7 +9467,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9580,7 +9583,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9745,7 +9748,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9861,7 +9864,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10026,7 +10029,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10142,7 +10145,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10307,7 +10310,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10423,7 +10426,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10588,7 +10591,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10704,7 +10707,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10869,7 +10872,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10985,7 +10988,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11150,7 +11153,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11272,7 +11275,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11437,7 +11440,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11559,7 +11562,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11724,7 +11727,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11846,7 +11849,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -12011,7 +12014,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12133,7 +12136,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12298,7 +12301,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12420,7 +12423,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12585,7 +12588,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12707,7 +12710,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12872,7 +12875,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12994,7 +12997,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13159,7 +13162,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13281,7 +13284,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13446,7 +13449,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13568,7 +13571,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13733,7 +13736,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13855,7 +13858,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -14020,7 +14023,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14142,7 +14145,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14307,7 +14310,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14429,7 +14432,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14594,7 +14597,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14716,7 +14719,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14881,7 +14884,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -15003,7 +15006,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15168,7 +15171,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15290,7 +15293,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15455,7 +15458,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15577,7 +15580,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15742,7 +15745,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15864,7 +15867,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16029,7 +16032,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16151,7 +16154,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16316,7 +16319,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16438,7 +16441,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16603,7 +16606,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16725,7 +16728,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16890,7 +16893,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -17009,7 +17012,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17174,7 +17177,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17290,7 +17293,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17455,7 +17458,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17568,7 +17571,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17733,7 +17736,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17846,7 +17849,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -18011,7 +18014,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18124,7 +18127,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18289,7 +18292,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18402,7 +18405,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18567,7 +18570,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18680,7 +18683,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18845,7 +18848,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18958,7 +18961,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19123,7 +19126,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19236,7 +19239,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19401,7 +19404,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19514,7 +19517,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19679,7 +19682,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19792,7 +19795,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19957,7 +19960,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20070,7 +20073,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20241,7 +20244,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20354,7 +20357,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20525,7 +20528,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20638,7 +20641,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20809,7 +20812,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20922,7 +20925,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21093,7 +21096,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21203,7 +21206,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21374,7 +21377,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21481,7 +21484,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21652,7 +21655,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21756,7 +21759,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21927,7 +21930,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22031,7 +22034,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22202,7 +22205,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22306,7 +22309,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22477,7 +22480,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22581,7 +22584,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22752,7 +22755,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22856,7 +22859,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23027,7 +23030,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23131,7 +23134,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23302,7 +23305,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23403,7 +23406,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23574,7 +23577,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23675,7 +23678,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23846,7 +23849,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23947,7 +23950,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24118,7 +24121,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24219,7 +24222,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24390,7 +24393,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24491,7 +24494,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24662,7 +24665,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24763,7 +24766,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24934,7 +24937,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25035,7 +25038,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25206,7 +25209,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25304,7 +25307,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25475,7 +25478,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25573,7 +25576,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25744,7 +25747,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25842,7 +25845,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -26013,7 +26016,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26111,7 +26114,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26282,7 +26285,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26380,7 +26383,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26551,7 +26554,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26649,7 +26652,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26820,7 +26823,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26918,7 +26921,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27089,7 +27092,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27187,7 +27190,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27358,7 +27361,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27456,7 +27459,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27627,7 +27630,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27725,7 +27728,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27896,7 +27899,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27994,7 +27997,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28165,7 +28168,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28263,7 +28266,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28434,7 +28437,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28532,7 +28535,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28703,7 +28706,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28801,7 +28804,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28972,7 +28975,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29070,7 +29073,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29241,7 +29244,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29339,7 +29342,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29510,7 +29513,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29608,7 +29611,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29779,7 +29782,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29877,7 +29880,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30048,7 +30051,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30146,7 +30149,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30317,7 +30320,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30415,7 +30418,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30586,7 +30589,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30684,7 +30687,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30855,7 +30858,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30953,7 +30956,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31124,7 +31127,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31222,7 +31225,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31393,7 +31396,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31491,7 +31494,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31662,7 +31665,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31760,7 +31763,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31931,7 +31934,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32029,7 +32032,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32200,7 +32203,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32298,7 +32301,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32469,7 +32472,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32567,7 +32570,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32738,7 +32741,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32836,7 +32839,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -33007,7 +33010,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33105,7 +33108,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33276,7 +33279,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33374,7 +33377,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33545,7 +33548,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33643,7 +33646,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33814,7 +33817,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33912,7 +33915,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34083,7 +34086,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34181,7 +34184,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34352,7 +34355,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34450,7 +34453,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34621,7 +34624,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34719,7 +34722,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34890,7 +34893,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34988,7 +34991,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35159,7 +35162,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35257,7 +35260,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35428,7 +35431,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35526,7 +35529,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35697,7 +35700,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35795,7 +35798,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35966,7 +35969,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36064,7 +36067,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36235,7 +36238,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36333,7 +36336,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36504,7 +36507,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36602,7 +36605,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36773,7 +36776,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36871,7 +36874,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37042,7 +37045,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37140,7 +37143,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37311,7 +37314,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37409,7 +37412,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37580,7 +37583,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37678,7 +37681,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37849,7 +37852,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37947,7 +37950,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38118,7 +38121,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38216,7 +38219,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38387,7 +38390,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38485,7 +38488,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38656,7 +38659,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38754,7 +38757,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38925,7 +38928,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -39023,7 +39026,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39194,7 +39197,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39292,7 +39295,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39463,7 +39466,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39561,7 +39564,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39732,7 +39735,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39830,7 +39833,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -40001,7 +40004,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40099,7 +40102,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40270,7 +40273,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40368,7 +40371,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40539,7 +40542,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40637,7 +40640,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40808,7 +40811,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40906,7 +40909,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41077,7 +41080,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41175,7 +41178,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41346,7 +41349,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41444,7 +41447,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41615,7 +41618,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41713,7 +41716,7 @@
         <v>0.01422843894993598</v>
       </c>
       <c r="AM146" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN146">
         <v>0.3570285831928028</v>
@@ -41982,7 +41985,7 @@
         <v>0.01287672421329242</v>
       </c>
       <c r="AM147" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN147">
         <v>0.1138938544209247</v>
@@ -42251,7 +42254,7 @@
         <v>0.01129449859594168</v>
       </c>
       <c r="AM148" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN148">
         <v>0.01929055864963264</v>
@@ -42520,7 +42523,7 @@
         <v>0.01268293743279473</v>
       </c>
       <c r="AM149" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN149">
         <v>0.02713293780673231</v>
@@ -42789,7 +42792,7 @@
         <v>0.006815186142663594</v>
       </c>
       <c r="AM150" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN150">
         <v>0.06060596226028341</v>
@@ -43058,7 +43061,7 @@
         <v>0.01172718359151741</v>
       </c>
       <c r="AM151" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN151">
         <v>0.09142880750409497</v>
@@ -43327,7 +43330,7 @@
         <v>0.01464508407647874</v>
       </c>
       <c r="AM152" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN152">
         <v>0.3981395839245215</v>
@@ -43596,7 +43599,7 @@
         <v>0.01424145384485694</v>
       </c>
       <c r="AM153" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN153">
         <v>0.1335188651800471</v>
@@ -43865,7 +43868,7 @@
         <v>0.008636072468123625</v>
       </c>
       <c r="AM154" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN154">
         <v>0.06745759346973818</v>
@@ -44134,7 +44137,7 @@
         <v>0.01257263323646787</v>
       </c>
       <c r="AM155" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN155">
         <v>0.1015263162251083</v>
@@ -44403,7 +44406,7 @@
         <v>0.01192789588635882</v>
       </c>
       <c r="AM156" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN156">
         <v>0.08086717939318311</v>
@@ -44672,7 +44675,7 @@
         <v>0.01186799249853062</v>
       </c>
       <c r="AM157" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN157">
         <v>0.07213994227012922</v>
@@ -44941,7 +44944,7 @@
         <v>0.01449742321347242</v>
       </c>
       <c r="AM158" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN158">
         <v>0.1112845525409627</v>
@@ -45119,6 +45122,275 @@
       </c>
       <c r="CU158">
         <v>-0.6649766371082574</v>
+      </c>
+    </row>
+    <row r="159" spans="10:99">
+      <c r="J159" t="s">
+        <v>256</v>
+      </c>
+      <c r="K159">
+        <v>0.002758067374948991</v>
+      </c>
+      <c r="L159">
+        <v>0.002758067374948991</v>
+      </c>
+      <c r="M159">
+        <v>0.001009970955282213</v>
+      </c>
+      <c r="N159">
+        <v>0.001009970955282213</v>
+      </c>
+      <c r="O159">
+        <v>0.003347269879370529</v>
+      </c>
+      <c r="P159">
+        <v>0.003347269879370529</v>
+      </c>
+      <c r="Q159">
+        <v>0.001172963308390806</v>
+      </c>
+      <c r="R159">
+        <v>0.001172963308390806</v>
+      </c>
+      <c r="S159">
+        <v>5.644837502034616</v>
+      </c>
+      <c r="T159">
+        <v>12.78389669578428</v>
+      </c>
+      <c r="U159">
+        <v>1</v>
+      </c>
+      <c r="V159">
+        <v>0.7858431491042077</v>
+      </c>
+      <c r="W159">
+        <v>0.09999679449937755</v>
+      </c>
+      <c r="X159">
+        <v>0.09490082656760303</v>
+      </c>
+      <c r="Y159">
+        <v>0.1151253228040793</v>
+      </c>
+      <c r="Z159">
+        <v>0.1191571267604236</v>
+      </c>
+      <c r="AA159">
+        <v>0.9893205645975773</v>
+      </c>
+      <c r="AB159">
+        <v>0.8938376006991946</v>
+      </c>
+      <c r="AC159">
+        <v>0.8973189804924766</v>
+      </c>
+      <c r="AD159">
+        <v>0.9962213871942949</v>
+      </c>
+      <c r="AE159">
+        <v>0.8851134529587228</v>
+      </c>
+      <c r="AF159">
+        <v>0.8834459320445649</v>
+      </c>
+      <c r="AG159">
+        <v>0.0202328691234658</v>
+      </c>
+      <c r="AH159">
+        <v>0.01458063833474489</v>
+      </c>
+      <c r="AI159">
+        <v>0.9893205645975773</v>
+      </c>
+      <c r="AJ159">
+        <v>0.9962213871942949</v>
+      </c>
+      <c r="AK159">
+        <v>0.0202328691234658</v>
+      </c>
+      <c r="AL159">
+        <v>0.01458063833474489</v>
+      </c>
+      <c r="AM159" t="s">
+        <v>257</v>
+      </c>
+      <c r="AN159">
+        <v>0.182085969558268</v>
+      </c>
+      <c r="AO159">
+        <v>0.08111770949339026</v>
+      </c>
+      <c r="AP159">
+        <v>-43.246691886</v>
+      </c>
+      <c r="AQ159">
+        <v>-44.095630878</v>
+      </c>
+      <c r="AR159">
+        <v>13258.07936811399</v>
+      </c>
+      <c r="AS159">
+        <v>11088.94115912199</v>
+      </c>
+      <c r="AT159">
+        <v>13127.41241811399</v>
+      </c>
+      <c r="AU159">
+        <v>11088.94115912199</v>
+      </c>
+      <c r="AV159">
+        <v>0.3258079368113995</v>
+      </c>
+      <c r="AW159">
+        <v>0.1088941159121988</v>
+      </c>
+      <c r="AX159">
+        <v>4.254361640670133</v>
+      </c>
+      <c r="AY159">
+        <v>1.876274209989806</v>
+      </c>
+      <c r="AZ159">
+        <v>22.5</v>
+      </c>
+      <c r="BA159">
+        <v>45.13333333333333</v>
+      </c>
+      <c r="BB159">
+        <v>0.05986542155710243</v>
+      </c>
+      <c r="BC159">
+        <v>0.1039703716842554</v>
+      </c>
+      <c r="BD159">
+        <v>-210.2201969920973</v>
+      </c>
+      <c r="BE159">
+        <v>-131.471384947021</v>
+      </c>
+      <c r="BF159">
+        <v>219</v>
+      </c>
+      <c r="BG159">
+        <v>404</v>
+      </c>
+      <c r="BH159">
+        <v>102.3944444444444</v>
+      </c>
+      <c r="BI159">
+        <v>359</v>
+      </c>
+      <c r="BJ159">
+        <v>905</v>
+      </c>
+      <c r="BK159">
+        <v>578</v>
+      </c>
+      <c r="BL159">
+        <v>1309</v>
+      </c>
+      <c r="BM159">
+        <v>0</v>
+      </c>
+      <c r="BN159">
+        <v>0</v>
+      </c>
+      <c r="BO159">
+        <v>96</v>
+      </c>
+      <c r="BP159">
+        <v>119</v>
+      </c>
+      <c r="BQ159">
+        <v>0</v>
+      </c>
+      <c r="BR159">
+        <v>0</v>
+      </c>
+      <c r="BS159">
+        <v>123</v>
+      </c>
+      <c r="BT159">
+        <v>285</v>
+      </c>
+      <c r="BU159">
+        <v>359</v>
+      </c>
+      <c r="BV159">
+        <v>905</v>
+      </c>
+      <c r="BW159">
+        <v>3258.079368114004</v>
+      </c>
+      <c r="BX159">
+        <v>1088.941159121998</v>
+      </c>
+      <c r="BY159">
+        <v>0.2514594405147345</v>
+      </c>
+      <c r="BZ159">
+        <v>0.08535337142663287</v>
+      </c>
+      <c r="CA159">
+        <v>0.3363917172926917</v>
+      </c>
+      <c r="CB159">
+        <v>0.1036772172248619</v>
+      </c>
+      <c r="CC159">
+        <v>0.04464549222672994</v>
+      </c>
+      <c r="CD159">
+        <v>0.01710434616468156</v>
+      </c>
+      <c r="CE159">
+        <v>0.04666673003086644</v>
+      </c>
+      <c r="CF159">
+        <v>0.0169104535315157</v>
+      </c>
+      <c r="CG159">
+        <v>3301.326060000004</v>
+      </c>
+      <c r="CH159">
+        <v>1133.036789999999</v>
+      </c>
+      <c r="CI159">
+        <v>3511.546256992101</v>
+      </c>
+      <c r="CJ159">
+        <v>1264.50817494702</v>
+      </c>
+      <c r="CK159">
+        <v>0.1464327077984825</v>
+      </c>
+      <c r="CL159">
+        <v>0.06367131048874407</v>
+      </c>
+      <c r="CM159">
+        <v>10000</v>
+      </c>
+      <c r="CO159">
+        <v>0.002846685644570964</v>
+      </c>
+      <c r="CP159">
+        <v>0.05530703538023587</v>
+      </c>
+      <c r="CQ159">
+        <v>1150640.528656262</v>
+      </c>
+      <c r="CR159">
+        <v>1971216.259841402</v>
+      </c>
+      <c r="CS159" s="2">
+        <v>45567.21099284347</v>
+      </c>
+      <c r="CT159">
+        <v>-0.4239993530325838</v>
+      </c>
+      <c r="CU159">
+        <v>-0.5350284955665463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update METISUSDT.json at 2024-10-02_07-35-51 bestfile_scores 0.0009676241688939102 bestfile_sharp 0.08447403422936871
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="402">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -785,6 +785,9 @@
   </si>
   <si>
     <t>ZROUSDT</t>
+  </si>
+  <si>
+    <t>RDNTUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1578,7 +1581,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU159"/>
+  <dimension ref="A1:CU160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1996,7 +1999,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2161,7 +2164,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2277,7 +2280,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2442,7 +2445,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2558,7 +2561,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2723,7 +2726,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2839,7 +2842,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -3004,7 +3007,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3120,7 +3123,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3285,7 +3288,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3401,7 +3404,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3566,7 +3569,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3682,7 +3685,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3847,7 +3850,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3963,7 +3966,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4128,7 +4131,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4244,7 +4247,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4409,7 +4412,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4525,7 +4528,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4690,7 +4693,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4806,7 +4809,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4971,7 +4974,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5087,7 +5090,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5252,7 +5255,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5368,7 +5371,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5533,7 +5536,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5649,7 +5652,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5814,7 +5817,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5930,7 +5933,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6095,7 +6098,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6211,7 +6214,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6376,7 +6379,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6492,7 +6495,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6657,7 +6660,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6773,7 +6776,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6938,7 +6941,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7054,7 +7057,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7219,7 +7222,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7335,7 +7338,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7500,7 +7503,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7616,7 +7619,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7781,7 +7784,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7897,7 +7900,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8062,7 +8065,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8178,7 +8181,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8343,7 +8346,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8459,7 +8462,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8624,7 +8627,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8740,7 +8743,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8905,7 +8908,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -9021,7 +9024,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9186,7 +9189,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9302,7 +9305,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9467,7 +9470,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9583,7 +9586,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9748,7 +9751,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9864,7 +9867,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10029,7 +10032,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10145,7 +10148,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10310,7 +10313,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10426,7 +10429,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10591,7 +10594,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10707,7 +10710,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10872,7 +10875,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10988,7 +10991,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11153,7 +11156,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11275,7 +11278,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11440,7 +11443,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11562,7 +11565,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11727,7 +11730,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11849,7 +11852,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -12014,7 +12017,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12136,7 +12139,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12301,7 +12304,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12423,7 +12426,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12588,7 +12591,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12710,7 +12713,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12875,7 +12878,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12997,7 +13000,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13162,7 +13165,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13284,7 +13287,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13449,7 +13452,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13571,7 +13574,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13736,7 +13739,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13858,7 +13861,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -14023,7 +14026,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14145,7 +14148,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14310,7 +14313,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14432,7 +14435,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14597,7 +14600,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14719,7 +14722,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14884,7 +14887,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -15006,7 +15009,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15171,7 +15174,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15293,7 +15296,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15458,7 +15461,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15580,7 +15583,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15745,7 +15748,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15867,7 +15870,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16032,7 +16035,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16154,7 +16157,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16319,7 +16322,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16441,7 +16444,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16606,7 +16609,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16728,7 +16731,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16893,7 +16896,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -17012,7 +17015,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17177,7 +17180,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17293,7 +17296,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17458,7 +17461,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17571,7 +17574,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17736,7 +17739,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17849,7 +17852,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -18014,7 +18017,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18127,7 +18130,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18292,7 +18295,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18405,7 +18408,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18570,7 +18573,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18683,7 +18686,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18848,7 +18851,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18961,7 +18964,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19126,7 +19129,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19239,7 +19242,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19404,7 +19407,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19517,7 +19520,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19682,7 +19685,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19795,7 +19798,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19960,7 +19963,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20073,7 +20076,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20244,7 +20247,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20357,7 +20360,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20528,7 +20531,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20641,7 +20644,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20812,7 +20815,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20925,7 +20928,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21096,7 +21099,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21206,7 +21209,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21377,7 +21380,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21484,7 +21487,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21655,7 +21658,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21759,7 +21762,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21930,7 +21933,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22034,7 +22037,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22205,7 +22208,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22309,7 +22312,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22480,7 +22483,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22584,7 +22587,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22755,7 +22758,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22859,7 +22862,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23030,7 +23033,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23134,7 +23137,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23305,7 +23308,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23406,7 +23409,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23577,7 +23580,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23678,7 +23681,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23849,7 +23852,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23950,7 +23953,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24121,7 +24124,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24222,7 +24225,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24393,7 +24396,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24494,7 +24497,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24665,7 +24668,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24766,7 +24769,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24937,7 +24940,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25038,7 +25041,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25209,7 +25212,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25307,7 +25310,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25478,7 +25481,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25576,7 +25579,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25747,7 +25750,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25845,7 +25848,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -26016,7 +26019,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26114,7 +26117,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26285,7 +26288,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26383,7 +26386,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26554,7 +26557,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26652,7 +26655,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26823,7 +26826,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26921,7 +26924,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27092,7 +27095,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27190,7 +27193,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27361,7 +27364,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27459,7 +27462,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27630,7 +27633,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27728,7 +27731,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27899,7 +27902,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27997,7 +28000,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28168,7 +28171,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28266,7 +28269,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28437,7 +28440,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28535,7 +28538,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28706,7 +28709,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28804,7 +28807,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28975,7 +28978,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29073,7 +29076,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29244,7 +29247,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29342,7 +29345,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29513,7 +29516,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29611,7 +29614,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29782,7 +29785,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29880,7 +29883,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30051,7 +30054,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30149,7 +30152,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30320,7 +30323,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30418,7 +30421,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30589,7 +30592,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30687,7 +30690,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30858,7 +30861,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30956,7 +30959,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31127,7 +31130,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31225,7 +31228,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31396,7 +31399,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31494,7 +31497,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31665,7 +31668,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31763,7 +31766,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31934,7 +31937,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32032,7 +32035,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32203,7 +32206,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32301,7 +32304,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32472,7 +32475,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32570,7 +32573,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32741,7 +32744,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32839,7 +32842,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -33010,7 +33013,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33108,7 +33111,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33279,7 +33282,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33377,7 +33380,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33548,7 +33551,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33646,7 +33649,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33817,7 +33820,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33915,7 +33918,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34086,7 +34089,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34184,7 +34187,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34355,7 +34358,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34453,7 +34456,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34624,7 +34627,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34722,7 +34725,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34893,7 +34896,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34991,7 +34994,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35162,7 +35165,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35260,7 +35263,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35431,7 +35434,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35529,7 +35532,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35700,7 +35703,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35798,7 +35801,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35969,7 +35972,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36067,7 +36070,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36238,7 +36241,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36336,7 +36339,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36507,7 +36510,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36605,7 +36608,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36776,7 +36779,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36874,7 +36877,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37045,7 +37048,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37143,7 +37146,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37314,7 +37317,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37412,7 +37415,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37583,7 +37586,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37681,7 +37684,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37852,7 +37855,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37950,7 +37953,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38121,7 +38124,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38219,7 +38222,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38390,7 +38393,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38488,7 +38491,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38659,7 +38662,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38757,7 +38760,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38928,7 +38931,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -39026,7 +39029,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39197,7 +39200,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39295,7 +39298,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39466,7 +39469,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39564,7 +39567,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39735,7 +39738,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39833,7 +39836,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -40004,7 +40007,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40102,7 +40105,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40273,7 +40276,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40371,7 +40374,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40542,7 +40545,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40640,7 +40643,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40811,7 +40814,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40909,7 +40912,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41080,7 +41083,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41178,7 +41181,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41349,7 +41352,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41447,7 +41450,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41618,7 +41621,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41716,7 +41719,7 @@
         <v>0.01422843894993598</v>
       </c>
       <c r="AM146" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN146">
         <v>0.3570285831928028</v>
@@ -41985,7 +41988,7 @@
         <v>0.01287672421329242</v>
       </c>
       <c r="AM147" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN147">
         <v>0.1138938544209247</v>
@@ -42254,7 +42257,7 @@
         <v>0.01129449859594168</v>
       </c>
       <c r="AM148" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN148">
         <v>0.01929055864963264</v>
@@ -42523,7 +42526,7 @@
         <v>0.01268293743279473</v>
       </c>
       <c r="AM149" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN149">
         <v>0.02713293780673231</v>
@@ -42792,7 +42795,7 @@
         <v>0.006815186142663594</v>
       </c>
       <c r="AM150" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN150">
         <v>0.06060596226028341</v>
@@ -43061,7 +43064,7 @@
         <v>0.01172718359151741</v>
       </c>
       <c r="AM151" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN151">
         <v>0.09142880750409497</v>
@@ -43330,7 +43333,7 @@
         <v>0.01464508407647874</v>
       </c>
       <c r="AM152" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN152">
         <v>0.3981395839245215</v>
@@ -43599,7 +43602,7 @@
         <v>0.01424145384485694</v>
       </c>
       <c r="AM153" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN153">
         <v>0.1335188651800471</v>
@@ -43868,7 +43871,7 @@
         <v>0.008636072468123625</v>
       </c>
       <c r="AM154" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN154">
         <v>0.06745759346973818</v>
@@ -44137,7 +44140,7 @@
         <v>0.01257263323646787</v>
       </c>
       <c r="AM155" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN155">
         <v>0.1015263162251083</v>
@@ -44406,7 +44409,7 @@
         <v>0.01192789588635882</v>
       </c>
       <c r="AM156" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN156">
         <v>0.08086717939318311</v>
@@ -44675,7 +44678,7 @@
         <v>0.01186799249853062</v>
       </c>
       <c r="AM157" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN157">
         <v>0.07213994227012922</v>
@@ -44944,7 +44947,7 @@
         <v>0.01449742321347242</v>
       </c>
       <c r="AM158" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN158">
         <v>0.1112845525409627</v>
@@ -45213,7 +45216,7 @@
         <v>0.01458063833474489</v>
       </c>
       <c r="AM159" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN159">
         <v>0.182085969558268</v>
@@ -45391,6 +45394,275 @@
       </c>
       <c r="CU159">
         <v>-0.5350284955665463</v>
+      </c>
+    </row>
+    <row r="160" spans="10:99">
+      <c r="J160" t="s">
+        <v>257</v>
+      </c>
+      <c r="K160">
+        <v>0.0004334713670646195</v>
+      </c>
+      <c r="L160">
+        <v>0.0004334713670646195</v>
+      </c>
+      <c r="M160">
+        <v>0.002444868493271191</v>
+      </c>
+      <c r="N160">
+        <v>0.002444868493271191</v>
+      </c>
+      <c r="O160">
+        <v>0.0005442242282440723</v>
+      </c>
+      <c r="P160">
+        <v>0.0005442242282440723</v>
+      </c>
+      <c r="Q160">
+        <v>0.002578131277199658</v>
+      </c>
+      <c r="R160">
+        <v>0.002578131277199658</v>
+      </c>
+      <c r="S160">
+        <v>6.161631878461071</v>
+      </c>
+      <c r="T160">
+        <v>11.24704429916411</v>
+      </c>
+      <c r="U160">
+        <v>0.9911593797186379</v>
+      </c>
+      <c r="V160">
+        <v>0.7664591128210272</v>
+      </c>
+      <c r="W160">
+        <v>0.09258825473082477</v>
+      </c>
+      <c r="X160">
+        <v>0.09340818042662685</v>
+      </c>
+      <c r="Y160">
+        <v>0.2243833618893161</v>
+      </c>
+      <c r="Z160">
+        <v>0.1342584911555272</v>
+      </c>
+      <c r="AA160">
+        <v>0.9984916952823659</v>
+      </c>
+      <c r="AB160">
+        <v>0.8070197401218737</v>
+      </c>
+      <c r="AC160">
+        <v>0.8804590293723861</v>
+      </c>
+      <c r="AD160">
+        <v>0.9971186125700052</v>
+      </c>
+      <c r="AE160">
+        <v>0.7761239307879453</v>
+      </c>
+      <c r="AF160">
+        <v>0.8677933487846073</v>
+      </c>
+      <c r="AG160">
+        <v>0.01026475346738024</v>
+      </c>
+      <c r="AH160">
+        <v>0.01203015543742209</v>
+      </c>
+      <c r="AI160">
+        <v>0.9984916952823659</v>
+      </c>
+      <c r="AJ160">
+        <v>0.9971186125700052</v>
+      </c>
+      <c r="AK160">
+        <v>0.01026475346738024</v>
+      </c>
+      <c r="AL160">
+        <v>0.01203015543742209</v>
+      </c>
+      <c r="AM160" t="s">
+        <v>258</v>
+      </c>
+      <c r="AN160">
+        <v>0.04025259423397862</v>
+      </c>
+      <c r="AO160">
+        <v>0.1196555143668329</v>
+      </c>
+      <c r="AP160">
+        <v>-101.290028982</v>
+      </c>
+      <c r="AQ160">
+        <v>-972.5843283600001</v>
+      </c>
+      <c r="AR160">
+        <v>12661.40652101798</v>
+      </c>
+      <c r="AS160">
+        <v>37795.41887164005</v>
+      </c>
+      <c r="AT160">
+        <v>12656.11273101798</v>
+      </c>
+      <c r="AU160">
+        <v>37795.41887164005</v>
+      </c>
+      <c r="AV160">
+        <v>0.2661406521017977</v>
+      </c>
+      <c r="AW160">
+        <v>2.779541887164005</v>
+      </c>
+      <c r="AX160">
+        <v>3.895627111906182</v>
+      </c>
+      <c r="AY160">
+        <v>2.134079155098263</v>
+      </c>
+      <c r="AZ160">
+        <v>48.7</v>
+      </c>
+      <c r="BA160">
+        <v>41.06666666666667</v>
+      </c>
+      <c r="BB160">
+        <v>0.1388691343718976</v>
+      </c>
+      <c r="BC160">
+        <v>0.04609182593706302</v>
+      </c>
+      <c r="BD160">
+        <v>-445.5226188540968</v>
+      </c>
+      <c r="BE160">
+        <v>-1390.039242879773</v>
+      </c>
+      <c r="BF160">
+        <v>1582</v>
+      </c>
+      <c r="BG160">
+        <v>2456</v>
+      </c>
+      <c r="BH160">
+        <v>544.4986111111111</v>
+      </c>
+      <c r="BI160">
+        <v>1773</v>
+      </c>
+      <c r="BJ160">
+        <v>3668</v>
+      </c>
+      <c r="BK160">
+        <v>3355</v>
+      </c>
+      <c r="BL160">
+        <v>6124</v>
+      </c>
+      <c r="BM160">
+        <v>0</v>
+      </c>
+      <c r="BN160">
+        <v>0</v>
+      </c>
+      <c r="BO160">
+        <v>26</v>
+      </c>
+      <c r="BP160">
+        <v>1490</v>
+      </c>
+      <c r="BQ160">
+        <v>0</v>
+      </c>
+      <c r="BR160">
+        <v>0</v>
+      </c>
+      <c r="BS160">
+        <v>1556</v>
+      </c>
+      <c r="BT160">
+        <v>966</v>
+      </c>
+      <c r="BU160">
+        <v>1773</v>
+      </c>
+      <c r="BV160">
+        <v>3668</v>
+      </c>
+      <c r="BW160">
+        <v>2661.406521017997</v>
+      </c>
+      <c r="BX160">
+        <v>27795.41887163999</v>
+      </c>
+      <c r="BY160">
+        <v>0.1029623572489861</v>
+      </c>
+      <c r="BZ160">
+        <v>0.08207943623972055</v>
+      </c>
+      <c r="CA160">
+        <v>0.288451000093932</v>
+      </c>
+      <c r="CB160">
+        <v>0.1167685748473511</v>
+      </c>
+      <c r="CC160">
+        <v>0.01461356802735315</v>
+      </c>
+      <c r="CD160">
+        <v>0.009184092139635646</v>
+      </c>
+      <c r="CE160">
+        <v>0.01769311833305812</v>
+      </c>
+      <c r="CF160">
+        <v>0.01200380731445641</v>
+      </c>
+      <c r="CG160">
+        <v>2762.696549999996</v>
+      </c>
+      <c r="CH160">
+        <v>28768.00319999999</v>
+      </c>
+      <c r="CI160">
+        <v>3208.219168854093</v>
+      </c>
+      <c r="CJ160">
+        <v>30158.04244287976</v>
+      </c>
+      <c r="CK160">
+        <v>0.04413544954082176</v>
+      </c>
+      <c r="CL160">
+        <v>0.1741132501882998</v>
+      </c>
+      <c r="CM160">
+        <v>10000</v>
+      </c>
+      <c r="CO160">
+        <v>0.01920575407452751</v>
+      </c>
+      <c r="CP160">
+        <v>0.06335603336138955</v>
+      </c>
+      <c r="CQ160">
+        <v>3302948.080610289</v>
+      </c>
+      <c r="CR160">
+        <v>18609944.41800443</v>
+      </c>
+      <c r="CS160" s="2">
+        <v>45567.28155661427</v>
+      </c>
+      <c r="CT160">
+        <v>-0.7522678488492383</v>
+      </c>
+      <c r="CU160">
+        <v>-0.5261894562865548</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update LPTUSDT.json at 2024-10-02_10-59-41 bestfile_scores 0.0007680516463811238 bestfile_sharp 0.10430655866055508
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="403">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -788,6 +788,9 @@
   </si>
   <si>
     <t>RDNTUSDT</t>
+  </si>
+  <si>
+    <t>METISUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1581,7 +1584,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU160"/>
+  <dimension ref="A1:CU161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1999,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2164,7 +2167,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2280,7 +2283,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2445,7 +2448,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2561,7 +2564,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2726,7 +2729,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2842,7 +2845,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -3007,7 +3010,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3123,7 +3126,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3288,7 +3291,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3404,7 +3407,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3569,7 +3572,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3685,7 +3688,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3850,7 +3853,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3966,7 +3969,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4131,7 +4134,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4247,7 +4250,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4412,7 +4415,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4528,7 +4531,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4693,7 +4696,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4809,7 +4812,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4974,7 +4977,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5090,7 +5093,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5255,7 +5258,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5371,7 +5374,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5536,7 +5539,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5652,7 +5655,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5817,7 +5820,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5933,7 +5936,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6098,7 +6101,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6214,7 +6217,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6379,7 +6382,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6495,7 +6498,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6660,7 +6663,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6776,7 +6779,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6941,7 +6944,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7057,7 +7060,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7222,7 +7225,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7338,7 +7341,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7503,7 +7506,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7619,7 +7622,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7784,7 +7787,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7900,7 +7903,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8065,7 +8068,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8181,7 +8184,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8346,7 +8349,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8462,7 +8465,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8627,7 +8630,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8743,7 +8746,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8908,7 +8911,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -9024,7 +9027,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9189,7 +9192,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9305,7 +9308,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9470,7 +9473,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9586,7 +9589,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9751,7 +9754,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9867,7 +9870,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10032,7 +10035,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10148,7 +10151,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10313,7 +10316,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10429,7 +10432,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10594,7 +10597,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10710,7 +10713,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10875,7 +10878,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10991,7 +10994,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11156,7 +11159,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11278,7 +11281,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11443,7 +11446,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11565,7 +11568,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11730,7 +11733,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11852,7 +11855,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -12017,7 +12020,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12139,7 +12142,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12304,7 +12307,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12426,7 +12429,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12591,7 +12594,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12713,7 +12716,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12878,7 +12881,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -13000,7 +13003,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13165,7 +13168,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13287,7 +13290,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13452,7 +13455,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13574,7 +13577,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13739,7 +13742,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13861,7 +13864,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -14026,7 +14029,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14148,7 +14151,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14313,7 +14316,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14435,7 +14438,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14600,7 +14603,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14722,7 +14725,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14887,7 +14890,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -15009,7 +15012,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15174,7 +15177,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15296,7 +15299,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15461,7 +15464,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15583,7 +15586,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15748,7 +15751,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15870,7 +15873,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16035,7 +16038,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16157,7 +16160,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16322,7 +16325,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16444,7 +16447,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16609,7 +16612,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16731,7 +16734,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16896,7 +16899,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -17015,7 +17018,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17180,7 +17183,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17296,7 +17299,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17461,7 +17464,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17574,7 +17577,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17739,7 +17742,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17852,7 +17855,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -18017,7 +18020,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18130,7 +18133,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18295,7 +18298,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18408,7 +18411,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18573,7 +18576,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18686,7 +18689,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18851,7 +18854,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18964,7 +18967,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19129,7 +19132,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19242,7 +19245,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19407,7 +19410,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19520,7 +19523,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19685,7 +19688,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19798,7 +19801,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19963,7 +19966,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20076,7 +20079,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20247,7 +20250,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20360,7 +20363,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20531,7 +20534,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20644,7 +20647,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20815,7 +20818,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20928,7 +20931,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21099,7 +21102,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21209,7 +21212,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21380,7 +21383,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21487,7 +21490,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21658,7 +21661,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21762,7 +21765,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21933,7 +21936,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22037,7 +22040,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22208,7 +22211,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22312,7 +22315,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22483,7 +22486,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22587,7 +22590,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22758,7 +22761,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22862,7 +22865,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23033,7 +23036,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23137,7 +23140,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23308,7 +23311,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23409,7 +23412,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23580,7 +23583,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23681,7 +23684,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23852,7 +23855,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23953,7 +23956,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24124,7 +24127,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24225,7 +24228,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24396,7 +24399,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24497,7 +24500,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24668,7 +24671,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24769,7 +24772,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24940,7 +24943,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25041,7 +25044,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25212,7 +25215,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25310,7 +25313,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25481,7 +25484,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25579,7 +25582,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25750,7 +25753,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25848,7 +25851,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -26019,7 +26022,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26117,7 +26120,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26288,7 +26291,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26386,7 +26389,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26557,7 +26560,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26655,7 +26658,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26826,7 +26829,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26924,7 +26927,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27095,7 +27098,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27193,7 +27196,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27364,7 +27367,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27462,7 +27465,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27633,7 +27636,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27731,7 +27734,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27902,7 +27905,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -28000,7 +28003,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28171,7 +28174,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28269,7 +28272,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28440,7 +28443,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28538,7 +28541,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28709,7 +28712,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28807,7 +28810,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28978,7 +28981,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29076,7 +29079,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29247,7 +29250,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29345,7 +29348,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29516,7 +29519,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29614,7 +29617,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29785,7 +29788,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29883,7 +29886,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30054,7 +30057,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30152,7 +30155,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30323,7 +30326,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30421,7 +30424,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30592,7 +30595,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30690,7 +30693,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30861,7 +30864,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30959,7 +30962,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31130,7 +31133,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31228,7 +31231,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31399,7 +31402,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31497,7 +31500,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31668,7 +31671,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31766,7 +31769,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31937,7 +31940,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32035,7 +32038,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32206,7 +32209,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32304,7 +32307,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32475,7 +32478,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32573,7 +32576,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32744,7 +32747,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32842,7 +32845,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -33013,7 +33016,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33111,7 +33114,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33282,7 +33285,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33380,7 +33383,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33551,7 +33554,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33649,7 +33652,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33820,7 +33823,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33918,7 +33921,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34089,7 +34092,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34187,7 +34190,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34358,7 +34361,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34456,7 +34459,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34627,7 +34630,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34725,7 +34728,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34896,7 +34899,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34994,7 +34997,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35165,7 +35168,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35263,7 +35266,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35434,7 +35437,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35532,7 +35535,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35703,7 +35706,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35801,7 +35804,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35972,7 +35975,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36070,7 +36073,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36241,7 +36244,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36339,7 +36342,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36510,7 +36513,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36608,7 +36611,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36779,7 +36782,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36877,7 +36880,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37048,7 +37051,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37146,7 +37149,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37317,7 +37320,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37415,7 +37418,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37586,7 +37589,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37684,7 +37687,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37855,7 +37858,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37953,7 +37956,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38124,7 +38127,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38222,7 +38225,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38393,7 +38396,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38491,7 +38494,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38662,7 +38665,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38760,7 +38763,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38931,7 +38934,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -39029,7 +39032,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39200,7 +39203,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39298,7 +39301,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39469,7 +39472,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39567,7 +39570,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39738,7 +39741,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39836,7 +39839,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -40007,7 +40010,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40105,7 +40108,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40276,7 +40279,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40374,7 +40377,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40545,7 +40548,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40643,7 +40646,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40814,7 +40817,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40912,7 +40915,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41083,7 +41086,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41181,7 +41184,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41352,7 +41355,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41450,7 +41453,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41621,7 +41624,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41719,7 +41722,7 @@
         <v>0.01422843894993598</v>
       </c>
       <c r="AM146" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN146">
         <v>0.3570285831928028</v>
@@ -41988,7 +41991,7 @@
         <v>0.01287672421329242</v>
       </c>
       <c r="AM147" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN147">
         <v>0.1138938544209247</v>
@@ -42257,7 +42260,7 @@
         <v>0.01129449859594168</v>
       </c>
       <c r="AM148" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN148">
         <v>0.01929055864963264</v>
@@ -42526,7 +42529,7 @@
         <v>0.01268293743279473</v>
       </c>
       <c r="AM149" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN149">
         <v>0.02713293780673231</v>
@@ -42795,7 +42798,7 @@
         <v>0.006815186142663594</v>
       </c>
       <c r="AM150" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN150">
         <v>0.06060596226028341</v>
@@ -43064,7 +43067,7 @@
         <v>0.01172718359151741</v>
       </c>
       <c r="AM151" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN151">
         <v>0.09142880750409497</v>
@@ -43333,7 +43336,7 @@
         <v>0.01464508407647874</v>
       </c>
       <c r="AM152" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN152">
         <v>0.3981395839245215</v>
@@ -43602,7 +43605,7 @@
         <v>0.01424145384485694</v>
       </c>
       <c r="AM153" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN153">
         <v>0.1335188651800471</v>
@@ -43871,7 +43874,7 @@
         <v>0.008636072468123625</v>
       </c>
       <c r="AM154" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN154">
         <v>0.06745759346973818</v>
@@ -44140,7 +44143,7 @@
         <v>0.01257263323646787</v>
       </c>
       <c r="AM155" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN155">
         <v>0.1015263162251083</v>
@@ -44409,7 +44412,7 @@
         <v>0.01192789588635882</v>
       </c>
       <c r="AM156" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN156">
         <v>0.08086717939318311</v>
@@ -44678,7 +44681,7 @@
         <v>0.01186799249853062</v>
       </c>
       <c r="AM157" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN157">
         <v>0.07213994227012922</v>
@@ -44947,7 +44950,7 @@
         <v>0.01449742321347242</v>
       </c>
       <c r="AM158" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN158">
         <v>0.1112845525409627</v>
@@ -45216,7 +45219,7 @@
         <v>0.01458063833474489</v>
       </c>
       <c r="AM159" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN159">
         <v>0.182085969558268</v>
@@ -45485,7 +45488,7 @@
         <v>0.01203015543742209</v>
       </c>
       <c r="AM160" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN160">
         <v>0.04025259423397862</v>
@@ -45663,6 +45666,275 @@
       </c>
       <c r="CU160">
         <v>-0.5261894562865548</v>
+      </c>
+    </row>
+    <row r="161" spans="10:99">
+      <c r="J161" t="s">
+        <v>258</v>
+      </c>
+      <c r="K161">
+        <v>0.0004137416325991072</v>
+      </c>
+      <c r="L161">
+        <v>0.0004137416325991072</v>
+      </c>
+      <c r="M161">
+        <v>0.001329440734463949</v>
+      </c>
+      <c r="N161">
+        <v>0.001329440734463949</v>
+      </c>
+      <c r="O161">
+        <v>0.0001846271807166122</v>
+      </c>
+      <c r="P161">
+        <v>0.0001846271807166122</v>
+      </c>
+      <c r="Q161">
+        <v>0.001942687127795972</v>
+      </c>
+      <c r="R161">
+        <v>0.001942687127795972</v>
+      </c>
+      <c r="S161">
+        <v>5.600943085864679</v>
+      </c>
+      <c r="T161">
+        <v>10.05702379646891</v>
+      </c>
+      <c r="U161">
+        <v>0.9902297765505657</v>
+      </c>
+      <c r="V161">
+        <v>0.7586885893381883</v>
+      </c>
+      <c r="W161">
+        <v>0.03701324750988488</v>
+      </c>
+      <c r="X161">
+        <v>0.09694366587681902</v>
+      </c>
+      <c r="Y161">
+        <v>0.09483106907169973</v>
+      </c>
+      <c r="Z161">
+        <v>0.1398132706016705</v>
+      </c>
+      <c r="AA161">
+        <v>0.9994780856571323</v>
+      </c>
+      <c r="AB161">
+        <v>0.9340854555952806</v>
+      </c>
+      <c r="AC161">
+        <v>0.8798969595508586</v>
+      </c>
+      <c r="AD161">
+        <v>0.9953083025256662</v>
+      </c>
+      <c r="AE161">
+        <v>0.9052924170960746</v>
+      </c>
+      <c r="AF161">
+        <v>0.8642061049043722</v>
+      </c>
+      <c r="AG161">
+        <v>0.003987180988716563</v>
+      </c>
+      <c r="AH161">
+        <v>0.01488877514152119</v>
+      </c>
+      <c r="AI161">
+        <v>0.9994780856571323</v>
+      </c>
+      <c r="AJ161">
+        <v>0.9953083025256662</v>
+      </c>
+      <c r="AK161">
+        <v>0.003987180988716563</v>
+      </c>
+      <c r="AL161">
+        <v>0.01488877514152119</v>
+      </c>
+      <c r="AM161" t="s">
+        <v>259</v>
+      </c>
+      <c r="AN161">
+        <v>0.01931426172613477</v>
+      </c>
+      <c r="AO161">
+        <v>0.160244058259244</v>
+      </c>
+      <c r="AP161">
+        <v>-35.65562034</v>
+      </c>
+      <c r="AQ161">
+        <v>-72.10192409999999</v>
+      </c>
+      <c r="AR161">
+        <v>10874.38687966002</v>
+      </c>
+      <c r="AS161">
+        <v>13089.49437590001</v>
+      </c>
+      <c r="AT161">
+        <v>10868.26187966002</v>
+      </c>
+      <c r="AU161">
+        <v>13089.49437590001</v>
+      </c>
+      <c r="AV161">
+        <v>0.08743868796600207</v>
+      </c>
+      <c r="AW161">
+        <v>0.3089494375900006</v>
+      </c>
+      <c r="AX161">
+        <v>4.277013521457966</v>
+      </c>
+      <c r="AY161">
+        <v>2.387080674194076</v>
+      </c>
+      <c r="AZ161">
+        <v>83.11666666666666</v>
+      </c>
+      <c r="BA161">
+        <v>37.73333333333333</v>
+      </c>
+      <c r="BB161">
+        <v>0.1679251024910572</v>
+      </c>
+      <c r="BC161">
+        <v>0.07157125758007946</v>
+      </c>
+      <c r="BD161">
+        <v>-183.6601254781601</v>
+      </c>
+      <c r="BE161">
+        <v>-243.7229835880945</v>
+      </c>
+      <c r="BF161">
+        <v>465</v>
+      </c>
+      <c r="BG161">
+        <v>921</v>
+      </c>
+      <c r="BH161">
+        <v>202.6444444444444</v>
+      </c>
+      <c r="BI161">
+        <v>670</v>
+      </c>
+      <c r="BJ161">
+        <v>1117</v>
+      </c>
+      <c r="BK161">
+        <v>1135</v>
+      </c>
+      <c r="BL161">
+        <v>2038</v>
+      </c>
+      <c r="BM161">
+        <v>0</v>
+      </c>
+      <c r="BN161">
+        <v>0</v>
+      </c>
+      <c r="BO161">
+        <v>8</v>
+      </c>
+      <c r="BP161">
+        <v>52</v>
+      </c>
+      <c r="BQ161">
+        <v>0</v>
+      </c>
+      <c r="BR161">
+        <v>0</v>
+      </c>
+      <c r="BS161">
+        <v>457</v>
+      </c>
+      <c r="BT161">
+        <v>869</v>
+      </c>
+      <c r="BU161">
+        <v>670</v>
+      </c>
+      <c r="BV161">
+        <v>1117</v>
+      </c>
+      <c r="BW161">
+        <v>874.3868796600102</v>
+      </c>
+      <c r="BX161">
+        <v>3089.49437589999</v>
+      </c>
+      <c r="BY161">
+        <v>0.06268542483383106</v>
+      </c>
+      <c r="BZ161">
+        <v>0.08282910685375881</v>
+      </c>
+      <c r="CA161">
+        <v>0.1363684156933809</v>
+      </c>
+      <c r="CB161">
+        <v>0.1192137825990478</v>
+      </c>
+      <c r="CC161">
+        <v>0.01671360694027366</v>
+      </c>
+      <c r="CD161">
+        <v>0.01562794613524056</v>
+      </c>
+      <c r="CE161">
+        <v>0.01433048378261276</v>
+      </c>
+      <c r="CF161">
+        <v>0.01557070406445176</v>
+      </c>
+      <c r="CG161">
+        <v>910.0425000000103</v>
+      </c>
+      <c r="CH161">
+        <v>3161.59629999999</v>
+      </c>
+      <c r="CI161">
+        <v>1093.70262547817</v>
+      </c>
+      <c r="CJ161">
+        <v>3405.319283588085</v>
+      </c>
+      <c r="CK161">
+        <v>0.08447403422936871</v>
+      </c>
+      <c r="CL161">
+        <v>0.0895087503205767</v>
+      </c>
+      <c r="CM161">
+        <v>10000</v>
+      </c>
+      <c r="CO161">
+        <v>0.007399794450154163</v>
+      </c>
+      <c r="CP161">
+        <v>0.07173689619732786</v>
+      </c>
+      <c r="CQ161">
+        <v>788633.4795472159</v>
+      </c>
+      <c r="CR161">
+        <v>4987525.511984727</v>
+      </c>
+      <c r="CS161" s="2">
+        <v>45567.31659491234</v>
+      </c>
+      <c r="CT161">
+        <v>-0.933102572242228</v>
+      </c>
+      <c r="CU161">
+        <v>-0.5457182029235589</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update FXSUSDT.json at 2024-10-02_14-24-23 bestfile_scores 0.0013374246123236677 bestfile_sharp 0.1373634478132738
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="404">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -791,6 +791,9 @@
   </si>
   <si>
     <t>METISUSDT</t>
+  </si>
+  <si>
+    <t>LPTUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1584,7 +1587,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU161"/>
+  <dimension ref="A1:CU162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2002,7 +2005,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2167,7 +2170,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2283,7 +2286,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2448,7 +2451,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2564,7 +2567,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2729,7 +2732,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2845,7 +2848,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -3010,7 +3013,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3126,7 +3129,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3291,7 +3294,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3407,7 +3410,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3572,7 +3575,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3688,7 +3691,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3853,7 +3856,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3969,7 +3972,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4134,7 +4137,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4250,7 +4253,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4415,7 +4418,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4531,7 +4534,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4696,7 +4699,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4812,7 +4815,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4977,7 +4980,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5093,7 +5096,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5258,7 +5261,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5374,7 +5377,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5539,7 +5542,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5655,7 +5658,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5820,7 +5823,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5936,7 +5939,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6101,7 +6104,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6217,7 +6220,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6382,7 +6385,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6498,7 +6501,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6663,7 +6666,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6779,7 +6782,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6944,7 +6947,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7060,7 +7063,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7225,7 +7228,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7341,7 +7344,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7506,7 +7509,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7622,7 +7625,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7787,7 +7790,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7903,7 +7906,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8068,7 +8071,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8184,7 +8187,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8349,7 +8352,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8465,7 +8468,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8630,7 +8633,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8746,7 +8749,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8911,7 +8914,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -9027,7 +9030,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9192,7 +9195,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9308,7 +9311,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9473,7 +9476,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9589,7 +9592,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9754,7 +9757,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9870,7 +9873,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10035,7 +10038,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10151,7 +10154,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10316,7 +10319,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10432,7 +10435,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10597,7 +10600,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10713,7 +10716,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10878,7 +10881,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10994,7 +10997,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11159,7 +11162,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11281,7 +11284,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11446,7 +11449,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11568,7 +11571,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11733,7 +11736,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11855,7 +11858,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -12020,7 +12023,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12142,7 +12145,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12307,7 +12310,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12429,7 +12432,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12594,7 +12597,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12716,7 +12719,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12881,7 +12884,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -13003,7 +13006,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13168,7 +13171,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13290,7 +13293,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13455,7 +13458,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13577,7 +13580,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13742,7 +13745,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13864,7 +13867,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -14029,7 +14032,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14151,7 +14154,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14316,7 +14319,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14438,7 +14441,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14603,7 +14606,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14725,7 +14728,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14890,7 +14893,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -15012,7 +15015,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15177,7 +15180,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15299,7 +15302,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15464,7 +15467,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15586,7 +15589,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15751,7 +15754,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15873,7 +15876,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16038,7 +16041,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16160,7 +16163,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16325,7 +16328,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16447,7 +16450,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16612,7 +16615,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16734,7 +16737,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16899,7 +16902,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -17018,7 +17021,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17183,7 +17186,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17299,7 +17302,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17464,7 +17467,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17577,7 +17580,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17742,7 +17745,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17855,7 +17858,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -18020,7 +18023,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18133,7 +18136,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18298,7 +18301,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18411,7 +18414,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18576,7 +18579,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18689,7 +18692,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18854,7 +18857,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18967,7 +18970,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19132,7 +19135,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19245,7 +19248,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19410,7 +19413,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19523,7 +19526,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19688,7 +19691,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19801,7 +19804,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19966,7 +19969,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20079,7 +20082,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20250,7 +20253,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20363,7 +20366,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20534,7 +20537,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20647,7 +20650,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20818,7 +20821,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20931,7 +20934,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21102,7 +21105,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21212,7 +21215,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21383,7 +21386,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21490,7 +21493,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21661,7 +21664,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21765,7 +21768,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21936,7 +21939,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22040,7 +22043,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22211,7 +22214,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22315,7 +22318,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22486,7 +22489,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22590,7 +22593,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22761,7 +22764,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22865,7 +22868,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23036,7 +23039,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23140,7 +23143,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23311,7 +23314,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23412,7 +23415,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23583,7 +23586,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23684,7 +23687,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23855,7 +23858,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23956,7 +23959,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24127,7 +24130,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24228,7 +24231,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24399,7 +24402,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24500,7 +24503,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24671,7 +24674,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24772,7 +24775,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24943,7 +24946,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25044,7 +25047,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25215,7 +25218,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25313,7 +25316,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25484,7 +25487,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25582,7 +25585,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25753,7 +25756,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25851,7 +25854,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -26022,7 +26025,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26120,7 +26123,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26291,7 +26294,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26389,7 +26392,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26560,7 +26563,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26658,7 +26661,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26829,7 +26832,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26927,7 +26930,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27098,7 +27101,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27196,7 +27199,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27367,7 +27370,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27465,7 +27468,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27636,7 +27639,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27734,7 +27737,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27905,7 +27908,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -28003,7 +28006,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28174,7 +28177,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28272,7 +28275,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28443,7 +28446,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28541,7 +28544,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28712,7 +28715,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28810,7 +28813,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28981,7 +28984,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29079,7 +29082,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29250,7 +29253,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29348,7 +29351,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29519,7 +29522,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29617,7 +29620,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29788,7 +29791,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29886,7 +29889,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30057,7 +30060,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30155,7 +30158,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30326,7 +30329,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30424,7 +30427,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30595,7 +30598,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30693,7 +30696,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30864,7 +30867,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30962,7 +30965,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31133,7 +31136,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31231,7 +31234,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31402,7 +31405,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31500,7 +31503,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31671,7 +31674,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31769,7 +31772,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31940,7 +31943,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32038,7 +32041,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32209,7 +32212,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32307,7 +32310,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32478,7 +32481,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32576,7 +32579,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32747,7 +32750,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32845,7 +32848,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -33016,7 +33019,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33114,7 +33117,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33285,7 +33288,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33383,7 +33386,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33554,7 +33557,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33652,7 +33655,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33823,7 +33826,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33921,7 +33924,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34092,7 +34095,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34190,7 +34193,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34361,7 +34364,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34459,7 +34462,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34630,7 +34633,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34728,7 +34731,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34899,7 +34902,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34997,7 +35000,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35168,7 +35171,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35266,7 +35269,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35437,7 +35440,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35535,7 +35538,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35706,7 +35709,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35804,7 +35807,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35975,7 +35978,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36073,7 +36076,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36244,7 +36247,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36342,7 +36345,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36513,7 +36516,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36611,7 +36614,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36782,7 +36785,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36880,7 +36883,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37051,7 +37054,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37149,7 +37152,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37320,7 +37323,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37418,7 +37421,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37589,7 +37592,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37687,7 +37690,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37858,7 +37861,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37956,7 +37959,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38127,7 +38130,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38225,7 +38228,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38396,7 +38399,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38494,7 +38497,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38665,7 +38668,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38763,7 +38766,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38934,7 +38937,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -39032,7 +39035,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39203,7 +39206,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39301,7 +39304,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39472,7 +39475,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39570,7 +39573,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39741,7 +39744,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39839,7 +39842,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -40010,7 +40013,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40108,7 +40111,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40279,7 +40282,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40377,7 +40380,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40548,7 +40551,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40646,7 +40649,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40817,7 +40820,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40915,7 +40918,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41086,7 +41089,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41184,7 +41187,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41355,7 +41358,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41453,7 +41456,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41624,7 +41627,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41722,7 +41725,7 @@
         <v>0.01422843894993598</v>
       </c>
       <c r="AM146" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN146">
         <v>0.3570285831928028</v>
@@ -41991,7 +41994,7 @@
         <v>0.01287672421329242</v>
       </c>
       <c r="AM147" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN147">
         <v>0.1138938544209247</v>
@@ -42260,7 +42263,7 @@
         <v>0.01129449859594168</v>
       </c>
       <c r="AM148" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN148">
         <v>0.01929055864963264</v>
@@ -42529,7 +42532,7 @@
         <v>0.01268293743279473</v>
       </c>
       <c r="AM149" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN149">
         <v>0.02713293780673231</v>
@@ -42798,7 +42801,7 @@
         <v>0.006815186142663594</v>
       </c>
       <c r="AM150" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN150">
         <v>0.06060596226028341</v>
@@ -43067,7 +43070,7 @@
         <v>0.01172718359151741</v>
       </c>
       <c r="AM151" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN151">
         <v>0.09142880750409497</v>
@@ -43336,7 +43339,7 @@
         <v>0.01464508407647874</v>
       </c>
       <c r="AM152" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN152">
         <v>0.3981395839245215</v>
@@ -43605,7 +43608,7 @@
         <v>0.01424145384485694</v>
       </c>
       <c r="AM153" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN153">
         <v>0.1335188651800471</v>
@@ -43874,7 +43877,7 @@
         <v>0.008636072468123625</v>
       </c>
       <c r="AM154" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN154">
         <v>0.06745759346973818</v>
@@ -44143,7 +44146,7 @@
         <v>0.01257263323646787</v>
       </c>
       <c r="AM155" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN155">
         <v>0.1015263162251083</v>
@@ -44412,7 +44415,7 @@
         <v>0.01192789588635882</v>
       </c>
       <c r="AM156" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN156">
         <v>0.08086717939318311</v>
@@ -44681,7 +44684,7 @@
         <v>0.01186799249853062</v>
       </c>
       <c r="AM157" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN157">
         <v>0.07213994227012922</v>
@@ -44950,7 +44953,7 @@
         <v>0.01449742321347242</v>
       </c>
       <c r="AM158" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN158">
         <v>0.1112845525409627</v>
@@ -45219,7 +45222,7 @@
         <v>0.01458063833474489</v>
       </c>
       <c r="AM159" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN159">
         <v>0.182085969558268</v>
@@ -45488,7 +45491,7 @@
         <v>0.01203015543742209</v>
       </c>
       <c r="AM160" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN160">
         <v>0.04025259423397862</v>
@@ -45757,7 +45760,7 @@
         <v>0.01488877514152119</v>
       </c>
       <c r="AM161" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AN161">
         <v>0.01931426172613477</v>
@@ -45935,6 +45938,275 @@
       </c>
       <c r="CU161">
         <v>-0.5457182029235589</v>
+      </c>
+    </row>
+    <row r="162" spans="10:99">
+      <c r="J162" t="s">
+        <v>259</v>
+      </c>
+      <c r="K162">
+        <v>0.0009001144063058852</v>
+      </c>
+      <c r="L162">
+        <v>0.0009001144063058852</v>
+      </c>
+      <c r="M162">
+        <v>0.0005887970017741662</v>
+      </c>
+      <c r="N162">
+        <v>0.0005887970017741662</v>
+      </c>
+      <c r="O162">
+        <v>0.0009922594615237035</v>
+      </c>
+      <c r="P162">
+        <v>0.0009922594615237035</v>
+      </c>
+      <c r="Q162">
+        <v>0.0005910357159207402</v>
+      </c>
+      <c r="R162">
+        <v>0.0005910357159207402</v>
+      </c>
+      <c r="S162">
+        <v>10.02319965661348</v>
+      </c>
+      <c r="T162">
+        <v>3.800530353103513</v>
+      </c>
+      <c r="U162">
+        <v>1</v>
+      </c>
+      <c r="V162">
+        <v>0.8365282386645743</v>
+      </c>
+      <c r="W162">
+        <v>0.09997728636516762</v>
+      </c>
+      <c r="X162">
+        <v>0.09967457026184179</v>
+      </c>
+      <c r="Y162">
+        <v>0.2160527480814721</v>
+      </c>
+      <c r="Z162">
+        <v>0.2064858139840652</v>
+      </c>
+      <c r="AA162">
+        <v>0.9979751796709645</v>
+      </c>
+      <c r="AB162">
+        <v>0.803595709048731</v>
+      </c>
+      <c r="AC162">
+        <v>0.8093706312415898</v>
+      </c>
+      <c r="AD162">
+        <v>0.9970549251097668</v>
+      </c>
+      <c r="AE162">
+        <v>0.7878368396957853</v>
+      </c>
+      <c r="AF162">
+        <v>0.796396927481158</v>
+      </c>
+      <c r="AG162">
+        <v>0.01073712475082089</v>
+      </c>
+      <c r="AH162">
+        <v>0.01132277626110294</v>
+      </c>
+      <c r="AI162">
+        <v>0.9979751796709645</v>
+      </c>
+      <c r="AJ162">
+        <v>0.9970549251097668</v>
+      </c>
+      <c r="AK162">
+        <v>0.01073712475082089</v>
+      </c>
+      <c r="AL162">
+        <v>0.01132277626110294</v>
+      </c>
+      <c r="AM162" t="s">
+        <v>260</v>
+      </c>
+      <c r="AN162">
+        <v>0.06043490875273809</v>
+      </c>
+      <c r="AO162">
+        <v>0.0542866135802059</v>
+      </c>
+      <c r="AP162">
+        <v>-475.01057804</v>
+      </c>
+      <c r="AQ162">
+        <v>-381.4949457</v>
+      </c>
+      <c r="AR162">
+        <v>25832.83112195987</v>
+      </c>
+      <c r="AS162">
+        <v>18606.22995429991</v>
+      </c>
+      <c r="AT162">
+        <v>25770.69282195987</v>
+      </c>
+      <c r="AU162">
+        <v>18606.22995429991</v>
+      </c>
+      <c r="AV162">
+        <v>1.583283112195986</v>
+      </c>
+      <c r="AW162">
+        <v>0.8606229954299907</v>
+      </c>
+      <c r="AX162">
+        <v>2.394510657081599</v>
+      </c>
+      <c r="AY162">
+        <v>6.312799401197605</v>
+      </c>
+      <c r="AZ162">
+        <v>51.05</v>
+      </c>
+      <c r="BA162">
+        <v>87.05</v>
+      </c>
+      <c r="BB162">
+        <v>0.08752792640599417</v>
+      </c>
+      <c r="BC162">
+        <v>0.1824369115439868</v>
+      </c>
+      <c r="BD162">
+        <v>-1564.312606890044</v>
+      </c>
+      <c r="BE162">
+        <v>-2005.585618670219</v>
+      </c>
+      <c r="BF162">
+        <v>3615</v>
+      </c>
+      <c r="BG162">
+        <v>2529</v>
+      </c>
+      <c r="BH162">
+        <v>1054.852777777778</v>
+      </c>
+      <c r="BI162">
+        <v>6958</v>
+      </c>
+      <c r="BJ162">
+        <v>1480</v>
+      </c>
+      <c r="BK162">
+        <v>10573</v>
+      </c>
+      <c r="BL162">
+        <v>4009</v>
+      </c>
+      <c r="BM162">
+        <v>0</v>
+      </c>
+      <c r="BN162">
+        <v>0</v>
+      </c>
+      <c r="BO162">
+        <v>314</v>
+      </c>
+      <c r="BP162">
+        <v>1063</v>
+      </c>
+      <c r="BQ162">
+        <v>0</v>
+      </c>
+      <c r="BR162">
+        <v>0</v>
+      </c>
+      <c r="BS162">
+        <v>3301</v>
+      </c>
+      <c r="BT162">
+        <v>1466</v>
+      </c>
+      <c r="BU162">
+        <v>6958</v>
+      </c>
+      <c r="BV162">
+        <v>1480</v>
+      </c>
+      <c r="BW162">
+        <v>15832.83112196</v>
+      </c>
+      <c r="BX162">
+        <v>8606.229954300004</v>
+      </c>
+      <c r="BY162">
+        <v>0.1133596962789828</v>
+      </c>
+      <c r="BZ162">
+        <v>0.2674553621114902</v>
+      </c>
+      <c r="CA162">
+        <v>0.2950740536275655</v>
+      </c>
+      <c r="CB162">
+        <v>0.5068985130158035</v>
+      </c>
+      <c r="CC162">
+        <v>0.01598159185900528</v>
+      </c>
+      <c r="CD162">
+        <v>0.0331925292183551</v>
+      </c>
+      <c r="CE162">
+        <v>0.01667907178627192</v>
+      </c>
+      <c r="CF162">
+        <v>0.04355013740535307</v>
+      </c>
+      <c r="CG162">
+        <v>16307.8417</v>
+      </c>
+      <c r="CH162">
+        <v>8987.724900000005</v>
+      </c>
+      <c r="CI162">
+        <v>17872.15430689004</v>
+      </c>
+      <c r="CJ162">
+        <v>10993.31051867022</v>
+      </c>
+      <c r="CK162">
+        <v>0.1043065586605551</v>
+      </c>
+      <c r="CL162">
+        <v>0.07067719779354581</v>
+      </c>
+      <c r="CM162">
+        <v>10000</v>
+      </c>
+      <c r="CO162">
+        <v>0.01587803144008216</v>
+      </c>
+      <c r="CP162">
+        <v>0.0001974879532348527</v>
+      </c>
+      <c r="CQ162">
+        <v>23175841.68417671</v>
+      </c>
+      <c r="CR162">
+        <v>2896139.159554843</v>
+      </c>
+      <c r="CS162" s="2">
+        <v>45567.45814918268</v>
+      </c>
+      <c r="CT162">
+        <v>-0.7828348096637191</v>
+      </c>
+      <c r="CU162">
+        <v>-0.7842491568660279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update COMBOUSDT.json at 2024-10-02_18-12-53 bestfile_scores 0.0021057748463523874 bestfile_sharp 0.08090285344291481
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="405">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -794,6 +794,9 @@
   </si>
   <si>
     <t>LPTUSDT</t>
+  </si>
+  <si>
+    <t>FXSUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1587,7 +1590,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU162"/>
+  <dimension ref="A1:CU163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2005,7 +2008,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2170,7 +2173,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2286,7 +2289,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2451,7 +2454,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2567,7 +2570,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2732,7 +2735,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2848,7 +2851,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -3013,7 +3016,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3129,7 +3132,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3294,7 +3297,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3410,7 +3413,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3575,7 +3578,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3691,7 +3694,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3856,7 +3859,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3972,7 +3975,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4137,7 +4140,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4253,7 +4256,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4418,7 +4421,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4534,7 +4537,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4699,7 +4702,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4815,7 +4818,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4980,7 +4983,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5096,7 +5099,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5261,7 +5264,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5377,7 +5380,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5542,7 +5545,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5658,7 +5661,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5823,7 +5826,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5939,7 +5942,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6104,7 +6107,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6220,7 +6223,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6385,7 +6388,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6501,7 +6504,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6666,7 +6669,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6782,7 +6785,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6947,7 +6950,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7063,7 +7066,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7228,7 +7231,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7344,7 +7347,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7509,7 +7512,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7625,7 +7628,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7790,7 +7793,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7906,7 +7909,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8071,7 +8074,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8187,7 +8190,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8352,7 +8355,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8468,7 +8471,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8633,7 +8636,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8749,7 +8752,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8914,7 +8917,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -9030,7 +9033,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9195,7 +9198,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9311,7 +9314,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9476,7 +9479,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9592,7 +9595,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9757,7 +9760,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9873,7 +9876,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10038,7 +10041,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10154,7 +10157,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10319,7 +10322,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10435,7 +10438,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10600,7 +10603,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10716,7 +10719,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10881,7 +10884,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10997,7 +11000,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11162,7 +11165,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11284,7 +11287,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11449,7 +11452,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11571,7 +11574,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11736,7 +11739,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11858,7 +11861,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -12023,7 +12026,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12145,7 +12148,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12310,7 +12313,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12432,7 +12435,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12597,7 +12600,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12719,7 +12722,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12884,7 +12887,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -13006,7 +13009,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13171,7 +13174,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13293,7 +13296,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13458,7 +13461,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13580,7 +13583,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13745,7 +13748,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13867,7 +13870,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -14032,7 +14035,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14154,7 +14157,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14319,7 +14322,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14441,7 +14444,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14606,7 +14609,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14728,7 +14731,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14893,7 +14896,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -15015,7 +15018,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15180,7 +15183,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15302,7 +15305,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15467,7 +15470,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15589,7 +15592,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15754,7 +15757,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15876,7 +15879,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16041,7 +16044,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16163,7 +16166,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16328,7 +16331,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16450,7 +16453,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16615,7 +16618,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16737,7 +16740,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16902,7 +16905,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -17021,7 +17024,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17186,7 +17189,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17302,7 +17305,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17467,7 +17470,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17580,7 +17583,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17745,7 +17748,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17858,7 +17861,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -18023,7 +18026,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18136,7 +18139,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18301,7 +18304,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18414,7 +18417,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18579,7 +18582,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18692,7 +18695,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18857,7 +18860,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18970,7 +18973,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19135,7 +19138,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19248,7 +19251,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19413,7 +19416,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19526,7 +19529,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19691,7 +19694,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19804,7 +19807,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19969,7 +19972,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20082,7 +20085,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20253,7 +20256,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20366,7 +20369,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20537,7 +20540,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20650,7 +20653,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20821,7 +20824,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20934,7 +20937,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21105,7 +21108,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21215,7 +21218,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21386,7 +21389,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21493,7 +21496,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21664,7 +21667,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21768,7 +21771,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21939,7 +21942,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22043,7 +22046,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22214,7 +22217,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22318,7 +22321,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22489,7 +22492,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22593,7 +22596,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22764,7 +22767,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22868,7 +22871,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23039,7 +23042,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23143,7 +23146,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23314,7 +23317,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23415,7 +23418,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23586,7 +23589,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23687,7 +23690,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23858,7 +23861,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23959,7 +23962,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24130,7 +24133,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24231,7 +24234,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24402,7 +24405,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24503,7 +24506,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24674,7 +24677,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24775,7 +24778,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24946,7 +24949,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25047,7 +25050,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25218,7 +25221,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25316,7 +25319,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25487,7 +25490,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25585,7 +25588,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25756,7 +25759,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25854,7 +25857,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -26025,7 +26028,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26123,7 +26126,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26294,7 +26297,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26392,7 +26395,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26563,7 +26566,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26661,7 +26664,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26832,7 +26835,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26930,7 +26933,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27101,7 +27104,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27199,7 +27202,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27370,7 +27373,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27468,7 +27471,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27639,7 +27642,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27737,7 +27740,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27908,7 +27911,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -28006,7 +28009,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28177,7 +28180,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28275,7 +28278,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28446,7 +28449,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28544,7 +28547,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28715,7 +28718,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28813,7 +28816,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28984,7 +28987,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29082,7 +29085,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29253,7 +29256,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29351,7 +29354,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29522,7 +29525,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29620,7 +29623,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29791,7 +29794,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29889,7 +29892,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30060,7 +30063,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30158,7 +30161,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30329,7 +30332,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30427,7 +30430,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30598,7 +30601,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30696,7 +30699,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30867,7 +30870,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30965,7 +30968,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31136,7 +31139,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31234,7 +31237,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31405,7 +31408,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31503,7 +31506,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31674,7 +31677,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31772,7 +31775,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31943,7 +31946,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32041,7 +32044,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32212,7 +32215,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32310,7 +32313,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32481,7 +32484,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32579,7 +32582,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32750,7 +32753,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32848,7 +32851,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -33019,7 +33022,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33117,7 +33120,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33288,7 +33291,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33386,7 +33389,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33557,7 +33560,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33655,7 +33658,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33826,7 +33829,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33924,7 +33927,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34095,7 +34098,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34193,7 +34196,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34364,7 +34367,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34462,7 +34465,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34633,7 +34636,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34731,7 +34734,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34902,7 +34905,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -35000,7 +35003,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35171,7 +35174,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35269,7 +35272,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35440,7 +35443,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35538,7 +35541,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35709,7 +35712,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35807,7 +35810,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35978,7 +35981,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36076,7 +36079,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36247,7 +36250,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36345,7 +36348,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36516,7 +36519,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36614,7 +36617,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36785,7 +36788,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36883,7 +36886,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37054,7 +37057,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37152,7 +37155,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37323,7 +37326,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37421,7 +37424,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37592,7 +37595,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37690,7 +37693,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37861,7 +37864,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37959,7 +37962,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38130,7 +38133,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38228,7 +38231,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38399,7 +38402,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38497,7 +38500,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38668,7 +38671,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38766,7 +38769,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38937,7 +38940,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -39035,7 +39038,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39206,7 +39209,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39304,7 +39307,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39475,7 +39478,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39573,7 +39576,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39744,7 +39747,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39842,7 +39845,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -40013,7 +40016,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40111,7 +40114,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40282,7 +40285,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40380,7 +40383,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40551,7 +40554,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40649,7 +40652,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40820,7 +40823,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40918,7 +40921,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41089,7 +41092,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41187,7 +41190,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41358,7 +41361,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41456,7 +41459,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41627,7 +41630,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41725,7 +41728,7 @@
         <v>0.01422843894993598</v>
       </c>
       <c r="AM146" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN146">
         <v>0.3570285831928028</v>
@@ -41994,7 +41997,7 @@
         <v>0.01287672421329242</v>
       </c>
       <c r="AM147" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN147">
         <v>0.1138938544209247</v>
@@ -42263,7 +42266,7 @@
         <v>0.01129449859594168</v>
       </c>
       <c r="AM148" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN148">
         <v>0.01929055864963264</v>
@@ -42532,7 +42535,7 @@
         <v>0.01268293743279473</v>
       </c>
       <c r="AM149" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN149">
         <v>0.02713293780673231</v>
@@ -42801,7 +42804,7 @@
         <v>0.006815186142663594</v>
       </c>
       <c r="AM150" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN150">
         <v>0.06060596226028341</v>
@@ -43070,7 +43073,7 @@
         <v>0.01172718359151741</v>
       </c>
       <c r="AM151" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN151">
         <v>0.09142880750409497</v>
@@ -43339,7 +43342,7 @@
         <v>0.01464508407647874</v>
       </c>
       <c r="AM152" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN152">
         <v>0.3981395839245215</v>
@@ -43608,7 +43611,7 @@
         <v>0.01424145384485694</v>
       </c>
       <c r="AM153" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN153">
         <v>0.1335188651800471</v>
@@ -43877,7 +43880,7 @@
         <v>0.008636072468123625</v>
       </c>
       <c r="AM154" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN154">
         <v>0.06745759346973818</v>
@@ -44146,7 +44149,7 @@
         <v>0.01257263323646787</v>
       </c>
       <c r="AM155" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN155">
         <v>0.1015263162251083</v>
@@ -44415,7 +44418,7 @@
         <v>0.01192789588635882</v>
       </c>
       <c r="AM156" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN156">
         <v>0.08086717939318311</v>
@@ -44684,7 +44687,7 @@
         <v>0.01186799249853062</v>
       </c>
       <c r="AM157" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN157">
         <v>0.07213994227012922</v>
@@ -44953,7 +44956,7 @@
         <v>0.01449742321347242</v>
       </c>
       <c r="AM158" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN158">
         <v>0.1112845525409627</v>
@@ -45222,7 +45225,7 @@
         <v>0.01458063833474489</v>
       </c>
       <c r="AM159" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN159">
         <v>0.182085969558268</v>
@@ -45491,7 +45494,7 @@
         <v>0.01203015543742209</v>
       </c>
       <c r="AM160" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN160">
         <v>0.04025259423397862</v>
@@ -45760,7 +45763,7 @@
         <v>0.01488877514152119</v>
       </c>
       <c r="AM161" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN161">
         <v>0.01931426172613477</v>
@@ -46029,7 +46032,7 @@
         <v>0.01132277626110294</v>
       </c>
       <c r="AM162" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN162">
         <v>0.06043490875273809</v>
@@ -46207,6 +46210,275 @@
       </c>
       <c r="CU162">
         <v>-0.7842491568660279</v>
+      </c>
+    </row>
+    <row r="163" spans="10:99">
+      <c r="J163" t="s">
+        <v>260</v>
+      </c>
+      <c r="K163">
+        <v>0.000703728758751021</v>
+      </c>
+      <c r="L163">
+        <v>0.000703728758751021</v>
+      </c>
+      <c r="M163">
+        <v>0.001844867908288306</v>
+      </c>
+      <c r="N163">
+        <v>0.001844867908288306</v>
+      </c>
+      <c r="O163">
+        <v>0.0008269801575081281</v>
+      </c>
+      <c r="P163">
+        <v>0.0008269801575081281</v>
+      </c>
+      <c r="Q163">
+        <v>0.001974121624747216</v>
+      </c>
+      <c r="R163">
+        <v>0.001974121624747216</v>
+      </c>
+      <c r="S163">
+        <v>7.168930874730722</v>
+      </c>
+      <c r="T163">
+        <v>5.775732670587367</v>
+      </c>
+      <c r="U163">
+        <v>0.9918861768682095</v>
+      </c>
+      <c r="V163">
+        <v>0.7986030961865679</v>
+      </c>
+      <c r="W163">
+        <v>0.02482147045576369</v>
+      </c>
+      <c r="X163">
+        <v>0.08058317516553877</v>
+      </c>
+      <c r="Y163">
+        <v>0.08447779265391459</v>
+      </c>
+      <c r="Z163">
+        <v>0.1150513070791521</v>
+      </c>
+      <c r="AA163">
+        <v>0.9993731955592845</v>
+      </c>
+      <c r="AB163">
+        <v>0.9399688530646839</v>
+      </c>
+      <c r="AC163">
+        <v>0.8988027390491377</v>
+      </c>
+      <c r="AD163">
+        <v>0.995903941822592</v>
+      </c>
+      <c r="AE163">
+        <v>0.9160099810646035</v>
+      </c>
+      <c r="AF163">
+        <v>0.8880238535595312</v>
+      </c>
+      <c r="AG163">
+        <v>0.002879813727897104</v>
+      </c>
+      <c r="AH163">
+        <v>0.011946015255795</v>
+      </c>
+      <c r="AI163">
+        <v>0.9993731955592845</v>
+      </c>
+      <c r="AJ163">
+        <v>0.995903941822592</v>
+      </c>
+      <c r="AK163">
+        <v>0.002879813727897104</v>
+      </c>
+      <c r="AL163">
+        <v>0.011946015255795</v>
+      </c>
+      <c r="AM163" t="s">
+        <v>261</v>
+      </c>
+      <c r="AN163">
+        <v>0.04010539941927226</v>
+      </c>
+      <c r="AO163">
+        <v>0.1526173787152363</v>
+      </c>
+      <c r="AP163">
+        <v>-202.727699332</v>
+      </c>
+      <c r="AQ163">
+        <v>-620.3769173120002</v>
+      </c>
+      <c r="AR163">
+        <v>15477.046290668</v>
+      </c>
+      <c r="AS163">
+        <v>31404.76420268797</v>
+      </c>
+      <c r="AT163">
+        <v>15424.193600668</v>
+      </c>
+      <c r="AU163">
+        <v>31404.76420268797</v>
+      </c>
+      <c r="AV163">
+        <v>0.5477046290668002</v>
+      </c>
+      <c r="AW163">
+        <v>2.140476420268797</v>
+      </c>
+      <c r="AX163">
+        <v>3.347790262172285</v>
+      </c>
+      <c r="AY163">
+        <v>4.153854021385402</v>
+      </c>
+      <c r="AZ163">
+        <v>25.5</v>
+      </c>
+      <c r="BA163">
+        <v>40.73333333333333</v>
+      </c>
+      <c r="BB163">
+        <v>0.1319000477781516</v>
+      </c>
+      <c r="BC163">
+        <v>0.05771280138936623</v>
+      </c>
+      <c r="BD163">
+        <v>-862.9910170282442</v>
+      </c>
+      <c r="BE163">
+        <v>-1348.986377938233</v>
+      </c>
+      <c r="BF163">
+        <v>2321</v>
+      </c>
+      <c r="BG163">
+        <v>2243</v>
+      </c>
+      <c r="BH163">
+        <v>620.8736111111111</v>
+      </c>
+      <c r="BI163">
+        <v>2130</v>
+      </c>
+      <c r="BJ163">
+        <v>1343</v>
+      </c>
+      <c r="BK163">
+        <v>4451</v>
+      </c>
+      <c r="BL163">
+        <v>3586</v>
+      </c>
+      <c r="BM163">
+        <v>0</v>
+      </c>
+      <c r="BN163">
+        <v>0</v>
+      </c>
+      <c r="BO163">
+        <v>757</v>
+      </c>
+      <c r="BP163">
+        <v>428</v>
+      </c>
+      <c r="BQ163">
+        <v>0</v>
+      </c>
+      <c r="BR163">
+        <v>0</v>
+      </c>
+      <c r="BS163">
+        <v>1564</v>
+      </c>
+      <c r="BT163">
+        <v>1815</v>
+      </c>
+      <c r="BU163">
+        <v>2130</v>
+      </c>
+      <c r="BV163">
+        <v>1343</v>
+      </c>
+      <c r="BW163">
+        <v>5477.046290668003</v>
+      </c>
+      <c r="BX163">
+        <v>21404.76420268799</v>
+      </c>
+      <c r="BY163">
+        <v>0.04422580835061127</v>
+      </c>
+      <c r="BZ163">
+        <v>0.07276979404395911</v>
+      </c>
+      <c r="CA163">
+        <v>0.09369722042969926</v>
+      </c>
+      <c r="CB163">
+        <v>0.1007005576347439</v>
+      </c>
+      <c r="CC163">
+        <v>0.01139607036115643</v>
+      </c>
+      <c r="CD163">
+        <v>0.01565659926798499</v>
+      </c>
+      <c r="CE163">
+        <v>0.009247515845401861</v>
+      </c>
+      <c r="CF163">
+        <v>0.01430420350422968</v>
+      </c>
+      <c r="CG163">
+        <v>5679.773990000003</v>
+      </c>
+      <c r="CH163">
+        <v>22025.14112</v>
+      </c>
+      <c r="CI163">
+        <v>6542.765007028247</v>
+      </c>
+      <c r="CJ163">
+        <v>23374.12749793823</v>
+      </c>
+      <c r="CK163">
+        <v>0.1373634478132738</v>
+      </c>
+      <c r="CL163">
+        <v>0.1554969557816263</v>
+      </c>
+      <c r="CM163">
+        <v>10000</v>
+      </c>
+      <c r="CO163">
+        <v>0.00362367467454033</v>
+      </c>
+      <c r="CP163">
+        <v>0.05811300496577641</v>
+      </c>
+      <c r="CQ163">
+        <v>3591967.686310469</v>
+      </c>
+      <c r="CR163">
+        <v>8361158.583184867</v>
+      </c>
+      <c r="CS163" s="2">
+        <v>45567.60029945114</v>
+      </c>
+      <c r="CT163">
+        <v>-0.9033952272211854</v>
+      </c>
+      <c r="CU163">
+        <v>-0.63284104473326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update OMNIUSDT.json at 2024-10-02_18-53-52 bestfile_scores 0.003498977923309582 bestfile_sharp 0.13436113751534692
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="406">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -797,6 +797,9 @@
   </si>
   <si>
     <t>FXSUSDT</t>
+  </si>
+  <si>
+    <t>COMBOUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1590,7 +1593,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU163"/>
+  <dimension ref="A1:CU164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2008,7 +2011,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2173,7 +2176,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2289,7 +2292,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2454,7 +2457,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2570,7 +2573,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2735,7 +2738,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2851,7 +2854,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -3016,7 +3019,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3132,7 +3135,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3297,7 +3300,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3413,7 +3416,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3578,7 +3581,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3694,7 +3697,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3859,7 +3862,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3975,7 +3978,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4140,7 +4143,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4256,7 +4259,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4421,7 +4424,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4537,7 +4540,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4702,7 +4705,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4818,7 +4821,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4983,7 +4986,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5099,7 +5102,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5264,7 +5267,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5380,7 +5383,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5545,7 +5548,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5661,7 +5664,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5826,7 +5829,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5942,7 +5945,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6107,7 +6110,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6223,7 +6226,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6388,7 +6391,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6504,7 +6507,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6669,7 +6672,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6785,7 +6788,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6950,7 +6953,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7066,7 +7069,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7231,7 +7234,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7347,7 +7350,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7512,7 +7515,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7628,7 +7631,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7793,7 +7796,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7909,7 +7912,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8074,7 +8077,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8190,7 +8193,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8355,7 +8358,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8471,7 +8474,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8636,7 +8639,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8752,7 +8755,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8917,7 +8920,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -9033,7 +9036,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9198,7 +9201,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9314,7 +9317,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9479,7 +9482,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9595,7 +9598,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9760,7 +9763,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9876,7 +9879,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10041,7 +10044,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10157,7 +10160,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10322,7 +10325,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10438,7 +10441,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10603,7 +10606,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10719,7 +10722,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10884,7 +10887,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -11000,7 +11003,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11165,7 +11168,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11287,7 +11290,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11452,7 +11455,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11574,7 +11577,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11739,7 +11742,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11861,7 +11864,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -12026,7 +12029,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12148,7 +12151,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12313,7 +12316,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12435,7 +12438,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12600,7 +12603,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12722,7 +12725,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12887,7 +12890,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -13009,7 +13012,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13174,7 +13177,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13296,7 +13299,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13461,7 +13464,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13583,7 +13586,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13748,7 +13751,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13870,7 +13873,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -14035,7 +14038,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14157,7 +14160,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14322,7 +14325,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14444,7 +14447,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14609,7 +14612,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14731,7 +14734,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14896,7 +14899,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -15018,7 +15021,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15183,7 +15186,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15305,7 +15308,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15470,7 +15473,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15592,7 +15595,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15757,7 +15760,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15879,7 +15882,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16044,7 +16047,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16166,7 +16169,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16331,7 +16334,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16453,7 +16456,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16618,7 +16621,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16740,7 +16743,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16905,7 +16908,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -17024,7 +17027,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17189,7 +17192,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17305,7 +17308,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17470,7 +17473,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17583,7 +17586,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17748,7 +17751,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17861,7 +17864,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -18026,7 +18029,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18139,7 +18142,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18304,7 +18307,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18417,7 +18420,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18582,7 +18585,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18695,7 +18698,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18860,7 +18863,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18973,7 +18976,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19138,7 +19141,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19251,7 +19254,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19416,7 +19419,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19529,7 +19532,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19694,7 +19697,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19807,7 +19810,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19972,7 +19975,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20085,7 +20088,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20256,7 +20259,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20369,7 +20372,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20540,7 +20543,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20653,7 +20656,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20824,7 +20827,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20937,7 +20940,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21108,7 +21111,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21218,7 +21221,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21389,7 +21392,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21496,7 +21499,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21667,7 +21670,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21771,7 +21774,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21942,7 +21945,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22046,7 +22049,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22217,7 +22220,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22321,7 +22324,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22492,7 +22495,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22596,7 +22599,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22767,7 +22770,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22871,7 +22874,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23042,7 +23045,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23146,7 +23149,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23317,7 +23320,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23418,7 +23421,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23589,7 +23592,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23690,7 +23693,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23861,7 +23864,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23962,7 +23965,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24133,7 +24136,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24234,7 +24237,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24405,7 +24408,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24506,7 +24509,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24677,7 +24680,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24778,7 +24781,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24949,7 +24952,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25050,7 +25053,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25221,7 +25224,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25319,7 +25322,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25490,7 +25493,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25588,7 +25591,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25759,7 +25762,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25857,7 +25860,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -26028,7 +26031,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26126,7 +26129,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26297,7 +26300,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26395,7 +26398,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26566,7 +26569,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26664,7 +26667,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26835,7 +26838,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26933,7 +26936,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27104,7 +27107,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27202,7 +27205,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27373,7 +27376,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27471,7 +27474,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27642,7 +27645,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27740,7 +27743,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27911,7 +27914,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -28009,7 +28012,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28180,7 +28183,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28278,7 +28281,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28449,7 +28452,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28547,7 +28550,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28718,7 +28721,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28816,7 +28819,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28987,7 +28990,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29085,7 +29088,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29256,7 +29259,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29354,7 +29357,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29525,7 +29528,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29623,7 +29626,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29794,7 +29797,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29892,7 +29895,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30063,7 +30066,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30161,7 +30164,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30332,7 +30335,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30430,7 +30433,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30601,7 +30604,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30699,7 +30702,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30870,7 +30873,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30968,7 +30971,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31139,7 +31142,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31237,7 +31240,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31408,7 +31411,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31506,7 +31509,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31677,7 +31680,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31775,7 +31778,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31946,7 +31949,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32044,7 +32047,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32215,7 +32218,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32313,7 +32316,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32484,7 +32487,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32582,7 +32585,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32753,7 +32756,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32851,7 +32854,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -33022,7 +33025,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33120,7 +33123,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33291,7 +33294,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33389,7 +33392,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33560,7 +33563,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33658,7 +33661,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33829,7 +33832,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33927,7 +33930,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34098,7 +34101,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34196,7 +34199,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34367,7 +34370,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34465,7 +34468,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34636,7 +34639,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34734,7 +34737,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34905,7 +34908,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -35003,7 +35006,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35174,7 +35177,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35272,7 +35275,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35443,7 +35446,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35541,7 +35544,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35712,7 +35715,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35810,7 +35813,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35981,7 +35984,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36079,7 +36082,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36250,7 +36253,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36348,7 +36351,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36519,7 +36522,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36617,7 +36620,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36788,7 +36791,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36886,7 +36889,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37057,7 +37060,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37155,7 +37158,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37326,7 +37329,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37424,7 +37427,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37595,7 +37598,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37693,7 +37696,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37864,7 +37867,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37962,7 +37965,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38133,7 +38136,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38231,7 +38234,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38402,7 +38405,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38500,7 +38503,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38671,7 +38674,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38769,7 +38772,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38940,7 +38943,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -39038,7 +39041,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39209,7 +39212,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39307,7 +39310,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39478,7 +39481,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39576,7 +39579,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39747,7 +39750,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39845,7 +39848,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -40016,7 +40019,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40114,7 +40117,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40285,7 +40288,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40383,7 +40386,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40554,7 +40557,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40652,7 +40655,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40823,7 +40826,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40921,7 +40924,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41092,7 +41095,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41190,7 +41193,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41361,7 +41364,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41459,7 +41462,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41630,7 +41633,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41728,7 +41731,7 @@
         <v>0.01422843894993598</v>
       </c>
       <c r="AM146" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN146">
         <v>0.3570285831928028</v>
@@ -41997,7 +42000,7 @@
         <v>0.01287672421329242</v>
       </c>
       <c r="AM147" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN147">
         <v>0.1138938544209247</v>
@@ -42266,7 +42269,7 @@
         <v>0.01129449859594168</v>
       </c>
       <c r="AM148" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN148">
         <v>0.01929055864963264</v>
@@ -42535,7 +42538,7 @@
         <v>0.01268293743279473</v>
       </c>
       <c r="AM149" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN149">
         <v>0.02713293780673231</v>
@@ -42804,7 +42807,7 @@
         <v>0.006815186142663594</v>
       </c>
       <c r="AM150" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN150">
         <v>0.06060596226028341</v>
@@ -43073,7 +43076,7 @@
         <v>0.01172718359151741</v>
       </c>
       <c r="AM151" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN151">
         <v>0.09142880750409497</v>
@@ -43342,7 +43345,7 @@
         <v>0.01464508407647874</v>
       </c>
       <c r="AM152" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN152">
         <v>0.3981395839245215</v>
@@ -43611,7 +43614,7 @@
         <v>0.01424145384485694</v>
       </c>
       <c r="AM153" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN153">
         <v>0.1335188651800471</v>
@@ -43880,7 +43883,7 @@
         <v>0.008636072468123625</v>
       </c>
       <c r="AM154" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN154">
         <v>0.06745759346973818</v>
@@ -44149,7 +44152,7 @@
         <v>0.01257263323646787</v>
       </c>
       <c r="AM155" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN155">
         <v>0.1015263162251083</v>
@@ -44418,7 +44421,7 @@
         <v>0.01192789588635882</v>
       </c>
       <c r="AM156" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN156">
         <v>0.08086717939318311</v>
@@ -44687,7 +44690,7 @@
         <v>0.01186799249853062</v>
       </c>
       <c r="AM157" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN157">
         <v>0.07213994227012922</v>
@@ -44956,7 +44959,7 @@
         <v>0.01449742321347242</v>
       </c>
       <c r="AM158" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN158">
         <v>0.1112845525409627</v>
@@ -45225,7 +45228,7 @@
         <v>0.01458063833474489</v>
       </c>
       <c r="AM159" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN159">
         <v>0.182085969558268</v>
@@ -45494,7 +45497,7 @@
         <v>0.01203015543742209</v>
       </c>
       <c r="AM160" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN160">
         <v>0.04025259423397862</v>
@@ -45763,7 +45766,7 @@
         <v>0.01488877514152119</v>
       </c>
       <c r="AM161" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN161">
         <v>0.01931426172613477</v>
@@ -46032,7 +46035,7 @@
         <v>0.01132277626110294</v>
       </c>
       <c r="AM162" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN162">
         <v>0.06043490875273809</v>
@@ -46301,7 +46304,7 @@
         <v>0.011946015255795</v>
       </c>
       <c r="AM163" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN163">
         <v>0.04010539941927226</v>
@@ -46479,6 +46482,275 @@
       </c>
       <c r="CU163">
         <v>-0.63284104473326</v>
+      </c>
+    </row>
+    <row r="164" spans="10:99">
+      <c r="J164" t="s">
+        <v>261</v>
+      </c>
+      <c r="K164">
+        <v>0.0009201569956158728</v>
+      </c>
+      <c r="L164">
+        <v>0.0009201569956158728</v>
+      </c>
+      <c r="M164">
+        <v>0.003314448984685914</v>
+      </c>
+      <c r="N164">
+        <v>0.003314448984685914</v>
+      </c>
+      <c r="O164">
+        <v>0.0007260192702664315</v>
+      </c>
+      <c r="P164">
+        <v>0.0007260192702664315</v>
+      </c>
+      <c r="Q164">
+        <v>0.003462474134841331</v>
+      </c>
+      <c r="R164">
+        <v>0.003462474134841331</v>
+      </c>
+      <c r="S164">
+        <v>5.546682469180824</v>
+      </c>
+      <c r="T164">
+        <v>7.99797150419232</v>
+      </c>
+      <c r="U164">
+        <v>0.9881240611752308</v>
+      </c>
+      <c r="V164">
+        <v>0.6346115047758485</v>
+      </c>
+      <c r="W164">
+        <v>0.086871319500276</v>
+      </c>
+      <c r="X164">
+        <v>0.08929699777390226</v>
+      </c>
+      <c r="Y164">
+        <v>0.1845818072682003</v>
+      </c>
+      <c r="Z164">
+        <v>0.2332382135535822</v>
+      </c>
+      <c r="AA164">
+        <v>0.9980127790748595</v>
+      </c>
+      <c r="AB164">
+        <v>0.8411333506540203</v>
+      </c>
+      <c r="AC164">
+        <v>0.8392151998275809</v>
+      </c>
+      <c r="AD164">
+        <v>0.9981602813714707</v>
+      </c>
+      <c r="AE164">
+        <v>0.8160900108443542</v>
+      </c>
+      <c r="AF164">
+        <v>0.7734616286360604</v>
+      </c>
+      <c r="AG164">
+        <v>0.01010546235187185</v>
+      </c>
+      <c r="AH164">
+        <v>0.01042329697569886</v>
+      </c>
+      <c r="AI164">
+        <v>0.9980127790748595</v>
+      </c>
+      <c r="AJ164">
+        <v>0.9981602813714707</v>
+      </c>
+      <c r="AK164">
+        <v>0.01010546235187185</v>
+      </c>
+      <c r="AL164">
+        <v>0.01042329697569886</v>
+      </c>
+      <c r="AM164" t="s">
+        <v>262</v>
+      </c>
+      <c r="AN164">
+        <v>0.07892284657150772</v>
+      </c>
+      <c r="AO164">
+        <v>0.1374818838500218</v>
+      </c>
+      <c r="AP164">
+        <v>-136.034424948</v>
+      </c>
+      <c r="AQ164">
+        <v>-578.754721182</v>
+      </c>
+      <c r="AR164">
+        <v>15657.56359505204</v>
+      </c>
+      <c r="AS164">
+        <v>50184.31592881793</v>
+      </c>
+      <c r="AT164">
+        <v>15515.64303505204</v>
+      </c>
+      <c r="AU164">
+        <v>50184.31592881793</v>
+      </c>
+      <c r="AV164">
+        <v>0.5657563595052042</v>
+      </c>
+      <c r="AW164">
+        <v>4.018431592881793</v>
+      </c>
+      <c r="AX164">
+        <v>4.328049081267728</v>
+      </c>
+      <c r="AY164">
+        <v>2.999106379339833</v>
+      </c>
+      <c r="AZ164">
+        <v>25.61666666666667</v>
+      </c>
+      <c r="BA164">
+        <v>40.1</v>
+      </c>
+      <c r="BB164">
+        <v>0.1160715581269541</v>
+      </c>
+      <c r="BC164">
+        <v>0.03819837556230792</v>
+      </c>
+      <c r="BD164">
+        <v>-760.7764582364479</v>
+      </c>
+      <c r="BE164">
+        <v>-1618.923322854568</v>
+      </c>
+      <c r="BF164">
+        <v>848</v>
+      </c>
+      <c r="BG164">
+        <v>1267</v>
+      </c>
+      <c r="BH164">
+        <v>487.4986111111111</v>
+      </c>
+      <c r="BI164">
+        <v>1856</v>
+      </c>
+      <c r="BJ164">
+        <v>2632</v>
+      </c>
+      <c r="BK164">
+        <v>2704</v>
+      </c>
+      <c r="BL164">
+        <v>3899</v>
+      </c>
+      <c r="BM164">
+        <v>0</v>
+      </c>
+      <c r="BN164">
+        <v>0</v>
+      </c>
+      <c r="BO164">
+        <v>234</v>
+      </c>
+      <c r="BP164">
+        <v>412</v>
+      </c>
+      <c r="BQ164">
+        <v>0</v>
+      </c>
+      <c r="BR164">
+        <v>0</v>
+      </c>
+      <c r="BS164">
+        <v>614</v>
+      </c>
+      <c r="BT164">
+        <v>855</v>
+      </c>
+      <c r="BU164">
+        <v>1856</v>
+      </c>
+      <c r="BV164">
+        <v>2632</v>
+      </c>
+      <c r="BW164">
+        <v>5657.563595052014</v>
+      </c>
+      <c r="BX164">
+        <v>40184.31592881796</v>
+      </c>
+      <c r="BY164">
+        <v>0.09638325967538793</v>
+      </c>
+      <c r="BZ164">
+        <v>0.07344103697111412</v>
+      </c>
+      <c r="CA164">
+        <v>0.2226910572543913</v>
+      </c>
+      <c r="CB164">
+        <v>0.1858707031068316</v>
+      </c>
+      <c r="CC164">
+        <v>0.01641712395957907</v>
+      </c>
+      <c r="CD164">
+        <v>0.01330922199856043</v>
+      </c>
+      <c r="CE164">
+        <v>0.01523761234266956</v>
+      </c>
+      <c r="CF164">
+        <v>0.01237925259482096</v>
+      </c>
+      <c r="CG164">
+        <v>5793.598020000014</v>
+      </c>
+      <c r="CH164">
+        <v>40763.07064999996</v>
+      </c>
+      <c r="CI164">
+        <v>6554.374478236462</v>
+      </c>
+      <c r="CJ164">
+        <v>42381.99397285453</v>
+      </c>
+      <c r="CK164">
+        <v>0.08090285344291481</v>
+      </c>
+      <c r="CL164">
+        <v>0.2065055817984873</v>
+      </c>
+      <c r="CM164">
+        <v>10000</v>
+      </c>
+      <c r="CO164">
+        <v>0.02324587642081873</v>
+      </c>
+      <c r="CP164">
+        <v>0.0416203743269806</v>
+      </c>
+      <c r="CQ164">
+        <v>4642874.124941684</v>
+      </c>
+      <c r="CR164">
+        <v>25642029.77414152</v>
+      </c>
+      <c r="CS164" s="2">
+        <v>45567.75898843661</v>
+      </c>
+      <c r="CT164">
+        <v>-0.6843531623931977</v>
+      </c>
+      <c r="CU164">
+        <v>-0.4488480053756655</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update SYSUSDT.json at 2024-10-02_19-21-16 bestfile_scores 0.010180040317356857 bestfile_sharp 0.33614397602227825
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="407">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -800,6 +800,9 @@
   </si>
   <si>
     <t>COMBOUSDT</t>
+  </si>
+  <si>
+    <t>OMNIUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1593,7 +1596,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU164"/>
+  <dimension ref="A1:CU165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2011,7 +2014,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2176,7 +2179,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2292,7 +2295,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2457,7 +2460,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2573,7 +2576,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2738,7 +2741,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2854,7 +2857,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -3019,7 +3022,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3135,7 +3138,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3300,7 +3303,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3416,7 +3419,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3581,7 +3584,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3697,7 +3700,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3862,7 +3865,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3978,7 +3981,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4143,7 +4146,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4259,7 +4262,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4424,7 +4427,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4540,7 +4543,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4705,7 +4708,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4821,7 +4824,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4986,7 +4989,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5102,7 +5105,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5267,7 +5270,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5383,7 +5386,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5548,7 +5551,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5664,7 +5667,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5829,7 +5832,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5945,7 +5948,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6110,7 +6113,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6226,7 +6229,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6391,7 +6394,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6507,7 +6510,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6672,7 +6675,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6788,7 +6791,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6953,7 +6956,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7069,7 +7072,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7234,7 +7237,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7350,7 +7353,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7515,7 +7518,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7631,7 +7634,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7796,7 +7799,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7912,7 +7915,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8077,7 +8080,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8193,7 +8196,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8358,7 +8361,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8474,7 +8477,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8639,7 +8642,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8755,7 +8758,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8920,7 +8923,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -9036,7 +9039,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9201,7 +9204,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9317,7 +9320,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9482,7 +9485,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9598,7 +9601,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9763,7 +9766,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9879,7 +9882,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10044,7 +10047,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10160,7 +10163,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10325,7 +10328,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10441,7 +10444,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10606,7 +10609,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10722,7 +10725,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10887,7 +10890,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -11003,7 +11006,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11168,7 +11171,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11290,7 +11293,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11455,7 +11458,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11577,7 +11580,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11742,7 +11745,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11864,7 +11867,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -12029,7 +12032,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12151,7 +12154,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12316,7 +12319,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12438,7 +12441,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12603,7 +12606,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12725,7 +12728,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12890,7 +12893,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -13012,7 +13015,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13177,7 +13180,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13299,7 +13302,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13464,7 +13467,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13586,7 +13589,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13751,7 +13754,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13873,7 +13876,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -14038,7 +14041,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14160,7 +14163,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14325,7 +14328,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14447,7 +14450,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14612,7 +14615,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14734,7 +14737,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14899,7 +14902,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -15021,7 +15024,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15186,7 +15189,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15308,7 +15311,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15473,7 +15476,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15595,7 +15598,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15760,7 +15763,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15882,7 +15885,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16047,7 +16050,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16169,7 +16172,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16334,7 +16337,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16456,7 +16459,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16621,7 +16624,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16743,7 +16746,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16908,7 +16911,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -17027,7 +17030,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17192,7 +17195,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17308,7 +17311,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17473,7 +17476,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17586,7 +17589,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17751,7 +17754,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17864,7 +17867,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -18029,7 +18032,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18142,7 +18145,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18307,7 +18310,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18420,7 +18423,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18585,7 +18588,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18698,7 +18701,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18863,7 +18866,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18976,7 +18979,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19141,7 +19144,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19254,7 +19257,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19419,7 +19422,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19532,7 +19535,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19697,7 +19700,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19810,7 +19813,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19975,7 +19978,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20088,7 +20091,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20259,7 +20262,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20372,7 +20375,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20543,7 +20546,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20656,7 +20659,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20827,7 +20830,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20940,7 +20943,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21111,7 +21114,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21221,7 +21224,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21392,7 +21395,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21499,7 +21502,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21670,7 +21673,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21774,7 +21777,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21945,7 +21948,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22049,7 +22052,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22220,7 +22223,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22324,7 +22327,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22495,7 +22498,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22599,7 +22602,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22770,7 +22773,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22874,7 +22877,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23045,7 +23048,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23149,7 +23152,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23320,7 +23323,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23421,7 +23424,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23592,7 +23595,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23693,7 +23696,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23864,7 +23867,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23965,7 +23968,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24136,7 +24139,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24237,7 +24240,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24408,7 +24411,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24509,7 +24512,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24680,7 +24683,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24781,7 +24784,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24952,7 +24955,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25053,7 +25056,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25224,7 +25227,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25322,7 +25325,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25493,7 +25496,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25591,7 +25594,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25762,7 +25765,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25860,7 +25863,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -26031,7 +26034,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26129,7 +26132,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26300,7 +26303,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26398,7 +26401,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26569,7 +26572,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26667,7 +26670,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26838,7 +26841,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26936,7 +26939,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27107,7 +27110,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27205,7 +27208,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27376,7 +27379,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27474,7 +27477,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27645,7 +27648,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27743,7 +27746,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27914,7 +27917,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -28012,7 +28015,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28183,7 +28186,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28281,7 +28284,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28452,7 +28455,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28550,7 +28553,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28721,7 +28724,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28819,7 +28822,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28990,7 +28993,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29088,7 +29091,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29259,7 +29262,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29357,7 +29360,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29528,7 +29531,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29626,7 +29629,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29797,7 +29800,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29895,7 +29898,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30066,7 +30069,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30164,7 +30167,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30335,7 +30338,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30433,7 +30436,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30604,7 +30607,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30702,7 +30705,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30873,7 +30876,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30971,7 +30974,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31142,7 +31145,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31240,7 +31243,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31411,7 +31414,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31509,7 +31512,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31680,7 +31683,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31778,7 +31781,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31949,7 +31952,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32047,7 +32050,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32218,7 +32221,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32316,7 +32319,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32487,7 +32490,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32585,7 +32588,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32756,7 +32759,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32854,7 +32857,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -33025,7 +33028,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33123,7 +33126,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33294,7 +33297,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33392,7 +33395,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33563,7 +33566,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33661,7 +33664,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33832,7 +33835,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33930,7 +33933,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34101,7 +34104,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34199,7 +34202,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34370,7 +34373,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34468,7 +34471,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34639,7 +34642,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34737,7 +34740,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34908,7 +34911,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -35006,7 +35009,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35177,7 +35180,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35275,7 +35278,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35446,7 +35449,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35544,7 +35547,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35715,7 +35718,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35813,7 +35816,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35984,7 +35987,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36082,7 +36085,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36253,7 +36256,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36351,7 +36354,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36522,7 +36525,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36620,7 +36623,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36791,7 +36794,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36889,7 +36892,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37060,7 +37063,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37158,7 +37161,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37329,7 +37332,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37427,7 +37430,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37598,7 +37601,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37696,7 +37699,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37867,7 +37870,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37965,7 +37968,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38136,7 +38139,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38234,7 +38237,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38405,7 +38408,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38503,7 +38506,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38674,7 +38677,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38772,7 +38775,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38943,7 +38946,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -39041,7 +39044,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39212,7 +39215,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39310,7 +39313,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39481,7 +39484,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39579,7 +39582,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39750,7 +39753,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39848,7 +39851,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -40019,7 +40022,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40117,7 +40120,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40288,7 +40291,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40386,7 +40389,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40557,7 +40560,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40655,7 +40658,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40826,7 +40829,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40924,7 +40927,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41095,7 +41098,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41193,7 +41196,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41364,7 +41367,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41462,7 +41465,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41633,7 +41636,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41731,7 +41734,7 @@
         <v>0.01422843894993598</v>
       </c>
       <c r="AM146" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN146">
         <v>0.3570285831928028</v>
@@ -42000,7 +42003,7 @@
         <v>0.01287672421329242</v>
       </c>
       <c r="AM147" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN147">
         <v>0.1138938544209247</v>
@@ -42269,7 +42272,7 @@
         <v>0.01129449859594168</v>
       </c>
       <c r="AM148" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN148">
         <v>0.01929055864963264</v>
@@ -42538,7 +42541,7 @@
         <v>0.01268293743279473</v>
       </c>
       <c r="AM149" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN149">
         <v>0.02713293780673231</v>
@@ -42807,7 +42810,7 @@
         <v>0.006815186142663594</v>
       </c>
       <c r="AM150" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN150">
         <v>0.06060596226028341</v>
@@ -43076,7 +43079,7 @@
         <v>0.01172718359151741</v>
       </c>
       <c r="AM151" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN151">
         <v>0.09142880750409497</v>
@@ -43345,7 +43348,7 @@
         <v>0.01464508407647874</v>
       </c>
       <c r="AM152" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN152">
         <v>0.3981395839245215</v>
@@ -43614,7 +43617,7 @@
         <v>0.01424145384485694</v>
       </c>
       <c r="AM153" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN153">
         <v>0.1335188651800471</v>
@@ -43883,7 +43886,7 @@
         <v>0.008636072468123625</v>
       </c>
       <c r="AM154" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN154">
         <v>0.06745759346973818</v>
@@ -44152,7 +44155,7 @@
         <v>0.01257263323646787</v>
       </c>
       <c r="AM155" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN155">
         <v>0.1015263162251083</v>
@@ -44421,7 +44424,7 @@
         <v>0.01192789588635882</v>
       </c>
       <c r="AM156" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN156">
         <v>0.08086717939318311</v>
@@ -44690,7 +44693,7 @@
         <v>0.01186799249853062</v>
       </c>
       <c r="AM157" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN157">
         <v>0.07213994227012922</v>
@@ -44959,7 +44962,7 @@
         <v>0.01449742321347242</v>
       </c>
       <c r="AM158" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN158">
         <v>0.1112845525409627</v>
@@ -45228,7 +45231,7 @@
         <v>0.01458063833474489</v>
       </c>
       <c r="AM159" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN159">
         <v>0.182085969558268</v>
@@ -45497,7 +45500,7 @@
         <v>0.01203015543742209</v>
       </c>
       <c r="AM160" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN160">
         <v>0.04025259423397862</v>
@@ -45766,7 +45769,7 @@
         <v>0.01488877514152119</v>
       </c>
       <c r="AM161" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN161">
         <v>0.01931426172613477</v>
@@ -46035,7 +46038,7 @@
         <v>0.01132277626110294</v>
       </c>
       <c r="AM162" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN162">
         <v>0.06043490875273809</v>
@@ -46304,7 +46307,7 @@
         <v>0.011946015255795</v>
       </c>
       <c r="AM163" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN163">
         <v>0.04010539941927226</v>
@@ -46573,7 +46576,7 @@
         <v>0.01042329697569886</v>
       </c>
       <c r="AM164" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN164">
         <v>0.07892284657150772</v>
@@ -46751,6 +46754,275 @@
       </c>
       <c r="CU164">
         <v>-0.4488480053756655</v>
+      </c>
+    </row>
+    <row r="165" spans="10:99">
+      <c r="J165" t="s">
+        <v>262</v>
+      </c>
+      <c r="K165">
+        <v>0.001810106199435557</v>
+      </c>
+      <c r="L165">
+        <v>0.001810106199435557</v>
+      </c>
+      <c r="M165">
+        <v>0.004421816445275395</v>
+      </c>
+      <c r="N165">
+        <v>0.004421816445275395</v>
+      </c>
+      <c r="O165">
+        <v>0.001443954780242129</v>
+      </c>
+      <c r="P165">
+        <v>0.001443954780242129</v>
+      </c>
+      <c r="Q165">
+        <v>0.006320034268285246</v>
+      </c>
+      <c r="R165">
+        <v>0.006320034268285246</v>
+      </c>
+      <c r="S165">
+        <v>27.10624777043115</v>
+      </c>
+      <c r="T165">
+        <v>23.98227959415625</v>
+      </c>
+      <c r="U165">
+        <v>0.9999890613075754</v>
+      </c>
+      <c r="V165">
+        <v>0.801501972718889</v>
+      </c>
+      <c r="W165">
+        <v>0.09322124194369853</v>
+      </c>
+      <c r="X165">
+        <v>0.08563076108503589</v>
+      </c>
+      <c r="Y165">
+        <v>0.1242056599068399</v>
+      </c>
+      <c r="Z165">
+        <v>0.1106118444965417</v>
+      </c>
+      <c r="AA165">
+        <v>0.9978108206567343</v>
+      </c>
+      <c r="AB165">
+        <v>0.8920415402294454</v>
+      </c>
+      <c r="AC165">
+        <v>0.902181732192429</v>
+      </c>
+      <c r="AD165">
+        <v>0.9972376649631125</v>
+      </c>
+      <c r="AE165">
+        <v>0.8759694989305363</v>
+      </c>
+      <c r="AF165">
+        <v>0.8898180956527305</v>
+      </c>
+      <c r="AG165">
+        <v>0.0114398795295447</v>
+      </c>
+      <c r="AH165">
+        <v>0.01136039741545648</v>
+      </c>
+      <c r="AI165">
+        <v>0.9978108206567343</v>
+      </c>
+      <c r="AJ165">
+        <v>0.9972376649631125</v>
+      </c>
+      <c r="AK165">
+        <v>0.0114398795295447</v>
+      </c>
+      <c r="AL165">
+        <v>0.01136039741545648</v>
+      </c>
+      <c r="AM165" t="s">
+        <v>263</v>
+      </c>
+      <c r="AN165">
+        <v>0.06727405626523143</v>
+      </c>
+      <c r="AO165">
+        <v>0.1159721027407887</v>
+      </c>
+      <c r="AP165">
+        <v>-240.322717888</v>
+      </c>
+      <c r="AQ165">
+        <v>-468.8080221980001</v>
+      </c>
+      <c r="AR165">
+        <v>13535.97003211203</v>
+      </c>
+      <c r="AS165">
+        <v>20931.03194780203</v>
+      </c>
+      <c r="AT165">
+        <v>13533.74306211203</v>
+      </c>
+      <c r="AU165">
+        <v>20931.03194780203</v>
+      </c>
+      <c r="AV165">
+        <v>0.3535970032112035</v>
+      </c>
+      <c r="AW165">
+        <v>1.093103194780203</v>
+      </c>
+      <c r="AX165">
+        <v>0.8854860039673793</v>
+      </c>
+      <c r="AY165">
+        <v>0.9975253280186015</v>
+      </c>
+      <c r="AZ165">
+        <v>39.78333333333333</v>
+      </c>
+      <c r="BA165">
+        <v>58.55</v>
+      </c>
+      <c r="BB165">
+        <v>0.03167231218472315</v>
+      </c>
+      <c r="BC165">
+        <v>0.03527881138271168</v>
+      </c>
+      <c r="BD165">
+        <v>-123.5159588886229</v>
+      </c>
+      <c r="BE165">
+        <v>-416.8798289494947</v>
+      </c>
+      <c r="BF165">
+        <v>1158</v>
+      </c>
+      <c r="BG165">
+        <v>1288</v>
+      </c>
+      <c r="BH165">
+        <v>167.4152777777778</v>
+      </c>
+      <c r="BI165">
+        <v>3380</v>
+      </c>
+      <c r="BJ165">
+        <v>2727</v>
+      </c>
+      <c r="BK165">
+        <v>4538</v>
+      </c>
+      <c r="BL165">
+        <v>4015</v>
+      </c>
+      <c r="BM165">
+        <v>0</v>
+      </c>
+      <c r="BN165">
+        <v>0</v>
+      </c>
+      <c r="BO165">
+        <v>992</v>
+      </c>
+      <c r="BP165">
+        <v>679</v>
+      </c>
+      <c r="BQ165">
+        <v>0</v>
+      </c>
+      <c r="BR165">
+        <v>0</v>
+      </c>
+      <c r="BS165">
+        <v>166</v>
+      </c>
+      <c r="BT165">
+        <v>609</v>
+      </c>
+      <c r="BU165">
+        <v>3380</v>
+      </c>
+      <c r="BV165">
+        <v>2727</v>
+      </c>
+      <c r="BW165">
+        <v>3535.970032112009</v>
+      </c>
+      <c r="BX165">
+        <v>10931.03194780202</v>
+      </c>
+      <c r="BY165">
+        <v>0.1026286213667018</v>
+      </c>
+      <c r="BZ165">
+        <v>0.0776133637307516</v>
+      </c>
+      <c r="CA165">
+        <v>0.1415922883057632</v>
+      </c>
+      <c r="CB165">
+        <v>0.09924614269333266</v>
+      </c>
+      <c r="CC165">
+        <v>0.01003013146683454</v>
+      </c>
+      <c r="CD165">
+        <v>0.009096707201308134</v>
+      </c>
+      <c r="CE165">
+        <v>0.01745311849162336</v>
+      </c>
+      <c r="CF165">
+        <v>0.01348032641111211</v>
+      </c>
+      <c r="CG165">
+        <v>3776.292750000009</v>
+      </c>
+      <c r="CH165">
+        <v>11399.83997000002</v>
+      </c>
+      <c r="CI165">
+        <v>3899.808708888631</v>
+      </c>
+      <c r="CJ165">
+        <v>11816.71979894952</v>
+      </c>
+      <c r="CK165">
+        <v>0.1343611375153469</v>
+      </c>
+      <c r="CL165">
+        <v>0.2667006619437886</v>
+      </c>
+      <c r="CM165">
+        <v>10000</v>
+      </c>
+      <c r="CO165">
+        <v>0.04304553371485444</v>
+      </c>
+      <c r="CP165">
+        <v>0.07962179646678279</v>
+      </c>
+      <c r="CQ165">
+        <v>5314146.879435077</v>
+      </c>
+      <c r="CR165">
+        <v>8511259.049831672</v>
+      </c>
+      <c r="CS165" s="2">
+        <v>45567.78744035306</v>
+      </c>
+      <c r="CT165">
+        <v>-0.5872903381105973</v>
+      </c>
+      <c r="CU165">
+        <v>-0.3596428817468907</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update GUSDT.json at 2024-10-02_19-47-03 bestfile_scores 0.005363301402332094 bestfile_sharp 0.3616240190195784
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="408">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -803,6 +803,9 @@
   </si>
   <si>
     <t>OMNIUSDT</t>
+  </si>
+  <si>
+    <t>SYSUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1596,7 +1599,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU165"/>
+  <dimension ref="A1:CU166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2014,7 +2017,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2179,7 +2182,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2295,7 +2298,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2460,7 +2463,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2576,7 +2579,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2741,7 +2744,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2857,7 +2860,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -3022,7 +3025,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3138,7 +3141,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3303,7 +3306,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3419,7 +3422,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3584,7 +3587,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3700,7 +3703,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3865,7 +3868,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3981,7 +3984,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4146,7 +4149,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4262,7 +4265,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4427,7 +4430,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4543,7 +4546,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4708,7 +4711,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4824,7 +4827,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4989,7 +4992,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5105,7 +5108,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5270,7 +5273,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5386,7 +5389,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5551,7 +5554,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5667,7 +5670,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5832,7 +5835,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5948,7 +5951,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6113,7 +6116,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6229,7 +6232,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6394,7 +6397,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6510,7 +6513,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6675,7 +6678,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6791,7 +6794,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6956,7 +6959,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7072,7 +7075,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7237,7 +7240,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7353,7 +7356,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7518,7 +7521,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7634,7 +7637,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7799,7 +7802,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7915,7 +7918,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8080,7 +8083,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8196,7 +8199,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8361,7 +8364,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8477,7 +8480,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8642,7 +8645,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8758,7 +8761,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8923,7 +8926,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -9039,7 +9042,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9204,7 +9207,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9320,7 +9323,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9485,7 +9488,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9601,7 +9604,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9766,7 +9769,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9882,7 +9885,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10047,7 +10050,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10163,7 +10166,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10328,7 +10331,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10444,7 +10447,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10609,7 +10612,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10725,7 +10728,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10890,7 +10893,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -11006,7 +11009,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11171,7 +11174,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11293,7 +11296,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11458,7 +11461,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11580,7 +11583,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11745,7 +11748,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11867,7 +11870,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -12032,7 +12035,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12154,7 +12157,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12319,7 +12322,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12441,7 +12444,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12606,7 +12609,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12728,7 +12731,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12893,7 +12896,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -13015,7 +13018,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13180,7 +13183,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13302,7 +13305,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13467,7 +13470,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13589,7 +13592,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13754,7 +13757,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13876,7 +13879,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -14041,7 +14044,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14163,7 +14166,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14328,7 +14331,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14450,7 +14453,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14615,7 +14618,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14737,7 +14740,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14902,7 +14905,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -15024,7 +15027,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15189,7 +15192,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15311,7 +15314,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15476,7 +15479,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15598,7 +15601,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15763,7 +15766,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15885,7 +15888,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16050,7 +16053,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16172,7 +16175,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16337,7 +16340,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16459,7 +16462,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16624,7 +16627,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16746,7 +16749,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16911,7 +16914,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -17030,7 +17033,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17195,7 +17198,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17311,7 +17314,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17476,7 +17479,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17589,7 +17592,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17754,7 +17757,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17867,7 +17870,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -18032,7 +18035,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18145,7 +18148,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18310,7 +18313,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18423,7 +18426,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18588,7 +18591,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18701,7 +18704,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18866,7 +18869,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18979,7 +18982,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19144,7 +19147,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19257,7 +19260,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19422,7 +19425,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19535,7 +19538,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19700,7 +19703,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19813,7 +19816,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19978,7 +19981,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20091,7 +20094,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20262,7 +20265,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20375,7 +20378,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20546,7 +20549,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20659,7 +20662,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20830,7 +20833,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20943,7 +20946,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21114,7 +21117,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21224,7 +21227,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21395,7 +21398,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21502,7 +21505,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21673,7 +21676,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21777,7 +21780,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21948,7 +21951,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22052,7 +22055,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22223,7 +22226,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22327,7 +22330,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22498,7 +22501,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22602,7 +22605,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22773,7 +22776,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22877,7 +22880,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23048,7 +23051,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23152,7 +23155,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23323,7 +23326,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23424,7 +23427,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23595,7 +23598,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23696,7 +23699,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23867,7 +23870,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23968,7 +23971,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24139,7 +24142,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24240,7 +24243,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24411,7 +24414,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24512,7 +24515,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24683,7 +24686,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24784,7 +24787,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24955,7 +24958,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25056,7 +25059,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25227,7 +25230,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25325,7 +25328,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25496,7 +25499,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25594,7 +25597,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25765,7 +25768,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25863,7 +25866,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -26034,7 +26037,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26132,7 +26135,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26303,7 +26306,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26401,7 +26404,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26572,7 +26575,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26670,7 +26673,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26841,7 +26844,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26939,7 +26942,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27110,7 +27113,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27208,7 +27211,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27379,7 +27382,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27477,7 +27480,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27648,7 +27651,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27746,7 +27749,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27917,7 +27920,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -28015,7 +28018,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28186,7 +28189,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28284,7 +28287,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28455,7 +28458,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28553,7 +28556,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28724,7 +28727,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28822,7 +28825,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28993,7 +28996,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29091,7 +29094,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29262,7 +29265,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29360,7 +29363,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29531,7 +29534,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29629,7 +29632,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29800,7 +29803,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29898,7 +29901,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30069,7 +30072,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30167,7 +30170,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30338,7 +30341,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30436,7 +30439,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30607,7 +30610,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30705,7 +30708,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30876,7 +30879,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30974,7 +30977,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31145,7 +31148,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31243,7 +31246,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31414,7 +31417,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31512,7 +31515,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31683,7 +31686,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31781,7 +31784,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31952,7 +31955,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32050,7 +32053,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32221,7 +32224,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32319,7 +32322,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32490,7 +32493,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32588,7 +32591,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32759,7 +32762,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32857,7 +32860,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -33028,7 +33031,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33126,7 +33129,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33297,7 +33300,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33395,7 +33398,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33566,7 +33569,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33664,7 +33667,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33835,7 +33838,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33933,7 +33936,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34104,7 +34107,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34202,7 +34205,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34373,7 +34376,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34471,7 +34474,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34642,7 +34645,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34740,7 +34743,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34911,7 +34914,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -35009,7 +35012,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35180,7 +35183,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35278,7 +35281,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35449,7 +35452,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35547,7 +35550,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35718,7 +35721,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35816,7 +35819,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35987,7 +35990,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36085,7 +36088,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36256,7 +36259,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36354,7 +36357,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36525,7 +36528,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36623,7 +36626,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36794,7 +36797,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36892,7 +36895,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37063,7 +37066,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37161,7 +37164,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37332,7 +37335,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37430,7 +37433,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37601,7 +37604,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37699,7 +37702,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37870,7 +37873,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37968,7 +37971,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38139,7 +38142,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38237,7 +38240,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38408,7 +38411,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38506,7 +38509,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38677,7 +38680,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38775,7 +38778,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38946,7 +38949,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -39044,7 +39047,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39215,7 +39218,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39313,7 +39316,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39484,7 +39487,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39582,7 +39585,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39753,7 +39756,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39851,7 +39854,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -40022,7 +40025,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40120,7 +40123,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40291,7 +40294,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40389,7 +40392,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40560,7 +40563,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40658,7 +40661,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40829,7 +40832,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40927,7 +40930,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41098,7 +41101,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41196,7 +41199,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41367,7 +41370,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41465,7 +41468,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41636,7 +41639,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41734,7 +41737,7 @@
         <v>0.01422843894993598</v>
       </c>
       <c r="AM146" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN146">
         <v>0.3570285831928028</v>
@@ -42003,7 +42006,7 @@
         <v>0.01287672421329242</v>
       </c>
       <c r="AM147" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN147">
         <v>0.1138938544209247</v>
@@ -42272,7 +42275,7 @@
         <v>0.01129449859594168</v>
       </c>
       <c r="AM148" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN148">
         <v>0.01929055864963264</v>
@@ -42541,7 +42544,7 @@
         <v>0.01268293743279473</v>
       </c>
       <c r="AM149" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN149">
         <v>0.02713293780673231</v>
@@ -42810,7 +42813,7 @@
         <v>0.006815186142663594</v>
       </c>
       <c r="AM150" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN150">
         <v>0.06060596226028341</v>
@@ -43079,7 +43082,7 @@
         <v>0.01172718359151741</v>
       </c>
       <c r="AM151" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN151">
         <v>0.09142880750409497</v>
@@ -43348,7 +43351,7 @@
         <v>0.01464508407647874</v>
       </c>
       <c r="AM152" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN152">
         <v>0.3981395839245215</v>
@@ -43617,7 +43620,7 @@
         <v>0.01424145384485694</v>
       </c>
       <c r="AM153" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN153">
         <v>0.1335188651800471</v>
@@ -43886,7 +43889,7 @@
         <v>0.008636072468123625</v>
       </c>
       <c r="AM154" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN154">
         <v>0.06745759346973818</v>
@@ -44155,7 +44158,7 @@
         <v>0.01257263323646787</v>
       </c>
       <c r="AM155" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN155">
         <v>0.1015263162251083</v>
@@ -44424,7 +44427,7 @@
         <v>0.01192789588635882</v>
       </c>
       <c r="AM156" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN156">
         <v>0.08086717939318311</v>
@@ -44693,7 +44696,7 @@
         <v>0.01186799249853062</v>
       </c>
       <c r="AM157" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN157">
         <v>0.07213994227012922</v>
@@ -44962,7 +44965,7 @@
         <v>0.01449742321347242</v>
       </c>
       <c r="AM158" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN158">
         <v>0.1112845525409627</v>
@@ -45231,7 +45234,7 @@
         <v>0.01458063833474489</v>
       </c>
       <c r="AM159" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN159">
         <v>0.182085969558268</v>
@@ -45500,7 +45503,7 @@
         <v>0.01203015543742209</v>
       </c>
       <c r="AM160" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN160">
         <v>0.04025259423397862</v>
@@ -45769,7 +45772,7 @@
         <v>0.01488877514152119</v>
       </c>
       <c r="AM161" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN161">
         <v>0.01931426172613477</v>
@@ -46038,7 +46041,7 @@
         <v>0.01132277626110294</v>
       </c>
       <c r="AM162" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN162">
         <v>0.06043490875273809</v>
@@ -46307,7 +46310,7 @@
         <v>0.011946015255795</v>
       </c>
       <c r="AM163" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN163">
         <v>0.04010539941927226</v>
@@ -46576,7 +46579,7 @@
         <v>0.01042329697569886</v>
       </c>
       <c r="AM164" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN164">
         <v>0.07892284657150772</v>
@@ -46845,7 +46848,7 @@
         <v>0.01136039741545648</v>
       </c>
       <c r="AM165" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN165">
         <v>0.06727405626523143</v>
@@ -47023,6 +47026,275 @@
       </c>
       <c r="CU165">
         <v>-0.3596428817468907</v>
+      </c>
+    </row>
+    <row r="166" spans="10:99">
+      <c r="J166" t="s">
+        <v>263</v>
+      </c>
+      <c r="K166">
+        <v>0.00768970393425894</v>
+      </c>
+      <c r="L166">
+        <v>0.00768970393425894</v>
+      </c>
+      <c r="M166">
+        <v>0.01416367241540373</v>
+      </c>
+      <c r="N166">
+        <v>0.01416367241540373</v>
+      </c>
+      <c r="O166">
+        <v>0.006708268328842771</v>
+      </c>
+      <c r="P166">
+        <v>0.006708268328842771</v>
+      </c>
+      <c r="Q166">
+        <v>0.012158516590922</v>
+      </c>
+      <c r="R166">
+        <v>0.012158516590922</v>
+      </c>
+      <c r="S166">
+        <v>27.09430104778942</v>
+      </c>
+      <c r="T166">
+        <v>14.0531561461794</v>
+      </c>
+      <c r="U166">
+        <v>0.9951829496413584</v>
+      </c>
+      <c r="V166">
+        <v>0.8039724964349274</v>
+      </c>
+      <c r="W166">
+        <v>0.06960301187605133</v>
+      </c>
+      <c r="X166">
+        <v>0.09761164476215528</v>
+      </c>
+      <c r="Y166">
+        <v>0.07806036285617445</v>
+      </c>
+      <c r="Z166">
+        <v>0.1088365094161724</v>
+      </c>
+      <c r="AA166">
+        <v>0.9965790464952481</v>
+      </c>
+      <c r="AB166">
+        <v>0.9319593887833921</v>
+      </c>
+      <c r="AC166">
+        <v>0.9070828641268326</v>
+      </c>
+      <c r="AD166">
+        <v>0.9949176075973049</v>
+      </c>
+      <c r="AE166">
+        <v>0.9209317952921099</v>
+      </c>
+      <c r="AF166">
+        <v>0.8913417257128291</v>
+      </c>
+      <c r="AG166">
+        <v>0.01079828020398072</v>
+      </c>
+      <c r="AH166">
+        <v>0.01727984850524278</v>
+      </c>
+      <c r="AI166">
+        <v>0.9965790464952481</v>
+      </c>
+      <c r="AJ166">
+        <v>0.9949176075973049</v>
+      </c>
+      <c r="AK166">
+        <v>0.01079828020398072</v>
+      </c>
+      <c r="AL166">
+        <v>0.01727984850524278</v>
+      </c>
+      <c r="AM166" t="s">
+        <v>264</v>
+      </c>
+      <c r="AN166">
+        <v>0.1967611069668674</v>
+      </c>
+      <c r="AO166">
+        <v>0.4224353873448451</v>
+      </c>
+      <c r="AP166">
+        <v>-90.32622106000001</v>
+      </c>
+      <c r="AQ166">
+        <v>-111.70320254</v>
+      </c>
+      <c r="AR166">
+        <v>13952.20317893998</v>
+      </c>
+      <c r="AS166">
+        <v>18431.65949745997</v>
+      </c>
+      <c r="AT166">
+        <v>13519.68507893999</v>
+      </c>
+      <c r="AU166">
+        <v>18431.65949745997</v>
+      </c>
+      <c r="AV166">
+        <v>0.3952203178939984</v>
+      </c>
+      <c r="AW166">
+        <v>0.8431659497459969</v>
+      </c>
+      <c r="AX166">
+        <v>0.8798074199943359</v>
+      </c>
+      <c r="AY166">
+        <v>1.695601092896175</v>
+      </c>
+      <c r="AZ166">
+        <v>14.9</v>
+      </c>
+      <c r="BA166">
+        <v>21.88333333333333</v>
+      </c>
+      <c r="BB166">
+        <v>0.01024740223322827</v>
+      </c>
+      <c r="BC166">
+        <v>0.01092316014939273</v>
+      </c>
+      <c r="BD166">
+        <v>-41.85432288323486</v>
+      </c>
+      <c r="BE166">
+        <v>-94.35113150616647</v>
+      </c>
+      <c r="BF166">
+        <v>774</v>
+      </c>
+      <c r="BG166">
+        <v>372</v>
+      </c>
+      <c r="BH166">
+        <v>43.47777777777778</v>
+      </c>
+      <c r="BI166">
+        <v>404</v>
+      </c>
+      <c r="BJ166">
+        <v>239</v>
+      </c>
+      <c r="BK166">
+        <v>1178</v>
+      </c>
+      <c r="BL166">
+        <v>611</v>
+      </c>
+      <c r="BM166">
+        <v>0</v>
+      </c>
+      <c r="BN166">
+        <v>0</v>
+      </c>
+      <c r="BO166">
+        <v>92</v>
+      </c>
+      <c r="BP166">
+        <v>207</v>
+      </c>
+      <c r="BQ166">
+        <v>0</v>
+      </c>
+      <c r="BR166">
+        <v>0</v>
+      </c>
+      <c r="BS166">
+        <v>682</v>
+      </c>
+      <c r="BT166">
+        <v>165</v>
+      </c>
+      <c r="BU166">
+        <v>404</v>
+      </c>
+      <c r="BV166">
+        <v>239</v>
+      </c>
+      <c r="BW166">
+        <v>3952.20317894</v>
+      </c>
+      <c r="BX166">
+        <v>8431.659497459994</v>
+      </c>
+      <c r="BY166">
+        <v>0.07303874930229157</v>
+      </c>
+      <c r="BZ166">
+        <v>0.08497207703199364</v>
+      </c>
+      <c r="CA166">
+        <v>0.08322096881383569</v>
+      </c>
+      <c r="CB166">
+        <v>0.09800760080776559</v>
+      </c>
+      <c r="CC166">
+        <v>0.0118157017135484</v>
+      </c>
+      <c r="CD166">
+        <v>0.01524450034864163</v>
+      </c>
+      <c r="CE166">
+        <v>0.01179969262853249</v>
+      </c>
+      <c r="CF166">
+        <v>0.01622486598713134</v>
+      </c>
+      <c r="CG166">
+        <v>4042.5294</v>
+      </c>
+      <c r="CH166">
+        <v>8543.362699999994</v>
+      </c>
+      <c r="CI166">
+        <v>4084.383722883235</v>
+      </c>
+      <c r="CJ166">
+        <v>8637.71383150616</v>
+      </c>
+      <c r="CK166">
+        <v>0.3361439760222782</v>
+      </c>
+      <c r="CL166">
+        <v>0.4218718312154179</v>
+      </c>
+      <c r="CM166">
+        <v>10000</v>
+      </c>
+      <c r="CO166">
+        <v>0.08229665071770335</v>
+      </c>
+      <c r="CP166">
+        <v>0.230622009569378</v>
+      </c>
+      <c r="CQ166">
+        <v>3127712.26621667</v>
+      </c>
+      <c r="CR166">
+        <v>3364116.785869008</v>
+      </c>
+      <c r="CS166" s="2">
+        <v>45567.80646056199</v>
+      </c>
+      <c r="CT166">
+        <v>-0.2296421337289892</v>
+      </c>
+      <c r="CU166">
+        <v>0.1400528478845656</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Git commited DOGEUSDT at 2024-10-02 21:57:08
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="409">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -808,6 +808,9 @@
     <t>SYSUSDT</t>
   </si>
   <si>
+    <t>GUSDT</t>
+  </si>
+  <si>
     <t>binance</t>
   </si>
   <si>
@@ -1599,7 +1602,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU166"/>
+  <dimension ref="A1:CU167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2017,7 +2020,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2182,7 +2185,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2298,7 +2301,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2463,7 +2466,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2579,7 +2582,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2744,7 +2747,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2860,7 +2863,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -3025,7 +3028,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3141,7 +3144,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3306,7 +3309,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3422,7 +3425,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3587,7 +3590,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3703,7 +3706,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3868,7 +3871,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3984,7 +3987,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4149,7 +4152,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4265,7 +4268,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4430,7 +4433,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4546,7 +4549,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4711,7 +4714,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4827,7 +4830,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4992,7 +4995,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5108,7 +5111,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5273,7 +5276,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5389,7 +5392,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5554,7 +5557,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5670,7 +5673,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5835,7 +5838,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5951,7 +5954,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6116,7 +6119,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6232,7 +6235,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6397,7 +6400,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6513,7 +6516,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6678,7 +6681,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6794,7 +6797,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6959,7 +6962,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7075,7 +7078,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7240,7 +7243,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7356,7 +7359,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7521,7 +7524,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7637,7 +7640,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7802,7 +7805,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7918,7 +7921,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8083,7 +8086,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8199,7 +8202,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8364,7 +8367,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8480,7 +8483,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8645,7 +8648,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8761,7 +8764,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8926,7 +8929,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -9042,7 +9045,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9207,7 +9210,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9323,7 +9326,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9488,7 +9491,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9604,7 +9607,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9769,7 +9772,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9885,7 +9888,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10050,7 +10053,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10166,7 +10169,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10331,7 +10334,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10447,7 +10450,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10612,7 +10615,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10728,7 +10731,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10893,7 +10896,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -11009,7 +11012,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11174,7 +11177,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11296,7 +11299,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11461,7 +11464,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11583,7 +11586,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11748,7 +11751,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11870,7 +11873,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -12035,7 +12038,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12157,7 +12160,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12322,7 +12325,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12444,7 +12447,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12609,7 +12612,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12731,7 +12734,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12896,7 +12899,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -13018,7 +13021,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13183,7 +13186,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13305,7 +13308,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13470,7 +13473,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13592,7 +13595,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13757,7 +13760,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13879,7 +13882,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -14044,7 +14047,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14166,7 +14169,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14331,7 +14334,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14453,7 +14456,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14618,7 +14621,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14740,7 +14743,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14905,7 +14908,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -15027,7 +15030,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15192,7 +15195,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15314,7 +15317,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15479,7 +15482,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15601,7 +15604,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15766,7 +15769,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15888,7 +15891,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16053,7 +16056,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16175,7 +16178,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16340,7 +16343,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16462,7 +16465,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16627,7 +16630,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16749,7 +16752,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16914,7 +16917,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -17033,7 +17036,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17198,7 +17201,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17314,7 +17317,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17479,7 +17482,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17592,7 +17595,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17757,7 +17760,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17870,7 +17873,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -18035,7 +18038,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18148,7 +18151,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18313,7 +18316,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18426,7 +18429,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18591,7 +18594,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18704,7 +18707,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18869,7 +18872,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18982,7 +18985,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19147,7 +19150,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19260,7 +19263,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19425,7 +19428,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19538,7 +19541,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19703,7 +19706,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19816,7 +19819,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19981,7 +19984,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20094,7 +20097,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20265,7 +20268,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20378,7 +20381,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20549,7 +20552,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20662,7 +20665,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20833,7 +20836,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20946,7 +20949,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21117,7 +21120,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21227,7 +21230,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21398,7 +21401,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21505,7 +21508,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21676,7 +21679,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21780,7 +21783,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21951,7 +21954,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22055,7 +22058,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22226,7 +22229,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22330,7 +22333,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22501,7 +22504,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22605,7 +22608,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22776,7 +22779,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22880,7 +22883,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23051,7 +23054,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23155,7 +23158,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23326,7 +23329,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23427,7 +23430,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23598,7 +23601,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23699,7 +23702,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23870,7 +23873,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23971,7 +23974,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24142,7 +24145,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24243,7 +24246,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24414,7 +24417,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24515,7 +24518,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24686,7 +24689,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24787,7 +24790,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24958,7 +24961,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25059,7 +25062,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25230,7 +25233,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25328,7 +25331,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25499,7 +25502,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25597,7 +25600,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25768,7 +25771,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25866,7 +25869,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -26037,7 +26040,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26135,7 +26138,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26306,7 +26309,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26404,7 +26407,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26575,7 +26578,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26673,7 +26676,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26844,7 +26847,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26942,7 +26945,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27113,7 +27116,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27211,7 +27214,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27382,7 +27385,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27480,7 +27483,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27651,7 +27654,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27749,7 +27752,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27920,7 +27923,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -28018,7 +28021,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28189,7 +28192,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28287,7 +28290,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28458,7 +28461,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28556,7 +28559,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28727,7 +28730,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28825,7 +28828,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28996,7 +28999,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29094,7 +29097,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29265,7 +29268,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29363,7 +29366,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29534,7 +29537,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29632,7 +29635,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29803,7 +29806,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29901,7 +29904,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30072,7 +30075,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30170,7 +30173,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30341,7 +30344,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30439,7 +30442,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30610,7 +30613,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30708,7 +30711,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30879,7 +30882,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30977,7 +30980,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31148,7 +31151,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31246,7 +31249,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31417,7 +31420,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31515,7 +31518,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31686,7 +31689,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31784,7 +31787,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31955,7 +31958,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32053,7 +32056,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32224,7 +32227,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32322,7 +32325,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32493,7 +32496,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32591,7 +32594,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32762,7 +32765,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32860,7 +32863,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -33031,7 +33034,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33129,7 +33132,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33300,7 +33303,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33398,7 +33401,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33569,7 +33572,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33667,7 +33670,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33838,7 +33841,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33936,7 +33939,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34107,7 +34110,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34205,7 +34208,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34376,7 +34379,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34474,7 +34477,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34645,7 +34648,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34743,7 +34746,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34914,7 +34917,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -35012,7 +35015,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35183,7 +35186,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35281,7 +35284,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35452,7 +35455,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35550,7 +35553,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35721,7 +35724,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35819,7 +35822,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35990,7 +35993,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36088,7 +36091,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36259,7 +36262,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36357,7 +36360,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36528,7 +36531,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36626,7 +36629,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36797,7 +36800,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36895,7 +36898,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37066,7 +37069,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37164,7 +37167,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37335,7 +37338,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37433,7 +37436,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37604,7 +37607,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37702,7 +37705,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37873,7 +37876,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37971,7 +37974,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38142,7 +38145,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38240,7 +38243,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38411,7 +38414,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38509,7 +38512,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38680,7 +38683,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38778,7 +38781,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38949,7 +38952,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -39047,7 +39050,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39218,7 +39221,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39316,7 +39319,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39487,7 +39490,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39585,7 +39588,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39756,7 +39759,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39854,7 +39857,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -40025,7 +40028,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40123,7 +40126,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40294,7 +40297,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40392,7 +40395,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40563,7 +40566,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40661,7 +40664,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40832,7 +40835,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40930,7 +40933,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41101,7 +41104,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41199,7 +41202,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41370,7 +41373,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41468,7 +41471,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41639,7 +41642,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41737,7 +41740,7 @@
         <v>0.01422843894993598</v>
       </c>
       <c r="AM146" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN146">
         <v>0.3570285831928028</v>
@@ -42006,7 +42009,7 @@
         <v>0.01287672421329242</v>
       </c>
       <c r="AM147" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN147">
         <v>0.1138938544209247</v>
@@ -42275,7 +42278,7 @@
         <v>0.01129449859594168</v>
       </c>
       <c r="AM148" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN148">
         <v>0.01929055864963264</v>
@@ -42544,7 +42547,7 @@
         <v>0.01268293743279473</v>
       </c>
       <c r="AM149" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN149">
         <v>0.02713293780673231</v>
@@ -42813,7 +42816,7 @@
         <v>0.006815186142663594</v>
       </c>
       <c r="AM150" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN150">
         <v>0.06060596226028341</v>
@@ -43082,7 +43085,7 @@
         <v>0.01172718359151741</v>
       </c>
       <c r="AM151" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN151">
         <v>0.09142880750409497</v>
@@ -43351,7 +43354,7 @@
         <v>0.01464508407647874</v>
       </c>
       <c r="AM152" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN152">
         <v>0.3981395839245215</v>
@@ -43620,7 +43623,7 @@
         <v>0.01424145384485694</v>
       </c>
       <c r="AM153" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN153">
         <v>0.1335188651800471</v>
@@ -43889,7 +43892,7 @@
         <v>0.008636072468123625</v>
       </c>
       <c r="AM154" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN154">
         <v>0.06745759346973818</v>
@@ -44158,7 +44161,7 @@
         <v>0.01257263323646787</v>
       </c>
       <c r="AM155" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN155">
         <v>0.1015263162251083</v>
@@ -44427,7 +44430,7 @@
         <v>0.01192789588635882</v>
       </c>
       <c r="AM156" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN156">
         <v>0.08086717939318311</v>
@@ -44696,7 +44699,7 @@
         <v>0.01186799249853062</v>
       </c>
       <c r="AM157" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN157">
         <v>0.07213994227012922</v>
@@ -44965,7 +44968,7 @@
         <v>0.01449742321347242</v>
       </c>
       <c r="AM158" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN158">
         <v>0.1112845525409627</v>
@@ -45234,7 +45237,7 @@
         <v>0.01458063833474489</v>
       </c>
       <c r="AM159" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN159">
         <v>0.182085969558268</v>
@@ -45503,7 +45506,7 @@
         <v>0.01203015543742209</v>
       </c>
       <c r="AM160" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN160">
         <v>0.04025259423397862</v>
@@ -45772,7 +45775,7 @@
         <v>0.01488877514152119</v>
       </c>
       <c r="AM161" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN161">
         <v>0.01931426172613477</v>
@@ -46041,7 +46044,7 @@
         <v>0.01132277626110294</v>
       </c>
       <c r="AM162" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN162">
         <v>0.06043490875273809</v>
@@ -46310,7 +46313,7 @@
         <v>0.011946015255795</v>
       </c>
       <c r="AM163" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN163">
         <v>0.04010539941927226</v>
@@ -46579,7 +46582,7 @@
         <v>0.01042329697569886</v>
       </c>
       <c r="AM164" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN164">
         <v>0.07892284657150772</v>
@@ -46848,7 +46851,7 @@
         <v>0.01136039741545648</v>
       </c>
       <c r="AM165" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN165">
         <v>0.06727405626523143</v>
@@ -47117,7 +47120,7 @@
         <v>0.01727984850524278</v>
       </c>
       <c r="AM166" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN166">
         <v>0.1967611069668674</v>
@@ -47295,6 +47298,275 @@
       </c>
       <c r="CU166">
         <v>0.1400528478845656</v>
+      </c>
+    </row>
+    <row r="167" spans="10:99">
+      <c r="J167" t="s">
+        <v>264</v>
+      </c>
+      <c r="K167">
+        <v>0.004149211964134647</v>
+      </c>
+      <c r="L167">
+        <v>0.004149211964134647</v>
+      </c>
+      <c r="M167">
+        <v>0.006013456004538398</v>
+      </c>
+      <c r="N167">
+        <v>0.006013456004538398</v>
+      </c>
+      <c r="O167">
+        <v>0.004963468865797194</v>
+      </c>
+      <c r="P167">
+        <v>0.004963468865797194</v>
+      </c>
+      <c r="Q167">
+        <v>0.006327068774858136</v>
+      </c>
+      <c r="R167">
+        <v>0.006327068774858136</v>
+      </c>
+      <c r="S167">
+        <v>29.65597940556986</v>
+      </c>
+      <c r="T167">
+        <v>14.30142756845308</v>
+      </c>
+      <c r="U167">
+        <v>0.9999756790075592</v>
+      </c>
+      <c r="V167">
+        <v>0.8677329386867014</v>
+      </c>
+      <c r="W167">
+        <v>0.05263264612240953</v>
+      </c>
+      <c r="X167">
+        <v>0.06335499149294982</v>
+      </c>
+      <c r="Y167">
+        <v>0.06715833291094069</v>
+      </c>
+      <c r="Z167">
+        <v>0.07150144267862329</v>
+      </c>
+      <c r="AA167">
+        <v>0.9969108001094261</v>
+      </c>
+      <c r="AB167">
+        <v>0.9469632747940429</v>
+      </c>
+      <c r="AC167">
+        <v>0.9367996816395034</v>
+      </c>
+      <c r="AD167">
+        <v>0.9932486045631714</v>
+      </c>
+      <c r="AE167">
+        <v>0.9329923559311198</v>
+      </c>
+      <c r="AF167">
+        <v>0.9291944568344969</v>
+      </c>
+      <c r="AG167">
+        <v>0.008745110419745289</v>
+      </c>
+      <c r="AH167">
+        <v>0.0134271753582951</v>
+      </c>
+      <c r="AI167">
+        <v>0.9969108001094261</v>
+      </c>
+      <c r="AJ167">
+        <v>0.9932486045631714</v>
+      </c>
+      <c r="AK167">
+        <v>0.008745110419745289</v>
+      </c>
+      <c r="AL167">
+        <v>0.0134271753582951</v>
+      </c>
+      <c r="AM167" t="s">
+        <v>265</v>
+      </c>
+      <c r="AN167">
+        <v>0.209990341163658</v>
+      </c>
+      <c r="AO167">
+        <v>0.4075173640201666</v>
+      </c>
+      <c r="AP167">
+        <v>-286.80805531</v>
+      </c>
+      <c r="AQ167">
+        <v>-85.09751703400001</v>
+      </c>
+      <c r="AR167">
+        <v>12172.42193468996</v>
+      </c>
+      <c r="AS167">
+        <v>13292.973792966</v>
+      </c>
+      <c r="AT167">
+        <v>12171.36467468996</v>
+      </c>
+      <c r="AU167">
+        <v>13292.973792966</v>
+      </c>
+      <c r="AV167">
+        <v>0.2172421934689965</v>
+      </c>
+      <c r="AW167">
+        <v>0.3292973792965999</v>
+      </c>
+      <c r="AX167">
+        <v>0.8097488746742478</v>
+      </c>
+      <c r="AY167">
+        <v>1.666863323500492</v>
+      </c>
+      <c r="AZ167">
+        <v>17.38333333333333</v>
+      </c>
+      <c r="BA167">
+        <v>25.8</v>
+      </c>
+      <c r="BB167">
+        <v>0.009479655092901437</v>
+      </c>
+      <c r="BC167">
+        <v>0.03635341051044376</v>
+      </c>
+      <c r="BD167">
+        <v>-23.5357630150503</v>
+      </c>
+      <c r="BE167">
+        <v>-127.4371895313115</v>
+      </c>
+      <c r="BF167">
+        <v>594</v>
+      </c>
+      <c r="BG167">
+        <v>499</v>
+      </c>
+      <c r="BH167">
+        <v>47.47777777777778</v>
+      </c>
+      <c r="BI167">
+        <v>814</v>
+      </c>
+      <c r="BJ167">
+        <v>180</v>
+      </c>
+      <c r="BK167">
+        <v>1408</v>
+      </c>
+      <c r="BL167">
+        <v>679</v>
+      </c>
+      <c r="BM167">
+        <v>0</v>
+      </c>
+      <c r="BN167">
+        <v>0</v>
+      </c>
+      <c r="BO167">
+        <v>496</v>
+      </c>
+      <c r="BP167">
+        <v>114</v>
+      </c>
+      <c r="BQ167">
+        <v>0</v>
+      </c>
+      <c r="BR167">
+        <v>0</v>
+      </c>
+      <c r="BS167">
+        <v>98</v>
+      </c>
+      <c r="BT167">
+        <v>385</v>
+      </c>
+      <c r="BU167">
+        <v>814</v>
+      </c>
+      <c r="BV167">
+        <v>180</v>
+      </c>
+      <c r="BW167">
+        <v>2172.421934689991</v>
+      </c>
+      <c r="BX167">
+        <v>3292.973792966</v>
+      </c>
+      <c r="BY167">
+        <v>0.05532973182634315</v>
+      </c>
+      <c r="BZ167">
+        <v>0.05895497831614305</v>
+      </c>
+      <c r="CA167">
+        <v>0.07181941934132559</v>
+      </c>
+      <c r="CB167">
+        <v>0.06612211426187349</v>
+      </c>
+      <c r="CC167">
+        <v>0.007455555953407559</v>
+      </c>
+      <c r="CD167">
+        <v>0.01269809952706124</v>
+      </c>
+      <c r="CE167">
+        <v>0.009854789240745789</v>
+      </c>
+      <c r="CF167">
+        <v>0.01169902787421558</v>
+      </c>
+      <c r="CG167">
+        <v>2459.229989999991</v>
+      </c>
+      <c r="CH167">
+        <v>3378.07131</v>
+      </c>
+      <c r="CI167">
+        <v>2482.765753015041</v>
+      </c>
+      <c r="CJ167">
+        <v>3505.508499531312</v>
+      </c>
+      <c r="CK167">
+        <v>0.3616240190195784</v>
+      </c>
+      <c r="CL167">
+        <v>0.3495913032222542</v>
+      </c>
+      <c r="CM167">
+        <v>10000</v>
+      </c>
+      <c r="CO167">
+        <v>0.1349693251533742</v>
+      </c>
+      <c r="CP167">
+        <v>0.2541630148992112</v>
+      </c>
+      <c r="CQ167">
+        <v>1775882.93455477</v>
+      </c>
+      <c r="CR167">
+        <v>2685328.117906907</v>
+      </c>
+      <c r="CS167" s="2">
+        <v>45567.824369977</v>
+      </c>
+      <c r="CT167">
+        <v>-0.4155903099182516</v>
+      </c>
+      <c r="CU167">
+        <v>-0.2422663676567164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update NTRNUSDT.json at 2024-10-09_14-21-17 bestfile_scores 0.0012651427403998885 bestfile_sharp 0.10196585733032616
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="389">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -746,6 +746,9 @@
   </si>
   <si>
     <t>1000PEPEUSDT</t>
+  </si>
+  <si>
+    <t>STXUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1539,7 +1542,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU146"/>
+  <dimension ref="A1:CU147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1957,7 +1960,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2122,7 +2125,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2238,7 +2241,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2403,7 +2406,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2519,7 +2522,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2684,7 +2687,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2800,7 +2803,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -2965,7 +2968,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3081,7 +3084,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3246,7 +3249,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3362,7 +3365,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3527,7 +3530,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3643,7 +3646,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3808,7 +3811,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3924,7 +3927,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4089,7 +4092,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4205,7 +4208,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4370,7 +4373,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4486,7 +4489,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4651,7 +4654,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4767,7 +4770,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4932,7 +4935,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5048,7 +5051,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5213,7 +5216,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5329,7 +5332,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5494,7 +5497,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5610,7 +5613,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5775,7 +5778,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5891,7 +5894,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6056,7 +6059,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6172,7 +6175,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6337,7 +6340,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6453,7 +6456,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6618,7 +6621,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6734,7 +6737,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6899,7 +6902,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7015,7 +7018,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7180,7 +7183,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7296,7 +7299,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7461,7 +7464,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7577,7 +7580,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7742,7 +7745,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7858,7 +7861,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8023,7 +8026,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8139,7 +8142,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8304,7 +8307,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8420,7 +8423,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8585,7 +8588,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8701,7 +8704,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8866,7 +8869,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -8982,7 +8985,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9147,7 +9150,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9263,7 +9266,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9428,7 +9431,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9544,7 +9547,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9709,7 +9712,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9825,7 +9828,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -9990,7 +9993,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10106,7 +10109,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10271,7 +10274,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10387,7 +10390,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10552,7 +10555,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10668,7 +10671,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10833,7 +10836,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10949,7 +10952,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11114,7 +11117,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11236,7 +11239,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11401,7 +11404,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11523,7 +11526,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11688,7 +11691,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11810,7 +11813,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -11975,7 +11978,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12097,7 +12100,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12262,7 +12265,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12384,7 +12387,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12549,7 +12552,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12671,7 +12674,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12836,7 +12839,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12958,7 +12961,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13123,7 +13126,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13245,7 +13248,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13410,7 +13413,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13532,7 +13535,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13697,7 +13700,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13819,7 +13822,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -13984,7 +13987,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14106,7 +14109,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14271,7 +14274,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14393,7 +14396,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14558,7 +14561,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14680,7 +14683,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14845,7 +14848,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -14967,7 +14970,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15132,7 +15135,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15254,7 +15257,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15419,7 +15422,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15541,7 +15544,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15706,7 +15709,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15828,7 +15831,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -15993,7 +15996,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16115,7 +16118,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16280,7 +16283,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16402,7 +16405,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16567,7 +16570,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16689,7 +16692,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16854,7 +16857,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -16973,7 +16976,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17138,7 +17141,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17254,7 +17257,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17419,7 +17422,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17532,7 +17535,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17697,7 +17700,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17810,7 +17813,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -17975,7 +17978,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18088,7 +18091,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18253,7 +18256,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18366,7 +18369,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18531,7 +18534,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18644,7 +18647,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18809,7 +18812,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18922,7 +18925,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19087,7 +19090,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19200,7 +19203,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19365,7 +19368,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19478,7 +19481,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19643,7 +19646,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19756,7 +19759,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19921,7 +19924,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20034,7 +20037,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20205,7 +20208,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20318,7 +20321,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20489,7 +20492,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20602,7 +20605,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20773,7 +20776,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20886,7 +20889,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21057,7 +21060,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21167,7 +21170,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21338,7 +21341,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21445,7 +21448,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21616,7 +21619,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21720,7 +21723,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21891,7 +21894,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -21995,7 +21998,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22166,7 +22169,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22270,7 +22273,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22441,7 +22444,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22545,7 +22548,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22716,7 +22719,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22820,7 +22823,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -22991,7 +22994,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23095,7 +23098,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23266,7 +23269,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23367,7 +23370,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23538,7 +23541,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23639,7 +23642,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23810,7 +23813,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23911,7 +23914,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24082,7 +24085,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24183,7 +24186,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24354,7 +24357,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24455,7 +24458,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24626,7 +24629,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24727,7 +24730,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24898,7 +24901,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -24999,7 +25002,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25170,7 +25173,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25268,7 +25271,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25439,7 +25442,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25537,7 +25540,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25708,7 +25711,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25806,7 +25809,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -25977,7 +25980,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26075,7 +26078,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26246,7 +26249,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26344,7 +26347,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26515,7 +26518,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26613,7 +26616,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26784,7 +26787,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26882,7 +26885,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27053,7 +27056,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27151,7 +27154,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27322,7 +27325,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27420,7 +27423,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27591,7 +27594,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27689,7 +27692,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27860,7 +27863,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27958,7 +27961,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28129,7 +28132,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28227,7 +28230,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28398,7 +28401,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28496,7 +28499,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28667,7 +28670,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28765,7 +28768,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28936,7 +28939,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29034,7 +29037,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29205,7 +29208,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29303,7 +29306,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29474,7 +29477,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29572,7 +29575,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29743,7 +29746,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29841,7 +29844,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30012,7 +30015,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30110,7 +30113,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30281,7 +30284,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30379,7 +30382,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30550,7 +30553,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30648,7 +30651,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30819,7 +30822,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30917,7 +30920,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31088,7 +31091,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31186,7 +31189,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31357,7 +31360,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31455,7 +31458,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31626,7 +31629,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31724,7 +31727,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31895,7 +31898,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -31993,7 +31996,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32164,7 +32167,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32262,7 +32265,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32433,7 +32436,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32531,7 +32534,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32702,7 +32705,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32800,7 +32803,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -32971,7 +32974,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33069,7 +33072,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33240,7 +33243,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33338,7 +33341,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33509,7 +33512,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33607,7 +33610,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33778,7 +33781,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33876,7 +33879,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34047,7 +34050,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34145,7 +34148,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34316,7 +34319,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34414,7 +34417,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34585,7 +34588,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34683,7 +34686,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34854,7 +34857,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34952,7 +34955,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35123,7 +35126,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35221,7 +35224,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35392,7 +35395,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35490,7 +35493,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35661,7 +35664,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35759,7 +35762,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35930,7 +35933,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36028,7 +36031,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36199,7 +36202,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36297,7 +36300,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36468,7 +36471,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36566,7 +36569,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36737,7 +36740,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36835,7 +36838,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37006,7 +37009,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37104,7 +37107,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37275,7 +37278,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37373,7 +37376,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37544,7 +37547,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37642,7 +37645,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37813,7 +37816,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37911,7 +37914,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38082,7 +38085,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38180,7 +38183,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38351,7 +38354,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38449,7 +38452,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38620,7 +38623,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38718,7 +38721,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38889,7 +38892,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -38987,7 +38990,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39158,7 +39161,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39256,7 +39259,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39427,7 +39430,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39525,7 +39528,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39696,7 +39699,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39794,7 +39797,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -39965,7 +39968,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40063,7 +40066,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40234,7 +40237,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40332,7 +40335,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40503,7 +40506,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40601,7 +40604,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40772,7 +40775,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40870,7 +40873,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41041,7 +41044,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41139,7 +41142,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41310,7 +41313,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41408,7 +41411,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41579,7 +41582,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41677,7 +41680,7 @@
         <v>0.006328270379966137</v>
       </c>
       <c r="AM146" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN146">
         <v>0.08370784758312214</v>
@@ -41855,6 +41858,275 @@
       </c>
       <c r="CU146">
         <v>-0.9207553417203316</v>
+      </c>
+    </row>
+    <row r="147" spans="10:99">
+      <c r="J147" t="s">
+        <v>244</v>
+      </c>
+      <c r="K147">
+        <v>0.0008686252022698238</v>
+      </c>
+      <c r="L147">
+        <v>0.0008686252022698238</v>
+      </c>
+      <c r="M147">
+        <v>0.0008719031808308575</v>
+      </c>
+      <c r="N147">
+        <v>0.0008719031808308575</v>
+      </c>
+      <c r="O147">
+        <v>0.0007598065414332833</v>
+      </c>
+      <c r="P147">
+        <v>0.0007598065414332833</v>
+      </c>
+      <c r="Q147">
+        <v>0.0007485129188969264</v>
+      </c>
+      <c r="R147">
+        <v>0.0007485129188969264</v>
+      </c>
+      <c r="S147">
+        <v>14.27625010497243</v>
+      </c>
+      <c r="T147">
+        <v>5.131052243610678</v>
+      </c>
+      <c r="U147">
+        <v>0.9898686983128189</v>
+      </c>
+      <c r="V147">
+        <v>0.6402604860412664</v>
+      </c>
+      <c r="W147">
+        <v>0.0946379156503491</v>
+      </c>
+      <c r="X147">
+        <v>0.09760094303516567</v>
+      </c>
+      <c r="Y147">
+        <v>0.2432485236910339</v>
+      </c>
+      <c r="Z147">
+        <v>0.2196420118562086</v>
+      </c>
+      <c r="AA147">
+        <v>0.9977224313621884</v>
+      </c>
+      <c r="AB147">
+        <v>0.8112995632767273</v>
+      </c>
+      <c r="AC147">
+        <v>0.806309389779946</v>
+      </c>
+      <c r="AD147">
+        <v>0.9980373393310574</v>
+      </c>
+      <c r="AE147">
+        <v>0.7569380656689977</v>
+      </c>
+      <c r="AF147">
+        <v>0.7806773604261499</v>
+      </c>
+      <c r="AG147">
+        <v>0.0107615197926094</v>
+      </c>
+      <c r="AH147">
+        <v>0.0110592804278049</v>
+      </c>
+      <c r="AI147">
+        <v>0.9977224313621884</v>
+      </c>
+      <c r="AJ147">
+        <v>0.9980373393310574</v>
+      </c>
+      <c r="AK147">
+        <v>0.0107615197926094</v>
+      </c>
+      <c r="AL147">
+        <v>0.0110592804278049</v>
+      </c>
+      <c r="AM147" t="s">
+        <v>245</v>
+      </c>
+      <c r="AN147">
+        <v>0.07581655721931389</v>
+      </c>
+      <c r="AO147">
+        <v>0.05609019558171888</v>
+      </c>
+      <c r="AP147">
+        <v>-357.92265994</v>
+      </c>
+      <c r="AQ147">
+        <v>-205.33789268</v>
+      </c>
+      <c r="AR147">
+        <v>16769.05506105329</v>
+      </c>
+      <c r="AS147">
+        <v>16801.78650732002</v>
+      </c>
+      <c r="AT147">
+        <v>16740.32784006006</v>
+      </c>
+      <c r="AU147">
+        <v>16801.78650732002</v>
+      </c>
+      <c r="AV147">
+        <v>0.6769055061053288</v>
+      </c>
+      <c r="AW147">
+        <v>0.6801786507320022</v>
+      </c>
+      <c r="AX147">
+        <v>1.680736949445033</v>
+      </c>
+      <c r="AY147">
+        <v>4.678710980135342</v>
+      </c>
+      <c r="AZ147">
+        <v>26.26666666666667</v>
+      </c>
+      <c r="BA147">
+        <v>57.56666666666667</v>
+      </c>
+      <c r="BB147">
+        <v>0.08581217558606696</v>
+      </c>
+      <c r="BC147">
+        <v>0.07259380077378652</v>
+      </c>
+      <c r="BD147">
+        <v>-668.9888524646784</v>
+      </c>
+      <c r="BE147">
+        <v>-548.4908264740449</v>
+      </c>
+      <c r="BF147">
+        <v>3740</v>
+      </c>
+      <c r="BG147">
+        <v>1361</v>
+      </c>
+      <c r="BH147">
+        <v>595.3944444444445</v>
+      </c>
+      <c r="BI147">
+        <v>4760</v>
+      </c>
+      <c r="BJ147">
+        <v>1694</v>
+      </c>
+      <c r="BK147">
+        <v>8500</v>
+      </c>
+      <c r="BL147">
+        <v>3055</v>
+      </c>
+      <c r="BM147">
+        <v>0</v>
+      </c>
+      <c r="BN147">
+        <v>0</v>
+      </c>
+      <c r="BO147">
+        <v>1961</v>
+      </c>
+      <c r="BP147">
+        <v>485</v>
+      </c>
+      <c r="BQ147">
+        <v>0</v>
+      </c>
+      <c r="BR147">
+        <v>0</v>
+      </c>
+      <c r="BS147">
+        <v>1779</v>
+      </c>
+      <c r="BT147">
+        <v>876</v>
+      </c>
+      <c r="BU147">
+        <v>4760</v>
+      </c>
+      <c r="BV147">
+        <v>1694</v>
+      </c>
+      <c r="BW147">
+        <v>6769.055061053225</v>
+      </c>
+      <c r="BX147">
+        <v>6801.786507320002</v>
+      </c>
+      <c r="BY147">
+        <v>0.1038858197339511</v>
+      </c>
+      <c r="BZ147">
+        <v>0.08889487512642701</v>
+      </c>
+      <c r="CA147">
+        <v>0.3211130024098212</v>
+      </c>
+      <c r="CB147">
+        <v>0.179874077220266</v>
+      </c>
+      <c r="CC147">
+        <v>0.01504746909508449</v>
+      </c>
+      <c r="CD147">
+        <v>0.01647280608903716</v>
+      </c>
+      <c r="CE147">
+        <v>0.01501812685954315</v>
+      </c>
+      <c r="CF147">
+        <v>0.01645745860712478</v>
+      </c>
+      <c r="CG147">
+        <v>7126.977720993224</v>
+      </c>
+      <c r="CH147">
+        <v>7007.124400000002</v>
+      </c>
+      <c r="CI147">
+        <v>7795.966573457903</v>
+      </c>
+      <c r="CJ147">
+        <v>7555.615226474047</v>
+      </c>
+      <c r="CK147">
+        <v>0.0876608537421346</v>
+      </c>
+      <c r="CL147">
+        <v>0.09438173766495386</v>
+      </c>
+      <c r="CM147">
+        <v>10000</v>
+      </c>
+      <c r="CO147">
+        <v>0.02610034287313694</v>
+      </c>
+      <c r="CP147">
+        <v>0.01644391575117207</v>
+      </c>
+      <c r="CQ147">
+        <v>6471383.18612241</v>
+      </c>
+      <c r="CR147">
+        <v>3041853.6398008</v>
+      </c>
+      <c r="CS147" s="2">
+        <v>45574.54011241355</v>
+      </c>
+      <c r="CT147">
+        <v>-0.7102224815550879</v>
+      </c>
+      <c r="CU147">
+        <v>-0.7396324181909387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update TLMUSDT.json at 2024-10-10_02-05-01 bestfile_scores 0.0012425193506455546 bestfile_sharp 0.05688459322482251
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="392">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -755,6 +755,9 @@
   </si>
   <si>
     <t>BELUSDT</t>
+  </si>
+  <si>
+    <t>QNTUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1548,7 +1551,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU149"/>
+  <dimension ref="A1:CU150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1966,7 +1969,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2131,7 +2134,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2247,7 +2250,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2412,7 +2415,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2528,7 +2531,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2693,7 +2696,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2809,7 +2812,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -2974,7 +2977,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3090,7 +3093,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3255,7 +3258,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3371,7 +3374,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3536,7 +3539,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3652,7 +3655,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3817,7 +3820,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3933,7 +3936,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4098,7 +4101,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4214,7 +4217,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4379,7 +4382,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4495,7 +4498,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4660,7 +4663,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4776,7 +4779,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4941,7 +4944,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5057,7 +5060,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5222,7 +5225,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5338,7 +5341,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5503,7 +5506,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5619,7 +5622,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5784,7 +5787,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5900,7 +5903,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6065,7 +6068,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6181,7 +6184,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6346,7 +6349,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6462,7 +6465,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6627,7 +6630,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6743,7 +6746,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6908,7 +6911,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7024,7 +7027,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7189,7 +7192,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7305,7 +7308,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7470,7 +7473,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7586,7 +7589,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7751,7 +7754,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7867,7 +7870,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8032,7 +8035,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8148,7 +8151,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8313,7 +8316,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8429,7 +8432,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8594,7 +8597,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8710,7 +8713,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8875,7 +8878,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -8991,7 +8994,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9156,7 +9159,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9272,7 +9275,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9437,7 +9440,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9553,7 +9556,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9718,7 +9721,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9834,7 +9837,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -9999,7 +10002,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10115,7 +10118,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10280,7 +10283,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10396,7 +10399,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10561,7 +10564,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10677,7 +10680,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10842,7 +10845,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10958,7 +10961,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11123,7 +11126,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11245,7 +11248,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11410,7 +11413,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11532,7 +11535,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11697,7 +11700,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11819,7 +11822,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -11984,7 +11987,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12106,7 +12109,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12271,7 +12274,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12393,7 +12396,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12558,7 +12561,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12680,7 +12683,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12845,7 +12848,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12967,7 +12970,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13132,7 +13135,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13254,7 +13257,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13419,7 +13422,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13541,7 +13544,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13706,7 +13709,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13828,7 +13831,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -13993,7 +13996,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14115,7 +14118,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14280,7 +14283,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14402,7 +14405,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14567,7 +14570,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14689,7 +14692,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14854,7 +14857,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -14976,7 +14979,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15141,7 +15144,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15263,7 +15266,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15428,7 +15431,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15550,7 +15553,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15715,7 +15718,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15837,7 +15840,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16002,7 +16005,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16124,7 +16127,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16289,7 +16292,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16411,7 +16414,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16576,7 +16579,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16698,7 +16701,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16863,7 +16866,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -16982,7 +16985,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17147,7 +17150,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17263,7 +17266,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17428,7 +17431,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17541,7 +17544,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17706,7 +17709,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17819,7 +17822,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -17984,7 +17987,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18097,7 +18100,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18262,7 +18265,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18375,7 +18378,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18540,7 +18543,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18653,7 +18656,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18818,7 +18821,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18931,7 +18934,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19096,7 +19099,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19209,7 +19212,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19374,7 +19377,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19487,7 +19490,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19652,7 +19655,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19765,7 +19768,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19930,7 +19933,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20043,7 +20046,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20214,7 +20217,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20327,7 +20330,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20498,7 +20501,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20611,7 +20614,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20782,7 +20785,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20895,7 +20898,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21066,7 +21069,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21176,7 +21179,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21347,7 +21350,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21454,7 +21457,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21625,7 +21628,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21729,7 +21732,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21900,7 +21903,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22004,7 +22007,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22175,7 +22178,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22279,7 +22282,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22450,7 +22453,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22554,7 +22557,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22725,7 +22728,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22829,7 +22832,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23000,7 +23003,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23104,7 +23107,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23275,7 +23278,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23376,7 +23379,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23547,7 +23550,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23648,7 +23651,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23819,7 +23822,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23920,7 +23923,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24091,7 +24094,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24192,7 +24195,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24363,7 +24366,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24464,7 +24467,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24635,7 +24638,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24736,7 +24739,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24907,7 +24910,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25008,7 +25011,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25179,7 +25182,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25277,7 +25280,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25448,7 +25451,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25546,7 +25549,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25717,7 +25720,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25815,7 +25818,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -25986,7 +25989,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26084,7 +26087,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26255,7 +26258,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26353,7 +26356,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26524,7 +26527,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26622,7 +26625,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26793,7 +26796,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26891,7 +26894,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27062,7 +27065,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27160,7 +27163,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27331,7 +27334,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27429,7 +27432,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27600,7 +27603,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27698,7 +27701,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27869,7 +27872,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27967,7 +27970,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28138,7 +28141,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28236,7 +28239,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28407,7 +28410,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28505,7 +28508,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28676,7 +28679,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28774,7 +28777,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28945,7 +28948,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29043,7 +29046,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29214,7 +29217,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29312,7 +29315,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29483,7 +29486,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29581,7 +29584,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29752,7 +29755,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29850,7 +29853,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30021,7 +30024,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30119,7 +30122,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30290,7 +30293,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30388,7 +30391,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30559,7 +30562,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30657,7 +30660,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30828,7 +30831,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30926,7 +30929,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31097,7 +31100,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31195,7 +31198,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31366,7 +31369,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31464,7 +31467,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31635,7 +31638,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31733,7 +31736,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31904,7 +31907,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32002,7 +32005,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32173,7 +32176,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32271,7 +32274,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32442,7 +32445,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32540,7 +32543,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32711,7 +32714,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32809,7 +32812,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -32980,7 +32983,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33078,7 +33081,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33249,7 +33252,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33347,7 +33350,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33518,7 +33521,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33616,7 +33619,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33787,7 +33790,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33885,7 +33888,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34056,7 +34059,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34154,7 +34157,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34325,7 +34328,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34423,7 +34426,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34594,7 +34597,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34692,7 +34695,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34863,7 +34866,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34961,7 +34964,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35132,7 +35135,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35230,7 +35233,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35401,7 +35404,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35499,7 +35502,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35670,7 +35673,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35768,7 +35771,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35939,7 +35942,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36037,7 +36040,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36208,7 +36211,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36306,7 +36309,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36477,7 +36480,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36575,7 +36578,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36746,7 +36749,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36844,7 +36847,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37015,7 +37018,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37113,7 +37116,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37284,7 +37287,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37382,7 +37385,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37553,7 +37556,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37651,7 +37654,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37822,7 +37825,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37920,7 +37923,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38091,7 +38094,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38189,7 +38192,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38360,7 +38363,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38458,7 +38461,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38629,7 +38632,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38727,7 +38730,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38898,7 +38901,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -38996,7 +38999,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39167,7 +39170,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39265,7 +39268,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39436,7 +39439,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39534,7 +39537,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39705,7 +39708,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39803,7 +39806,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -39974,7 +39977,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40072,7 +40075,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40243,7 +40246,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40341,7 +40344,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40512,7 +40515,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40610,7 +40613,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40781,7 +40784,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40879,7 +40882,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41050,7 +41053,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41148,7 +41151,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41319,7 +41322,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41417,7 +41420,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41588,7 +41591,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41686,7 +41689,7 @@
         <v>0.006328270379966137</v>
       </c>
       <c r="AM146" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN146">
         <v>0.08370784758312214</v>
@@ -41955,7 +41958,7 @@
         <v>0.0110592804278049</v>
       </c>
       <c r="AM147" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN147">
         <v>0.07581655721931389</v>
@@ -42224,7 +42227,7 @@
         <v>0.01450048649474174</v>
       </c>
       <c r="AM148" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN148">
         <v>0.09614621483891075</v>
@@ -42493,7 +42496,7 @@
         <v>0.01189559910110707</v>
       </c>
       <c r="AM149" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN149">
         <v>0.01288397198120313</v>
@@ -42671,6 +42674,275 @@
       </c>
       <c r="CU149">
         <v>-0.7929989904831393</v>
+      </c>
+    </row>
+    <row r="150" spans="10:99">
+      <c r="J150" t="s">
+        <v>247</v>
+      </c>
+      <c r="K150">
+        <v>0.002572313493031109</v>
+      </c>
+      <c r="L150">
+        <v>0.002572313493031109</v>
+      </c>
+      <c r="M150">
+        <v>0.0009196507343438576</v>
+      </c>
+      <c r="N150">
+        <v>0.0009196507343438576</v>
+      </c>
+      <c r="O150">
+        <v>0.002789027336181182</v>
+      </c>
+      <c r="P150">
+        <v>0.002789027336181182</v>
+      </c>
+      <c r="Q150">
+        <v>0.000921125949356938</v>
+      </c>
+      <c r="R150">
+        <v>0.000921125949356938</v>
+      </c>
+      <c r="S150">
+        <v>15.73008388575485</v>
+      </c>
+      <c r="T150">
+        <v>15.73841844097514</v>
+      </c>
+      <c r="U150">
+        <v>0.9993439316832068</v>
+      </c>
+      <c r="V150">
+        <v>0.7409268885301683</v>
+      </c>
+      <c r="W150">
+        <v>0.09711554770504344</v>
+      </c>
+      <c r="X150">
+        <v>0.09983291720478654</v>
+      </c>
+      <c r="Y150">
+        <v>0.2412842378627955</v>
+      </c>
+      <c r="Z150">
+        <v>0.1713396749397045</v>
+      </c>
+      <c r="AA150">
+        <v>0.9978380549226805</v>
+      </c>
+      <c r="AB150">
+        <v>0.8101480846350126</v>
+      </c>
+      <c r="AC150">
+        <v>0.8733509780190698</v>
+      </c>
+      <c r="AD150">
+        <v>0.9949325348498578</v>
+      </c>
+      <c r="AE150">
+        <v>0.75991717956208</v>
+      </c>
+      <c r="AF150">
+        <v>0.837602383023402</v>
+      </c>
+      <c r="AG150">
+        <v>0.01150286120135907</v>
+      </c>
+      <c r="AH150">
+        <v>0.0145803412240497</v>
+      </c>
+      <c r="AI150">
+        <v>0.9978380549226805</v>
+      </c>
+      <c r="AJ150">
+        <v>0.9949325348498578</v>
+      </c>
+      <c r="AK150">
+        <v>0.01150286120135907</v>
+      </c>
+      <c r="AL150">
+        <v>0.0145803412240497</v>
+      </c>
+      <c r="AM150" t="s">
+        <v>248</v>
+      </c>
+      <c r="AN150">
+        <v>0.1052173371212367</v>
+      </c>
+      <c r="AO150">
+        <v>0.1422908955763517</v>
+      </c>
+      <c r="AP150">
+        <v>-5437.8289288</v>
+      </c>
+      <c r="AQ150">
+        <v>-509.2341644</v>
+      </c>
+      <c r="AR150">
+        <v>63561.10107120041</v>
+      </c>
+      <c r="AS150">
+        <v>19381.75783559991</v>
+      </c>
+      <c r="AT150">
+        <v>63566.64507120042</v>
+      </c>
+      <c r="AU150">
+        <v>19378.62183559991</v>
+      </c>
+      <c r="AV150">
+        <v>5.356110107120041</v>
+      </c>
+      <c r="AW150">
+        <v>0.9381757835599907</v>
+      </c>
+      <c r="AX150">
+        <v>1.525780859018517</v>
+      </c>
+      <c r="AY150">
+        <v>1.524943360696737</v>
+      </c>
+      <c r="AZ150">
+        <v>87.7</v>
+      </c>
+      <c r="BA150">
+        <v>28.91666666666667</v>
+      </c>
+      <c r="BB150">
+        <v>0.02804992422942258</v>
+      </c>
+      <c r="BC150">
+        <v>0.101492898362162</v>
+      </c>
+      <c r="BD150">
+        <v>-1702.675432999957</v>
+      </c>
+      <c r="BE150">
+        <v>-1117.259333762713</v>
+      </c>
+      <c r="BF150">
+        <v>5099</v>
+      </c>
+      <c r="BG150">
+        <v>3180</v>
+      </c>
+      <c r="BH150">
+        <v>719.8944444444445</v>
+      </c>
+      <c r="BI150">
+        <v>6225</v>
+      </c>
+      <c r="BJ150">
+        <v>8150</v>
+      </c>
+      <c r="BK150">
+        <v>11324</v>
+      </c>
+      <c r="BL150">
+        <v>11330</v>
+      </c>
+      <c r="BM150">
+        <v>0</v>
+      </c>
+      <c r="BN150">
+        <v>0</v>
+      </c>
+      <c r="BO150">
+        <v>3707</v>
+      </c>
+      <c r="BP150">
+        <v>1498</v>
+      </c>
+      <c r="BQ150">
+        <v>0</v>
+      </c>
+      <c r="BR150">
+        <v>0</v>
+      </c>
+      <c r="BS150">
+        <v>1392</v>
+      </c>
+      <c r="BT150">
+        <v>1682</v>
+      </c>
+      <c r="BU150">
+        <v>6225</v>
+      </c>
+      <c r="BV150">
+        <v>8150</v>
+      </c>
+      <c r="BW150">
+        <v>53561.10107120006</v>
+      </c>
+      <c r="BX150">
+        <v>9381.757835599999</v>
+      </c>
+      <c r="BY150">
+        <v>0.1065560555224762</v>
+      </c>
+      <c r="BZ150">
+        <v>0.1288135907755846</v>
+      </c>
+      <c r="CA150">
+        <v>0.3159385223888543</v>
+      </c>
+      <c r="CB150">
+        <v>0.2044206398356833</v>
+      </c>
+      <c r="CC150">
+        <v>0.00761570951345348</v>
+      </c>
+      <c r="CD150">
+        <v>0.01632641140004124</v>
+      </c>
+      <c r="CE150">
+        <v>0.01819615986433238</v>
+      </c>
+      <c r="CF150">
+        <v>0.02158142171559226</v>
+      </c>
+      <c r="CG150">
+        <v>58998.93000000007</v>
+      </c>
+      <c r="CH150">
+        <v>9890.992</v>
+      </c>
+      <c r="CI150">
+        <v>60701.60543300002</v>
+      </c>
+      <c r="CJ150">
+        <v>11008.25133376271</v>
+      </c>
+      <c r="CK150">
+        <v>0.160877088081651</v>
+      </c>
+      <c r="CL150">
+        <v>0.08999420299093955</v>
+      </c>
+      <c r="CM150">
+        <v>10000</v>
+      </c>
+      <c r="CO150">
+        <v>0.06574454540193299</v>
+      </c>
+      <c r="CP150">
+        <v>0.01857746397360958</v>
+      </c>
+      <c r="CQ150">
+        <v>32833998.37467036</v>
+      </c>
+      <c r="CR150">
+        <v>17337418.88034286</v>
+      </c>
+      <c r="CS150" s="2">
+        <v>45575.00694019538</v>
+      </c>
+      <c r="CT150">
+        <v>-0.5012563658078123</v>
+      </c>
+      <c r="CU150">
+        <v>-0.6854369979414622</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update LOOMUSDT.json at 2024-10-10_04-06-35 bestfile_scores 0.001794934738583498 bestfile_sharp 0.11131064614801324
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="393">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -758,6 +758,9 @@
   </si>
   <si>
     <t>QNTUSDT</t>
+  </si>
+  <si>
+    <t>TLMUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1551,7 +1554,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU150"/>
+  <dimension ref="A1:CU151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1969,7 +1972,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2134,7 +2137,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2250,7 +2253,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2415,7 +2418,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2531,7 +2534,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2696,7 +2699,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2812,7 +2815,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -2977,7 +2980,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3093,7 +3096,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3258,7 +3261,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3374,7 +3377,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3539,7 +3542,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3655,7 +3658,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3820,7 +3823,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3936,7 +3939,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4101,7 +4104,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4217,7 +4220,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4382,7 +4385,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4498,7 +4501,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4663,7 +4666,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4779,7 +4782,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4944,7 +4947,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5060,7 +5063,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5225,7 +5228,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5341,7 +5344,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5506,7 +5509,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5622,7 +5625,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5787,7 +5790,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5903,7 +5906,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6068,7 +6071,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6184,7 +6187,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6349,7 +6352,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6465,7 +6468,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6630,7 +6633,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6746,7 +6749,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6911,7 +6914,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7027,7 +7030,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7192,7 +7195,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7308,7 +7311,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7473,7 +7476,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7589,7 +7592,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7754,7 +7757,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7870,7 +7873,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8035,7 +8038,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8151,7 +8154,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8316,7 +8319,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8432,7 +8435,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8597,7 +8600,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8713,7 +8716,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8878,7 +8881,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -8994,7 +8997,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9159,7 +9162,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9275,7 +9278,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9440,7 +9443,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9556,7 +9559,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9721,7 +9724,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9837,7 +9840,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10002,7 +10005,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10118,7 +10121,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10283,7 +10286,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10399,7 +10402,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10564,7 +10567,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10680,7 +10683,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10845,7 +10848,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10961,7 +10964,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11126,7 +11129,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11248,7 +11251,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11413,7 +11416,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11535,7 +11538,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11700,7 +11703,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11822,7 +11825,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -11987,7 +11990,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12109,7 +12112,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12274,7 +12277,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12396,7 +12399,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12561,7 +12564,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12683,7 +12686,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12848,7 +12851,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12970,7 +12973,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13135,7 +13138,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13257,7 +13260,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13422,7 +13425,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13544,7 +13547,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13709,7 +13712,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13831,7 +13834,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -13996,7 +13999,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14118,7 +14121,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14283,7 +14286,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14405,7 +14408,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14570,7 +14573,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14692,7 +14695,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14857,7 +14860,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -14979,7 +14982,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15144,7 +15147,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15266,7 +15269,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15431,7 +15434,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15553,7 +15556,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15718,7 +15721,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15840,7 +15843,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16005,7 +16008,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16127,7 +16130,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16292,7 +16295,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16414,7 +16417,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16579,7 +16582,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16701,7 +16704,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16866,7 +16869,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -16985,7 +16988,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17150,7 +17153,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17266,7 +17269,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17431,7 +17434,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17544,7 +17547,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17709,7 +17712,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17822,7 +17825,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -17987,7 +17990,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18100,7 +18103,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18265,7 +18268,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18378,7 +18381,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18543,7 +18546,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18656,7 +18659,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18821,7 +18824,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18934,7 +18937,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19099,7 +19102,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19212,7 +19215,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19377,7 +19380,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19490,7 +19493,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19655,7 +19658,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19768,7 +19771,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19933,7 +19936,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20046,7 +20049,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20217,7 +20220,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20330,7 +20333,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20501,7 +20504,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20614,7 +20617,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20785,7 +20788,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20898,7 +20901,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21069,7 +21072,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21179,7 +21182,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21350,7 +21353,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21457,7 +21460,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21628,7 +21631,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21732,7 +21735,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21903,7 +21906,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22007,7 +22010,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22178,7 +22181,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22282,7 +22285,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22453,7 +22456,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22557,7 +22560,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22728,7 +22731,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22832,7 +22835,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23003,7 +23006,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23107,7 +23110,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23278,7 +23281,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23379,7 +23382,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23550,7 +23553,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23651,7 +23654,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23822,7 +23825,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23923,7 +23926,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24094,7 +24097,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24195,7 +24198,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24366,7 +24369,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24467,7 +24470,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24638,7 +24641,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24739,7 +24742,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24910,7 +24913,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25011,7 +25014,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25182,7 +25185,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25280,7 +25283,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25451,7 +25454,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25549,7 +25552,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25720,7 +25723,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25818,7 +25821,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -25989,7 +25992,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26087,7 +26090,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26258,7 +26261,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26356,7 +26359,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26527,7 +26530,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26625,7 +26628,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26796,7 +26799,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26894,7 +26897,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27065,7 +27068,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27163,7 +27166,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27334,7 +27337,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27432,7 +27435,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27603,7 +27606,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27701,7 +27704,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27872,7 +27875,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27970,7 +27973,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28141,7 +28144,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28239,7 +28242,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28410,7 +28413,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28508,7 +28511,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28679,7 +28682,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28777,7 +28780,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28948,7 +28951,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29046,7 +29049,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29217,7 +29220,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29315,7 +29318,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29486,7 +29489,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29584,7 +29587,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29755,7 +29758,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29853,7 +29856,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30024,7 +30027,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30122,7 +30125,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30293,7 +30296,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30391,7 +30394,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30562,7 +30565,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30660,7 +30663,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30831,7 +30834,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30929,7 +30932,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31100,7 +31103,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31198,7 +31201,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31369,7 +31372,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31467,7 +31470,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31638,7 +31641,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31736,7 +31739,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31907,7 +31910,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32005,7 +32008,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32176,7 +32179,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32274,7 +32277,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32445,7 +32448,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32543,7 +32546,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32714,7 +32717,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32812,7 +32815,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -32983,7 +32986,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33081,7 +33084,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33252,7 +33255,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33350,7 +33353,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33521,7 +33524,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33619,7 +33622,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33790,7 +33793,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33888,7 +33891,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34059,7 +34062,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34157,7 +34160,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34328,7 +34331,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34426,7 +34429,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34597,7 +34600,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34695,7 +34698,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34866,7 +34869,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34964,7 +34967,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35135,7 +35138,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35233,7 +35236,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35404,7 +35407,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35502,7 +35505,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35673,7 +35676,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35771,7 +35774,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35942,7 +35945,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36040,7 +36043,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36211,7 +36214,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36309,7 +36312,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36480,7 +36483,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36578,7 +36581,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36749,7 +36752,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36847,7 +36850,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37018,7 +37021,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37116,7 +37119,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37287,7 +37290,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37385,7 +37388,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37556,7 +37559,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37654,7 +37657,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37825,7 +37828,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37923,7 +37926,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38094,7 +38097,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38192,7 +38195,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38363,7 +38366,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38461,7 +38464,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38632,7 +38635,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38730,7 +38733,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38901,7 +38904,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -38999,7 +39002,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39170,7 +39173,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39268,7 +39271,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39439,7 +39442,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39537,7 +39540,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39708,7 +39711,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39806,7 +39809,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -39977,7 +39980,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40075,7 +40078,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40246,7 +40249,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40344,7 +40347,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40515,7 +40518,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40613,7 +40616,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40784,7 +40787,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40882,7 +40885,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41053,7 +41056,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41151,7 +41154,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41322,7 +41325,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41420,7 +41423,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41591,7 +41594,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41689,7 +41692,7 @@
         <v>0.006328270379966137</v>
       </c>
       <c r="AM146" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN146">
         <v>0.08370784758312214</v>
@@ -41958,7 +41961,7 @@
         <v>0.0110592804278049</v>
       </c>
       <c r="AM147" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN147">
         <v>0.07581655721931389</v>
@@ -42227,7 +42230,7 @@
         <v>0.01450048649474174</v>
       </c>
       <c r="AM148" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN148">
         <v>0.09614621483891075</v>
@@ -42496,7 +42499,7 @@
         <v>0.01189559910110707</v>
       </c>
       <c r="AM149" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN149">
         <v>0.01288397198120313</v>
@@ -42765,7 +42768,7 @@
         <v>0.0145803412240497</v>
       </c>
       <c r="AM150" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN150">
         <v>0.1052173371212367</v>
@@ -42943,6 +42946,275 @@
       </c>
       <c r="CU150">
         <v>-0.6854369979414622</v>
+      </c>
+    </row>
+    <row r="151" spans="10:99">
+      <c r="J151" t="s">
+        <v>248</v>
+      </c>
+      <c r="K151">
+        <v>0.0004889751460581682</v>
+      </c>
+      <c r="L151">
+        <v>0.0004889751460581682</v>
+      </c>
+      <c r="M151">
+        <v>0.001709378566585373</v>
+      </c>
+      <c r="N151">
+        <v>0.001709378566585373</v>
+      </c>
+      <c r="O151">
+        <v>0.0007689356096738376</v>
+      </c>
+      <c r="P151">
+        <v>0.0007689356096738376</v>
+      </c>
+      <c r="Q151">
+        <v>0.002002788080264839</v>
+      </c>
+      <c r="R151">
+        <v>0.002002788080264839</v>
+      </c>
+      <c r="S151">
+        <v>7.223205936772576</v>
+      </c>
+      <c r="T151">
+        <v>16.9926188249806</v>
+      </c>
+      <c r="U151">
+        <v>0.989797691564847</v>
+      </c>
+      <c r="V151">
+        <v>0.6203927586512562</v>
+      </c>
+      <c r="W151">
+        <v>0.09704516324914551</v>
+      </c>
+      <c r="X151">
+        <v>0.08581802375544875</v>
+      </c>
+      <c r="Y151">
+        <v>0.2260118711704399</v>
+      </c>
+      <c r="Z151">
+        <v>0.2343469939091802</v>
+      </c>
+      <c r="AA151">
+        <v>0.997659412701151</v>
+      </c>
+      <c r="AB151">
+        <v>0.8383142336620037</v>
+      </c>
+      <c r="AC151">
+        <v>0.8345867302162592</v>
+      </c>
+      <c r="AD151">
+        <v>0.998162995191141</v>
+      </c>
+      <c r="AE151">
+        <v>0.7750113426019666</v>
+      </c>
+      <c r="AF151">
+        <v>0.7657348628169798</v>
+      </c>
+      <c r="AG151">
+        <v>0.01090935033557136</v>
+      </c>
+      <c r="AH151">
+        <v>0.01019614862437938</v>
+      </c>
+      <c r="AI151">
+        <v>0.997659412701151</v>
+      </c>
+      <c r="AJ151">
+        <v>0.998162995191141</v>
+      </c>
+      <c r="AK151">
+        <v>0.01090935033557136</v>
+      </c>
+      <c r="AL151">
+        <v>0.01019614862437938</v>
+      </c>
+      <c r="AM151" t="s">
+        <v>249</v>
+      </c>
+      <c r="AN151">
+        <v>0.07035209557900164</v>
+      </c>
+      <c r="AO151">
+        <v>0.0684678617479156</v>
+      </c>
+      <c r="AP151">
+        <v>-109.5132048776</v>
+      </c>
+      <c r="AQ151">
+        <v>-988.567962685</v>
+      </c>
+      <c r="AR151">
+        <v>13139.19966116715</v>
+      </c>
+      <c r="AS151">
+        <v>25956.44746031509</v>
+      </c>
+      <c r="AT151">
+        <v>13135.85989312238</v>
+      </c>
+      <c r="AU151">
+        <v>25956.44746031509</v>
+      </c>
+      <c r="AV151">
+        <v>0.3139199661167151</v>
+      </c>
+      <c r="AW151">
+        <v>1.595644746031509</v>
+      </c>
+      <c r="AX151">
+        <v>3.32312174559881</v>
+      </c>
+      <c r="AY151">
+        <v>1.411483472090491</v>
+      </c>
+      <c r="AZ151">
+        <v>39.68333333333333</v>
+      </c>
+      <c r="BA151">
+        <v>95.96666666666667</v>
+      </c>
+      <c r="BB151">
+        <v>0.1183423036579189</v>
+      </c>
+      <c r="BC151">
+        <v>0.06807842690570609</v>
+      </c>
+      <c r="BD151">
+        <v>-436.0651147105605</v>
+      </c>
+      <c r="BE151">
+        <v>-1237.861669046313</v>
+      </c>
+      <c r="BF151">
+        <v>2213</v>
+      </c>
+      <c r="BG151">
+        <v>3589</v>
+      </c>
+      <c r="BH151">
+        <v>558.4777777777778</v>
+      </c>
+      <c r="BI151">
+        <v>1821</v>
+      </c>
+      <c r="BJ151">
+        <v>5901</v>
+      </c>
+      <c r="BK151">
+        <v>4034</v>
+      </c>
+      <c r="BL151">
+        <v>9490</v>
+      </c>
+      <c r="BM151">
+        <v>0</v>
+      </c>
+      <c r="BN151">
+        <v>0</v>
+      </c>
+      <c r="BO151">
+        <v>23</v>
+      </c>
+      <c r="BP151">
+        <v>2253</v>
+      </c>
+      <c r="BQ151">
+        <v>0</v>
+      </c>
+      <c r="BR151">
+        <v>0</v>
+      </c>
+      <c r="BS151">
+        <v>2190</v>
+      </c>
+      <c r="BT151">
+        <v>1336</v>
+      </c>
+      <c r="BU151">
+        <v>1821</v>
+      </c>
+      <c r="BV151">
+        <v>5901</v>
+      </c>
+      <c r="BW151">
+        <v>3139.19966116717</v>
+      </c>
+      <c r="BX151">
+        <v>15956.44746031501</v>
+      </c>
+      <c r="BY151">
+        <v>0.1054376816774095</v>
+      </c>
+      <c r="BZ151">
+        <v>0.07499381052651015</v>
+      </c>
+      <c r="CA151">
+        <v>0.2873419284073879</v>
+      </c>
+      <c r="CB151">
+        <v>0.1897998925870064</v>
+      </c>
+      <c r="CC151">
+        <v>0.01685538478740925</v>
+      </c>
+      <c r="CD151">
+        <v>0.007799173724412807</v>
+      </c>
+      <c r="CE151">
+        <v>0.01760304476708733</v>
+      </c>
+      <c r="CF151">
+        <v>0.0124928651309224</v>
+      </c>
+      <c r="CG151">
+        <v>3248.71286604477</v>
+      </c>
+      <c r="CH151">
+        <v>16945.01542300001</v>
+      </c>
+      <c r="CI151">
+        <v>3684.777980755331</v>
+      </c>
+      <c r="CJ151">
+        <v>18182.87709204632</v>
+      </c>
+      <c r="CK151">
+        <v>0.05688459322482251</v>
+      </c>
+      <c r="CL151">
+        <v>0.1362652762028879</v>
+      </c>
+      <c r="CM151">
+        <v>10000</v>
+      </c>
+      <c r="CO151">
+        <v>0.0319283849309959</v>
+      </c>
+      <c r="CP151">
+        <v>0.04005967922417009</v>
+      </c>
+      <c r="CQ151">
+        <v>4095426.647085047</v>
+      </c>
+      <c r="CR151">
+        <v>15495136.44702353</v>
+      </c>
+      <c r="CS151" s="2">
+        <v>45575.08684452761</v>
+      </c>
+      <c r="CT151">
+        <v>-0.7729306388360467</v>
+      </c>
+      <c r="CU151">
+        <v>-0.5971770314221732</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update PENDLEUSDT.json at 2024-10-10_06-12-04 bestfile_scores 0.0016271703720683428 bestfile_sharp 0.12706596041596985
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="394">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -761,6 +761,9 @@
   </si>
   <si>
     <t>TLMUSDT</t>
+  </si>
+  <si>
+    <t>LOOMUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1554,7 +1557,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU151"/>
+  <dimension ref="A1:CU152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1972,7 +1975,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2137,7 +2140,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2253,7 +2256,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2418,7 +2421,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2534,7 +2537,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2699,7 +2702,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2815,7 +2818,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -2980,7 +2983,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3096,7 +3099,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3261,7 +3264,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3377,7 +3380,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3542,7 +3545,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3658,7 +3661,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3823,7 +3826,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3939,7 +3942,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4104,7 +4107,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4220,7 +4223,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4385,7 +4388,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4501,7 +4504,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4666,7 +4669,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4782,7 +4785,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4947,7 +4950,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5063,7 +5066,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5228,7 +5231,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5344,7 +5347,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5509,7 +5512,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5625,7 +5628,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5790,7 +5793,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5906,7 +5909,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6071,7 +6074,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6187,7 +6190,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6352,7 +6355,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6468,7 +6471,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6633,7 +6636,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6749,7 +6752,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6914,7 +6917,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7030,7 +7033,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7195,7 +7198,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7311,7 +7314,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7476,7 +7479,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7592,7 +7595,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7757,7 +7760,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7873,7 +7876,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8038,7 +8041,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8154,7 +8157,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8319,7 +8322,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8435,7 +8438,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8600,7 +8603,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8716,7 +8719,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8881,7 +8884,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -8997,7 +9000,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9162,7 +9165,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9278,7 +9281,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9443,7 +9446,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9559,7 +9562,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9724,7 +9727,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9840,7 +9843,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10005,7 +10008,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10121,7 +10124,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10286,7 +10289,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10402,7 +10405,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10567,7 +10570,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10683,7 +10686,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10848,7 +10851,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10964,7 +10967,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11129,7 +11132,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11251,7 +11254,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11416,7 +11419,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11538,7 +11541,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11703,7 +11706,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11825,7 +11828,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -11990,7 +11993,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12112,7 +12115,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12277,7 +12280,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12399,7 +12402,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12564,7 +12567,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12686,7 +12689,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12851,7 +12854,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12973,7 +12976,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13138,7 +13141,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13260,7 +13263,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13425,7 +13428,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13547,7 +13550,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13712,7 +13715,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13834,7 +13837,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -13999,7 +14002,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14121,7 +14124,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14286,7 +14289,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14408,7 +14411,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14573,7 +14576,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14695,7 +14698,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14860,7 +14863,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -14982,7 +14985,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15147,7 +15150,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15269,7 +15272,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15434,7 +15437,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15556,7 +15559,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15721,7 +15724,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15843,7 +15846,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16008,7 +16011,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16130,7 +16133,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16295,7 +16298,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16417,7 +16420,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16582,7 +16585,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16704,7 +16707,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16869,7 +16872,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -16988,7 +16991,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17153,7 +17156,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17269,7 +17272,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17434,7 +17437,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17547,7 +17550,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17712,7 +17715,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17825,7 +17828,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -17990,7 +17993,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18103,7 +18106,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18268,7 +18271,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18381,7 +18384,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18546,7 +18549,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18659,7 +18662,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18824,7 +18827,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18937,7 +18940,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19102,7 +19105,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19215,7 +19218,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19380,7 +19383,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19493,7 +19496,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19658,7 +19661,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19771,7 +19774,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19936,7 +19939,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20049,7 +20052,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20220,7 +20223,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20333,7 +20336,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20504,7 +20507,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20617,7 +20620,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20788,7 +20791,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20901,7 +20904,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21072,7 +21075,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21182,7 +21185,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21353,7 +21356,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21460,7 +21463,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21631,7 +21634,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21735,7 +21738,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21906,7 +21909,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22010,7 +22013,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22181,7 +22184,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22285,7 +22288,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22456,7 +22459,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22560,7 +22563,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22731,7 +22734,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22835,7 +22838,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23006,7 +23009,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23110,7 +23113,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23281,7 +23284,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23382,7 +23385,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23553,7 +23556,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23654,7 +23657,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23825,7 +23828,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23926,7 +23929,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24097,7 +24100,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24198,7 +24201,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24369,7 +24372,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24470,7 +24473,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24641,7 +24644,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24742,7 +24745,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24913,7 +24916,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25014,7 +25017,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25185,7 +25188,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25283,7 +25286,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25454,7 +25457,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25552,7 +25555,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25723,7 +25726,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25821,7 +25824,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -25992,7 +25995,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26090,7 +26093,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26261,7 +26264,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26359,7 +26362,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26530,7 +26533,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26628,7 +26631,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26799,7 +26802,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26897,7 +26900,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27068,7 +27071,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27166,7 +27169,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27337,7 +27340,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27435,7 +27438,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27606,7 +27609,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27704,7 +27707,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27875,7 +27878,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27973,7 +27976,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28144,7 +28147,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28242,7 +28245,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28413,7 +28416,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28511,7 +28514,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28682,7 +28685,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28780,7 +28783,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28951,7 +28954,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29049,7 +29052,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29220,7 +29223,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29318,7 +29321,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29489,7 +29492,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29587,7 +29590,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29758,7 +29761,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29856,7 +29859,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30027,7 +30030,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30125,7 +30128,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30296,7 +30299,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30394,7 +30397,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30565,7 +30568,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30663,7 +30666,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30834,7 +30837,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30932,7 +30935,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31103,7 +31106,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31201,7 +31204,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31372,7 +31375,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31470,7 +31473,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31641,7 +31644,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31739,7 +31742,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31910,7 +31913,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32008,7 +32011,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32179,7 +32182,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32277,7 +32280,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32448,7 +32451,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32546,7 +32549,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32717,7 +32720,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32815,7 +32818,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -32986,7 +32989,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33084,7 +33087,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33255,7 +33258,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33353,7 +33356,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33524,7 +33527,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33622,7 +33625,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33793,7 +33796,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33891,7 +33894,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34062,7 +34065,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34160,7 +34163,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34331,7 +34334,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34429,7 +34432,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34600,7 +34603,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34698,7 +34701,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34869,7 +34872,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34967,7 +34970,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35138,7 +35141,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35236,7 +35239,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35407,7 +35410,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35505,7 +35508,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35676,7 +35679,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35774,7 +35777,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35945,7 +35948,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36043,7 +36046,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36214,7 +36217,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36312,7 +36315,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36483,7 +36486,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36581,7 +36584,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36752,7 +36755,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36850,7 +36853,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37021,7 +37024,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37119,7 +37122,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37290,7 +37293,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37388,7 +37391,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37559,7 +37562,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37657,7 +37660,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37828,7 +37831,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37926,7 +37929,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38097,7 +38100,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38195,7 +38198,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38366,7 +38369,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38464,7 +38467,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38635,7 +38638,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38733,7 +38736,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38904,7 +38907,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -39002,7 +39005,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39173,7 +39176,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39271,7 +39274,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39442,7 +39445,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39540,7 +39543,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39711,7 +39714,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39809,7 +39812,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -39980,7 +39983,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40078,7 +40081,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40249,7 +40252,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40347,7 +40350,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40518,7 +40521,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40616,7 +40619,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40787,7 +40790,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40885,7 +40888,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41056,7 +41059,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41154,7 +41157,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41325,7 +41328,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41423,7 +41426,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41594,7 +41597,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41692,7 +41695,7 @@
         <v>0.006328270379966137</v>
       </c>
       <c r="AM146" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN146">
         <v>0.08370784758312214</v>
@@ -41961,7 +41964,7 @@
         <v>0.0110592804278049</v>
       </c>
       <c r="AM147" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN147">
         <v>0.07581655721931389</v>
@@ -42230,7 +42233,7 @@
         <v>0.01450048649474174</v>
       </c>
       <c r="AM148" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN148">
         <v>0.09614621483891075</v>
@@ -42499,7 +42502,7 @@
         <v>0.01189559910110707</v>
       </c>
       <c r="AM149" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN149">
         <v>0.01288397198120313</v>
@@ -42768,7 +42771,7 @@
         <v>0.0145803412240497</v>
       </c>
       <c r="AM150" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN150">
         <v>0.1052173371212367</v>
@@ -43037,7 +43040,7 @@
         <v>0.01019614862437938</v>
       </c>
       <c r="AM151" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN151">
         <v>0.07035209557900164</v>
@@ -43215,6 +43218,275 @@
       </c>
       <c r="CU151">
         <v>-0.5971770314221732</v>
+      </c>
+    </row>
+    <row r="152" spans="10:99">
+      <c r="J152" t="s">
+        <v>249</v>
+      </c>
+      <c r="K152">
+        <v>0.001173357377818318</v>
+      </c>
+      <c r="L152">
+        <v>0.001173357377818318</v>
+      </c>
+      <c r="M152">
+        <v>0.002129192517102529</v>
+      </c>
+      <c r="N152">
+        <v>0.002129192517102529</v>
+      </c>
+      <c r="O152">
+        <v>0.001094071234133698</v>
+      </c>
+      <c r="P152">
+        <v>0.001094071234133698</v>
+      </c>
+      <c r="Q152">
+        <v>0.002783117825279446</v>
+      </c>
+      <c r="R152">
+        <v>0.002783117825279446</v>
+      </c>
+      <c r="S152">
+        <v>8.723303419914082</v>
+      </c>
+      <c r="T152">
+        <v>9.903838803870908</v>
+      </c>
+      <c r="U152">
+        <v>0.9908408582089593</v>
+      </c>
+      <c r="V152">
+        <v>0.6466825812721239</v>
+      </c>
+      <c r="W152">
+        <v>0.0962517256195405</v>
+      </c>
+      <c r="X152">
+        <v>0.09715084619866743</v>
+      </c>
+      <c r="Y152">
+        <v>0.190330478027451</v>
+      </c>
+      <c r="Z152">
+        <v>0.216596380733302</v>
+      </c>
+      <c r="AA152">
+        <v>0.9971575779271823</v>
+      </c>
+      <c r="AB152">
+        <v>0.8318663458843295</v>
+      </c>
+      <c r="AC152">
+        <v>0.8463690609989255</v>
+      </c>
+      <c r="AD152">
+        <v>0.997739566636169</v>
+      </c>
+      <c r="AE152">
+        <v>0.810127869857635</v>
+      </c>
+      <c r="AF152">
+        <v>0.7854470833588312</v>
+      </c>
+      <c r="AG152">
+        <v>0.0124811775556087</v>
+      </c>
+      <c r="AH152">
+        <v>0.01085520881764603</v>
+      </c>
+      <c r="AI152">
+        <v>0.9971575779271823</v>
+      </c>
+      <c r="AJ152">
+        <v>0.997739566636169</v>
+      </c>
+      <c r="AK152">
+        <v>0.0124811775556087</v>
+      </c>
+      <c r="AL152">
+        <v>0.01085520881764603</v>
+      </c>
+      <c r="AM152" t="s">
+        <v>250</v>
+      </c>
+      <c r="AN152">
+        <v>0.0930850934199607</v>
+      </c>
+      <c r="AO152">
+        <v>0.1035385465850781</v>
+      </c>
+      <c r="AP152">
+        <v>-226.385296326</v>
+      </c>
+      <c r="AQ152">
+        <v>-399.77997479</v>
+      </c>
+      <c r="AR152">
+        <v>15313.37586648095</v>
+      </c>
+      <c r="AS152">
+        <v>21660.69385520996</v>
+      </c>
+      <c r="AT152">
+        <v>15316.29103367401</v>
+      </c>
+      <c r="AU152">
+        <v>21649.77829520996</v>
+      </c>
+      <c r="AV152">
+        <v>0.5313375866480952</v>
+      </c>
+      <c r="AW152">
+        <v>1.166069385520996</v>
+      </c>
+      <c r="AX152">
+        <v>2.752093194488272</v>
+      </c>
+      <c r="AY152">
+        <v>2.423105428942005</v>
+      </c>
+      <c r="AZ152">
+        <v>71.43333333333334</v>
+      </c>
+      <c r="BA152">
+        <v>46.81666666666667</v>
+      </c>
+      <c r="BB152">
+        <v>0.04668199064095184</v>
+      </c>
+      <c r="BC152">
+        <v>0.08403656921949275</v>
+      </c>
+      <c r="BD152">
+        <v>-271.270526955778</v>
+      </c>
+      <c r="BE152">
+        <v>-1106.507978130787</v>
+      </c>
+      <c r="BF152">
+        <v>1229</v>
+      </c>
+      <c r="BG152">
+        <v>2313</v>
+      </c>
+      <c r="BH152">
+        <v>363.3944444444444</v>
+      </c>
+      <c r="BI152">
+        <v>1941</v>
+      </c>
+      <c r="BJ152">
+        <v>1286</v>
+      </c>
+      <c r="BK152">
+        <v>3170</v>
+      </c>
+      <c r="BL152">
+        <v>3599</v>
+      </c>
+      <c r="BM152">
+        <v>0</v>
+      </c>
+      <c r="BN152">
+        <v>0</v>
+      </c>
+      <c r="BO152">
+        <v>854</v>
+      </c>
+      <c r="BP152">
+        <v>363</v>
+      </c>
+      <c r="BQ152">
+        <v>0</v>
+      </c>
+      <c r="BR152">
+        <v>0</v>
+      </c>
+      <c r="BS152">
+        <v>375</v>
+      </c>
+      <c r="BT152">
+        <v>1950</v>
+      </c>
+      <c r="BU152">
+        <v>1941</v>
+      </c>
+      <c r="BV152">
+        <v>1286</v>
+      </c>
+      <c r="BW152">
+        <v>5313.375866480946</v>
+      </c>
+      <c r="BX152">
+        <v>11660.69385521003</v>
+      </c>
+      <c r="BY152">
+        <v>0.1073635732580613</v>
+      </c>
+      <c r="BZ152">
+        <v>0.08574876154539714</v>
+      </c>
+      <c r="CA152">
+        <v>0.2343685863867914</v>
+      </c>
+      <c r="CB152">
+        <v>0.1766479714453114</v>
+      </c>
+      <c r="CC152">
+        <v>0.01163497331758421</v>
+      </c>
+      <c r="CD152">
+        <v>0.01114707901096373</v>
+      </c>
+      <c r="CE152">
+        <v>0.01727189610731973</v>
+      </c>
+      <c r="CF152">
+        <v>0.01231652404133699</v>
+      </c>
+      <c r="CG152">
+        <v>5539.761162806945</v>
+      </c>
+      <c r="CH152">
+        <v>12060.47383000003</v>
+      </c>
+      <c r="CI152">
+        <v>5811.031689762724</v>
+      </c>
+      <c r="CJ152">
+        <v>13166.98180813082</v>
+      </c>
+      <c r="CK152">
+        <v>0.1113106461480132</v>
+      </c>
+      <c r="CL152">
+        <v>0.1254283168267084</v>
+      </c>
+      <c r="CM152">
+        <v>10000</v>
+      </c>
+      <c r="CO152">
+        <v>0.06041499484122435</v>
+      </c>
+      <c r="CP152">
+        <v>0.02762810959532271</v>
+      </c>
+      <c r="CQ152">
+        <v>5301113.447515012</v>
+      </c>
+      <c r="CR152">
+        <v>7433235.41422287</v>
+      </c>
+      <c r="CS152" s="2">
+        <v>45575.1712671494</v>
+      </c>
+      <c r="CT152">
+        <v>-0.6607322796180672</v>
+      </c>
+      <c r="CU152">
+        <v>-0.4916064901626342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update RADUSDT.json at 2024-10-10_08-38-11 bestfile_scores 0.0009969173786225193 bestfile_sharp 0.12467836925057742
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="395">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -764,6 +764,9 @@
   </si>
   <si>
     <t>LOOMUSDT</t>
+  </si>
+  <si>
+    <t>PENDLEUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1557,7 +1560,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU152"/>
+  <dimension ref="A1:CU153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1975,7 +1978,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2140,7 +2143,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2256,7 +2259,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2421,7 +2424,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2537,7 +2540,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2702,7 +2705,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2818,7 +2821,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -2983,7 +2986,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3099,7 +3102,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3264,7 +3267,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3380,7 +3383,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3545,7 +3548,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3661,7 +3664,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3826,7 +3829,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3942,7 +3945,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4107,7 +4110,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4223,7 +4226,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4388,7 +4391,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4504,7 +4507,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4669,7 +4672,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4785,7 +4788,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4950,7 +4953,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5066,7 +5069,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5231,7 +5234,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5347,7 +5350,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5512,7 +5515,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5628,7 +5631,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5793,7 +5796,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5909,7 +5912,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6074,7 +6077,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6190,7 +6193,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6355,7 +6358,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6471,7 +6474,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6636,7 +6639,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6752,7 +6755,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6917,7 +6920,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7033,7 +7036,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7198,7 +7201,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7314,7 +7317,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7479,7 +7482,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7595,7 +7598,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7760,7 +7763,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7876,7 +7879,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8041,7 +8044,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8157,7 +8160,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8322,7 +8325,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8438,7 +8441,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8603,7 +8606,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8719,7 +8722,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8884,7 +8887,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -9000,7 +9003,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9165,7 +9168,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9281,7 +9284,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9446,7 +9449,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9562,7 +9565,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9727,7 +9730,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9843,7 +9846,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10008,7 +10011,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10124,7 +10127,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10289,7 +10292,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10405,7 +10408,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10570,7 +10573,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10686,7 +10689,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10851,7 +10854,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10967,7 +10970,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11132,7 +11135,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11254,7 +11257,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11419,7 +11422,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11541,7 +11544,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11706,7 +11709,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11828,7 +11831,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -11993,7 +11996,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12115,7 +12118,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12280,7 +12283,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12402,7 +12405,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12567,7 +12570,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12689,7 +12692,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12854,7 +12857,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12976,7 +12979,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13141,7 +13144,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13263,7 +13266,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13428,7 +13431,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13550,7 +13553,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13715,7 +13718,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13837,7 +13840,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -14002,7 +14005,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14124,7 +14127,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14289,7 +14292,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14411,7 +14414,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14576,7 +14579,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14698,7 +14701,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14863,7 +14866,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -14985,7 +14988,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15150,7 +15153,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15272,7 +15275,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15437,7 +15440,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15559,7 +15562,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15724,7 +15727,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15846,7 +15849,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16011,7 +16014,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16133,7 +16136,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16298,7 +16301,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16420,7 +16423,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16585,7 +16588,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16707,7 +16710,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16872,7 +16875,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -16991,7 +16994,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17156,7 +17159,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17272,7 +17275,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17437,7 +17440,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17550,7 +17553,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17715,7 +17718,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17828,7 +17831,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -17993,7 +17996,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18106,7 +18109,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18271,7 +18274,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18384,7 +18387,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18549,7 +18552,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18662,7 +18665,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18827,7 +18830,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18940,7 +18943,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19105,7 +19108,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19218,7 +19221,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19383,7 +19386,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19496,7 +19499,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19661,7 +19664,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19774,7 +19777,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19939,7 +19942,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20052,7 +20055,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20223,7 +20226,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20336,7 +20339,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20507,7 +20510,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20620,7 +20623,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20791,7 +20794,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20904,7 +20907,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21075,7 +21078,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21185,7 +21188,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21356,7 +21359,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21463,7 +21466,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21634,7 +21637,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21738,7 +21741,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21909,7 +21912,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22013,7 +22016,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22184,7 +22187,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22288,7 +22291,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22459,7 +22462,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22563,7 +22566,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22734,7 +22737,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22838,7 +22841,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23009,7 +23012,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23113,7 +23116,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23284,7 +23287,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23385,7 +23388,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23556,7 +23559,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23657,7 +23660,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23828,7 +23831,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23929,7 +23932,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24100,7 +24103,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24201,7 +24204,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24372,7 +24375,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24473,7 +24476,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24644,7 +24647,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24745,7 +24748,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24916,7 +24919,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25017,7 +25020,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25188,7 +25191,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25286,7 +25289,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25457,7 +25460,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25555,7 +25558,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25726,7 +25729,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25824,7 +25827,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -25995,7 +25998,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26093,7 +26096,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26264,7 +26267,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26362,7 +26365,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26533,7 +26536,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26631,7 +26634,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26802,7 +26805,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26900,7 +26903,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27071,7 +27074,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27169,7 +27172,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27340,7 +27343,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27438,7 +27441,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27609,7 +27612,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27707,7 +27710,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27878,7 +27881,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27976,7 +27979,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28147,7 +28150,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28245,7 +28248,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28416,7 +28419,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28514,7 +28517,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28685,7 +28688,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28783,7 +28786,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28954,7 +28957,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29052,7 +29055,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29223,7 +29226,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29321,7 +29324,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29492,7 +29495,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29590,7 +29593,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29761,7 +29764,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29859,7 +29862,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30030,7 +30033,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30128,7 +30131,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30299,7 +30302,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30397,7 +30400,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30568,7 +30571,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30666,7 +30669,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30837,7 +30840,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30935,7 +30938,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31106,7 +31109,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31204,7 +31207,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31375,7 +31378,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31473,7 +31476,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31644,7 +31647,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31742,7 +31745,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31913,7 +31916,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32011,7 +32014,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32182,7 +32185,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32280,7 +32283,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32451,7 +32454,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32549,7 +32552,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32720,7 +32723,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32818,7 +32821,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -32989,7 +32992,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33087,7 +33090,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33258,7 +33261,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33356,7 +33359,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33527,7 +33530,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33625,7 +33628,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33796,7 +33799,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33894,7 +33897,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34065,7 +34068,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34163,7 +34166,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34334,7 +34337,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34432,7 +34435,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34603,7 +34606,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34701,7 +34704,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34872,7 +34875,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34970,7 +34973,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35141,7 +35144,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35239,7 +35242,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35410,7 +35413,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35508,7 +35511,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35679,7 +35682,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35777,7 +35780,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35948,7 +35951,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36046,7 +36049,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36217,7 +36220,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36315,7 +36318,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36486,7 +36489,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36584,7 +36587,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36755,7 +36758,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36853,7 +36856,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37024,7 +37027,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37122,7 +37125,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37293,7 +37296,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37391,7 +37394,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37562,7 +37565,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37660,7 +37663,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37831,7 +37834,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37929,7 +37932,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38100,7 +38103,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38198,7 +38201,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38369,7 +38372,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38467,7 +38470,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38638,7 +38641,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38736,7 +38739,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38907,7 +38910,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -39005,7 +39008,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39176,7 +39179,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39274,7 +39277,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39445,7 +39448,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39543,7 +39546,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39714,7 +39717,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39812,7 +39815,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -39983,7 +39986,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40081,7 +40084,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40252,7 +40255,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40350,7 +40353,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40521,7 +40524,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40619,7 +40622,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40790,7 +40793,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40888,7 +40891,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41059,7 +41062,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41157,7 +41160,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41328,7 +41331,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41426,7 +41429,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41597,7 +41600,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41695,7 +41698,7 @@
         <v>0.006328270379966137</v>
       </c>
       <c r="AM146" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN146">
         <v>0.08370784758312214</v>
@@ -41964,7 +41967,7 @@
         <v>0.0110592804278049</v>
       </c>
       <c r="AM147" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN147">
         <v>0.07581655721931389</v>
@@ -42233,7 +42236,7 @@
         <v>0.01450048649474174</v>
       </c>
       <c r="AM148" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN148">
         <v>0.09614621483891075</v>
@@ -42502,7 +42505,7 @@
         <v>0.01189559910110707</v>
       </c>
       <c r="AM149" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN149">
         <v>0.01288397198120313</v>
@@ -42771,7 +42774,7 @@
         <v>0.0145803412240497</v>
       </c>
       <c r="AM150" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN150">
         <v>0.1052173371212367</v>
@@ -43040,7 +43043,7 @@
         <v>0.01019614862437938</v>
       </c>
       <c r="AM151" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN151">
         <v>0.07035209557900164</v>
@@ -43309,7 +43312,7 @@
         <v>0.01085520881764603</v>
       </c>
       <c r="AM152" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN152">
         <v>0.0930850934199607</v>
@@ -43487,6 +43490,275 @@
       </c>
       <c r="CU152">
         <v>-0.4916064901626342</v>
+      </c>
+    </row>
+    <row r="153" spans="10:99">
+      <c r="J153" t="s">
+        <v>250</v>
+      </c>
+      <c r="K153">
+        <v>0.001368070472775651</v>
+      </c>
+      <c r="L153">
+        <v>0.001368070472775651</v>
+      </c>
+      <c r="M153">
+        <v>0.001894336599113755</v>
+      </c>
+      <c r="N153">
+        <v>0.001894336599113755</v>
+      </c>
+      <c r="O153">
+        <v>0.00144770463850652</v>
+      </c>
+      <c r="P153">
+        <v>0.00144770463850652</v>
+      </c>
+      <c r="Q153">
+        <v>0.001798569777877446</v>
+      </c>
+      <c r="R153">
+        <v>0.001798569777877446</v>
+      </c>
+      <c r="S153">
+        <v>13.65476386374856</v>
+      </c>
+      <c r="T153">
+        <v>8.790268477614207</v>
+      </c>
+      <c r="U153">
+        <v>0.9999603357121986</v>
+      </c>
+      <c r="V153">
+        <v>0.7195180969786101</v>
+      </c>
+      <c r="W153">
+        <v>0.09668684538324265</v>
+      </c>
+      <c r="X153">
+        <v>0.09115035791347474</v>
+      </c>
+      <c r="Y153">
+        <v>0.1305585229068082</v>
+      </c>
+      <c r="Z153">
+        <v>0.1645183356280085</v>
+      </c>
+      <c r="AA153">
+        <v>0.9972976145357619</v>
+      </c>
+      <c r="AB153">
+        <v>0.8825129210704101</v>
+      </c>
+      <c r="AC153">
+        <v>0.8518653830518763</v>
+      </c>
+      <c r="AD153">
+        <v>0.9971296998885323</v>
+      </c>
+      <c r="AE153">
+        <v>0.8724565352491152</v>
+      </c>
+      <c r="AF153">
+        <v>0.836900826996775</v>
+      </c>
+      <c r="AG153">
+        <v>0.01123461828456636</v>
+      </c>
+      <c r="AH153">
+        <v>0.01194275707748435</v>
+      </c>
+      <c r="AI153">
+        <v>0.9972976145357619</v>
+      </c>
+      <c r="AJ153">
+        <v>0.9971296998885323</v>
+      </c>
+      <c r="AK153">
+        <v>0.01123461828456636</v>
+      </c>
+      <c r="AL153">
+        <v>0.01194275707748435</v>
+      </c>
+      <c r="AM153" t="s">
+        <v>251</v>
+      </c>
+      <c r="AN153">
+        <v>0.0823051935622205</v>
+      </c>
+      <c r="AO153">
+        <v>0.09863175818738529</v>
+      </c>
+      <c r="AP153">
+        <v>-252.20926748</v>
+      </c>
+      <c r="AQ153">
+        <v>-366.1669847</v>
+      </c>
+      <c r="AR153">
+        <v>18221.7015427258</v>
+      </c>
+      <c r="AS153">
+        <v>22947.57821530013</v>
+      </c>
+      <c r="AT153">
+        <v>18213.56733251996</v>
+      </c>
+      <c r="AU153">
+        <v>22950.13291530013</v>
+      </c>
+      <c r="AV153">
+        <v>0.8221701542725806</v>
+      </c>
+      <c r="AW153">
+        <v>1.294757821530013</v>
+      </c>
+      <c r="AX153">
+        <v>1.756255562972853</v>
+      </c>
+      <c r="AY153">
+        <v>2.730386310604097</v>
+      </c>
+      <c r="AZ153">
+        <v>25</v>
+      </c>
+      <c r="BA153">
+        <v>92.3</v>
+      </c>
+      <c r="BB153">
+        <v>0.06016275141192162</v>
+      </c>
+      <c r="BC153">
+        <v>0.03927219744365017</v>
+      </c>
+      <c r="BD153">
+        <v>-542.4490147917694</v>
+      </c>
+      <c r="BE153">
+        <v>-544.2332665064964</v>
+      </c>
+      <c r="BF153">
+        <v>3547</v>
+      </c>
+      <c r="BG153">
+        <v>1071</v>
+      </c>
+      <c r="BH153">
+        <v>438.8944444444444</v>
+      </c>
+      <c r="BI153">
+        <v>2446</v>
+      </c>
+      <c r="BJ153">
+        <v>2787</v>
+      </c>
+      <c r="BK153">
+        <v>5993</v>
+      </c>
+      <c r="BL153">
+        <v>3858</v>
+      </c>
+      <c r="BM153">
+        <v>0</v>
+      </c>
+      <c r="BN153">
+        <v>0</v>
+      </c>
+      <c r="BO153">
+        <v>357</v>
+      </c>
+      <c r="BP153">
+        <v>375</v>
+      </c>
+      <c r="BQ153">
+        <v>0</v>
+      </c>
+      <c r="BR153">
+        <v>0</v>
+      </c>
+      <c r="BS153">
+        <v>3190</v>
+      </c>
+      <c r="BT153">
+        <v>696</v>
+      </c>
+      <c r="BU153">
+        <v>2446</v>
+      </c>
+      <c r="BV153">
+        <v>2787</v>
+      </c>
+      <c r="BW153">
+        <v>8221.701542725858</v>
+      </c>
+      <c r="BX153">
+        <v>12947.57821530002</v>
+      </c>
+      <c r="BY153">
+        <v>0.1022785433278477</v>
+      </c>
+      <c r="BZ153">
+        <v>0.08149525946946853</v>
+      </c>
+      <c r="CA153">
+        <v>0.1461850891198415</v>
+      </c>
+      <c r="CB153">
+        <v>0.1402230739802073</v>
+      </c>
+      <c r="CC153">
+        <v>0.0164587231047277</v>
+      </c>
+      <c r="CD153">
+        <v>0.01324916542716602</v>
+      </c>
+      <c r="CE153">
+        <v>0.01524421302410333</v>
+      </c>
+      <c r="CF153">
+        <v>0.01418823828161815</v>
+      </c>
+      <c r="CG153">
+        <v>8473.910810205858</v>
+      </c>
+      <c r="CH153">
+        <v>13313.74520000002</v>
+      </c>
+      <c r="CI153">
+        <v>9016.359824997628</v>
+      </c>
+      <c r="CJ153">
+        <v>13857.97846650652</v>
+      </c>
+      <c r="CK153">
+        <v>0.1270659604159698</v>
+      </c>
+      <c r="CL153">
+        <v>0.1338716715152697</v>
+      </c>
+      <c r="CM153">
+        <v>10000</v>
+      </c>
+      <c r="CO153">
+        <v>0.02553393450403417</v>
+      </c>
+      <c r="CP153">
+        <v>0.05154247745609872</v>
+      </c>
+      <c r="CQ153">
+        <v>7299645.936587103</v>
+      </c>
+      <c r="CR153">
+        <v>9637623.88185947</v>
+      </c>
+      <c r="CS153" s="2">
+        <v>45575.2584111198</v>
+      </c>
+      <c r="CT153">
+        <v>-0.6858826598981475</v>
+      </c>
+      <c r="CU153">
+        <v>-0.5360388336727706</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update ZKUSDT.json at 2024-10-10_09-22-15 bestfile_scores 0.005968839666992176 bestfile_sharp 0.315701294602746
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="396">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -767,6 +767,9 @@
   </si>
   <si>
     <t>PENDLEUSDT</t>
+  </si>
+  <si>
+    <t>RADUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1560,7 +1563,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU153"/>
+  <dimension ref="A1:CU154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1978,7 +1981,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2143,7 +2146,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2259,7 +2262,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2424,7 +2427,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2540,7 +2543,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2705,7 +2708,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2821,7 +2824,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -2986,7 +2989,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3102,7 +3105,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3267,7 +3270,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3383,7 +3386,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3548,7 +3551,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3664,7 +3667,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3829,7 +3832,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3945,7 +3948,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4110,7 +4113,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4226,7 +4229,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4391,7 +4394,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4507,7 +4510,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4672,7 +4675,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4788,7 +4791,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4953,7 +4956,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5069,7 +5072,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5234,7 +5237,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5350,7 +5353,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5515,7 +5518,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5631,7 +5634,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5796,7 +5799,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5912,7 +5915,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6077,7 +6080,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6193,7 +6196,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6358,7 +6361,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6474,7 +6477,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6639,7 +6642,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6755,7 +6758,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6920,7 +6923,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7036,7 +7039,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7201,7 +7204,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7317,7 +7320,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7482,7 +7485,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7598,7 +7601,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7763,7 +7766,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7879,7 +7882,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8044,7 +8047,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8160,7 +8163,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8325,7 +8328,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8441,7 +8444,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8606,7 +8609,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8722,7 +8725,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8887,7 +8890,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -9003,7 +9006,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9168,7 +9171,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9284,7 +9287,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9449,7 +9452,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9565,7 +9568,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9730,7 +9733,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9846,7 +9849,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10011,7 +10014,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10127,7 +10130,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10292,7 +10295,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10408,7 +10411,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10573,7 +10576,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10689,7 +10692,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10854,7 +10857,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10970,7 +10973,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11135,7 +11138,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11257,7 +11260,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11422,7 +11425,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11544,7 +11547,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11709,7 +11712,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11831,7 +11834,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -11996,7 +11999,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12118,7 +12121,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12283,7 +12286,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12405,7 +12408,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12570,7 +12573,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12692,7 +12695,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12857,7 +12860,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12979,7 +12982,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13144,7 +13147,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13266,7 +13269,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13431,7 +13434,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13553,7 +13556,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13718,7 +13721,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13840,7 +13843,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -14005,7 +14008,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14127,7 +14130,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14292,7 +14295,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14414,7 +14417,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14579,7 +14582,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14701,7 +14704,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14866,7 +14869,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -14988,7 +14991,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15153,7 +15156,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15275,7 +15278,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15440,7 +15443,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15562,7 +15565,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15727,7 +15730,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15849,7 +15852,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16014,7 +16017,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16136,7 +16139,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16301,7 +16304,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16423,7 +16426,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16588,7 +16591,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16710,7 +16713,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16875,7 +16878,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -16994,7 +16997,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17159,7 +17162,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17275,7 +17278,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17440,7 +17443,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17553,7 +17556,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17718,7 +17721,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17831,7 +17834,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -17996,7 +17999,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18109,7 +18112,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18274,7 +18277,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18387,7 +18390,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18552,7 +18555,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18665,7 +18668,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18830,7 +18833,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18943,7 +18946,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19108,7 +19111,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19221,7 +19224,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19386,7 +19389,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19499,7 +19502,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19664,7 +19667,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19777,7 +19780,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19942,7 +19945,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20055,7 +20058,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20226,7 +20229,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20339,7 +20342,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20510,7 +20513,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20623,7 +20626,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20794,7 +20797,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20907,7 +20910,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21078,7 +21081,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21188,7 +21191,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21359,7 +21362,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21466,7 +21469,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21637,7 +21640,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21741,7 +21744,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21912,7 +21915,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22016,7 +22019,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22187,7 +22190,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22291,7 +22294,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22462,7 +22465,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22566,7 +22569,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22737,7 +22740,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22841,7 +22844,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23012,7 +23015,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23116,7 +23119,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23287,7 +23290,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23388,7 +23391,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23559,7 +23562,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23660,7 +23663,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23831,7 +23834,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23932,7 +23935,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24103,7 +24106,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24204,7 +24207,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24375,7 +24378,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24476,7 +24479,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24647,7 +24650,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24748,7 +24751,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24919,7 +24922,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25020,7 +25023,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25191,7 +25194,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25289,7 +25292,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25460,7 +25463,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25558,7 +25561,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25729,7 +25732,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25827,7 +25830,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -25998,7 +26001,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26096,7 +26099,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26267,7 +26270,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26365,7 +26368,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26536,7 +26539,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26634,7 +26637,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26805,7 +26808,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26903,7 +26906,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27074,7 +27077,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27172,7 +27175,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27343,7 +27346,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27441,7 +27444,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27612,7 +27615,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27710,7 +27713,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27881,7 +27884,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27979,7 +27982,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28150,7 +28153,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28248,7 +28251,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28419,7 +28422,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28517,7 +28520,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28688,7 +28691,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28786,7 +28789,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28957,7 +28960,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29055,7 +29058,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29226,7 +29229,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29324,7 +29327,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29495,7 +29498,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29593,7 +29596,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29764,7 +29767,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29862,7 +29865,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30033,7 +30036,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30131,7 +30134,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30302,7 +30305,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30400,7 +30403,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30571,7 +30574,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30669,7 +30672,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30840,7 +30843,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30938,7 +30941,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31109,7 +31112,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31207,7 +31210,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31378,7 +31381,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31476,7 +31479,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31647,7 +31650,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31745,7 +31748,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31916,7 +31919,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32014,7 +32017,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32185,7 +32188,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32283,7 +32286,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32454,7 +32457,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32552,7 +32555,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32723,7 +32726,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32821,7 +32824,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -32992,7 +32995,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33090,7 +33093,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33261,7 +33264,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33359,7 +33362,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33530,7 +33533,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33628,7 +33631,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33799,7 +33802,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33897,7 +33900,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34068,7 +34071,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34166,7 +34169,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34337,7 +34340,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34435,7 +34438,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34606,7 +34609,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34704,7 +34707,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34875,7 +34878,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34973,7 +34976,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35144,7 +35147,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35242,7 +35245,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35413,7 +35416,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35511,7 +35514,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35682,7 +35685,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35780,7 +35783,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35951,7 +35954,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36049,7 +36052,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36220,7 +36223,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36318,7 +36321,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36489,7 +36492,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36587,7 +36590,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36758,7 +36761,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36856,7 +36859,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37027,7 +37030,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37125,7 +37128,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37296,7 +37299,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37394,7 +37397,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37565,7 +37568,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37663,7 +37666,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37834,7 +37837,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37932,7 +37935,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38103,7 +38106,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38201,7 +38204,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38372,7 +38375,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38470,7 +38473,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38641,7 +38644,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38739,7 +38742,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38910,7 +38913,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -39008,7 +39011,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39179,7 +39182,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39277,7 +39280,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39448,7 +39451,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39546,7 +39549,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39717,7 +39720,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39815,7 +39818,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -39986,7 +39989,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40084,7 +40087,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40255,7 +40258,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40353,7 +40356,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40524,7 +40527,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40622,7 +40625,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40793,7 +40796,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40891,7 +40894,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41062,7 +41065,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41160,7 +41163,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41331,7 +41334,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41429,7 +41432,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41600,7 +41603,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41698,7 +41701,7 @@
         <v>0.006328270379966137</v>
       </c>
       <c r="AM146" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN146">
         <v>0.08370784758312214</v>
@@ -41967,7 +41970,7 @@
         <v>0.0110592804278049</v>
       </c>
       <c r="AM147" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN147">
         <v>0.07581655721931389</v>
@@ -42236,7 +42239,7 @@
         <v>0.01450048649474174</v>
       </c>
       <c r="AM148" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN148">
         <v>0.09614621483891075</v>
@@ -42505,7 +42508,7 @@
         <v>0.01189559910110707</v>
       </c>
       <c r="AM149" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN149">
         <v>0.01288397198120313</v>
@@ -42774,7 +42777,7 @@
         <v>0.0145803412240497</v>
       </c>
       <c r="AM150" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN150">
         <v>0.1052173371212367</v>
@@ -43043,7 +43046,7 @@
         <v>0.01019614862437938</v>
       </c>
       <c r="AM151" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN151">
         <v>0.07035209557900164</v>
@@ -43312,7 +43315,7 @@
         <v>0.01085520881764603</v>
       </c>
       <c r="AM152" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN152">
         <v>0.0930850934199607</v>
@@ -43581,7 +43584,7 @@
         <v>0.01194275707748435</v>
       </c>
       <c r="AM153" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN153">
         <v>0.0823051935622205</v>
@@ -43759,6 +43762,275 @@
       </c>
       <c r="CU153">
         <v>-0.5360388336727706</v>
+      </c>
+    </row>
+    <row r="154" spans="10:99">
+      <c r="J154" t="s">
+        <v>251</v>
+      </c>
+      <c r="K154">
+        <v>0.00131026978251958</v>
+      </c>
+      <c r="L154">
+        <v>0.00131026978251958</v>
+      </c>
+      <c r="M154">
+        <v>0.0020549970689967</v>
+      </c>
+      <c r="N154">
+        <v>0.0020549970689967</v>
+      </c>
+      <c r="O154">
+        <v>0.0002416960083684972</v>
+      </c>
+      <c r="P154">
+        <v>0.0002416960083684972</v>
+      </c>
+      <c r="Q154">
+        <v>0.0003807066546053006</v>
+      </c>
+      <c r="R154">
+        <v>0.0003807066546053006</v>
+      </c>
+      <c r="S154">
+        <v>2.270537494732944</v>
+      </c>
+      <c r="T154">
+        <v>6.069581507196744</v>
+      </c>
+      <c r="U154">
+        <v>0.9999626451036483</v>
+      </c>
+      <c r="V154">
+        <v>0.7639533538599218</v>
+      </c>
+      <c r="W154">
+        <v>0.07691948422434937</v>
+      </c>
+      <c r="X154">
+        <v>0.07646698838976666</v>
+      </c>
+      <c r="Y154">
+        <v>0.09699735372266169</v>
+      </c>
+      <c r="Z154">
+        <v>0.1338379761000623</v>
+      </c>
+      <c r="AA154">
+        <v>0.9947557151680528</v>
+      </c>
+      <c r="AB154">
+        <v>0.9115208077823811</v>
+      </c>
+      <c r="AC154">
+        <v>0.8911011433398611</v>
+      </c>
+      <c r="AD154">
+        <v>0.9967972086535123</v>
+      </c>
+      <c r="AE154">
+        <v>0.9075449958514359</v>
+      </c>
+      <c r="AF154">
+        <v>0.8662075224476194</v>
+      </c>
+      <c r="AG154">
+        <v>0.01120522946710938</v>
+      </c>
+      <c r="AH154">
+        <v>0.01004172771237574</v>
+      </c>
+      <c r="AI154">
+        <v>0.9947557151680528</v>
+      </c>
+      <c r="AJ154">
+        <v>0.9967972086535123</v>
+      </c>
+      <c r="AK154">
+        <v>0.01120522946710938</v>
+      </c>
+      <c r="AL154">
+        <v>0.01004172771237574</v>
+      </c>
+      <c r="AM154" t="s">
+        <v>252</v>
+      </c>
+      <c r="AN154">
+        <v>0.2004871827431348</v>
+      </c>
+      <c r="AO154">
+        <v>0.1753529663308173</v>
+      </c>
+      <c r="AP154">
+        <v>-137.61045332</v>
+      </c>
+      <c r="AQ154">
+        <v>-645.3098396600001</v>
+      </c>
+      <c r="AR154">
+        <v>19691.83436719411</v>
+      </c>
+      <c r="AS154">
+        <v>28932.10896034004</v>
+      </c>
+      <c r="AT154">
+        <v>19584.71534667999</v>
+      </c>
+      <c r="AU154">
+        <v>28932.73806034003</v>
+      </c>
+      <c r="AV154">
+        <v>0.9691834367194108</v>
+      </c>
+      <c r="AW154">
+        <v>1.893210896034004</v>
+      </c>
+      <c r="AX154">
+        <v>7.561314593980693</v>
+      </c>
+      <c r="AY154">
+        <v>2.827043524416136</v>
+      </c>
+      <c r="AZ154">
+        <v>24.05</v>
+      </c>
+      <c r="BA154">
+        <v>29.45</v>
+      </c>
+      <c r="BB154">
+        <v>0.08692581115910371</v>
+      </c>
+      <c r="BC154">
+        <v>0.02050925775043352</v>
+      </c>
+      <c r="BD154">
+        <v>-935.77550949228</v>
+      </c>
+      <c r="BE154">
+        <v>-409.9255980053758</v>
+      </c>
+      <c r="BF154">
+        <v>589</v>
+      </c>
+      <c r="BG154">
+        <v>1640</v>
+      </c>
+      <c r="BH154">
+        <v>517.4986111111111</v>
+      </c>
+      <c r="BI154">
+        <v>586</v>
+      </c>
+      <c r="BJ154">
+        <v>1501</v>
+      </c>
+      <c r="BK154">
+        <v>1175</v>
+      </c>
+      <c r="BL154">
+        <v>3141</v>
+      </c>
+      <c r="BM154">
+        <v>0</v>
+      </c>
+      <c r="BN154">
+        <v>0</v>
+      </c>
+      <c r="BO154">
+        <v>198</v>
+      </c>
+      <c r="BP154">
+        <v>1214</v>
+      </c>
+      <c r="BQ154">
+        <v>0</v>
+      </c>
+      <c r="BR154">
+        <v>0</v>
+      </c>
+      <c r="BS154">
+        <v>391</v>
+      </c>
+      <c r="BT154">
+        <v>426</v>
+      </c>
+      <c r="BU154">
+        <v>586</v>
+      </c>
+      <c r="BV154">
+        <v>1501</v>
+      </c>
+      <c r="BW154">
+        <v>9691.834367194117</v>
+      </c>
+      <c r="BX154">
+        <v>18932.10896034</v>
+      </c>
+      <c r="BY154">
+        <v>0.2245211555236802</v>
+      </c>
+      <c r="BZ154">
+        <v>0.06944166639146315</v>
+      </c>
+      <c r="CA154">
+        <v>0.5086487976873659</v>
+      </c>
+      <c r="CB154">
+        <v>0.1179985272565561</v>
+      </c>
+      <c r="CC154">
+        <v>0.02960686380471667</v>
+      </c>
+      <c r="CD154">
+        <v>0.009072356870513325</v>
+      </c>
+      <c r="CE154">
+        <v>0.02978583392586601</v>
+      </c>
+      <c r="CF154">
+        <v>0.01168818562725964</v>
+      </c>
+      <c r="CG154">
+        <v>9829.444820514116</v>
+      </c>
+      <c r="CH154">
+        <v>19577.4188</v>
+      </c>
+      <c r="CI154">
+        <v>10765.2203300064</v>
+      </c>
+      <c r="CJ154">
+        <v>19987.34439800537</v>
+      </c>
+      <c r="CK154">
+        <v>0.1246783692505774</v>
+      </c>
+      <c r="CL154">
+        <v>0.186248412969152</v>
+      </c>
+      <c r="CM154">
+        <v>10000</v>
+      </c>
+      <c r="CO154">
+        <v>0.03952982851622253</v>
+      </c>
+      <c r="CP154">
+        <v>0.06988165204089848</v>
+      </c>
+      <c r="CQ154">
+        <v>3441632.619619544</v>
+      </c>
+      <c r="CR154">
+        <v>10813896.21182788</v>
+      </c>
+      <c r="CS154" s="2">
+        <v>45575.35987348158</v>
+      </c>
+      <c r="CT154">
+        <v>-0.6752991164432082</v>
+      </c>
+      <c r="CU154">
+        <v>-0.6077761306030433</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update ILVUSDT.json at 2024-10-10_11-06-19 bestfile_scores 0.0014919833922750702 bestfile_sharp 0.09800701910134668
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="397">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -770,6 +770,9 @@
   </si>
   <si>
     <t>RADUSDT</t>
+  </si>
+  <si>
+    <t>ZKUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1563,7 +1566,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU154"/>
+  <dimension ref="A1:CU155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1981,7 +1984,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2146,7 +2149,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2262,7 +2265,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2427,7 +2430,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2543,7 +2546,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2708,7 +2711,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2824,7 +2827,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -2989,7 +2992,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3105,7 +3108,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3270,7 +3273,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3386,7 +3389,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3551,7 +3554,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3667,7 +3670,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3832,7 +3835,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3948,7 +3951,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4113,7 +4116,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4229,7 +4232,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4394,7 +4397,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4510,7 +4513,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4675,7 +4678,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4791,7 +4794,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4956,7 +4959,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5072,7 +5075,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5237,7 +5240,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5353,7 +5356,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5518,7 +5521,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5634,7 +5637,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5799,7 +5802,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5915,7 +5918,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6080,7 +6083,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6196,7 +6199,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6361,7 +6364,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6477,7 +6480,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6642,7 +6645,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6758,7 +6761,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6923,7 +6926,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7039,7 +7042,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7204,7 +7207,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7320,7 +7323,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7485,7 +7488,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7601,7 +7604,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7766,7 +7769,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7882,7 +7885,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8047,7 +8050,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8163,7 +8166,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8328,7 +8331,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8444,7 +8447,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8609,7 +8612,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8725,7 +8728,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8890,7 +8893,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -9006,7 +9009,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9171,7 +9174,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9287,7 +9290,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9452,7 +9455,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9568,7 +9571,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9733,7 +9736,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9849,7 +9852,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10014,7 +10017,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10130,7 +10133,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10295,7 +10298,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10411,7 +10414,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10576,7 +10579,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10692,7 +10695,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10857,7 +10860,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10973,7 +10976,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11138,7 +11141,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11260,7 +11263,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11425,7 +11428,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11547,7 +11550,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11712,7 +11715,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11834,7 +11837,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -11999,7 +12002,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12121,7 +12124,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12286,7 +12289,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12408,7 +12411,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12573,7 +12576,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12695,7 +12698,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12860,7 +12863,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12982,7 +12985,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13147,7 +13150,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13269,7 +13272,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13434,7 +13437,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13556,7 +13559,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13721,7 +13724,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13843,7 +13846,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -14008,7 +14011,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14130,7 +14133,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14295,7 +14298,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14417,7 +14420,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14582,7 +14585,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14704,7 +14707,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14869,7 +14872,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -14991,7 +14994,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15156,7 +15159,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15278,7 +15281,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15443,7 +15446,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15565,7 +15568,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15730,7 +15733,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15852,7 +15855,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16017,7 +16020,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16139,7 +16142,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16304,7 +16307,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16426,7 +16429,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16591,7 +16594,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16713,7 +16716,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16878,7 +16881,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -16997,7 +17000,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17162,7 +17165,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17278,7 +17281,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17443,7 +17446,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17556,7 +17559,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17721,7 +17724,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17834,7 +17837,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -17999,7 +18002,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18112,7 +18115,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18277,7 +18280,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18390,7 +18393,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18555,7 +18558,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18668,7 +18671,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18833,7 +18836,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18946,7 +18949,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19111,7 +19114,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19224,7 +19227,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19389,7 +19392,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19502,7 +19505,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19667,7 +19670,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19780,7 +19783,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19945,7 +19948,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20058,7 +20061,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20229,7 +20232,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20342,7 +20345,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20513,7 +20516,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20626,7 +20629,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20797,7 +20800,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20910,7 +20913,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21081,7 +21084,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21191,7 +21194,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21362,7 +21365,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21469,7 +21472,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21640,7 +21643,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21744,7 +21747,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21915,7 +21918,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22019,7 +22022,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22190,7 +22193,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22294,7 +22297,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22465,7 +22468,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22569,7 +22572,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22740,7 +22743,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22844,7 +22847,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23015,7 +23018,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23119,7 +23122,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23290,7 +23293,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23391,7 +23394,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23562,7 +23565,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23663,7 +23666,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23834,7 +23837,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23935,7 +23938,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24106,7 +24109,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24207,7 +24210,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24378,7 +24381,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24479,7 +24482,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24650,7 +24653,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24751,7 +24754,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24922,7 +24925,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25023,7 +25026,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25194,7 +25197,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25292,7 +25295,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25463,7 +25466,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25561,7 +25564,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25732,7 +25735,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25830,7 +25833,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -26001,7 +26004,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26099,7 +26102,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26270,7 +26273,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26368,7 +26371,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26539,7 +26542,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26637,7 +26640,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26808,7 +26811,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26906,7 +26909,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27077,7 +27080,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27175,7 +27178,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27346,7 +27349,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27444,7 +27447,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27615,7 +27618,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27713,7 +27716,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27884,7 +27887,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27982,7 +27985,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28153,7 +28156,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28251,7 +28254,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28422,7 +28425,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28520,7 +28523,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28691,7 +28694,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28789,7 +28792,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28960,7 +28963,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29058,7 +29061,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29229,7 +29232,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29327,7 +29330,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29498,7 +29501,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29596,7 +29599,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29767,7 +29770,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29865,7 +29868,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30036,7 +30039,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30134,7 +30137,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30305,7 +30308,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30403,7 +30406,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30574,7 +30577,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30672,7 +30675,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30843,7 +30846,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30941,7 +30944,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31112,7 +31115,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31210,7 +31213,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31381,7 +31384,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31479,7 +31482,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31650,7 +31653,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31748,7 +31751,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31919,7 +31922,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32017,7 +32020,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32188,7 +32191,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32286,7 +32289,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32457,7 +32460,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32555,7 +32558,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32726,7 +32729,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32824,7 +32827,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -32995,7 +32998,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33093,7 +33096,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33264,7 +33267,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33362,7 +33365,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33533,7 +33536,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33631,7 +33634,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33802,7 +33805,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33900,7 +33903,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34071,7 +34074,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34169,7 +34172,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34340,7 +34343,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34438,7 +34441,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34609,7 +34612,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34707,7 +34710,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34878,7 +34881,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34976,7 +34979,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35147,7 +35150,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35245,7 +35248,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35416,7 +35419,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35514,7 +35517,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35685,7 +35688,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35783,7 +35786,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35954,7 +35957,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36052,7 +36055,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36223,7 +36226,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36321,7 +36324,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36492,7 +36495,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36590,7 +36593,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36761,7 +36764,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36859,7 +36862,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37030,7 +37033,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37128,7 +37131,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37299,7 +37302,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37397,7 +37400,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37568,7 +37571,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37666,7 +37669,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37837,7 +37840,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37935,7 +37938,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38106,7 +38109,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38204,7 +38207,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38375,7 +38378,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38473,7 +38476,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38644,7 +38647,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38742,7 +38745,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38913,7 +38916,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -39011,7 +39014,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39182,7 +39185,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39280,7 +39283,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39451,7 +39454,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39549,7 +39552,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39720,7 +39723,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39818,7 +39821,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -39989,7 +39992,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40087,7 +40090,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40258,7 +40261,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40356,7 +40359,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40527,7 +40530,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40625,7 +40628,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40796,7 +40799,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40894,7 +40897,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41065,7 +41068,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41163,7 +41166,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41334,7 +41337,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41432,7 +41435,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41603,7 +41606,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41701,7 +41704,7 @@
         <v>0.006328270379966137</v>
       </c>
       <c r="AM146" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN146">
         <v>0.08370784758312214</v>
@@ -41970,7 +41973,7 @@
         <v>0.0110592804278049</v>
       </c>
       <c r="AM147" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN147">
         <v>0.07581655721931389</v>
@@ -42239,7 +42242,7 @@
         <v>0.01450048649474174</v>
       </c>
       <c r="AM148" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN148">
         <v>0.09614621483891075</v>
@@ -42508,7 +42511,7 @@
         <v>0.01189559910110707</v>
       </c>
       <c r="AM149" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN149">
         <v>0.01288397198120313</v>
@@ -42777,7 +42780,7 @@
         <v>0.0145803412240497</v>
       </c>
       <c r="AM150" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN150">
         <v>0.1052173371212367</v>
@@ -43046,7 +43049,7 @@
         <v>0.01019614862437938</v>
       </c>
       <c r="AM151" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN151">
         <v>0.07035209557900164</v>
@@ -43315,7 +43318,7 @@
         <v>0.01085520881764603</v>
       </c>
       <c r="AM152" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN152">
         <v>0.0930850934199607</v>
@@ -43584,7 +43587,7 @@
         <v>0.01194275707748435</v>
       </c>
       <c r="AM153" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN153">
         <v>0.0823051935622205</v>
@@ -43853,7 +43856,7 @@
         <v>0.01004172771237574</v>
       </c>
       <c r="AM154" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN154">
         <v>0.2004871827431348</v>
@@ -44031,6 +44034,275 @@
       </c>
       <c r="CU154">
         <v>-0.6077761306030433</v>
+      </c>
+    </row>
+    <row r="155" spans="10:99">
+      <c r="J155" t="s">
+        <v>252</v>
+      </c>
+      <c r="K155">
+        <v>0.005616545586630384</v>
+      </c>
+      <c r="L155">
+        <v>0.005616545586630384</v>
+      </c>
+      <c r="M155">
+        <v>0.006476595427910459</v>
+      </c>
+      <c r="N155">
+        <v>0.006476595427910459</v>
+      </c>
+      <c r="O155">
+        <v>0.004867432906441116</v>
+      </c>
+      <c r="P155">
+        <v>0.004867432906441116</v>
+      </c>
+      <c r="Q155">
+        <v>0.006914784746986746</v>
+      </c>
+      <c r="R155">
+        <v>0.006914784746986746</v>
+      </c>
+      <c r="S155">
+        <v>50.5957036578933</v>
+      </c>
+      <c r="T155">
+        <v>27.58098841333649</v>
+      </c>
+      <c r="U155">
+        <v>0.9978265712781789</v>
+      </c>
+      <c r="V155">
+        <v>0.8006731821209783</v>
+      </c>
+      <c r="W155">
+        <v>0.09997814192638384</v>
+      </c>
+      <c r="X155">
+        <v>0.09770361230111213</v>
+      </c>
+      <c r="Y155">
+        <v>0.1565586427483908</v>
+      </c>
+      <c r="Z155">
+        <v>0.1171375436272742</v>
+      </c>
+      <c r="AA155">
+        <v>0.9957146111894505</v>
+      </c>
+      <c r="AB155">
+        <v>0.8757135276582304</v>
+      </c>
+      <c r="AC155">
+        <v>0.9000755740134636</v>
+      </c>
+      <c r="AD155">
+        <v>0.9923962464108029</v>
+      </c>
+      <c r="AE155">
+        <v>0.8429847877104543</v>
+      </c>
+      <c r="AF155">
+        <v>0.8893066961297036</v>
+      </c>
+      <c r="AG155">
+        <v>0.01329298856981823</v>
+      </c>
+      <c r="AH155">
+        <v>0.01933638311795493</v>
+      </c>
+      <c r="AI155">
+        <v>0.9957146111894505</v>
+      </c>
+      <c r="AJ155">
+        <v>0.9923962464108029</v>
+      </c>
+      <c r="AK155">
+        <v>0.01329298856981823</v>
+      </c>
+      <c r="AL155">
+        <v>0.01933638311795493</v>
+      </c>
+      <c r="AM155" t="s">
+        <v>253</v>
+      </c>
+      <c r="AN155">
+        <v>0.1986348331383821</v>
+      </c>
+      <c r="AO155">
+        <v>0.2926845629357868</v>
+      </c>
+      <c r="AP155">
+        <v>-857.738232636</v>
+      </c>
+      <c r="AQ155">
+        <v>-276.683987938</v>
+      </c>
+      <c r="AR155">
+        <v>18993.15544736399</v>
+      </c>
+      <c r="AS155">
+        <v>20946.94480206195</v>
+      </c>
+      <c r="AT155">
+        <v>18962.13930736399</v>
+      </c>
+      <c r="AU155">
+        <v>20946.94480206195</v>
+      </c>
+      <c r="AV155">
+        <v>0.8993155447363987</v>
+      </c>
+      <c r="AW155">
+        <v>1.094694480206195</v>
+      </c>
+      <c r="AX155">
+        <v>0.4738896559659417</v>
+      </c>
+      <c r="AY155">
+        <v>0.8651256069242137</v>
+      </c>
+      <c r="AZ155">
+        <v>14.08333333333333</v>
+      </c>
+      <c r="BA155">
+        <v>72.23333333333333</v>
+      </c>
+      <c r="BB155">
+        <v>0.05304922177260152</v>
+      </c>
+      <c r="BC155">
+        <v>0.03204470745561996</v>
+      </c>
+      <c r="BD155">
+        <v>-551.8578742464967</v>
+      </c>
+      <c r="BE155">
+        <v>-371.5645794142227</v>
+      </c>
+      <c r="BF155">
+        <v>3080</v>
+      </c>
+      <c r="BG155">
+        <v>2024</v>
+      </c>
+      <c r="BH155">
+        <v>114.5354166666667</v>
+      </c>
+      <c r="BI155">
+        <v>2715</v>
+      </c>
+      <c r="BJ155">
+        <v>1135</v>
+      </c>
+      <c r="BK155">
+        <v>5795</v>
+      </c>
+      <c r="BL155">
+        <v>3159</v>
+      </c>
+      <c r="BM155">
+        <v>0</v>
+      </c>
+      <c r="BN155">
+        <v>0</v>
+      </c>
+      <c r="BO155">
+        <v>2886</v>
+      </c>
+      <c r="BP155">
+        <v>256</v>
+      </c>
+      <c r="BQ155">
+        <v>0</v>
+      </c>
+      <c r="BR155">
+        <v>0</v>
+      </c>
+      <c r="BS155">
+        <v>194</v>
+      </c>
+      <c r="BT155">
+        <v>1768</v>
+      </c>
+      <c r="BU155">
+        <v>2715</v>
+      </c>
+      <c r="BV155">
+        <v>1135</v>
+      </c>
+      <c r="BW155">
+        <v>8993.155447363986</v>
+      </c>
+      <c r="BX155">
+        <v>10946.94480206199</v>
+      </c>
+      <c r="BY155">
+        <v>0.1130760405416129</v>
+      </c>
+      <c r="BZ155">
+        <v>0.08505983029521307</v>
+      </c>
+      <c r="CA155">
+        <v>0.1862567521454727</v>
+      </c>
+      <c r="CB155">
+        <v>0.09966096087551353</v>
+      </c>
+      <c r="CC155">
+        <v>0.0115610794668569</v>
+      </c>
+      <c r="CD155">
+        <v>0.01600521536383607</v>
+      </c>
+      <c r="CE155">
+        <v>0.0142791136897049</v>
+      </c>
+      <c r="CF155">
+        <v>0.01971441465681235</v>
+      </c>
+      <c r="CG155">
+        <v>9850.893679999986</v>
+      </c>
+      <c r="CH155">
+        <v>11223.62878999999</v>
+      </c>
+      <c r="CI155">
+        <v>10402.75155424648</v>
+      </c>
+      <c r="CJ155">
+        <v>11595.19336941421</v>
+      </c>
+      <c r="CK155">
+        <v>0.315701294602746</v>
+      </c>
+      <c r="CL155">
+        <v>0.2472877155160815</v>
+      </c>
+      <c r="CM155">
+        <v>10000</v>
+      </c>
+      <c r="CO155">
+        <v>0.08945454545454545</v>
+      </c>
+      <c r="CP155">
+        <v>0.1967272727272727</v>
+      </c>
+      <c r="CQ155">
+        <v>12145210.00336875</v>
+      </c>
+      <c r="CR155">
+        <v>12324453.83990518</v>
+      </c>
+      <c r="CS155" s="2">
+        <v>45575.39047404622</v>
+      </c>
+      <c r="CT155">
+        <v>-0.2599727167384927</v>
+      </c>
+      <c r="CU155">
+        <v>-0.1345707965930885</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update ATAUSDT.json at 2024-10-10_15-32-07 bestfile_scores 0.0010116162552585351 bestfile_sharp 0.0910179440555702
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="398">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -773,6 +773,9 @@
   </si>
   <si>
     <t>ZKUSDT</t>
+  </si>
+  <si>
+    <t>ILVUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1566,7 +1569,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU155"/>
+  <dimension ref="A1:CU156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1984,7 +1987,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2149,7 +2152,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2265,7 +2268,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2430,7 +2433,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2546,7 +2549,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2711,7 +2714,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2827,7 +2830,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -2992,7 +2995,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3108,7 +3111,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3273,7 +3276,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3389,7 +3392,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3554,7 +3557,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3670,7 +3673,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3835,7 +3838,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3951,7 +3954,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4116,7 +4119,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4232,7 +4235,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4397,7 +4400,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4513,7 +4516,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4678,7 +4681,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4794,7 +4797,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4959,7 +4962,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5075,7 +5078,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5240,7 +5243,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5356,7 +5359,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5521,7 +5524,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5637,7 +5640,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5802,7 +5805,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5918,7 +5921,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6083,7 +6086,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6199,7 +6202,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6364,7 +6367,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6480,7 +6483,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6645,7 +6648,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6761,7 +6764,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6926,7 +6929,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7042,7 +7045,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7207,7 +7210,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7323,7 +7326,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7488,7 +7491,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7604,7 +7607,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7769,7 +7772,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7885,7 +7888,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8050,7 +8053,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8166,7 +8169,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8331,7 +8334,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8447,7 +8450,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8612,7 +8615,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8728,7 +8731,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8893,7 +8896,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -9009,7 +9012,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9174,7 +9177,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9290,7 +9293,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9455,7 +9458,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9571,7 +9574,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9736,7 +9739,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9852,7 +9855,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10017,7 +10020,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10133,7 +10136,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10298,7 +10301,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10414,7 +10417,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10579,7 +10582,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10695,7 +10698,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10860,7 +10863,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10976,7 +10979,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11141,7 +11144,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11263,7 +11266,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11428,7 +11431,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11550,7 +11553,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11715,7 +11718,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11837,7 +11840,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -12002,7 +12005,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12124,7 +12127,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12289,7 +12292,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12411,7 +12414,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12576,7 +12579,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12698,7 +12701,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12863,7 +12866,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12985,7 +12988,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13150,7 +13153,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13272,7 +13275,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13437,7 +13440,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13559,7 +13562,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13724,7 +13727,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13846,7 +13849,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -14011,7 +14014,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14133,7 +14136,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14298,7 +14301,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14420,7 +14423,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14585,7 +14588,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14707,7 +14710,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14872,7 +14875,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -14994,7 +14997,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15159,7 +15162,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15281,7 +15284,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15446,7 +15449,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15568,7 +15571,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15733,7 +15736,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15855,7 +15858,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16020,7 +16023,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16142,7 +16145,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16307,7 +16310,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16429,7 +16432,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16594,7 +16597,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16716,7 +16719,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16881,7 +16884,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -17000,7 +17003,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17165,7 +17168,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17281,7 +17284,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17446,7 +17449,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17559,7 +17562,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17724,7 +17727,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17837,7 +17840,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -18002,7 +18005,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18115,7 +18118,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18280,7 +18283,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18393,7 +18396,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18558,7 +18561,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18671,7 +18674,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18836,7 +18839,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18949,7 +18952,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19114,7 +19117,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19227,7 +19230,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19392,7 +19395,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19505,7 +19508,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19670,7 +19673,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19783,7 +19786,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19948,7 +19951,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20061,7 +20064,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20232,7 +20235,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20345,7 +20348,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20516,7 +20519,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20629,7 +20632,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20800,7 +20803,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20913,7 +20916,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21084,7 +21087,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21194,7 +21197,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21365,7 +21368,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21472,7 +21475,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21643,7 +21646,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21747,7 +21750,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21918,7 +21921,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22022,7 +22025,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22193,7 +22196,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22297,7 +22300,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22468,7 +22471,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22572,7 +22575,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22743,7 +22746,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22847,7 +22850,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23018,7 +23021,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23122,7 +23125,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23293,7 +23296,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23394,7 +23397,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23565,7 +23568,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23666,7 +23669,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23837,7 +23840,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23938,7 +23941,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24109,7 +24112,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24210,7 +24213,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24381,7 +24384,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24482,7 +24485,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24653,7 +24656,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24754,7 +24757,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24925,7 +24928,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25026,7 +25029,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25197,7 +25200,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25295,7 +25298,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25466,7 +25469,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25564,7 +25567,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25735,7 +25738,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25833,7 +25836,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -26004,7 +26007,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26102,7 +26105,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26273,7 +26276,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26371,7 +26374,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26542,7 +26545,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26640,7 +26643,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26811,7 +26814,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26909,7 +26912,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27080,7 +27083,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27178,7 +27181,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27349,7 +27352,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27447,7 +27450,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27618,7 +27621,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27716,7 +27719,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27887,7 +27890,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27985,7 +27988,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28156,7 +28159,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28254,7 +28257,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28425,7 +28428,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28523,7 +28526,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28694,7 +28697,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28792,7 +28795,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28963,7 +28966,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29061,7 +29064,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29232,7 +29235,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29330,7 +29333,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29501,7 +29504,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29599,7 +29602,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29770,7 +29773,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29868,7 +29871,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30039,7 +30042,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30137,7 +30140,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30308,7 +30311,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30406,7 +30409,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30577,7 +30580,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30675,7 +30678,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30846,7 +30849,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30944,7 +30947,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31115,7 +31118,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31213,7 +31216,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31384,7 +31387,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31482,7 +31485,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31653,7 +31656,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31751,7 +31754,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31922,7 +31925,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32020,7 +32023,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32191,7 +32194,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32289,7 +32292,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32460,7 +32463,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32558,7 +32561,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32729,7 +32732,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32827,7 +32830,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -32998,7 +33001,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33096,7 +33099,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33267,7 +33270,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33365,7 +33368,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33536,7 +33539,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33634,7 +33637,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33805,7 +33808,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33903,7 +33906,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34074,7 +34077,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34172,7 +34175,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34343,7 +34346,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34441,7 +34444,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34612,7 +34615,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34710,7 +34713,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34881,7 +34884,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34979,7 +34982,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35150,7 +35153,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35248,7 +35251,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35419,7 +35422,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35517,7 +35520,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35688,7 +35691,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35786,7 +35789,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35957,7 +35960,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36055,7 +36058,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36226,7 +36229,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36324,7 +36327,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36495,7 +36498,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36593,7 +36596,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36764,7 +36767,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36862,7 +36865,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37033,7 +37036,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37131,7 +37134,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37302,7 +37305,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37400,7 +37403,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37571,7 +37574,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37669,7 +37672,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37840,7 +37843,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37938,7 +37941,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38109,7 +38112,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38207,7 +38210,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38378,7 +38381,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38476,7 +38479,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38647,7 +38650,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38745,7 +38748,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38916,7 +38919,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -39014,7 +39017,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39185,7 +39188,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39283,7 +39286,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39454,7 +39457,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39552,7 +39555,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39723,7 +39726,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39821,7 +39824,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -39992,7 +39995,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40090,7 +40093,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40261,7 +40264,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40359,7 +40362,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40530,7 +40533,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40628,7 +40631,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40799,7 +40802,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40897,7 +40900,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41068,7 +41071,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41166,7 +41169,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41337,7 +41340,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41435,7 +41438,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41606,7 +41609,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41704,7 +41707,7 @@
         <v>0.006328270379966137</v>
       </c>
       <c r="AM146" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN146">
         <v>0.08370784758312214</v>
@@ -41973,7 +41976,7 @@
         <v>0.0110592804278049</v>
       </c>
       <c r="AM147" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN147">
         <v>0.07581655721931389</v>
@@ -42242,7 +42245,7 @@
         <v>0.01450048649474174</v>
       </c>
       <c r="AM148" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN148">
         <v>0.09614621483891075</v>
@@ -42511,7 +42514,7 @@
         <v>0.01189559910110707</v>
       </c>
       <c r="AM149" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN149">
         <v>0.01288397198120313</v>
@@ -42780,7 +42783,7 @@
         <v>0.0145803412240497</v>
       </c>
       <c r="AM150" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN150">
         <v>0.1052173371212367</v>
@@ -43049,7 +43052,7 @@
         <v>0.01019614862437938</v>
       </c>
       <c r="AM151" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN151">
         <v>0.07035209557900164</v>
@@ -43318,7 +43321,7 @@
         <v>0.01085520881764603</v>
       </c>
       <c r="AM152" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN152">
         <v>0.0930850934199607</v>
@@ -43587,7 +43590,7 @@
         <v>0.01194275707748435</v>
       </c>
       <c r="AM153" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN153">
         <v>0.0823051935622205</v>
@@ -43856,7 +43859,7 @@
         <v>0.01004172771237574</v>
       </c>
       <c r="AM154" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN154">
         <v>0.2004871827431348</v>
@@ -44125,7 +44128,7 @@
         <v>0.01933638311795493</v>
       </c>
       <c r="AM155" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN155">
         <v>0.1986348331383821</v>
@@ -44303,6 +44306,275 @@
       </c>
       <c r="CU155">
         <v>-0.1345707965930885</v>
+      </c>
+    </row>
+    <row r="156" spans="10:99">
+      <c r="J156" t="s">
+        <v>253</v>
+      </c>
+      <c r="K156">
+        <v>0.001083920185847465</v>
+      </c>
+      <c r="L156">
+        <v>0.001083920185847465</v>
+      </c>
+      <c r="M156">
+        <v>0.002070190644179348</v>
+      </c>
+      <c r="N156">
+        <v>0.002070190644179348</v>
+      </c>
+      <c r="O156">
+        <v>0.0009097731295870659</v>
+      </c>
+      <c r="P156">
+        <v>0.0009097731295870659</v>
+      </c>
+      <c r="Q156">
+        <v>0.001904049609486402</v>
+      </c>
+      <c r="R156">
+        <v>0.001904049609486402</v>
+      </c>
+      <c r="S156">
+        <v>7.549853762297262</v>
+      </c>
+      <c r="T156">
+        <v>5.491890454666312</v>
+      </c>
+      <c r="U156">
+        <v>0.9996017766581576</v>
+      </c>
+      <c r="V156">
+        <v>0.8170018552134358</v>
+      </c>
+      <c r="W156">
+        <v>0.09746497393682627</v>
+      </c>
+      <c r="X156">
+        <v>0.08343869904196256</v>
+      </c>
+      <c r="Y156">
+        <v>0.202357539161326</v>
+      </c>
+      <c r="Z156">
+        <v>0.1070332460934421</v>
+      </c>
+      <c r="AA156">
+        <v>0.9983143282371996</v>
+      </c>
+      <c r="AB156">
+        <v>0.836005411183805</v>
+      </c>
+      <c r="AC156">
+        <v>0.9058076243782643</v>
+      </c>
+      <c r="AD156">
+        <v>0.9979172269121082</v>
+      </c>
+      <c r="AE156">
+        <v>0.7978300438801056</v>
+      </c>
+      <c r="AF156">
+        <v>0.8992688269300005</v>
+      </c>
+      <c r="AG156">
+        <v>0.01046787686260407</v>
+      </c>
+      <c r="AH156">
+        <v>0.01041289954961886</v>
+      </c>
+      <c r="AI156">
+        <v>0.9983143282371996</v>
+      </c>
+      <c r="AJ156">
+        <v>0.9979172269121082</v>
+      </c>
+      <c r="AK156">
+        <v>0.01046787686260407</v>
+      </c>
+      <c r="AL156">
+        <v>0.01041289954961886</v>
+      </c>
+      <c r="AM156" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN156">
+        <v>0.05962444025709573</v>
+      </c>
+      <c r="AO156">
+        <v>0.1341841005423368</v>
+      </c>
+      <c r="AP156">
+        <v>-189.027906</v>
+      </c>
+      <c r="AQ156">
+        <v>-169.75363242</v>
+      </c>
+      <c r="AR156">
+        <v>14364.43569400002</v>
+      </c>
+      <c r="AS156">
+        <v>19964.53476758</v>
+      </c>
+      <c r="AT156">
+        <v>14349.66769400002</v>
+      </c>
+      <c r="AU156">
+        <v>19975.03566758</v>
+      </c>
+      <c r="AV156">
+        <v>0.4364435694000015</v>
+      </c>
+      <c r="AW156">
+        <v>0.9964534767580004</v>
+      </c>
+      <c r="AX156">
+        <v>3.178907385387766</v>
+      </c>
+      <c r="AY156">
+        <v>4.36495004541326</v>
+      </c>
+      <c r="AZ156">
+        <v>72.46666666666667</v>
+      </c>
+      <c r="BA156">
+        <v>20.96666666666667</v>
+      </c>
+      <c r="BB156">
+        <v>0.104746345137463</v>
+      </c>
+      <c r="BC156">
+        <v>0.08636889709946935</v>
+      </c>
+      <c r="BD156">
+        <v>-532.7637225783903</v>
+      </c>
+      <c r="BE156">
+        <v>-958.0314299908853</v>
+      </c>
+      <c r="BF156">
+        <v>1090</v>
+      </c>
+      <c r="BG156">
+        <v>559</v>
+      </c>
+      <c r="BH156">
+        <v>334.3111111111111</v>
+      </c>
+      <c r="BI156">
+        <v>1434</v>
+      </c>
+      <c r="BJ156">
+        <v>1277</v>
+      </c>
+      <c r="BK156">
+        <v>2524</v>
+      </c>
+      <c r="BL156">
+        <v>1836</v>
+      </c>
+      <c r="BM156">
+        <v>0</v>
+      </c>
+      <c r="BN156">
+        <v>0</v>
+      </c>
+      <c r="BO156">
+        <v>12</v>
+      </c>
+      <c r="BP156">
+        <v>200</v>
+      </c>
+      <c r="BQ156">
+        <v>0</v>
+      </c>
+      <c r="BR156">
+        <v>0</v>
+      </c>
+      <c r="BS156">
+        <v>1078</v>
+      </c>
+      <c r="BT156">
+        <v>359</v>
+      </c>
+      <c r="BU156">
+        <v>1434</v>
+      </c>
+      <c r="BV156">
+        <v>1277</v>
+      </c>
+      <c r="BW156">
+        <v>4364.435694000001</v>
+      </c>
+      <c r="BX156">
+        <v>9964.534767579991</v>
+      </c>
+      <c r="BY156">
+        <v>0.1065310812612241</v>
+      </c>
+      <c r="BZ156">
+        <v>0.07307763902091662</v>
+      </c>
+      <c r="CA156">
+        <v>0.2534003607285024</v>
+      </c>
+      <c r="CB156">
+        <v>0.2006000003113123</v>
+      </c>
+      <c r="CC156">
+        <v>0.0135904414768199</v>
+      </c>
+      <c r="CD156">
+        <v>0.01767464493812843</v>
+      </c>
+      <c r="CE156">
+        <v>0.0169826253261859</v>
+      </c>
+      <c r="CF156">
+        <v>0.01416444814275574</v>
+      </c>
+      <c r="CG156">
+        <v>4553.463600000001</v>
+      </c>
+      <c r="CH156">
+        <v>10134.28839999999</v>
+      </c>
+      <c r="CI156">
+        <v>5086.227322578391</v>
+      </c>
+      <c r="CJ156">
+        <v>11092.31982999088</v>
+      </c>
+      <c r="CK156">
+        <v>0.09800701910134668</v>
+      </c>
+      <c r="CL156">
+        <v>0.1625768930767786</v>
+      </c>
+      <c r="CM156">
+        <v>10000</v>
+      </c>
+      <c r="CO156">
+        <v>0.02130841121495327</v>
+      </c>
+      <c r="CP156">
+        <v>0.03800623052959502</v>
+      </c>
+      <c r="CQ156">
+        <v>2855225.816503792</v>
+      </c>
+      <c r="CR156">
+        <v>4644270.091909833</v>
+      </c>
+      <c r="CS156" s="2">
+        <v>45575.46274252641</v>
+      </c>
+      <c r="CT156">
+        <v>-0.6669894744619533</v>
+      </c>
+      <c r="CU156">
+        <v>-0.5741664034478539</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update SUIUSDT.json at 2024-10-10_18-23-25 bestfile_scores 0.0010434723655505158 bestfile_sharp 0.15063333263529108
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="399">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -776,6 +776,9 @@
   </si>
   <si>
     <t>ILVUSDT</t>
+  </si>
+  <si>
+    <t>ATAUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1569,7 +1572,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU156"/>
+  <dimension ref="A1:CU157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1987,7 +1990,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2152,7 +2155,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2268,7 +2271,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2433,7 +2436,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2549,7 +2552,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2714,7 +2717,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2830,7 +2833,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -2995,7 +2998,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3111,7 +3114,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3276,7 +3279,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3392,7 +3395,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3557,7 +3560,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3673,7 +3676,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3838,7 +3841,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3954,7 +3957,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4119,7 +4122,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4235,7 +4238,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4400,7 +4403,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4516,7 +4519,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4681,7 +4684,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4797,7 +4800,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4962,7 +4965,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5078,7 +5081,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5243,7 +5246,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5359,7 +5362,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5524,7 +5527,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5640,7 +5643,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5805,7 +5808,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5921,7 +5924,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6086,7 +6089,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6202,7 +6205,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6367,7 +6370,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6483,7 +6486,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6648,7 +6651,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6764,7 +6767,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6929,7 +6932,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7045,7 +7048,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7210,7 +7213,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7326,7 +7329,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7491,7 +7494,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7607,7 +7610,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7772,7 +7775,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7888,7 +7891,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8053,7 +8056,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8169,7 +8172,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8334,7 +8337,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8450,7 +8453,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8615,7 +8618,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8731,7 +8734,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8896,7 +8899,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -9012,7 +9015,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9177,7 +9180,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9293,7 +9296,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9458,7 +9461,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9574,7 +9577,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9739,7 +9742,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9855,7 +9858,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10020,7 +10023,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10136,7 +10139,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10301,7 +10304,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10417,7 +10420,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10582,7 +10585,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10698,7 +10701,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10863,7 +10866,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10979,7 +10982,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11144,7 +11147,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11266,7 +11269,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11431,7 +11434,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11553,7 +11556,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11718,7 +11721,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11840,7 +11843,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -12005,7 +12008,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12127,7 +12130,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12292,7 +12295,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12414,7 +12417,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12579,7 +12582,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12701,7 +12704,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12866,7 +12869,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12988,7 +12991,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13153,7 +13156,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13275,7 +13278,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13440,7 +13443,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13562,7 +13565,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13727,7 +13730,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13849,7 +13852,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -14014,7 +14017,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14136,7 +14139,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14301,7 +14304,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14423,7 +14426,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14588,7 +14591,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14710,7 +14713,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14875,7 +14878,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -14997,7 +15000,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15162,7 +15165,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15284,7 +15287,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15449,7 +15452,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15571,7 +15574,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15736,7 +15739,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15858,7 +15861,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16023,7 +16026,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16145,7 +16148,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16310,7 +16313,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16432,7 +16435,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16597,7 +16600,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16719,7 +16722,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16884,7 +16887,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -17003,7 +17006,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17168,7 +17171,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17284,7 +17287,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17449,7 +17452,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17562,7 +17565,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17727,7 +17730,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17840,7 +17843,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -18005,7 +18008,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18118,7 +18121,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18283,7 +18286,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18396,7 +18399,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18561,7 +18564,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18674,7 +18677,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18839,7 +18842,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18952,7 +18955,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19117,7 +19120,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19230,7 +19233,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19395,7 +19398,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19508,7 +19511,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19673,7 +19676,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19786,7 +19789,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19951,7 +19954,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20064,7 +20067,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20235,7 +20238,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20348,7 +20351,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20519,7 +20522,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20632,7 +20635,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20803,7 +20806,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20916,7 +20919,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21087,7 +21090,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21197,7 +21200,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21368,7 +21371,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21475,7 +21478,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21646,7 +21649,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21750,7 +21753,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21921,7 +21924,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22025,7 +22028,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22196,7 +22199,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22300,7 +22303,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22471,7 +22474,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22575,7 +22578,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22746,7 +22749,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22850,7 +22853,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23021,7 +23024,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23125,7 +23128,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23296,7 +23299,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23397,7 +23400,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23568,7 +23571,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23669,7 +23672,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23840,7 +23843,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23941,7 +23944,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24112,7 +24115,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24213,7 +24216,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24384,7 +24387,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24485,7 +24488,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24656,7 +24659,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24757,7 +24760,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24928,7 +24931,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25029,7 +25032,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25200,7 +25203,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25298,7 +25301,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25469,7 +25472,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25567,7 +25570,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25738,7 +25741,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25836,7 +25839,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -26007,7 +26010,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26105,7 +26108,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26276,7 +26279,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26374,7 +26377,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26545,7 +26548,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26643,7 +26646,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26814,7 +26817,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26912,7 +26915,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27083,7 +27086,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27181,7 +27184,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27352,7 +27355,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27450,7 +27453,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27621,7 +27624,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27719,7 +27722,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27890,7 +27893,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27988,7 +27991,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28159,7 +28162,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28257,7 +28260,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28428,7 +28431,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28526,7 +28529,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28697,7 +28700,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28795,7 +28798,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28966,7 +28969,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29064,7 +29067,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29235,7 +29238,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29333,7 +29336,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29504,7 +29507,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29602,7 +29605,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29773,7 +29776,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29871,7 +29874,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30042,7 +30045,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30140,7 +30143,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30311,7 +30314,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30409,7 +30412,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30580,7 +30583,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30678,7 +30681,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30849,7 +30852,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30947,7 +30950,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31118,7 +31121,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31216,7 +31219,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31387,7 +31390,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31485,7 +31488,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31656,7 +31659,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31754,7 +31757,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31925,7 +31928,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32023,7 +32026,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32194,7 +32197,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32292,7 +32295,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32463,7 +32466,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32561,7 +32564,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32732,7 +32735,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32830,7 +32833,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -33001,7 +33004,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33099,7 +33102,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33270,7 +33273,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33368,7 +33371,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33539,7 +33542,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33637,7 +33640,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33808,7 +33811,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33906,7 +33909,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34077,7 +34080,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34175,7 +34178,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34346,7 +34349,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34444,7 +34447,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34615,7 +34618,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34713,7 +34716,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34884,7 +34887,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34982,7 +34985,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35153,7 +35156,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35251,7 +35254,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35422,7 +35425,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35520,7 +35523,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35691,7 +35694,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35789,7 +35792,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35960,7 +35963,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36058,7 +36061,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36229,7 +36232,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36327,7 +36330,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36498,7 +36501,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36596,7 +36599,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36767,7 +36770,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36865,7 +36868,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37036,7 +37039,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37134,7 +37137,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37305,7 +37308,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37403,7 +37406,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37574,7 +37577,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37672,7 +37675,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37843,7 +37846,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37941,7 +37944,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38112,7 +38115,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38210,7 +38213,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38381,7 +38384,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38479,7 +38482,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38650,7 +38653,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38748,7 +38751,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38919,7 +38922,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -39017,7 +39020,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39188,7 +39191,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39286,7 +39289,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39457,7 +39460,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39555,7 +39558,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39726,7 +39729,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39824,7 +39827,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -39995,7 +39998,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40093,7 +40096,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40264,7 +40267,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40362,7 +40365,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40533,7 +40536,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40631,7 +40634,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40802,7 +40805,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40900,7 +40903,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41071,7 +41074,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41169,7 +41172,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41340,7 +41343,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41438,7 +41441,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41609,7 +41612,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41707,7 +41710,7 @@
         <v>0.006328270379966137</v>
       </c>
       <c r="AM146" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN146">
         <v>0.08370784758312214</v>
@@ -41976,7 +41979,7 @@
         <v>0.0110592804278049</v>
       </c>
       <c r="AM147" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN147">
         <v>0.07581655721931389</v>
@@ -42245,7 +42248,7 @@
         <v>0.01450048649474174</v>
       </c>
       <c r="AM148" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN148">
         <v>0.09614621483891075</v>
@@ -42514,7 +42517,7 @@
         <v>0.01189559910110707</v>
       </c>
       <c r="AM149" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN149">
         <v>0.01288397198120313</v>
@@ -42783,7 +42786,7 @@
         <v>0.0145803412240497</v>
       </c>
       <c r="AM150" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN150">
         <v>0.1052173371212367</v>
@@ -43052,7 +43055,7 @@
         <v>0.01019614862437938</v>
       </c>
       <c r="AM151" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN151">
         <v>0.07035209557900164</v>
@@ -43321,7 +43324,7 @@
         <v>0.01085520881764603</v>
       </c>
       <c r="AM152" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN152">
         <v>0.0930850934199607</v>
@@ -43590,7 +43593,7 @@
         <v>0.01194275707748435</v>
       </c>
       <c r="AM153" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN153">
         <v>0.0823051935622205</v>
@@ -43859,7 +43862,7 @@
         <v>0.01004172771237574</v>
       </c>
       <c r="AM154" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN154">
         <v>0.2004871827431348</v>
@@ -44128,7 +44131,7 @@
         <v>0.01933638311795493</v>
       </c>
       <c r="AM155" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN155">
         <v>0.1986348331383821</v>
@@ -44397,7 +44400,7 @@
         <v>0.01041289954961886</v>
       </c>
       <c r="AM156" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN156">
         <v>0.05962444025709573</v>
@@ -44575,6 +44578,275 @@
       </c>
       <c r="CU156">
         <v>-0.5741664034478539</v>
+      </c>
+    </row>
+    <row r="157" spans="10:99">
+      <c r="J157" t="s">
+        <v>254</v>
+      </c>
+      <c r="K157">
+        <v>0.0007121969839867237</v>
+      </c>
+      <c r="L157">
+        <v>0.0007121969839867237</v>
+      </c>
+      <c r="M157">
+        <v>0.001419269556104608</v>
+      </c>
+      <c r="N157">
+        <v>0.001419269556104608</v>
+      </c>
+      <c r="O157">
+        <v>0.0007487340102616758</v>
+      </c>
+      <c r="P157">
+        <v>0.0007487340102616758</v>
+      </c>
+      <c r="Q157">
+        <v>0.001166264470681133</v>
+      </c>
+      <c r="R157">
+        <v>0.001166264470681133</v>
+      </c>
+      <c r="S157">
+        <v>8.14454142384454</v>
+      </c>
+      <c r="T157">
+        <v>18.2004221008689</v>
+      </c>
+      <c r="U157">
+        <v>0.9896336384785566</v>
+      </c>
+      <c r="V157">
+        <v>0.6016697212442377</v>
+      </c>
+      <c r="W157">
+        <v>0.09952701807673947</v>
+      </c>
+      <c r="X157">
+        <v>0.09583639027127948</v>
+      </c>
+      <c r="Y157">
+        <v>0.2051545658737408</v>
+      </c>
+      <c r="Z157">
+        <v>0.2499191646834295</v>
+      </c>
+      <c r="AA157">
+        <v>0.9985283610899658</v>
+      </c>
+      <c r="AB157">
+        <v>0.8228848677268346</v>
+      </c>
+      <c r="AC157">
+        <v>0.7702301267105844</v>
+      </c>
+      <c r="AD157">
+        <v>0.9981414580983481</v>
+      </c>
+      <c r="AE157">
+        <v>0.8077595383553803</v>
+      </c>
+      <c r="AF157">
+        <v>0.751303457613971</v>
+      </c>
+      <c r="AG157">
+        <v>0.009642313041340942</v>
+      </c>
+      <c r="AH157">
+        <v>0.01103085386133413</v>
+      </c>
+      <c r="AI157">
+        <v>0.9985283610899658</v>
+      </c>
+      <c r="AJ157">
+        <v>0.9981414580983481</v>
+      </c>
+      <c r="AK157">
+        <v>0.009642313041340942</v>
+      </c>
+      <c r="AL157">
+        <v>0.01103085386133413</v>
+      </c>
+      <c r="AM157" t="s">
+        <v>255</v>
+      </c>
+      <c r="AN157">
+        <v>0.04403544906999465</v>
+      </c>
+      <c r="AO157">
+        <v>0.06422505169703836</v>
+      </c>
+      <c r="AP157">
+        <v>-475.1671358</v>
+      </c>
+      <c r="AQ157">
+        <v>-4293.52220734</v>
+      </c>
+      <c r="AR157">
+        <v>22449.04526419995</v>
+      </c>
+      <c r="AS157">
+        <v>50075.07869266006</v>
+      </c>
+      <c r="AT157">
+        <v>22437.64966419995</v>
+      </c>
+      <c r="AU157">
+        <v>50075.07869266006</v>
+      </c>
+      <c r="AV157">
+        <v>1.244904526419996</v>
+      </c>
+      <c r="AW157">
+        <v>4.007507869266006</v>
+      </c>
+      <c r="AX157">
+        <v>2.946900900900901</v>
+      </c>
+      <c r="AY157">
+        <v>1.318146123581011</v>
+      </c>
+      <c r="AZ157">
+        <v>53.88333333333333</v>
+      </c>
+      <c r="BA157">
+        <v>44.78333333333333</v>
+      </c>
+      <c r="BB157">
+        <v>0.09738777154284545</v>
+      </c>
+      <c r="BC157">
+        <v>0.07277139019506668</v>
+      </c>
+      <c r="BD157">
+        <v>-1394.463984532814</v>
+      </c>
+      <c r="BE157">
+        <v>-3482.166894291953</v>
+      </c>
+      <c r="BF157">
+        <v>3178</v>
+      </c>
+      <c r="BG157">
+        <v>8363</v>
+      </c>
+      <c r="BH157">
+        <v>1135.852777777778</v>
+      </c>
+      <c r="BI157">
+        <v>6073</v>
+      </c>
+      <c r="BJ157">
+        <v>12310</v>
+      </c>
+      <c r="BK157">
+        <v>9251</v>
+      </c>
+      <c r="BL157">
+        <v>20673</v>
+      </c>
+      <c r="BM157">
+        <v>0</v>
+      </c>
+      <c r="BN157">
+        <v>0</v>
+      </c>
+      <c r="BO157">
+        <v>679</v>
+      </c>
+      <c r="BP157">
+        <v>7117</v>
+      </c>
+      <c r="BQ157">
+        <v>0</v>
+      </c>
+      <c r="BR157">
+        <v>0</v>
+      </c>
+      <c r="BS157">
+        <v>2499</v>
+      </c>
+      <c r="BT157">
+        <v>1246</v>
+      </c>
+      <c r="BU157">
+        <v>6073</v>
+      </c>
+      <c r="BV157">
+        <v>12310</v>
+      </c>
+      <c r="BW157">
+        <v>12449.04526419996</v>
+      </c>
+      <c r="BX157">
+        <v>40075.07869266005</v>
+      </c>
+      <c r="BY157">
+        <v>0.1001641043097407</v>
+      </c>
+      <c r="BZ157">
+        <v>0.08426660435854483</v>
+      </c>
+      <c r="CA157">
+        <v>0.2379864066748622</v>
+      </c>
+      <c r="CB157">
+        <v>0.1991647686635447</v>
+      </c>
+      <c r="CC157">
+        <v>0.01381080593744643</v>
+      </c>
+      <c r="CD157">
+        <v>0.009861563561261064</v>
+      </c>
+      <c r="CE157">
+        <v>0.01682855502295572</v>
+      </c>
+      <c r="CF157">
+        <v>0.01383126156290702</v>
+      </c>
+      <c r="CG157">
+        <v>12924.21239999996</v>
+      </c>
+      <c r="CH157">
+        <v>44368.60090000005</v>
+      </c>
+      <c r="CI157">
+        <v>14318.67638453278</v>
+      </c>
+      <c r="CJ157">
+        <v>47850.76779429201</v>
+      </c>
+      <c r="CK157">
+        <v>0.0910179440555702</v>
+      </c>
+      <c r="CL157">
+        <v>0.08716385368009834</v>
+      </c>
+      <c r="CM157">
+        <v>10000</v>
+      </c>
+      <c r="CO157">
+        <v>0.01558946518964126</v>
+      </c>
+      <c r="CP157">
+        <v>0.03110556819015479</v>
+      </c>
+      <c r="CQ157">
+        <v>16515088.19310524</v>
+      </c>
+      <c r="CR157">
+        <v>37368208.24219142</v>
+      </c>
+      <c r="CS157" s="2">
+        <v>45575.64733318567</v>
+      </c>
+      <c r="CT157">
+        <v>-0.7950022733063697</v>
+      </c>
+      <c r="CU157">
+        <v>-0.5515515516980466</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update PYTHUSDT.json at 2024-10-10_20-04-01 bestfile_scores 0.002321286492412078 bestfile_sharp 0.15654775440882573
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="400">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -779,6 +779,9 @@
   </si>
   <si>
     <t>ATAUSDT</t>
+  </si>
+  <si>
+    <t>SUIUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1572,7 +1575,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU157"/>
+  <dimension ref="A1:CU158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1990,7 +1993,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2155,7 +2158,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2271,7 +2274,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2436,7 +2439,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2552,7 +2555,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2717,7 +2720,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2833,7 +2836,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -2998,7 +3001,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3114,7 +3117,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3279,7 +3282,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3395,7 +3398,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3560,7 +3563,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3676,7 +3679,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3841,7 +3844,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3957,7 +3960,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4122,7 +4125,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4238,7 +4241,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4403,7 +4406,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4519,7 +4522,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4684,7 +4687,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4800,7 +4803,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4965,7 +4968,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5081,7 +5084,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5246,7 +5249,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5362,7 +5365,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5527,7 +5530,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5643,7 +5646,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5808,7 +5811,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5924,7 +5927,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6089,7 +6092,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6205,7 +6208,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6370,7 +6373,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6486,7 +6489,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6651,7 +6654,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6767,7 +6770,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6932,7 +6935,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7048,7 +7051,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7213,7 +7216,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7329,7 +7332,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7494,7 +7497,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7610,7 +7613,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7775,7 +7778,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7891,7 +7894,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8056,7 +8059,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8172,7 +8175,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8337,7 +8340,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8453,7 +8456,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8618,7 +8621,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8734,7 +8737,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8899,7 +8902,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -9015,7 +9018,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9180,7 +9183,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9296,7 +9299,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9461,7 +9464,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9577,7 +9580,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9742,7 +9745,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9858,7 +9861,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10023,7 +10026,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10139,7 +10142,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10304,7 +10307,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10420,7 +10423,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10585,7 +10588,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10701,7 +10704,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10866,7 +10869,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10982,7 +10985,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11147,7 +11150,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11269,7 +11272,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11434,7 +11437,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11556,7 +11559,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11721,7 +11724,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11843,7 +11846,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -12008,7 +12011,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12130,7 +12133,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12295,7 +12298,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12417,7 +12420,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12582,7 +12585,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12704,7 +12707,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12869,7 +12872,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12991,7 +12994,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13156,7 +13159,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13278,7 +13281,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13443,7 +13446,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13565,7 +13568,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13730,7 +13733,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13852,7 +13855,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -14017,7 +14020,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14139,7 +14142,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14304,7 +14307,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14426,7 +14429,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14591,7 +14594,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14713,7 +14716,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14878,7 +14881,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -15000,7 +15003,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15165,7 +15168,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15287,7 +15290,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15452,7 +15455,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15574,7 +15577,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15739,7 +15742,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15861,7 +15864,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16026,7 +16029,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16148,7 +16151,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16313,7 +16316,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16435,7 +16438,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16600,7 +16603,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16722,7 +16725,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16887,7 +16890,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -17006,7 +17009,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17171,7 +17174,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17287,7 +17290,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17452,7 +17455,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17565,7 +17568,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17730,7 +17733,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17843,7 +17846,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -18008,7 +18011,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18121,7 +18124,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18286,7 +18289,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18399,7 +18402,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18564,7 +18567,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18677,7 +18680,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18842,7 +18845,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18955,7 +18958,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19120,7 +19123,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19233,7 +19236,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19398,7 +19401,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19511,7 +19514,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19676,7 +19679,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19789,7 +19792,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19954,7 +19957,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20067,7 +20070,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20238,7 +20241,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20351,7 +20354,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20522,7 +20525,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20635,7 +20638,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20806,7 +20809,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20919,7 +20922,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21090,7 +21093,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21200,7 +21203,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21371,7 +21374,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21478,7 +21481,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21649,7 +21652,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21753,7 +21756,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21924,7 +21927,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22028,7 +22031,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22199,7 +22202,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22303,7 +22306,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22474,7 +22477,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22578,7 +22581,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22749,7 +22752,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22853,7 +22856,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23024,7 +23027,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23128,7 +23131,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23299,7 +23302,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23400,7 +23403,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23571,7 +23574,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23672,7 +23675,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23843,7 +23846,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23944,7 +23947,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24115,7 +24118,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24216,7 +24219,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24387,7 +24390,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24488,7 +24491,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24659,7 +24662,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24760,7 +24763,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24931,7 +24934,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25032,7 +25035,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25203,7 +25206,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25301,7 +25304,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25472,7 +25475,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25570,7 +25573,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25741,7 +25744,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25839,7 +25842,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -26010,7 +26013,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26108,7 +26111,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26279,7 +26282,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26377,7 +26380,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26548,7 +26551,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26646,7 +26649,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26817,7 +26820,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26915,7 +26918,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27086,7 +27089,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27184,7 +27187,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27355,7 +27358,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27453,7 +27456,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27624,7 +27627,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27722,7 +27725,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27893,7 +27896,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27991,7 +27994,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28162,7 +28165,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28260,7 +28263,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28431,7 +28434,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28529,7 +28532,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28700,7 +28703,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28798,7 +28801,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28969,7 +28972,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29067,7 +29070,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN99">
         <v>0.0224095392580651</v>
@@ -29238,7 +29241,7 @@
         <v>555000.5818001842</v>
       </c>
       <c r="CS99" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT99">
         <v>-0.7930559623825889</v>
@@ -29336,7 +29339,7 @@
         <v>0.0034227206580065</v>
       </c>
       <c r="AM100" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN100">
         <v>0.0120356538583077</v>
@@ -29507,7 +29510,7 @@
         <v>8829982.660321526</v>
       </c>
       <c r="CS100" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT100">
         <v>-0.8625963918106255</v>
@@ -29605,7 +29608,7 @@
         <v>0.0024512168149686</v>
       </c>
       <c r="AM101" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN101">
         <v>0.0237148028402029</v>
@@ -29776,7 +29779,7 @@
         <v>3109464.939265249</v>
       </c>
       <c r="CS101" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="CT101">
         <v>-0.8320151516141147</v>
@@ -29874,7 +29877,7 @@
         <v>0.0013136523187938</v>
       </c>
       <c r="AM102" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN102">
         <v>0.0039597254802618</v>
@@ -30045,7 +30048,7 @@
         <v>1199182.410839436</v>
       </c>
       <c r="CS102" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="CT102">
         <v>-0.9034091343725908</v>
@@ -30143,7 +30146,7 @@
         <v>0.0026660229792492</v>
       </c>
       <c r="AM103" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN103">
         <v>0.0062754689148565</v>
@@ -30314,7 +30317,7 @@
         <v>5608278.16173986</v>
       </c>
       <c r="CS103" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="CT103">
         <v>-0.8495964311677586</v>
@@ -30412,7 +30415,7 @@
         <v>0.0095889911638783</v>
       </c>
       <c r="AM104" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN104">
         <v>0.0276610340172863</v>
@@ -30583,7 +30586,7 @@
         <v>16198187.75410762</v>
       </c>
       <c r="CS104" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="CT104">
         <v>-0.8581350323980486</v>
@@ -30681,7 +30684,7 @@
         <v>0.0090102837599302</v>
       </c>
       <c r="AM105" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN105">
         <v>0.0216087690726687</v>
@@ -30852,7 +30855,7 @@
         <v>10577375.81046865</v>
       </c>
       <c r="CS105" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="CT105">
         <v>-0.8842562871250494</v>
@@ -30950,7 +30953,7 @@
         <v>0.0050995967216395</v>
       </c>
       <c r="AM106" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN106">
         <v>0.0064663828879011</v>
@@ -31121,7 +31124,7 @@
         <v>8161103.390277231</v>
       </c>
       <c r="CS106" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="CT106">
         <v>-0.8751724322696175</v>
@@ -31219,7 +31222,7 @@
         <v>0.008368149950938699</v>
       </c>
       <c r="AM107" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN107">
         <v>0.0044562593205472</v>
@@ -31390,7 +31393,7 @@
         <v>8562542.046147738</v>
       </c>
       <c r="CS107" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="CT107">
         <v>-0.9169005340500024</v>
@@ -31488,7 +31491,7 @@
         <v>0.0065618399294816</v>
       </c>
       <c r="AM108" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN108">
         <v>0.0115970759513037</v>
@@ -31659,7 +31662,7 @@
         <v>5094802.189709073</v>
       </c>
       <c r="CS108" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="CT108">
         <v>-0.807087633056609</v>
@@ -31757,7 +31760,7 @@
         <v>0.0039283848188842</v>
       </c>
       <c r="AM109" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN109">
         <v>0.0506122383924143</v>
@@ -31928,7 +31931,7 @@
         <v>2688942.923710383</v>
       </c>
       <c r="CS109" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="CT109">
         <v>-0.6156032480827009</v>
@@ -32026,7 +32029,7 @@
         <v>0.0110575018573894</v>
       </c>
       <c r="AM110" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN110">
         <v>0.0182408073926103</v>
@@ -32197,7 +32200,7 @@
         <v>7113237.577421894</v>
       </c>
       <c r="CS110" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="CT110">
         <v>-0.7629790982692873</v>
@@ -32295,7 +32298,7 @@
         <v>0.0079211631943229</v>
       </c>
       <c r="AM111" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN111">
         <v>0.0160665598628607</v>
@@ -32466,7 +32469,7 @@
         <v>7296357.590261763</v>
       </c>
       <c r="CS111" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="CT111">
         <v>-0.8942723506201351</v>
@@ -32564,7 +32567,7 @@
         <v>0.0045682228774332</v>
       </c>
       <c r="AM112" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN112">
         <v>0.037886406926907</v>
@@ -32735,7 +32738,7 @@
         <v>646350.5069878154</v>
       </c>
       <c r="CS112" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="CT112">
         <v>-0.0916621825765546</v>
@@ -32833,7 +32836,7 @@
         <v>0.0103540243512939</v>
       </c>
       <c r="AM113" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN113">
         <v>0.0123420077084287</v>
@@ -33004,7 +33007,7 @@
         <v>16980708.42353759</v>
       </c>
       <c r="CS113" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="CT113">
         <v>-0.8006705745635164</v>
@@ -33102,7 +33105,7 @@
         <v>0.0064839021721033</v>
       </c>
       <c r="AM114" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN114">
         <v>0.0163921516174475</v>
@@ -33273,7 +33276,7 @@
         <v>778558.4127862654</v>
       </c>
       <c r="CS114" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="CT114">
         <v>-0.7935423347142916</v>
@@ -33371,7 +33374,7 @@
         <v>0.0115121978063762</v>
       </c>
       <c r="AM115" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN115">
         <v>0.0122833373375532</v>
@@ -33542,7 +33545,7 @@
         <v>22312718.74654885</v>
       </c>
       <c r="CS115" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="CT115">
         <v>-0.833943178203995</v>
@@ -33640,7 +33643,7 @@
         <v>0.0085575638145724</v>
       </c>
       <c r="AM116" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN116">
         <v>0.0253654749054445</v>
@@ -33811,7 +33814,7 @@
         <v>55051148.20247716</v>
       </c>
       <c r="CS116" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="CT116">
         <v>-0.7450076808546802</v>
@@ -33909,7 +33912,7 @@
         <v>0.0073550550024841</v>
       </c>
       <c r="AM117" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN117">
         <v>0.0189839179655455</v>
@@ -34080,7 +34083,7 @@
         <v>7593228.666961946</v>
       </c>
       <c r="CS117" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="CT117">
         <v>-0.5920454049159357</v>
@@ -34178,7 +34181,7 @@
         <v>0.0080994776472478</v>
       </c>
       <c r="AM118" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN118">
         <v>0.0067043103411634</v>
@@ -34349,7 +34352,7 @@
         <v>8613700.914603613</v>
       </c>
       <c r="CS118" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="CT118">
         <v>-0.9326775287918464</v>
@@ -34447,7 +34450,7 @@
         <v>0.0068550971234694</v>
       </c>
       <c r="AM119" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN119">
         <v>0.009392776226783601</v>
@@ -34618,7 +34621,7 @@
         <v>2380328.733367264</v>
       </c>
       <c r="CS119" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="CT119">
         <v>-0.955941339278515</v>
@@ -34716,7 +34719,7 @@
         <v>0.0038610240640448</v>
       </c>
       <c r="AM120" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN120">
         <v>0.0077083561528932</v>
@@ -34887,7 +34890,7 @@
         <v>872704.4135421006</v>
       </c>
       <c r="CS120" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="CT120">
         <v>-0.8980421674690441</v>
@@ -34985,7 +34988,7 @@
         <v>0.007825344507997999</v>
       </c>
       <c r="AM121" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN121">
         <v>0.0327708854210512</v>
@@ -35156,7 +35159,7 @@
         <v>10271258.08902804</v>
       </c>
       <c r="CS121" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="CT121">
         <v>-0.7644558396778582</v>
@@ -35254,7 +35257,7 @@
         <v>0.0053863780237919</v>
       </c>
       <c r="AM122" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN122">
         <v>0.0318217118436193</v>
@@ -35425,7 +35428,7 @@
         <v>4219262.028734344</v>
       </c>
       <c r="CS122" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="CT122">
         <v>-0.7390744315992817</v>
@@ -35523,7 +35526,7 @@
         <v>0.008317099460099901</v>
       </c>
       <c r="AM123" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN123">
         <v>0.0412544366764669</v>
@@ -35694,7 +35697,7 @@
         <v>7884481.26725769</v>
       </c>
       <c r="CS123" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="CT123">
         <v>-0.7831546722232047</v>
@@ -35792,7 +35795,7 @@
         <v>0.0032418393755305</v>
       </c>
       <c r="AM124" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN124">
         <v>0.0499292345312228</v>
@@ -35963,7 +35966,7 @@
         <v>4199685.074142367</v>
       </c>
       <c r="CS124" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="CT124">
         <v>-0.7053510752114568</v>
@@ -36061,7 +36064,7 @@
         <v>0.0105307693727994</v>
       </c>
       <c r="AM125" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN125">
         <v>0.0209369586410007</v>
@@ -36232,7 +36235,7 @@
         <v>14590537.25038491</v>
       </c>
       <c r="CS125" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="CT125">
         <v>-0.7252315072660098</v>
@@ -36330,7 +36333,7 @@
         <v>0.0051130877078413</v>
       </c>
       <c r="AM126" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN126">
         <v>0.0123868401976321</v>
@@ -36501,7 +36504,7 @@
         <v>716228.3326648935</v>
       </c>
       <c r="CS126" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="CT126">
         <v>-0.892232561911074</v>
@@ -36599,7 +36602,7 @@
         <v>0.0103267254619839</v>
       </c>
       <c r="AM127" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN127">
         <v>0.0276741525944277</v>
@@ -36770,7 +36773,7 @@
         <v>7960049.437302528</v>
       </c>
       <c r="CS127" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="CT127">
         <v>-0.7368411844597273</v>
@@ -36868,7 +36871,7 @@
         <v>0.001129927884937</v>
       </c>
       <c r="AM128" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN128">
         <v>0.0069498164483821</v>
@@ -37039,7 +37042,7 @@
         <v>1259981.153790825</v>
       </c>
       <c r="CS128" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="CT128">
         <v>-0.9143802706411296</v>
@@ -37137,7 +37140,7 @@
         <v>0.0097288328816258</v>
       </c>
       <c r="AM129" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN129">
         <v>0.0275626982729415</v>
@@ -37308,7 +37311,7 @@
         <v>16803825.65057263</v>
       </c>
       <c r="CS129" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="CT129">
         <v>-0.8590793790924167</v>
@@ -37406,7 +37409,7 @@
         <v>0.0115638527937927</v>
       </c>
       <c r="AM130" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN130">
         <v>0.009514899377222301</v>
@@ -37577,7 +37580,7 @@
         <v>7461415.917733567</v>
       </c>
       <c r="CS130" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="CT130">
         <v>-0.7834455371012616</v>
@@ -37675,7 +37678,7 @@
         <v>0.0066617897392062</v>
       </c>
       <c r="AM131" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN131">
         <v>0.0175240810959318</v>
@@ -37846,7 +37849,7 @@
         <v>1295517.443775632</v>
       </c>
       <c r="CS131" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CT131">
         <v>-0.7832286955751367</v>
@@ -37944,7 +37947,7 @@
         <v>0.0073511543785546</v>
       </c>
       <c r="AM132" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN132">
         <v>0.0171480510071521</v>
@@ -38115,7 +38118,7 @@
         <v>7436893.530962305</v>
       </c>
       <c r="CS132" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="CT132">
         <v>-0.8091587172086132</v>
@@ -38213,7 +38216,7 @@
         <v>0.0033730418087468</v>
       </c>
       <c r="AM133" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN133">
         <v>0.009616489085314</v>
@@ -38384,7 +38387,7 @@
         <v>867003.1587181734</v>
       </c>
       <c r="CS133" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="CT133">
         <v>-0.9000180936758766</v>
@@ -38482,7 +38485,7 @@
         <v>0.0074087938346481</v>
       </c>
       <c r="AM134" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN134">
         <v>0.0409391807131387</v>
@@ -38653,7 +38656,7 @@
         <v>3390202.150984915</v>
       </c>
       <c r="CS134" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="CT134">
         <v>-0.6893066803315582</v>
@@ -38751,7 +38754,7 @@
         <v>0.0083849241650579</v>
       </c>
       <c r="AM135" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN135">
         <v>0.0422126511911422</v>
@@ -38922,7 +38925,7 @@
         <v>8715912.703511165</v>
       </c>
       <c r="CS135" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="CT135">
         <v>-0.8034449984146571</v>
@@ -39020,7 +39023,7 @@
         <v>0.008401051909799701</v>
       </c>
       <c r="AM136" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN136">
         <v>0.020710590359547</v>
@@ -39191,7 +39194,7 @@
         <v>15549669.36335931</v>
       </c>
       <c r="CS136" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="CT136">
         <v>-0.8182238609422743</v>
@@ -39289,7 +39292,7 @@
         <v>0.0077330551594838</v>
       </c>
       <c r="AM137" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN137">
         <v>0.0190728510027463</v>
@@ -39460,7 +39463,7 @@
         <v>8185952.559251163</v>
       </c>
       <c r="CS137" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="CT137">
         <v>-0.8729982178980289</v>
@@ -39558,7 +39561,7 @@
         <v>0.010898810531027</v>
       </c>
       <c r="AM138" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN138">
         <v>0.035028448432581</v>
@@ -39729,7 +39732,7 @@
         <v>1792741.222718281</v>
       </c>
       <c r="CS138" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="CT138">
         <v>-0.7176955593761354</v>
@@ -39827,7 +39830,7 @@
         <v>0.0049947080562063</v>
       </c>
       <c r="AM139" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN139">
         <v>0.0090224491293264</v>
@@ -39998,7 +40001,7 @@
         <v>4157882.239708048</v>
       </c>
       <c r="CS139" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="CT139">
         <v>-0.8723102032515645</v>
@@ -40096,7 +40099,7 @@
         <v>0.006652001977027</v>
       </c>
       <c r="AM140" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN140">
         <v>0.0486790527459496</v>
@@ -40267,7 +40270,7 @@
         <v>7172478.294001529</v>
       </c>
       <c r="CS140" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="CT140">
         <v>-0.5365809810110987</v>
@@ -40365,7 +40368,7 @@
         <v>0.009892196288343501</v>
       </c>
       <c r="AM141" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN141">
         <v>0.0262045792935156</v>
@@ -40536,7 +40539,7 @@
         <v>10598803.27492217</v>
       </c>
       <c r="CS141" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="CT141">
         <v>-0.8043091815774359</v>
@@ -40634,7 +40637,7 @@
         <v>0.0032840087191214</v>
       </c>
       <c r="AM142" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN142">
         <v>0.011024599092909</v>
@@ -40805,7 +40808,7 @@
         <v>1954441.87495541</v>
       </c>
       <c r="CS142" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="CT142">
         <v>-0.892071333585829</v>
@@ -40903,7 +40906,7 @@
         <v>0.0042924384175561</v>
       </c>
       <c r="AM143" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN143">
         <v>0.0289399933126468</v>
@@ -41074,7 +41077,7 @@
         <v>2325567.261086872</v>
       </c>
       <c r="CS143" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="CT143">
         <v>-0.7586823863673019</v>
@@ -41172,7 +41175,7 @@
         <v>0.0066499576490462</v>
       </c>
       <c r="AM144" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN144">
         <v>0.0173750820094196</v>
@@ -41343,7 +41346,7 @@
         <v>17826610.98082536</v>
       </c>
       <c r="CS144" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="CT144">
         <v>-0.9111405881388872</v>
@@ -41441,7 +41444,7 @@
         <v>0.0095523432691301</v>
       </c>
       <c r="AM145" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN145">
         <v>0.0220904013262179</v>
@@ -41612,7 +41615,7 @@
         <v>2190979.247087742</v>
       </c>
       <c r="CS145" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="CT145">
         <v>-0.6948709396994353</v>
@@ -41710,7 +41713,7 @@
         <v>0.006328270379966137</v>
       </c>
       <c r="AM146" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN146">
         <v>0.08370784758312214</v>
@@ -41979,7 +41982,7 @@
         <v>0.0110592804278049</v>
       </c>
       <c r="AM147" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN147">
         <v>0.07581655721931389</v>
@@ -42248,7 +42251,7 @@
         <v>0.01450048649474174</v>
       </c>
       <c r="AM148" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN148">
         <v>0.09614621483891075</v>
@@ -42517,7 +42520,7 @@
         <v>0.01189559910110707</v>
       </c>
       <c r="AM149" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN149">
         <v>0.01288397198120313</v>
@@ -42786,7 +42789,7 @@
         <v>0.0145803412240497</v>
       </c>
       <c r="AM150" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN150">
         <v>0.1052173371212367</v>
@@ -43055,7 +43058,7 @@
         <v>0.01019614862437938</v>
       </c>
       <c r="AM151" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN151">
         <v>0.07035209557900164</v>
@@ -43324,7 +43327,7 @@
         <v>0.01085520881764603</v>
       </c>
       <c r="AM152" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN152">
         <v>0.0930850934199607</v>
@@ -43593,7 +43596,7 @@
         <v>0.01194275707748435</v>
       </c>
       <c r="AM153" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN153">
         <v>0.0823051935622205</v>
@@ -43862,7 +43865,7 @@
         <v>0.01004172771237574</v>
       </c>
       <c r="AM154" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN154">
         <v>0.2004871827431348</v>
@@ -44131,7 +44134,7 @@
         <v>0.01933638311795493</v>
       </c>
       <c r="AM155" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN155">
         <v>0.1986348331383821</v>
@@ -44400,7 +44403,7 @@
         <v>0.01041289954961886</v>
       </c>
       <c r="AM156" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN156">
         <v>0.05962444025709573</v>
@@ -44669,7 +44672,7 @@
         <v>0.01103085386133413</v>
       </c>
       <c r="AM157" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN157">
         <v>0.04403544906999465</v>
@@ -44847,6 +44850,275 @@
       </c>
       <c r="CU157">
         <v>-0.5515515516980466</v>
+      </c>
+    </row>
+    <row r="158" spans="10:99">
+      <c r="J158" t="s">
+        <v>255</v>
+      </c>
+      <c r="K158">
+        <v>0.001724518098812799</v>
+      </c>
+      <c r="L158">
+        <v>0.001724518098812799</v>
+      </c>
+      <c r="M158">
+        <v>0.0001973708250251338</v>
+      </c>
+      <c r="N158">
+        <v>0.0001973708250251338</v>
+      </c>
+      <c r="O158">
+        <v>0.0020060252214682</v>
+      </c>
+      <c r="P158">
+        <v>0.0020060252214682</v>
+      </c>
+      <c r="Q158">
+        <v>0.00024597531689593</v>
+      </c>
+      <c r="R158">
+        <v>0.00024597531689593</v>
+      </c>
+      <c r="S158">
+        <v>10.78365795171836</v>
+      </c>
+      <c r="T158">
+        <v>3.84709138930676</v>
+      </c>
+      <c r="U158">
+        <v>0.9999784562024322</v>
+      </c>
+      <c r="V158">
+        <v>0.749570714780907</v>
+      </c>
+      <c r="W158">
+        <v>0.08404572731866602</v>
+      </c>
+      <c r="X158">
+        <v>0.03620840104408841</v>
+      </c>
+      <c r="Y158">
+        <v>0.2488446543080361</v>
+      </c>
+      <c r="Z158">
+        <v>0.1421672703276896</v>
+      </c>
+      <c r="AA158">
+        <v>0.9983373168544249</v>
+      </c>
+      <c r="AB158">
+        <v>0.8131951363428638</v>
+      </c>
+      <c r="AC158">
+        <v>0.9115979589664676</v>
+      </c>
+      <c r="AD158">
+        <v>0.9994176718502534</v>
+      </c>
+      <c r="AE158">
+        <v>0.7526907898139052</v>
+      </c>
+      <c r="AF158">
+        <v>0.8568656411905372</v>
+      </c>
+      <c r="AG158">
+        <v>0.009238942098331523</v>
+      </c>
+      <c r="AH158">
+        <v>0.004159002956563398</v>
+      </c>
+      <c r="AI158">
+        <v>0.9983373168544249</v>
+      </c>
+      <c r="AJ158">
+        <v>0.9994176718502534</v>
+      </c>
+      <c r="AK158">
+        <v>0.009238942098331523</v>
+      </c>
+      <c r="AL158">
+        <v>0.004159002956563398</v>
+      </c>
+      <c r="AM158" t="s">
+        <v>256</v>
+      </c>
+      <c r="AN158">
+        <v>0.07894730968642516</v>
+      </c>
+      <c r="AO158">
+        <v>0.01755229812691581</v>
+      </c>
+      <c r="AP158">
+        <v>-549.61676449</v>
+      </c>
+      <c r="AQ158">
+        <v>-59.450106714</v>
+      </c>
+      <c r="AR158">
+        <v>24723.37808550992</v>
+      </c>
+      <c r="AS158">
+        <v>11092.39858328597</v>
+      </c>
+      <c r="AT158">
+        <v>24694.11986550992</v>
+      </c>
+      <c r="AU158">
+        <v>11092.39858328597</v>
+      </c>
+      <c r="AV158">
+        <v>1.472337808550992</v>
+      </c>
+      <c r="AW158">
+        <v>0.1092398583285972</v>
+      </c>
+      <c r="AX158">
+        <v>2.225350164783428</v>
+      </c>
+      <c r="AY158">
+        <v>6.239306930693069</v>
+      </c>
+      <c r="AZ158">
+        <v>22.11666666666667</v>
+      </c>
+      <c r="BA158">
+        <v>91.95</v>
+      </c>
+      <c r="BB158">
+        <v>0.1030875138775118</v>
+      </c>
+      <c r="BC158">
+        <v>0.3396008749077266</v>
+      </c>
+      <c r="BD158">
+        <v>-1755.41660185509</v>
+      </c>
+      <c r="BE158">
+        <v>-592.3218369356009</v>
+      </c>
+      <c r="BF158">
+        <v>2561</v>
+      </c>
+      <c r="BG158">
+        <v>873</v>
+      </c>
+      <c r="BH158">
+        <v>525.3319444444445</v>
+      </c>
+      <c r="BI158">
+        <v>3104</v>
+      </c>
+      <c r="BJ158">
+        <v>1148</v>
+      </c>
+      <c r="BK158">
+        <v>5665</v>
+      </c>
+      <c r="BL158">
+        <v>2021</v>
+      </c>
+      <c r="BM158">
+        <v>0</v>
+      </c>
+      <c r="BN158">
+        <v>0</v>
+      </c>
+      <c r="BO158">
+        <v>92</v>
+      </c>
+      <c r="BP158">
+        <v>82</v>
+      </c>
+      <c r="BQ158">
+        <v>0</v>
+      </c>
+      <c r="BR158">
+        <v>0</v>
+      </c>
+      <c r="BS158">
+        <v>2469</v>
+      </c>
+      <c r="BT158">
+        <v>791</v>
+      </c>
+      <c r="BU158">
+        <v>3104</v>
+      </c>
+      <c r="BV158">
+        <v>1148</v>
+      </c>
+      <c r="BW158">
+        <v>14723.37808550998</v>
+      </c>
+      <c r="BX158">
+        <v>1092.398583286001</v>
+      </c>
+      <c r="BY158">
+        <v>0.09126729217002677</v>
+      </c>
+      <c r="BZ158">
+        <v>0.07211257369875604</v>
+      </c>
+      <c r="CA158">
+        <v>0.3285625216301712</v>
+      </c>
+      <c r="CB158">
+        <v>0.125211373271365</v>
+      </c>
+      <c r="CC158">
+        <v>0.01276532170544471</v>
+      </c>
+      <c r="CD158">
+        <v>0.0177856514147382</v>
+      </c>
+      <c r="CE158">
+        <v>0.01333489961129836</v>
+      </c>
+      <c r="CF158">
+        <v>0.01688639043027366</v>
+      </c>
+      <c r="CG158">
+        <v>15272.99484999998</v>
+      </c>
+      <c r="CH158">
+        <v>1151.848690000001</v>
+      </c>
+      <c r="CI158">
+        <v>17028.41145185507</v>
+      </c>
+      <c r="CJ158">
+        <v>1744.170526935602</v>
+      </c>
+      <c r="CK158">
+        <v>0.1506333326352911</v>
+      </c>
+      <c r="CL158">
+        <v>0.04333671196351721</v>
+      </c>
+      <c r="CM158">
+        <v>10000</v>
+      </c>
+      <c r="CO158">
+        <v>0.01530652708382901</v>
+      </c>
+      <c r="CP158">
+        <v>0.004124038385280355</v>
+      </c>
+      <c r="CQ158">
+        <v>8132538.948110002</v>
+      </c>
+      <c r="CR158">
+        <v>820713.9936883538</v>
+      </c>
+      <c r="CS158" s="2">
+        <v>45575.76629518008</v>
+      </c>
+      <c r="CT158">
+        <v>-0.6480148948828777</v>
+      </c>
+      <c r="CU158">
+        <v>-0.9365000460677725</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update ACHUSDT.json at 2024-10-11_02-54-02 bestfile_scores 0.0019887616169667497 bestfile_sharp 0.11810502922636139
</commit_message>
<xml_diff>
--- a/optimized/logs/analysis_clock.xlsx
+++ b/optimized/logs/analysis_clock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="402">
   <si>
     <t>Unnamed: 0.8</t>
   </si>
@@ -785,6 +785,9 @@
   </si>
   <si>
     <t>PYTHUSDT</t>
+  </si>
+  <si>
+    <t>ICXUSDT</t>
   </si>
   <si>
     <t>binance</t>
@@ -1578,7 +1581,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU159"/>
+  <dimension ref="A1:CU160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1996,7 +1999,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN2">
         <v>0.049606857</v>
@@ -2161,7 +2164,7 @@
         <v>0</v>
       </c>
       <c r="CS2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:99">
@@ -2277,7 +2280,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN3">
         <v>0.04006526</v>
@@ -2442,7 +2445,7 @@
         <v>0</v>
       </c>
       <c r="CS3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -2558,7 +2561,7 @@
         <v>0</v>
       </c>
       <c r="AM4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN4">
         <v>0.092575794</v>
@@ -2723,7 +2726,7 @@
         <v>0</v>
       </c>
       <c r="CS4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -2839,7 +2842,7 @@
         <v>0</v>
       </c>
       <c r="AM5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN5">
         <v>0.027448502</v>
@@ -3004,7 +3007,7 @@
         <v>0</v>
       </c>
       <c r="CS5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:99">
@@ -3120,7 +3123,7 @@
         <v>0</v>
       </c>
       <c r="AM6" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN6">
         <v>0.083929868</v>
@@ -3285,7 +3288,7 @@
         <v>0</v>
       </c>
       <c r="CS6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:99">
@@ -3401,7 +3404,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN7">
         <v>0.145376251</v>
@@ -3566,7 +3569,7 @@
         <v>0</v>
       </c>
       <c r="CS7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:99">
@@ -3682,7 +3685,7 @@
         <v>0</v>
       </c>
       <c r="AM8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN8">
         <v>0.087987204</v>
@@ -3847,7 +3850,7 @@
         <v>0</v>
       </c>
       <c r="CS8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:99">
@@ -3963,7 +3966,7 @@
         <v>0</v>
       </c>
       <c r="AM9" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN9">
         <v>0.118237951</v>
@@ -4128,7 +4131,7 @@
         <v>0</v>
       </c>
       <c r="CS9" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:99">
@@ -4244,7 +4247,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN10">
         <v>0.08106915200000001</v>
@@ -4409,7 +4412,7 @@
         <v>0</v>
       </c>
       <c r="CS10" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:99">
@@ -4525,7 +4528,7 @@
         <v>0</v>
       </c>
       <c r="AM11" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN11">
         <v>0.027960571</v>
@@ -4690,7 +4693,7 @@
         <v>0</v>
       </c>
       <c r="CS11" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:99">
@@ -4806,7 +4809,7 @@
         <v>0</v>
       </c>
       <c r="AM12" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN12">
         <v>0.032951036</v>
@@ -4971,7 +4974,7 @@
         <v>0</v>
       </c>
       <c r="CS12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:99">
@@ -5087,7 +5090,7 @@
         <v>0</v>
       </c>
       <c r="AM13" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN13">
         <v>0.179185242</v>
@@ -5252,7 +5255,7 @@
         <v>0</v>
       </c>
       <c r="CS13" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="14" spans="1:99">
@@ -5368,7 +5371,7 @@
         <v>0</v>
       </c>
       <c r="AM14" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN14">
         <v>0.143233482</v>
@@ -5533,7 +5536,7 @@
         <v>0</v>
       </c>
       <c r="CS14" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:99">
@@ -5649,7 +5652,7 @@
         <v>0</v>
       </c>
       <c r="AM15" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN15">
         <v>0.138115134</v>
@@ -5814,7 +5817,7 @@
         <v>0</v>
       </c>
       <c r="CS15" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="16" spans="1:99">
@@ -5930,7 +5933,7 @@
         <v>0</v>
       </c>
       <c r="AM16" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN16">
         <v>0.09650975000000001</v>
@@ -6095,7 +6098,7 @@
         <v>0</v>
       </c>
       <c r="CS16" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:97">
@@ -6211,7 +6214,7 @@
         <v>0</v>
       </c>
       <c r="AM17" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN17">
         <v>0.060693695</v>
@@ -6376,7 +6379,7 @@
         <v>0</v>
       </c>
       <c r="CS17" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="18" spans="1:97">
@@ -6492,7 +6495,7 @@
         <v>0</v>
       </c>
       <c r="AM18" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN18">
         <v>0.107514363</v>
@@ -6657,7 +6660,7 @@
         <v>0</v>
       </c>
       <c r="CS18" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19" spans="1:97">
@@ -6773,7 +6776,7 @@
         <v>0</v>
       </c>
       <c r="AM19" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN19">
         <v>0.014898256</v>
@@ -6938,7 +6941,7 @@
         <v>0</v>
       </c>
       <c r="CS19" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20" spans="1:97">
@@ -7054,7 +7057,7 @@
         <v>0</v>
       </c>
       <c r="AM20" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN20">
         <v>0.02858403</v>
@@ -7219,7 +7222,7 @@
         <v>0</v>
       </c>
       <c r="CS20" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21" spans="1:97">
@@ -7335,7 +7338,7 @@
         <v>0</v>
       </c>
       <c r="AM21" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN21">
         <v>0.082273481</v>
@@ -7500,7 +7503,7 @@
         <v>0</v>
       </c>
       <c r="CS21" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="22" spans="1:97">
@@ -7616,7 +7619,7 @@
         <v>0</v>
       </c>
       <c r="AM22" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN22">
         <v>0.012592558</v>
@@ -7781,7 +7784,7 @@
         <v>0</v>
       </c>
       <c r="CS22" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23" spans="1:97">
@@ -7897,7 +7900,7 @@
         <v>0</v>
       </c>
       <c r="AM23" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN23">
         <v>0.00903967</v>
@@ -8062,7 +8065,7 @@
         <v>0</v>
       </c>
       <c r="CS23" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:97">
@@ -8178,7 +8181,7 @@
         <v>0</v>
       </c>
       <c r="AM24" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN24">
         <v>0.030046089</v>
@@ -8343,7 +8346,7 @@
         <v>0</v>
       </c>
       <c r="CS24" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="25" spans="1:97">
@@ -8459,7 +8462,7 @@
         <v>0</v>
       </c>
       <c r="AM25" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN25">
         <v>0.010607012</v>
@@ -8624,7 +8627,7 @@
         <v>0</v>
       </c>
       <c r="CS25" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="26" spans="1:97">
@@ -8740,7 +8743,7 @@
         <v>0</v>
       </c>
       <c r="AM26" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN26">
         <v>0.053096335</v>
@@ -8905,7 +8908,7 @@
         <v>0</v>
       </c>
       <c r="CS26" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27" spans="1:97">
@@ -9021,7 +9024,7 @@
         <v>0</v>
       </c>
       <c r="AM27" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN27">
         <v>0.092674047</v>
@@ -9186,7 +9189,7 @@
         <v>0</v>
       </c>
       <c r="CS27" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="28" spans="1:97">
@@ -9302,7 +9305,7 @@
         <v>0</v>
       </c>
       <c r="AM28" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN28">
         <v>0.03099706</v>
@@ -9467,7 +9470,7 @@
         <v>0</v>
       </c>
       <c r="CS28" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="29" spans="1:97">
@@ -9583,7 +9586,7 @@
         <v>0</v>
       </c>
       <c r="AM29" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN29">
         <v>0.069423731</v>
@@ -9748,7 +9751,7 @@
         <v>0</v>
       </c>
       <c r="CS29" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="30" spans="1:97">
@@ -9864,7 +9867,7 @@
         <v>0</v>
       </c>
       <c r="AM30" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN30">
         <v>0.060424834</v>
@@ -10029,7 +10032,7 @@
         <v>0</v>
       </c>
       <c r="CS30" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="31" spans="1:97">
@@ -10145,7 +10148,7 @@
         <v>0</v>
       </c>
       <c r="AM31" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN31">
         <v>0.056666776</v>
@@ -10310,7 +10313,7 @@
         <v>0</v>
       </c>
       <c r="CS31" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="32" spans="1:97">
@@ -10426,7 +10429,7 @@
         <v>0</v>
       </c>
       <c r="AM32" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN32">
         <v>0.098888062</v>
@@ -10591,7 +10594,7 @@
         <v>0</v>
       </c>
       <c r="CS32" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="33" spans="1:99">
@@ -10707,7 +10710,7 @@
         <v>0</v>
       </c>
       <c r="AM33" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN33">
         <v>0.035815903</v>
@@ -10872,7 +10875,7 @@
         <v>0</v>
       </c>
       <c r="CS33" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="34" spans="1:99">
@@ -10988,7 +10991,7 @@
         <v>0</v>
       </c>
       <c r="AM34" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN34">
         <v>0.037311133</v>
@@ -11153,7 +11156,7 @@
         <v>0</v>
       </c>
       <c r="CS34" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CT34">
         <v>-0.814742818</v>
@@ -11275,7 +11278,7 @@
         <v>0</v>
       </c>
       <c r="AM35" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN35">
         <v>0.041330496</v>
@@ -11440,7 +11443,7 @@
         <v>0</v>
       </c>
       <c r="CS35" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CT35">
         <v>-0.753066891</v>
@@ -11562,7 +11565,7 @@
         <v>0</v>
       </c>
       <c r="AM36" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN36">
         <v>0.047772102</v>
@@ -11727,7 +11730,7 @@
         <v>0</v>
       </c>
       <c r="CS36" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CT36">
         <v>-0.872335259</v>
@@ -11849,7 +11852,7 @@
         <v>0</v>
       </c>
       <c r="AM37" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN37">
         <v>0.060484521</v>
@@ -12014,7 +12017,7 @@
         <v>0</v>
       </c>
       <c r="CS37" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CT37">
         <v>-0.759885442</v>
@@ -12136,7 +12139,7 @@
         <v>0</v>
       </c>
       <c r="AM38" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN38">
         <v>0.061007062</v>
@@ -12301,7 +12304,7 @@
         <v>0</v>
       </c>
       <c r="CS38" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CT38">
         <v>-0.838900609</v>
@@ -12423,7 +12426,7 @@
         <v>0</v>
       </c>
       <c r="AM39" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN39">
         <v>0.025236369</v>
@@ -12588,7 +12591,7 @@
         <v>0</v>
       </c>
       <c r="CS39" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CT39">
         <v>-0.780218664</v>
@@ -12710,7 +12713,7 @@
         <v>0</v>
       </c>
       <c r="AM40" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN40">
         <v>0.031804424</v>
@@ -12875,7 +12878,7 @@
         <v>0</v>
       </c>
       <c r="CS40" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CT40">
         <v>-0.79992089</v>
@@ -12997,7 +13000,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN41">
         <v>0.072404657</v>
@@ -13162,7 +13165,7 @@
         <v>0</v>
       </c>
       <c r="CS41" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CT41">
         <v>-0.528089775</v>
@@ -13284,7 +13287,7 @@
         <v>0</v>
       </c>
       <c r="AM42" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN42">
         <v>0.06821192299999999</v>
@@ -13449,7 +13452,7 @@
         <v>0</v>
       </c>
       <c r="CS42" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CT42">
         <v>-0.754849911</v>
@@ -13571,7 +13574,7 @@
         <v>0</v>
       </c>
       <c r="AM43" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN43">
         <v>0.069326524</v>
@@ -13736,7 +13739,7 @@
         <v>0</v>
       </c>
       <c r="CS43" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CT43">
         <v>-0.7655395739999999</v>
@@ -13858,7 +13861,7 @@
         <v>0</v>
       </c>
       <c r="AM44" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN44">
         <v>0.036991009</v>
@@ -14023,7 +14026,7 @@
         <v>0</v>
       </c>
       <c r="CS44" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CT44">
         <v>-0.829764531</v>
@@ -14145,7 +14148,7 @@
         <v>0</v>
       </c>
       <c r="AM45" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN45">
         <v>0.036729519</v>
@@ -14310,7 +14313,7 @@
         <v>0</v>
       </c>
       <c r="CS45" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CT45">
         <v>-0.404237806</v>
@@ -14432,7 +14435,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN46">
         <v>0.045071814</v>
@@ -14597,7 +14600,7 @@
         <v>0</v>
       </c>
       <c r="CS46" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CT46">
         <v>-0.703677808</v>
@@ -14719,7 +14722,7 @@
         <v>0</v>
       </c>
       <c r="AM47" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN47">
         <v>0.0580535</v>
@@ -14884,7 +14887,7 @@
         <v>0</v>
       </c>
       <c r="CS47" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CT47">
         <v>-0.753715321</v>
@@ -15006,7 +15009,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN48">
         <v>0.056639031</v>
@@ -15171,7 +15174,7 @@
         <v>0</v>
       </c>
       <c r="CS48" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CT48">
         <v>-0.71793867</v>
@@ -15293,7 +15296,7 @@
         <v>0</v>
       </c>
       <c r="AM49" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN49">
         <v>0.074241638</v>
@@ -15458,7 +15461,7 @@
         <v>0</v>
       </c>
       <c r="CS49" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CT49">
         <v>-0.655169358</v>
@@ -15580,7 +15583,7 @@
         <v>0</v>
       </c>
       <c r="AM50" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN50">
         <v>0.05430774</v>
@@ -15745,7 +15748,7 @@
         <v>0</v>
       </c>
       <c r="CS50" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CT50">
         <v>-0.6872439380000001</v>
@@ -15867,7 +15870,7 @@
         <v>0</v>
       </c>
       <c r="AM51" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN51">
         <v>0.080539377</v>
@@ -16032,7 +16035,7 @@
         <v>0</v>
       </c>
       <c r="CS51" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CT51">
         <v>-0.596275172</v>
@@ -16154,7 +16157,7 @@
         <v>0</v>
       </c>
       <c r="AM52" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN52">
         <v>0.032588051</v>
@@ -16319,7 +16322,7 @@
         <v>0</v>
       </c>
       <c r="CS52" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CT52">
         <v>-0.808081961</v>
@@ -16441,7 +16444,7 @@
         <v>0</v>
       </c>
       <c r="AM53" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN53">
         <v>0.026475554</v>
@@ -16606,7 +16609,7 @@
         <v>0</v>
       </c>
       <c r="CS53" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="CT53">
         <v>-0.77227813</v>
@@ -16728,7 +16731,7 @@
         <v>0</v>
       </c>
       <c r="AM54" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN54">
         <v>0.0245106310926154</v>
@@ -16893,7 +16896,7 @@
         <v>0</v>
       </c>
       <c r="CS54" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CT54">
         <v>-0.8664117478627688</v>
@@ -17012,7 +17015,7 @@
         <v>0</v>
       </c>
       <c r="AM55" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN55">
         <v>0.0779439577559576</v>
@@ -17177,7 +17180,7 @@
         <v>0</v>
       </c>
       <c r="CS55" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CT55">
         <v>-0.7108907987632488</v>
@@ -17293,7 +17296,7 @@
         <v>0</v>
       </c>
       <c r="AM56" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN56">
         <v>0.0402740604837066</v>
@@ -17458,7 +17461,7 @@
         <v>0</v>
       </c>
       <c r="CS56" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CT56">
         <v>-0.7447372903525753</v>
@@ -17571,7 +17574,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN57">
         <v>0.0441363962743036</v>
@@ -17736,7 +17739,7 @@
         <v>0</v>
       </c>
       <c r="CS57" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CT57">
         <v>-0.7777179486581601</v>
@@ -17849,7 +17852,7 @@
         <v>0</v>
       </c>
       <c r="AM58" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN58">
         <v>0.0589646348207879</v>
@@ -18014,7 +18017,7 @@
         <v>0</v>
       </c>
       <c r="CS58" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CT58">
         <v>-0.7757098341832183</v>
@@ -18127,7 +18130,7 @@
         <v>0</v>
       </c>
       <c r="AM59" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN59">
         <v>0.0088498418945465</v>
@@ -18292,7 +18295,7 @@
         <v>0</v>
       </c>
       <c r="CS59" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CT59">
         <v>-0.9614802262041642</v>
@@ -18405,7 +18408,7 @@
         <v>0</v>
       </c>
       <c r="AM60" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN60">
         <v>0.0438527807624406</v>
@@ -18570,7 +18573,7 @@
         <v>0</v>
       </c>
       <c r="CS60" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CT60">
         <v>-0.6569921650581255</v>
@@ -18683,7 +18686,7 @@
         <v>0</v>
       </c>
       <c r="AM61" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN61">
         <v>0.0175722673111926</v>
@@ -18848,7 +18851,7 @@
         <v>0</v>
       </c>
       <c r="CS61" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="CT61">
         <v>-0.924044412704054</v>
@@ -18961,7 +18964,7 @@
         <v>0</v>
       </c>
       <c r="AM62" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN62">
         <v>0.0551224625318549</v>
@@ -19126,7 +19129,7 @@
         <v>0</v>
       </c>
       <c r="CS62" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CT62">
         <v>-0.6213262971882773</v>
@@ -19239,7 +19242,7 @@
         <v>0</v>
       </c>
       <c r="AM63" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN63">
         <v>0.0157574961492794</v>
@@ -19404,7 +19407,7 @@
         <v>0</v>
       </c>
       <c r="CS63" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CT63">
         <v>-0.9477002142299265</v>
@@ -19517,7 +19520,7 @@
         <v>0</v>
       </c>
       <c r="AM64" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN64">
         <v>0.0348775184726272</v>
@@ -19682,7 +19685,7 @@
         <v>0</v>
       </c>
       <c r="CS64" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CT64">
         <v>-0.7774025388699596</v>
@@ -19795,7 +19798,7 @@
         <v>0</v>
       </c>
       <c r="AM65" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN65">
         <v>0.0617007650932976</v>
@@ -19960,7 +19963,7 @@
         <v>0</v>
       </c>
       <c r="CS65" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CT65">
         <v>-0.8140402180385446</v>
@@ -20073,7 +20076,7 @@
         <v>0.0108330657640134</v>
       </c>
       <c r="AM66" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN66">
         <v>0.0122896465671382</v>
@@ -20244,7 +20247,7 @@
         <v>28802806.1197283</v>
       </c>
       <c r="CS66" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CT66">
         <v>-0.7661604887809055</v>
@@ -20357,7 +20360,7 @@
         <v>0.009662114019183699</v>
       </c>
       <c r="AM67" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN67">
         <v>0.0157075521173083</v>
@@ -20528,7 +20531,7 @@
         <v>12816652.38654842</v>
       </c>
       <c r="CS67" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CT67">
         <v>-0.843107865610227</v>
@@ -20641,7 +20644,7 @@
         <v>0.009682496602030599</v>
       </c>
       <c r="AM68" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN68">
         <v>0.019453807476403</v>
@@ -20812,7 +20815,7 @@
         <v>362119.31393403</v>
       </c>
       <c r="CS68" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CT68">
         <v>-0.7040504011377985</v>
@@ -20925,7 +20928,7 @@
         <v>0.009502809785555901</v>
       </c>
       <c r="AM69" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN69">
         <v>0.0467996269477206</v>
@@ -21096,7 +21099,7 @@
         <v>3444392.687119505</v>
       </c>
       <c r="CS69" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CT69">
         <v>-0.5814104972412503</v>
@@ -21206,7 +21209,7 @@
         <v>0.0100375716524098</v>
       </c>
       <c r="AM70" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN70">
         <v>0.0260012684361012</v>
@@ -21377,7 +21380,7 @@
         <v>8020410.490554446</v>
       </c>
       <c r="CS70" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CT70">
         <v>-0.1225754953154068</v>
@@ -21484,7 +21487,7 @@
         <v>0.0030270679524292</v>
       </c>
       <c r="AM71" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN71">
         <v>0.007629803458883</v>
@@ -21655,7 +21658,7 @@
         <v>6690404.196816532</v>
       </c>
       <c r="CS71" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CT71">
         <v>-0.943556327266077</v>
@@ -21759,7 +21762,7 @@
         <v>0.0071318120684325</v>
       </c>
       <c r="AM72" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN72">
         <v>0.0106438024257861</v>
@@ -21930,7 +21933,7 @@
         <v>2333580.086114224</v>
       </c>
       <c r="CS72" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CT72">
         <v>-0.9017649135974464</v>
@@ -22034,7 +22037,7 @@
         <v>0.008671749707596699</v>
       </c>
       <c r="AM73" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN73">
         <v>0.008922434565822699</v>
@@ -22205,7 +22208,7 @@
         <v>4050354.030474017</v>
       </c>
       <c r="CS73" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CT73">
         <v>-0.9011542748767548</v>
@@ -22309,7 +22312,7 @@
         <v>0.0061287699408089</v>
       </c>
       <c r="AM74" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN74">
         <v>0.0100444206462455</v>
@@ -22480,7 +22483,7 @@
         <v>284228.7150822567</v>
       </c>
       <c r="CS74" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CT74">
         <v>-0.9022640234515124</v>
@@ -22584,7 +22587,7 @@
         <v>0.009112086818146899</v>
       </c>
       <c r="AM75" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN75">
         <v>0.0105885988628848</v>
@@ -22755,7 +22758,7 @@
         <v>9238253.926865038</v>
       </c>
       <c r="CS75" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CT75">
         <v>-0.8442464713130005</v>
@@ -22859,7 +22862,7 @@
         <v>0.0120332146147572</v>
       </c>
       <c r="AM76" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN76">
         <v>0.005689041712621</v>
@@ -23030,7 +23033,7 @@
         <v>103761437.1558867</v>
       </c>
       <c r="CS76" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CT76">
         <v>-0.9172425776350784</v>
@@ -23134,7 +23137,7 @@
         <v>0.009980777925547499</v>
       </c>
       <c r="AM77" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN77">
         <v>0.0213191472253163</v>
@@ -23305,7 +23308,7 @@
         <v>11075597.03060125</v>
       </c>
       <c r="CS77" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CT77">
         <v>-0.7048134977852135</v>
@@ -23406,7 +23409,7 @@
         <v>0.008640349693688199</v>
       </c>
       <c r="AM78" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN78">
         <v>0.0310379691662141</v>
@@ -23577,7 +23580,7 @@
         <v>4941591.885046311</v>
       </c>
       <c r="CS78" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CT78">
         <v>-0.6921566954508142</v>
@@ -23678,7 +23681,7 @@
         <v>0.0052151469726826</v>
       </c>
       <c r="AM79" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN79">
         <v>0.0187749711217366</v>
@@ -23849,7 +23852,7 @@
         <v>13794144.77050867</v>
       </c>
       <c r="CS79" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CT79">
         <v>-0.6546270123512354</v>
@@ -23950,7 +23953,7 @@
         <v>0.0083235819058295</v>
       </c>
       <c r="AM80" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN80">
         <v>0.0531066176371749</v>
@@ -24121,7 +24124,7 @@
         <v>1271425.087705649</v>
       </c>
       <c r="CS80" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CT80">
         <v>-0.3384511866527668</v>
@@ -24222,7 +24225,7 @@
         <v>0.0041067346844988</v>
       </c>
       <c r="AM81" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN81">
         <v>0.0376358519870464</v>
@@ -24393,7 +24396,7 @@
         <v>8472790.733285822</v>
       </c>
       <c r="CS81" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CT81">
         <v>-0.5869016106017596</v>
@@ -24494,7 +24497,7 @@
         <v>0.0055266741344329</v>
       </c>
       <c r="AM82" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN82">
         <v>0.0047447694558675</v>
@@ -24665,7 +24668,7 @@
         <v>6299784.652790904</v>
       </c>
       <c r="CS82" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CT82">
         <v>-0.9571664073286058</v>
@@ -24766,7 +24769,7 @@
         <v>0.0083610158619657</v>
       </c>
       <c r="AM83" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN83">
         <v>0.0075895877096284</v>
@@ -24937,7 +24940,7 @@
         <v>9553962.229671104</v>
       </c>
       <c r="CS83" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CT83">
         <v>-0.7975627900619038</v>
@@ -25038,7 +25041,7 @@
         <v>0.0110102665992773</v>
       </c>
       <c r="AM84" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN84">
         <v>0.0289129415567337</v>
@@ -25209,7 +25212,7 @@
         <v>9017755.465507764</v>
       </c>
       <c r="CS84" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT84">
         <v>-0.641321453686593</v>
@@ -25307,7 +25310,7 @@
         <v>0.001235474151197</v>
       </c>
       <c r="AM85" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN85">
         <v>0.0236860634403801</v>
@@ -25478,7 +25481,7 @@
         <v>395804.1998002621</v>
       </c>
       <c r="CS85" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CT85">
         <v>-0.8468525619890503</v>
@@ -25576,7 +25579,7 @@
         <v>0.0069339646256509</v>
       </c>
       <c r="AM86" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN86">
         <v>0.0046798420774097</v>
@@ -25747,7 +25750,7 @@
         <v>5470308.140646266</v>
       </c>
       <c r="CS86" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CT86">
         <v>-0.9414869172232342</v>
@@ -25845,7 +25848,7 @@
         <v>0.0084303895709902</v>
       </c>
       <c r="AM87" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN87">
         <v>0.0220548762227611</v>
@@ -26016,7 +26019,7 @@
         <v>10570112.91971009</v>
       </c>
       <c r="CS87" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CT87">
         <v>-0.8207903291654746</v>
@@ -26114,7 +26117,7 @@
         <v>0.0046858616922062</v>
       </c>
       <c r="AM88" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN88">
         <v>0.0514935425696241</v>
@@ -26285,7 +26288,7 @@
         <v>5725644.496349121</v>
       </c>
       <c r="CS88" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CT88">
         <v>-0.561712415905279</v>
@@ -26383,7 +26386,7 @@
         <v>0.0039939215766598</v>
       </c>
       <c r="AM89" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN89">
         <v>0.012222058764571</v>
@@ -26554,7 +26557,7 @@
         <v>1429804.32644608</v>
       </c>
       <c r="CS89" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT89">
         <v>-0.9176379634509604</v>
@@ -26652,7 +26655,7 @@
         <v>0.0042088758977745</v>
       </c>
       <c r="AM90" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN90">
         <v>0.019939030911244</v>
@@ -26823,7 +26826,7 @@
         <v>4722406.067514317</v>
       </c>
       <c r="CS90" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CT90">
         <v>-0.9278452363120948</v>
@@ -26921,7 +26924,7 @@
         <v>0.0090603002679094</v>
       </c>
       <c r="AM91" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN91">
         <v>0.0130335524359802</v>
@@ -27092,7 +27095,7 @@
         <v>2899232.912138085</v>
       </c>
       <c r="CS91" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CT91">
         <v>-0.8179686291978085</v>
@@ -27190,7 +27193,7 @@
         <v>0.0034278853232647</v>
       </c>
       <c r="AM92" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN92">
         <v>0.0267226315229668</v>
@@ -27361,7 +27364,7 @@
         <v>1448171.53934798</v>
       </c>
       <c r="CS92" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CT92">
         <v>-0.8215150584575165</v>
@@ -27459,7 +27462,7 @@
         <v>0.0078801601208179</v>
       </c>
       <c r="AM93" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN93">
         <v>0.0221393128933173</v>
@@ -27630,7 +27633,7 @@
         <v>16635452.15900955</v>
       </c>
       <c r="CS93" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CT93">
         <v>-0.7542388832888753</v>
@@ -27728,7 +27731,7 @@
         <v>0.0148358454007108</v>
       </c>
       <c r="AM94" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN94">
         <v>0.0142895129437342</v>
@@ -27899,7 +27902,7 @@
         <v>118847.66881</v>
       </c>
       <c r="CS94" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CT94">
         <v>-0.8706219162560768</v>
@@ -27997,7 +28000,7 @@
         <v>0.00777307269066</v>
       </c>
       <c r="AM95" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN95">
         <v>0.028345432375321</v>
@@ -28168,7 +28171,7 @@
         <v>9989976.067409206</v>
       </c>
       <c r="CS95" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CT95">
         <v>-0.7702665229627835</v>
@@ -28266,7 +28269,7 @@
         <v>0.005069566938105</v>
       </c>
       <c r="AM96" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN96">
         <v>0.0378882038525435</v>
@@ -28437,7 +28440,7 @@
         <v>4195010.116009732</v>
       </c>
       <c r="CS96" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="CT96">
         <v>-0.6208027078099908</v>
@@ -28535,7 +28538,7 @@
         <v>0.0109181034800677</v>
       </c>
       <c r="AM97" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN97">
         <v>0.0464479162381462</v>
@@ -28706,7 +28709,7 @@
         <v>1753546.300271091</v>
       </c>
       <c r="CS97" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CT97">
         <v>-0.6637406607330143</v>
@@ -28804,7 +28807,7 @@
         <v>0.0073561352130028</v>
       </c>
       <c r="AM98" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN98">
         <v>0.0129973328606765</v>
@@ -28975,7 +28978,7 @@
         <v>8525723.260530123</v>
       </c>
       <c r="CS98" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="CT98">
         <v>-0.6066396906320848</v>
@@ -29073,7 +29076,7 @@
         <v>0.0010483764611907</v>
       </c>
       <c r="AM99" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>